<commit_message>
python: variants.py and levels.py
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t xml:space="preserve">hayashi_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hirano_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hirano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_APARTMENTS_HIRANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hirano_m</t>
   </si>
   <si>
     <t xml:space="preserve">colour</t>
@@ -277,9 +289,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -346,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,7 +376,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,7 +401,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -516,7 +533,7 @@
       <c r="L2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2" t="str">
+      <c r="M2" s="4" t="str">
         <f aca="false">VLOOKUP(L2,dropdowns!D:E,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -595,7 +612,7 @@
       <c r="L3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="2" t="str">
+      <c r="M3" s="4" t="str">
         <f aca="false">VLOOKUP(L3,dropdowns!D:E,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -674,7 +691,7 @@
       <c r="L4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="2" t="str">
+      <c r="M4" s="4" t="str">
         <f aca="false">VLOOKUP(L4,dropdowns!D:E,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -753,7 +770,7 @@
       <c r="L5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="2" t="str">
+      <c r="M5" s="4" t="str">
         <f aca="false">VLOOKUP(L5,dropdowns!D:E,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -832,7 +849,7 @@
       <c r="L6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="2" t="str">
+      <c r="M6" s="4" t="str">
         <f aca="false">VLOOKUP(L6,dropdowns!D:E,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
@@ -909,7 +926,7 @@
       <c r="L7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="2" t="str">
+      <c r="M7" s="4" t="str">
         <f aca="false">VLOOKUP(L7,dropdowns!D:E,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -949,17 +966,171 @@
         <v>none</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>1960</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="4" t="str">
+        <f aca="false">VLOOKUP(L8,dropdowns!D:E,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <f aca="false">IF(D8="1X1",A8,"none")</f>
+        <v>hirano_s</v>
+      </c>
+      <c r="T8" s="1" t="str">
+        <f aca="false">IF(D8="1X1","none",CONCATENATE(A8,"_north"))</f>
+        <v>none</v>
+      </c>
+      <c r="U8" s="1" t="str">
+        <f aca="false">IF(D8="2X2",CONCATENATE(A8,"_east"),IF(D8="1X2",CONCATENATE(A8,"_east"),"none"))</f>
+        <v>none</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <f aca="false">IF(D8="2X2",CONCATENATE(A8,"_west"),IF(D8="2X1",CONCATENATE(A8,"_west"),"none"))</f>
+        <v>none</v>
+      </c>
+      <c r="W8" s="1" t="str">
+        <f aca="false">IF(D8="2X2",CONCATENATE(A8,"_south"),"none")</f>
+        <v>none</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>1960</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="4" t="str">
+        <f aca="false">VLOOKUP(L9,dropdowns!D:E,2,0)</f>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S9" s="1" t="str">
+        <f aca="false">IF(D9="1X1",A9,"none")</f>
+        <v>hirano_m</v>
+      </c>
+      <c r="T9" s="1" t="str">
+        <f aca="false">IF(D9="1X1","none",CONCATENATE(A9,"_north"))</f>
+        <v>none</v>
+      </c>
+      <c r="U9" s="1" t="str">
+        <f aca="false">IF(D9="2X2",CONCATENATE(A9,"_east"),IF(D9="1X2",CONCATENATE(A9,"_east"),"none"))</f>
+        <v>none</v>
+      </c>
+      <c r="V9" s="1" t="str">
+        <f aca="false">IF(D9="2X2",CONCATENATE(A9,"_west"),IF(D9="2X1",CONCATENATE(A9,"_west"),"none"))</f>
+        <v>none</v>
+      </c>
+      <c r="W9" s="1" t="str">
+        <f aca="false">IF(D9="2X2",CONCATENATE(A9,"_south"),"none")</f>
+        <v>none</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E7" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E9" type="list">
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L7" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L9" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P7" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P9" type="list">
       <formula1>dropdowns!$F:$F</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -991,499 +1162,595 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="str">
+      <c r="B1" s="1" t="str">
         <f aca="false">colour_dict!A2</f>
         <v>white</v>
       </c>
-      <c r="C1" s="0" t="str">
+      <c r="C1" s="1" t="str">
         <f aca="false">colour_dict!A3</f>
         <v>grey</v>
       </c>
-      <c r="D1" s="0" t="str">
+      <c r="D1" s="1" t="str">
         <f aca="false">colour_dict!A4</f>
         <v>brown1</v>
       </c>
-      <c r="E1" s="0" t="str">
+      <c r="E1" s="1" t="str">
         <f aca="false">colour_dict!A5</f>
         <v>brown2</v>
       </c>
-      <c r="F1" s="0" t="str">
+      <c r="F1" s="1" t="str">
         <f aca="false">colour_dict!A6</f>
         <v>mauve</v>
       </c>
-      <c r="G1" s="0" t="str">
+      <c r="G1" s="1" t="str">
         <f aca="false">colour_dict!A7</f>
         <v>dark_green</v>
       </c>
-      <c r="H1" s="0" t="str">
+      <c r="H1" s="1" t="str">
         <f aca="false">colour_dict!A8</f>
         <v>peach</v>
       </c>
-      <c r="I1" s="0" t="str">
+      <c r="I1" s="1" t="str">
         <f aca="false">colour_dict!A9</f>
         <v>pink</v>
       </c>
-      <c r="J1" s="0" t="str">
+      <c r="J1" s="1" t="str">
         <f aca="false">colour_dict!A10</f>
         <v>light_blue</v>
       </c>
-      <c r="K1" s="0" t="str">
+      <c r="K1" s="1" t="str">
         <f aca="false">colour_dict!A11</f>
         <v>dark_blue</v>
       </c>
-      <c r="L1" s="0" t="str">
+      <c r="L1" s="1" t="str">
         <f aca="false">colour_dict!A12</f>
         <v>light_green</v>
       </c>
-      <c r="M1" s="0" t="str">
+      <c r="M1" s="1" t="str">
         <f aca="false">colour_dict!A13</f>
         <v>black</v>
       </c>
-      <c r="N1" s="0" t="str">
+      <c r="N1" s="1" t="str">
         <f aca="false">colour_dict!A14</f>
         <v>gold</v>
       </c>
-      <c r="O1" s="0" t="str">
+      <c r="O1" s="1" t="str">
         <f aca="false">colour_dict!A15</f>
         <v>red_brown</v>
       </c>
-      <c r="P1" s="0" t="str">
+      <c r="P1" s="1" t="str">
         <f aca="false">colour_dict!A16</f>
         <v>red</v>
       </c>
-      <c r="Q1" s="0" t="str">
+      <c r="Q1" s="1" t="str">
         <f aca="false">colour_dict!A17</f>
         <v>midgrey</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
+      <c r="A2" s="1" t="str">
         <f aca="false">IF(items!A2="","",items!A2)</f>
         <v>fukuda_m</v>
       </c>
-      <c r="B2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="4" t="b">
+      <c r="B2" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
+      <c r="A3" s="1" t="str">
         <f aca="false">IF(items!A3="","",items!A3)</f>
         <v>fukuda_l</v>
       </c>
-      <c r="B3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4" t="b">
+      <c r="B3" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
+      <c r="A4" s="1" t="str">
         <f aca="false">IF(items!A4="","",items!A4)</f>
         <v>harada_m</v>
       </c>
-      <c r="B4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4" t="b">
+      <c r="B4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
+      <c r="A5" s="1" t="str">
         <f aca="false">IF(items!A5="","",items!A5)</f>
         <v>harada_l</v>
       </c>
-      <c r="B5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="b">
+      <c r="B5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="str">
+      <c r="A6" s="1" t="str">
         <f aca="false">IF(items!A6="","",items!A6)</f>
         <v>hayashi_s</v>
       </c>
-      <c r="B6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4" t="b">
+      <c r="B6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="str">
+      <c r="A7" s="1" t="str">
         <f aca="false">IF(items!A7="","",items!A7)</f>
         <v>hayashi_m</v>
       </c>
-      <c r="B7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4" t="b">
+      <c r="B7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="str">
+      <c r="A8" s="1" t="str">
         <f aca="false">IF(items!A8="","",items!A8)</f>
-        <v/>
+        <v>hirano_s</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="str">
+      <c r="A9" s="1" t="str">
         <f aca="false">IF(items!A9="","",items!A9)</f>
-        <v/>
+        <v>hirano_m</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="str">
+      <c r="A10" s="1" t="str">
         <f aca="false">IF(items!A10="","",items!A10)</f>
         <v/>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="str">
+      <c r="A11" s="1" t="str">
         <f aca="false">IF(items!A11="","",items!A11)</f>
         <v/>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="str">
+      <c r="A12" s="1" t="str">
         <f aca="false">IF(items!A12="","",items!A12)</f>
         <v/>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="str">
+      <c r="A13" s="1" t="str">
         <f aca="false">IF(items!A13="","",items!A13)</f>
         <v/>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="str">
+      <c r="A14" s="1" t="str">
         <f aca="false">IF(items!A14="","",items!A14)</f>
         <v/>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="str">
+      <c r="A15" s="1" t="str">
         <f aca="false">IF(items!A15="","",items!A15)</f>
         <v/>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="str">
+      <c r="A16" s="1" t="str">
         <f aca="false">IF(items!A16="","",items!A16)</f>
         <v/>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="str">
+      <c r="A17" s="1" t="str">
         <f aca="false">IF(items!A17="","",items!A17)</f>
         <v/>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="str">
+      <c r="A18" s="1" t="str">
         <f aca="false">IF(items!A18="","",items!A18)</f>
         <v/>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="str">
+      <c r="A19" s="1" t="str">
         <f aca="false">IF(items!A19="","",items!A19)</f>
         <v/>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="str">
+      <c r="A20" s="1" t="str">
         <f aca="false">IF(items!A20="","",items!A20)</f>
         <v/>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="str">
+      <c r="A21" s="1" t="str">
         <f aca="false">IF(items!A21="","",items!A21)</f>
         <v/>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="str">
+      <c r="A22" s="1" t="str">
         <f aca="false">IF(items!A22="","",items!A22)</f>
         <v/>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="str">
+      <c r="A23" s="1" t="str">
         <f aca="false">IF(items!A23="","",items!A23)</f>
         <v/>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="str">
+      <c r="A24" s="1" t="str">
         <f aca="false">IF(items!A24="","",items!A24)</f>
         <v/>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="str">
+      <c r="A25" s="1" t="str">
         <f aca="false">IF(items!A25="","",items!A25)</f>
         <v/>
       </c>
@@ -1535,143 +1802,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>45</v>
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="0" t="n">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="0" t="n">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1700,1101 +1967,1101 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>65</v>
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="str">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="str">
         <f aca="false">IF(C2="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C2" s="0" t="str">
+      <c r="C2" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A2,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">MAX(IF(C2="ID not in use",0,IF(C2="1X1",1,IF(C2="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="str">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="str">
         <f aca="false">IF(C3="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C3" s="0" t="str">
+      <c r="C3" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A3,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">MAX(IF(C3="ID not in use",0,IF(C3="1X1",1,IF(C3="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="str">
+      <c r="B4" s="1" t="str">
         <f aca="false">IF(C4="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C4" s="0" t="str">
+      <c r="C4" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A4,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <f aca="false">MAX(IF(C4="ID not in use",0,IF(C4="1X1",1,IF(C4="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="str">
+      <c r="B5" s="1" t="str">
         <f aca="false">IF(C5="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C5" s="0" t="str">
+      <c r="C5" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A5,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">MAX(IF(C5="ID not in use",0,IF(C5="1X1",1,IF(C5="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="str">
+      <c r="B6" s="1" t="str">
         <f aca="false">IF(C6="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C6" s="0" t="str">
+      <c r="C6" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A6,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">MAX(IF(C6="ID not in use",0,IF(C6="1X1",1,IF(C6="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="str">
+      <c r="B7" s="1" t="str">
         <f aca="false">IF(C7="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C7" s="0" t="str">
+      <c r="C7" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A7,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <f aca="false">MAX(IF(C7="ID not in use",0,IF(C7="1X1",1,IF(C7="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="str">
+      <c r="B8" s="1" t="str">
         <f aca="false">IF(C8="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C8" s="0" t="str">
+      <c r="C8" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A8,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">MAX(IF(C8="ID not in use",0,IF(C8="1X1",1,IF(C8="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="str">
+      <c r="B9" s="1" t="str">
         <f aca="false">IF(C9="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C9" s="0" t="str">
+      <c r="C9" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A9,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <f aca="false">MAX(IF(C9="ID not in use",0,IF(C9="1X1",1,IF(C9="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="str">
+      <c r="B10" s="1" t="str">
         <f aca="false">IF(C10="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C10" s="0" t="str">
+      <c r="C10" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A10,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <f aca="false">MAX(IF(C10="ID not in use",0,IF(C10="1X1",1,IF(C10="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="str">
+      <c r="B11" s="1" t="str">
         <f aca="false">IF(C11="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C11" s="0" t="str">
+      <c r="C11" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A11,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <f aca="false">MAX(IF(C11="ID not in use",0,IF(C11="1X1",1,IF(C11="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="str">
+      <c r="B12" s="1" t="str">
         <f aca="false">IF(C12="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C12" s="0" t="str">
+      <c r="C12" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A12,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <f aca="false">MAX(IF(C12="ID not in use",0,IF(C12="1X1",1,IF(C12="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="str">
+      <c r="B13" s="1" t="str">
         <f aca="false">IF(C13="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C13" s="0" t="str">
+      <c r="C13" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A13,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <f aca="false">MAX(IF(C13="ID not in use",0,IF(C13="1X1",1,IF(C13="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="str">
+      <c r="B14" s="1" t="str">
         <f aca="false">IF(C14="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C14" s="0" t="str">
+      <c r="C14" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A14,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <f aca="false">MAX(IF(C14="ID not in use",0,IF(C14="1X1",1,IF(C14="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="0" t="str">
+      <c r="B15" s="1" t="str">
         <f aca="false">IF(C15="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C15" s="0" t="str">
+      <c r="C15" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A15,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <f aca="false">MAX(IF(C15="ID not in use",0,IF(C15="1X1",1,IF(C15="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="0" t="str">
+      <c r="B16" s="1" t="str">
         <f aca="false">IF(C16="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C16" s="0" t="str">
+      <c r="C16" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A16,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <f aca="false">MAX(IF(C16="ID not in use",0,IF(C16="1X1",1,IF(C16="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="str">
+      <c r="B17" s="1" t="str">
         <f aca="false">IF(C17="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C17" s="0" t="str">
+      <c r="C17" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A17,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <f aca="false">MAX(IF(C17="ID not in use",0,IF(C17="1X1",1,IF(C17="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="0" t="str">
+      <c r="B18" s="1" t="str">
         <f aca="false">IF(C18="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C18" s="0" t="str">
+      <c r="C18" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A18,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <f aca="false">MAX(IF(C18="ID not in use",0,IF(C18="1X1",1,IF(C18="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="0" t="str">
+      <c r="B19" s="1" t="str">
         <f aca="false">IF(C19="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C19" s="0" t="str">
+      <c r="C19" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A19,items!C:D,2,0),"ID not in use")</f>
         <v>1X1</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <f aca="false">MAX(IF(C19="ID not in use",0,IF(C19="1X1",1,IF(C19="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="str">
+      <c r="B20" s="1" t="str">
         <f aca="false">IF(C20="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C20" s="0" t="str">
+      <c r="C20" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A20,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <f aca="false">MAX(IF(C20="ID not in use",0,IF(C20="1X1",1,IF(C20="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="0" t="str">
+      <c r="B21" s="1" t="str">
         <f aca="false">IF(C21="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C21" s="0" t="str">
+      <c r="C21" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A21,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <f aca="false">MAX(IF(C21="ID not in use",0,IF(C21="1X1",1,IF(C21="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="0" t="str">
+      <c r="B22" s="1" t="str">
         <f aca="false">IF(C22="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C22" s="0" t="str">
+      <c r="C22" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A22,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <f aca="false">MAX(IF(C22="ID not in use",0,IF(C22="1X1",1,IF(C22="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="0" t="str">
+      <c r="B23" s="1" t="str">
         <f aca="false">IF(C23="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C23" s="0" t="str">
+      <c r="C23" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A23,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <f aca="false">MAX(IF(C23="ID not in use",0,IF(C23="1X1",1,IF(C23="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="0" t="str">
+      <c r="B24" s="1" t="str">
         <f aca="false">IF(C24="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C24" s="0" t="str">
+      <c r="C24" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A24,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <f aca="false">MAX(IF(C24="ID not in use",0,IF(C24="1X1",1,IF(C24="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="0" t="str">
+      <c r="B25" s="1" t="str">
         <f aca="false">IF(C25="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C25" s="0" t="str">
+      <c r="C25" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A25,items!C:D,2,0),"ID not in use")</f>
         <v>1X1</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <f aca="false">MAX(IF(C25="ID not in use",0,IF(C25="1X1",1,IF(C25="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="0" t="str">
+      <c r="B26" s="1" t="str">
         <f aca="false">IF(C26="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C26" s="0" t="str">
+      <c r="C26" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A26,items!C:D,2,0),"ID not in use")</f>
         <v>1X1</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <f aca="false">MAX(IF(C26="ID not in use",0,IF(C26="1X1",1,IF(C26="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="0" t="str">
+      <c r="B27" s="1" t="str">
         <f aca="false">IF(C27="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C27" s="0" t="str">
+      <c r="C27" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A27,items!C:D,2,0),"ID not in use")</f>
         <v>1X1</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <f aca="false">MAX(IF(C27="ID not in use",0,IF(C27="1X1",1,IF(C27="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="0" t="str">
+      <c r="B28" s="1" t="str">
         <f aca="false">IF(C28="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C28" s="0" t="str">
+      <c r="C28" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A28,items!C:D,2,0),"ID not in use")</f>
         <v>1X1</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <f aca="false">MAX(IF(C28="ID not in use",0,IF(C28="1X1",1,IF(C28="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="0" t="str">
+      <c r="B29" s="1" t="str">
         <f aca="false">IF(C29="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C29" s="0" t="str">
+      <c r="C29" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A29,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <f aca="false">MAX(IF(C29="ID not in use",0,IF(C29="1X1",1,IF(C29="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="0" t="str">
+      <c r="B30" s="1" t="str">
         <f aca="false">IF(C30="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C30" s="0" t="str">
+      <c r="C30" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A30,items!C:D,2,0),"ID not in use")</f>
         <v>1X1</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <f aca="false">MAX(IF(C30="ID not in use",0,IF(C30="1X1",1,IF(C30="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="0" t="str">
+      <c r="B31" s="1" t="str">
         <f aca="false">IF(C31="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
-      </c>
-      <c r="C31" s="0" t="str">
+        <v>Used</v>
+      </c>
+      <c r="C31" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A31,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
-      </c>
-      <c r="D31" s="0" t="n">
+        <v>1X1</v>
+      </c>
+      <c r="D31" s="1" t="n">
         <f aca="false">MAX(IF(C31="ID not in use",0,IF(C31="1X1",1,IF(C31="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="0" t="str">
+      <c r="B32" s="1" t="str">
         <f aca="false">IF(C32="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C32" s="0" t="str">
+      <c r="C32" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A32,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <f aca="false">MAX(IF(C32="ID not in use",0,IF(C32="1X1",1,IF(C32="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="0" t="str">
+      <c r="B33" s="1" t="str">
         <f aca="false">IF(C33="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C33" s="0" t="str">
+      <c r="C33" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A33,items!C:D,2,0),"ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <f aca="false">MAX(IF(C33="ID not in use",0,IF(C33="1X1",1,IF(C33="2X2",4,2)))-1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="0" t="str">
+      <c r="B34" s="1" t="str">
         <f aca="false">IF(C34="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="0" t="n">
+      <c r="C34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="1" t="n">
         <f aca="false">MAX(IF(C34="ID not in use",0,IF(C34="1X1",1,IF(C34="2X2",4,2)))-1,0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="0" t="str">
+      <c r="B35" s="1" t="str">
         <f aca="false">IF(C35="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C35" s="0" t="str">
+      <c r="C35" s="1" t="str">
         <f aca="false">IF(D34&gt;0,"Multi-tile","ID not in use")</f>
         <v>Multi-tile</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <f aca="false">IF(C35="Multi-tile",D34-1,MAX(IF(C35="ID not in use",0,IF(C35="1X1",1,IF(C35="2X2",4,2)))-1,0))</f>
         <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="0" t="str">
+      <c r="B36" s="1" t="str">
         <f aca="false">IF(C36="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C36" s="0" t="str">
+      <c r="C36" s="1" t="str">
         <f aca="false">IF(D35&gt;0,"Multi-tile","ID not in use")</f>
         <v>Multi-tile</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <f aca="false">IF(C36="Multi-tile",D35-1,MAX(IF(C36="ID not in use",0,IF(C36="1X1",1,IF(C36="2X2",4,2)))-1,0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="0" t="str">
+      <c r="B37" s="1" t="str">
         <f aca="false">IF(C37="ID not in use","ID not in use","Used")</f>
         <v>Used</v>
       </c>
-      <c r="C37" s="0" t="str">
+      <c r="C37" s="1" t="str">
         <f aca="false">IF(D36&gt;0,"Multi-tile","ID not in use")</f>
         <v>Multi-tile</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="1" t="n">
         <f aca="false">IF(C37="Multi-tile",D36-1,MAX(IF(C37="ID not in use",0,IF(C37="1X1",1,IF(C37="2X2",4,2)))-1,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="0" t="str">
+      <c r="B38" s="1" t="str">
         <f aca="false">IF(C38="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C38" s="0" t="str">
+      <c r="C38" s="1" t="str">
         <f aca="false">IF(D37&gt;0,"Multi-tile","ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="1" t="n">
         <f aca="false">IF(C38="Multi-tile",D37-1,MAX(IF(C38="ID not in use",0,IF(C38="1X1",1,IF(C38="2X2",4,2)))-1,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="0" t="str">
+      <c r="B39" s="1" t="str">
         <f aca="false">IF(C39="ID not in use","ID not in use","Used")</f>
         <v>ID not in use</v>
       </c>
-      <c r="C39" s="0" t="str">
+      <c r="C39" s="1" t="str">
         <f aca="false">IF(D38&gt;0,"Multi-tile","ID not in use")</f>
         <v>ID not in use</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="1" t="n">
         <f aca="false">IF(C39="Multi-tile",D38-1,MAX(IF(C39="ID not in use",0,IF(C39="1X1",1,IF(C39="2X2",4,2)))-1,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+      <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+      <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
+      <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+      <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+      <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
+      <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+      <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
+      <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
+      <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
+      <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
+      <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
+      <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+      <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
+      <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
+      <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
+      <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
+      <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="n">
+      <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
+      <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="n">
+      <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
+      <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="n">
+      <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
+      <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="n">
+      <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
+      <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="n">
+      <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
+      <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="n">
+      <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="n">
+      <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="n">
+      <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="n">
+      <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="n">
+      <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="n">
+      <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
+      <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
+      <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="n">
+      <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="n">
+      <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="n">
+      <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="n">
+      <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="n">
+      <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="n">
+      <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="n">
+      <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="n">
+      <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="n">
+      <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="n">
+      <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="n">
+      <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="n">
+      <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="n">
+      <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="n">
+      <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="n">
+      <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="n">
+      <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="n">
+      <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="n">
+      <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="n">
+      <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="n">
+      <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="n">
+      <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="n">
+      <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="n">
+      <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="n">
+      <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="n">
+      <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="n">
+      <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
     </row>
@@ -2829,22 +3096,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2861,7 +3128,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>29</v>
@@ -2880,11 +3147,11 @@
       <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>74</v>
+      <c r="E3" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2898,29 +3165,29 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>79</v>
+      <c r="E5" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: farm & naganuma
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="137">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">medium</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME_APARTMENTS_FUKUDA</t>
+    <t xml:space="preserve">NAME_FUKUDA</t>
   </si>
   <si>
     <t xml:space="preserve">4,3,2</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">harada</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME_APARTMENTS_HARADA</t>
+    <t xml:space="preserve">NAME_HARADA</t>
   </si>
   <si>
     <t xml:space="preserve">0xFFFF</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">small</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME_APARTMENTS_HAYASHI</t>
+    <t xml:space="preserve">NAME_HAYASHI</t>
   </si>
   <si>
     <t xml:space="preserve">4,3,2,1</t>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">hirano</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME_APARTMENTS_HIRANO</t>
+    <t xml:space="preserve">NAME_HIRANO</t>
   </si>
   <si>
     <t xml:space="preserve">hirano_m</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">hirata</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME_APARTMENTS_HIRATA</t>
+    <t xml:space="preserve">NAME_HIRATA</t>
   </si>
   <si>
     <t xml:space="preserve">hirata_m</t>
@@ -218,12 +218,42 @@
     <t xml:space="preserve">[PASS, 8],[MAIL, 4],[GOOD, 4]</t>
   </si>
   <si>
+    <t xml:space="preserve">farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2X2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_FARM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitmask(HOUSE_FLAG_NOT_SLOPED)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PASS, 1],[MAIL, 1],[FOOD, 1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naganuma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_NAGANUMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single_house</t>
+  </si>
+  <si>
     <t xml:space="preserve">hospital</t>
   </si>
   <si>
-    <t xml:space="preserve">2X2</t>
-  </si>
-  <si>
     <t xml:space="preserve">landmark</t>
   </si>
   <si>
@@ -233,9 +263,6 @@
     <t xml:space="preserve">3,2</t>
   </si>
   <si>
-    <t xml:space="preserve">bitmask(HOUSE_FLAG_NOT_SLOPED)</t>
-  </si>
-  <si>
     <t xml:space="preserve">[PASS, 8], [MAIL, 4], [GOOD, 4], [RFPR, 8]</t>
   </si>
   <si>
@@ -363,6 +390,12 @@
   </si>
   <si>
     <t xml:space="preserve">bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</t>
   </si>
   <si>
     <t xml:space="preserve">Letter</t>
@@ -408,9 +441,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -477,7 +509,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -492,10 +524,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -515,7 +543,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -656,7 +684,7 @@
       <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="4" t="str">
+      <c r="M2" s="2" t="str">
         <f aca="false">VLOOKUP(L2,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -681,11 +709,11 @@
         <v>32</v>
       </c>
       <c r="T2" s="1" t="str">
-        <f aca="false">IF(NOT(D2="1X1"),"none",IF(E2="skyscraper",CONCATENATE(A2,"_c"),A2))</f>
+        <f aca="false">IF(NOT(D2="1X1"),"none",IF(E2="skyscraper",CONCATENATE(A2,"_c"),IF(E2="landmark",CONCATENATE(A2,"_k"),IF(E2="house",CONCATENATE(A2,"_h"),A2))))</f>
         <v>fukuda_m</v>
       </c>
       <c r="U2" s="1" t="str">
-        <f aca="false">IF(D2="1X1","none",IF(E2="skyscraper",CONCATENATE(A2,"_c_north"),IF(E2="landmark",CONCATENATE(A2,"_k_north"),CONCATENATE(A2,"_north"))))</f>
+        <f aca="false">IF(D2="1X1","none",IF(E2="skyscraper",CONCATENATE(A2,"_c_north"),IF(E2="landmark",CONCATENATE(A2,"_k_north"),IF(E2="house",CONCATENATE(A2,"_h_north"),CONCATENATE(A2,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V2" s="1" t="str">
@@ -741,7 +769,7 @@
       <c r="L3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="4" t="str">
+      <c r="M3" s="2" t="str">
         <f aca="false">VLOOKUP(L3,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -766,11 +794,11 @@
         <v>32</v>
       </c>
       <c r="T3" s="1" t="str">
-        <f aca="false">IF(NOT(D3="1X1"),"none",IF(E3="skyscraper",CONCATENATE(A3,"_c"),A3))</f>
+        <f aca="false">IF(NOT(D3="1X1"),"none",IF(E3="skyscraper",CONCATENATE(A3,"_c"),IF(E3="landmark",CONCATENATE(A3,"_k"),IF(E3="house",CONCATENATE(A3,"_h"),A3))))</f>
         <v>fukuda_l</v>
       </c>
       <c r="U3" s="1" t="str">
-        <f aca="false">IF(D3="1X1","none",IF(E3="skyscraper",CONCATENATE(A3,"_c_north"),IF(E3="landmark",CONCATENATE(A3,"_k_north"),CONCATENATE(A3,"_north"))))</f>
+        <f aca="false">IF(D3="1X1","none",IF(E3="skyscraper",CONCATENATE(A3,"_c_north"),IF(E3="landmark",CONCATENATE(A3,"_k_north"),IF(E3="house",CONCATENATE(A3,"_h_north"),CONCATENATE(A3,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V3" s="1" t="str">
@@ -826,7 +854,7 @@
       <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="4" t="str">
+      <c r="M4" s="2" t="str">
         <f aca="false">VLOOKUP(L4,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -851,11 +879,11 @@
         <v>32</v>
       </c>
       <c r="T4" s="1" t="str">
-        <f aca="false">IF(NOT(D4="1X1"),"none",IF(E4="skyscraper",CONCATENATE(A4,"_c"),A4))</f>
+        <f aca="false">IF(NOT(D4="1X1"),"none",IF(E4="skyscraper",CONCATENATE(A4,"_c"),IF(E4="landmark",CONCATENATE(A4,"_k"),IF(E4="house",CONCATENATE(A4,"_h"),A4))))</f>
         <v>harada_m</v>
       </c>
       <c r="U4" s="1" t="str">
-        <f aca="false">IF(D4="1X1","none",IF(E4="skyscraper",CONCATENATE(A4,"_c_north"),IF(E4="landmark",CONCATENATE(A4,"_k_north"),CONCATENATE(A4,"_north"))))</f>
+        <f aca="false">IF(D4="1X1","none",IF(E4="skyscraper",CONCATENATE(A4,"_c_north"),IF(E4="landmark",CONCATENATE(A4,"_k_north"),IF(E4="house",CONCATENATE(A4,"_h_north"),CONCATENATE(A4,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V4" s="1" t="str">
@@ -911,7 +939,7 @@
       <c r="L5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="4" t="str">
+      <c r="M5" s="2" t="str">
         <f aca="false">VLOOKUP(L5,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -936,11 +964,11 @@
         <v>32</v>
       </c>
       <c r="T5" s="1" t="str">
-        <f aca="false">IF(NOT(D5="1X1"),"none",IF(E5="skyscraper",CONCATENATE(A5,"_c"),A5))</f>
+        <f aca="false">IF(NOT(D5="1X1"),"none",IF(E5="skyscraper",CONCATENATE(A5,"_c"),IF(E5="landmark",CONCATENATE(A5,"_k"),IF(E5="house",CONCATENATE(A5,"_h"),A5))))</f>
         <v>harada_l</v>
       </c>
       <c r="U5" s="1" t="str">
-        <f aca="false">IF(D5="1X1","none",IF(E5="skyscraper",CONCATENATE(A5,"_c_north"),IF(E5="landmark",CONCATENATE(A5,"_k_north"),CONCATENATE(A5,"_north"))))</f>
+        <f aca="false">IF(D5="1X1","none",IF(E5="skyscraper",CONCATENATE(A5,"_c_north"),IF(E5="landmark",CONCATENATE(A5,"_k_north"),IF(E5="house",CONCATENATE(A5,"_h_north"),CONCATENATE(A5,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V5" s="1" t="str">
@@ -996,7 +1024,7 @@
       <c r="L6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="4" t="str">
+      <c r="M6" s="2" t="str">
         <f aca="false">VLOOKUP(L6,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -1021,11 +1049,11 @@
         <v>32</v>
       </c>
       <c r="T6" s="1" t="str">
-        <f aca="false">IF(NOT(D6="1X1"),"none",IF(E6="skyscraper",CONCATENATE(A6,"_c"),A6))</f>
+        <f aca="false">IF(NOT(D6="1X1"),"none",IF(E6="skyscraper",CONCATENATE(A6,"_c"),IF(E6="landmark",CONCATENATE(A6,"_k"),IF(E6="house",CONCATENATE(A6,"_h"),A6))))</f>
         <v>hayashi_s</v>
       </c>
       <c r="U6" s="1" t="str">
-        <f aca="false">IF(D6="1X1","none",IF(E6="skyscraper",CONCATENATE(A6,"_c_north"),IF(E6="landmark",CONCATENATE(A6,"_k_north"),CONCATENATE(A6,"_north"))))</f>
+        <f aca="false">IF(D6="1X1","none",IF(E6="skyscraper",CONCATENATE(A6,"_c_north"),IF(E6="landmark",CONCATENATE(A6,"_k_north"),IF(E6="house",CONCATENATE(A6,"_h_north"),CONCATENATE(A6,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V6" s="1" t="str">
@@ -1081,7 +1109,7 @@
       <c r="L7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="4" t="str">
+      <c r="M7" s="2" t="str">
         <f aca="false">VLOOKUP(L7,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -1106,11 +1134,11 @@
         <v>32</v>
       </c>
       <c r="T7" s="1" t="str">
-        <f aca="false">IF(NOT(D7="1X1"),"none",IF(E7="skyscraper",CONCATENATE(A7,"_c"),A7))</f>
+        <f aca="false">IF(NOT(D7="1X1"),"none",IF(E7="skyscraper",CONCATENATE(A7,"_c"),IF(E7="landmark",CONCATENATE(A7,"_k"),IF(E7="house",CONCATENATE(A7,"_h"),A7))))</f>
         <v>hayashi_m</v>
       </c>
       <c r="U7" s="1" t="str">
-        <f aca="false">IF(D7="1X1","none",IF(E7="skyscraper",CONCATENATE(A7,"_c_north"),IF(E7="landmark",CONCATENATE(A7,"_k_north"),CONCATENATE(A7,"_north"))))</f>
+        <f aca="false">IF(D7="1X1","none",IF(E7="skyscraper",CONCATENATE(A7,"_c_north"),IF(E7="landmark",CONCATENATE(A7,"_k_north"),IF(E7="house",CONCATENATE(A7,"_h_north"),CONCATENATE(A7,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V7" s="1" t="str">
@@ -1166,7 +1194,7 @@
       <c r="L8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="4" t="str">
+      <c r="M8" s="2" t="str">
         <f aca="false">VLOOKUP(L8,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -1191,11 +1219,11 @@
         <v>32</v>
       </c>
       <c r="T8" s="1" t="str">
-        <f aca="false">IF(NOT(D8="1X1"),"none",IF(E8="skyscraper",CONCATENATE(A8,"_c"),A8))</f>
+        <f aca="false">IF(NOT(D8="1X1"),"none",IF(E8="skyscraper",CONCATENATE(A8,"_c"),IF(E8="landmark",CONCATENATE(A8,"_k"),IF(E8="house",CONCATENATE(A8,"_h"),A8))))</f>
         <v>hirano_s</v>
       </c>
       <c r="U8" s="1" t="str">
-        <f aca="false">IF(D8="1X1","none",IF(E8="skyscraper",CONCATENATE(A8,"_c_north"),IF(E8="landmark",CONCATENATE(A8,"_k_north"),CONCATENATE(A8,"_north"))))</f>
+        <f aca="false">IF(D8="1X1","none",IF(E8="skyscraper",CONCATENATE(A8,"_c_north"),IF(E8="landmark",CONCATENATE(A8,"_k_north"),IF(E8="house",CONCATENATE(A8,"_h_north"),CONCATENATE(A8,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V8" s="1" t="str">
@@ -1251,7 +1279,7 @@
       <c r="L9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="4" t="str">
+      <c r="M9" s="2" t="str">
         <f aca="false">VLOOKUP(L9,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -1276,11 +1304,11 @@
         <v>32</v>
       </c>
       <c r="T9" s="1" t="str">
-        <f aca="false">IF(NOT(D9="1X1"),"none",IF(E9="skyscraper",CONCATENATE(A9,"_c"),A9))</f>
+        <f aca="false">IF(NOT(D9="1X1"),"none",IF(E9="skyscraper",CONCATENATE(A9,"_c"),IF(E9="landmark",CONCATENATE(A9,"_k"),IF(E9="house",CONCATENATE(A9,"_h"),A9))))</f>
         <v>hirano_m</v>
       </c>
       <c r="U9" s="1" t="str">
-        <f aca="false">IF(D9="1X1","none",IF(E9="skyscraper",CONCATENATE(A9,"_c_north"),IF(E9="landmark",CONCATENATE(A9,"_k_north"),CONCATENATE(A9,"_north"))))</f>
+        <f aca="false">IF(D9="1X1","none",IF(E9="skyscraper",CONCATENATE(A9,"_c_north"),IF(E9="landmark",CONCATENATE(A9,"_k_north"),IF(E9="house",CONCATENATE(A9,"_h_north"),CONCATENATE(A9,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V9" s="1" t="str">
@@ -1336,7 +1364,7 @@
       <c r="L10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="4" t="str">
+      <c r="M10" s="2" t="str">
         <f aca="false">VLOOKUP(L10,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -1361,11 +1389,11 @@
         <v>32</v>
       </c>
       <c r="T10" s="1" t="str">
-        <f aca="false">IF(NOT(D10="1X1"),"none",IF(E10="skyscraper",CONCATENATE(A10,"_c"),A10))</f>
+        <f aca="false">IF(NOT(D10="1X1"),"none",IF(E10="skyscraper",CONCATENATE(A10,"_c"),IF(E10="landmark",CONCATENATE(A10,"_k"),IF(E10="house",CONCATENATE(A10,"_h"),A10))))</f>
         <v>hirata_s</v>
       </c>
       <c r="U10" s="1" t="str">
-        <f aca="false">IF(D10="1X1","none",IF(E10="skyscraper",CONCATENATE(A10,"_c_north"),IF(E10="landmark",CONCATENATE(A10,"_k_north"),CONCATENATE(A10,"_north"))))</f>
+        <f aca="false">IF(D10="1X1","none",IF(E10="skyscraper",CONCATENATE(A10,"_c_north"),IF(E10="landmark",CONCATENATE(A10,"_k_north"),IF(E10="house",CONCATENATE(A10,"_h_north"),CONCATENATE(A10,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V10" s="1" t="str">
@@ -1421,7 +1449,7 @@
       <c r="L11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="4" t="str">
+      <c r="M11" s="2" t="str">
         <f aca="false">VLOOKUP(L11,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -1446,11 +1474,11 @@
         <v>32</v>
       </c>
       <c r="T11" s="1" t="str">
-        <f aca="false">IF(NOT(D11="1X1"),"none",IF(E11="skyscraper",CONCATENATE(A11,"_c"),A11))</f>
+        <f aca="false">IF(NOT(D11="1X1"),"none",IF(E11="skyscraper",CONCATENATE(A11,"_c"),IF(E11="landmark",CONCATENATE(A11,"_k"),IF(E11="house",CONCATENATE(A11,"_h"),A11))))</f>
         <v>hirata_m</v>
       </c>
       <c r="U11" s="1" t="str">
-        <f aca="false">IF(D11="1X1","none",IF(E11="skyscraper",CONCATENATE(A11,"_c_north"),IF(E11="landmark",CONCATENATE(A11,"_k_north"),CONCATENATE(A11,"_north"))))</f>
+        <f aca="false">IF(D11="1X1","none",IF(E11="skyscraper",CONCATENATE(A11,"_c_north"),IF(E11="landmark",CONCATENATE(A11,"_k_north"),IF(E11="house",CONCATENATE(A11,"_h_north"),CONCATENATE(A11,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V11" s="1" t="str">
@@ -1506,7 +1534,7 @@
       <c r="L12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="4" t="str">
+      <c r="M12" s="2" t="str">
         <f aca="false">VLOOKUP(L12,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -1529,11 +1557,11 @@
         <v>32</v>
       </c>
       <c r="T12" s="1" t="str">
-        <f aca="false">IF(NOT(D12="1X1"),"none",IF(E12="skyscraper",CONCATENATE(A12,"_c"),A12))</f>
+        <f aca="false">IF(NOT(D12="1X1"),"none",IF(E12="skyscraper",CONCATENATE(A12,"_c"),IF(E12="landmark",CONCATENATE(A12,"_k"),IF(E12="house",CONCATENATE(A12,"_h"),A12))))</f>
         <v>bank_building_c</v>
       </c>
       <c r="U12" s="1" t="str">
-        <f aca="false">IF(D12="1X1","none",IF(E12="skyscraper",CONCATENATE(A12,"_c_north"),IF(E12="landmark",CONCATENATE(A12,"_k_north"),CONCATENATE(A12,"_north"))))</f>
+        <f aca="false">IF(D12="1X1","none",IF(E12="skyscraper",CONCATENATE(A12,"_c_north"),IF(E12="landmark",CONCATENATE(A12,"_k_north"),IF(E12="house",CONCATENATE(A12,"_h_north"),CONCATENATE(A12,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V12" s="1" t="str">
@@ -1562,7 +1590,7 @@
       <c r="C13" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1589,7 +1617,7 @@
       <c r="L13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M13" s="4" t="str">
+      <c r="M13" s="2" t="str">
         <f aca="false">VLOOKUP(L13,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -1612,11 +1640,11 @@
         <v>63</v>
       </c>
       <c r="T13" s="1" t="str">
-        <f aca="false">IF(NOT(D13="1X1"),"none",IF(E13="skyscraper",CONCATENATE(A13,"_c"),A13))</f>
+        <f aca="false">IF(NOT(D13="1X1"),"none",IF(E13="skyscraper",CONCATENATE(A13,"_c"),IF(E13="landmark",CONCATENATE(A13,"_k"),IF(E13="house",CONCATENATE(A13,"_h"),A13))))</f>
         <v>none</v>
       </c>
       <c r="U13" s="1" t="str">
-        <f aca="false">IF(D13="1X1","none",IF(E13="skyscraper",CONCATENATE(A13,"_c_north"),IF(E13="landmark",CONCATENATE(A13,"_k_north"),CONCATENATE(A13,"_north"))))</f>
+        <f aca="false">IF(D13="1X1","none",IF(E13="skyscraper",CONCATENATE(A13,"_c_north"),IF(E13="landmark",CONCATENATE(A13,"_k_north"),IF(E13="house",CONCATENATE(A13,"_h_north"),CONCATENATE(A13,"_north")))))</f>
         <v>tsuno_building_c_north</v>
       </c>
       <c r="V13" s="1" t="str">
@@ -1643,7 +1671,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>65</v>
@@ -1655,64 +1683,64 @@
         <v>67</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="M14" s="4" t="str">
+      <c r="M14" s="2" t="str">
         <f aca="false">VLOOKUP(L14,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N14" s="1" t="n">
         <v>20</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>69</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R14" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>70</v>
       </c>
       <c r="T14" s="1" t="str">
-        <f aca="false">IF(NOT(D14="1X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c"),A14))</f>
+        <f aca="false">IF(NOT(D14="1X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c"),IF(E14="landmark",CONCATENATE(A14,"_k"),IF(E14="house",CONCATENATE(A14,"_h"),A14))))</f>
         <v>none</v>
       </c>
       <c r="U14" s="1" t="str">
-        <f aca="false">IF(D14="1X1","none",IF(E14="skyscraper",CONCATENATE(A14,"_c_north"),IF(E14="landmark",CONCATENATE(A14,"_k_north"),CONCATENATE(A14,"_north"))))</f>
-        <v>hospital_k_north</v>
+        <f aca="false">IF(D14="1X1","none",IF(E14="skyscraper",CONCATENATE(A14,"_c_north"),IF(E14="landmark",CONCATENATE(A14,"_k_north"),IF(E14="house",CONCATENATE(A14,"_h_north"),CONCATENATE(A14,"_north")))))</f>
+        <v>farm_h_north</v>
       </c>
       <c r="V14" s="1" t="str">
-        <f aca="false">IF(OR(D14="1X1",D14="2X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_east"),IF(E14="landmark",CONCATENATE(A14,"_k_east"),CONCATENATE(A14,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D14="1X1",D14="2X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_east"),IF(E14="landmark",CONCATENATE(A14,"_k_east"),IF(E14="house",CONCATENATE(A14,"_h_east"),CONCATENATE(A14,"_east")))))</f>
+        <v>farm_h_east</v>
       </c>
       <c r="W14" s="1" t="str">
-        <f aca="false">IF(OR(D14="1X1",D14="1X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_west"),IF(E14="landmark",CONCATENATE(A14,"_k_west"),CONCATENATE(A14,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D14="1X1",D14="1X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_west"),IF(E14="landmark",CONCATENATE(A14,"_k_west"),IF(E14="house",CONCATENATE(A14,"_h_west"),CONCATENATE(A14,"_west")))))</f>
+        <v>farm_h_west</v>
       </c>
       <c r="X14" s="1" t="str">
-        <f aca="false">IF(NOT(D14="2X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_south"),IF(E14="landmark",CONCATENATE(A14,"_k_south"),CONCATENATE(A14,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D14="2X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_south"),IF(E14="landmark",CONCATENATE(A14,"_k_south"),IF(E14="house",CONCATENATE(A14,"_h_south"),CONCATENATE(A14,"_south")))))</f>
+        <v>farm_h_south</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>64</v>
@@ -1726,10 +1754,10 @@
         <v>71</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>204</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>66</v>
@@ -1738,96 +1766,96 @@
         <v>72</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" s="4" t="str">
+        <v>73</v>
+      </c>
+      <c r="M15" s="2" t="str">
         <f aca="false">VLOOKUP(L15,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R15" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="T15" s="1" t="str">
-        <f aca="false">IF(NOT(D15="1X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c"),A15))</f>
+        <f aca="false">IF(NOT(D15="1X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c"),IF(E15="landmark",CONCATENATE(A15,"_k"),IF(E15="house",CONCATENATE(A15,"_h"),A15))))</f>
+        <v>naganuma_h</v>
+      </c>
+      <c r="U15" s="1" t="str">
+        <f aca="false">IF(D15="1X1","none",IF(E15="skyscraper",CONCATENATE(A15,"_c_north"),IF(E15="landmark",CONCATENATE(A15,"_k_north"),IF(E15="house",CONCATENATE(A15,"_h_north"),CONCATENATE(A15,"_north")))))</f>
         <v>none</v>
       </c>
-      <c r="U15" s="1" t="str">
-        <f aca="false">IF(D15="1X1","none",IF(E15="skyscraper",CONCATENATE(A15,"_c_north"),IF(E15="landmark",CONCATENATE(A15,"_k_north"),CONCATENATE(A15,"_north"))))</f>
-        <v>stadium_k_north</v>
-      </c>
       <c r="V15" s="1" t="str">
-        <f aca="false">IF(OR(D15="1X1",D15="2X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_east"),IF(E15="landmark",CONCATENATE(A15,"_k_east"),CONCATENATE(A15,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <f aca="false">IF(OR(D15="1X1",D15="2X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_east"),IF(E15="landmark",CONCATENATE(A15,"_k_east"),IF(E15="house",CONCATENATE(A15,"_h_east"),CONCATENATE(A15,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W15" s="1" t="str">
-        <f aca="false">IF(OR(D15="1X1",D15="1X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_west"),IF(E15="landmark",CONCATENATE(A15,"_k_west"),CONCATENATE(A15,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <f aca="false">IF(OR(D15="1X1",D15="1X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_west"),IF(E15="landmark",CONCATENATE(A15,"_k_west"),IF(E15="house",CONCATENATE(A15,"_h_west"),CONCATENATE(A15,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X15" s="1" t="str">
-        <f aca="false">IF(NOT(D15="2X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_south"),IF(E15="landmark",CONCATENATE(A15,"_k_south"),CONCATENATE(A15,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <f aca="false">IF(NOT(D15="2X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_south"),IF(E15="landmark",CONCATENATE(A15,"_k_south"),IF(E15="house",CONCATENATE(A15,"_h_south"),CONCATENATE(A15,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>39</v>
@@ -1836,11 +1864,11 @@
         <v>20</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="4" t="str">
+        <v>78</v>
+      </c>
+      <c r="M16" s="2" t="str">
         <f aca="false">VLOOKUP(L16,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N16" s="1" t="n">
         <v>20</v>
@@ -1849,45 +1877,206 @@
         <v>3</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="Q16" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R16" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="T16" s="1" t="str">
-        <f aca="false">IF(NOT(D16="1X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c"),A16))</f>
+        <f aca="false">IF(NOT(D16="1X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c"),IF(E16="landmark",CONCATENATE(A16,"_k"),IF(E16="house",CONCATENATE(A16,"_h"),A16))))</f>
         <v>none</v>
       </c>
       <c r="U16" s="1" t="str">
-        <f aca="false">IF(D16="1X1","none",IF(E16="skyscraper",CONCATENATE(A16,"_c_north"),IF(E16="landmark",CONCATENATE(A16,"_k_north"),CONCATENATE(A16,"_north"))))</f>
-        <v>temple_k_north</v>
+        <f aca="false">IF(D16="1X1","none",IF(E16="skyscraper",CONCATENATE(A16,"_c_north"),IF(E16="landmark",CONCATENATE(A16,"_k_north"),IF(E16="house",CONCATENATE(A16,"_h_north"),CONCATENATE(A16,"_north")))))</f>
+        <v>hospital_k_north</v>
       </c>
       <c r="V16" s="1" t="str">
         <f aca="false">IF(OR(D16="1X1",D16="2X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_east"),IF(E16="landmark",CONCATENATE(A16,"_k_east"),CONCATENATE(A16,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W16" s="1" t="str">
         <f aca="false">IF(OR(D16="1X1",D16="1X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_west"),IF(E16="landmark",CONCATENATE(A16,"_k_west"),CONCATENATE(A16,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X16" s="1" t="str">
         <f aca="false">IF(NOT(D16="2X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_south"),IF(E16="landmark",CONCATENATE(A16,"_k_south"),CONCATENATE(A16,"_south"))))</f>
+        <v>hospital_k_south</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="2" t="str">
+        <f aca="false">VLOOKUP(L17,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T17" s="1" t="str">
+        <f aca="false">IF(NOT(D17="1X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c"),IF(E17="landmark",CONCATENATE(A17,"_k"),IF(E17="house",CONCATENATE(A17,"_h"),A17))))</f>
+        <v>none</v>
+      </c>
+      <c r="U17" s="1" t="str">
+        <f aca="false">IF(D17="1X1","none",IF(E17="skyscraper",CONCATENATE(A17,"_c_north"),IF(E17="landmark",CONCATENATE(A17,"_k_north"),IF(E17="house",CONCATENATE(A17,"_h_north"),CONCATENATE(A17,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V17" s="1" t="str">
+        <f aca="false">IF(OR(D17="1X1",D17="2X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_east"),IF(E17="landmark",CONCATENATE(A17,"_k_east"),CONCATENATE(A17,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W17" s="1" t="str">
+        <f aca="false">IF(OR(D17="1X1",D17="1X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_west"),IF(E17="landmark",CONCATENATE(A17,"_k_west"),CONCATENATE(A17,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <f aca="false">IF(NOT(D17="2X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_south"),IF(E17="landmark",CONCATENATE(A17,"_k_south"),CONCATENATE(A17,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M18" s="2" t="str">
+        <f aca="false">VLOOKUP(L18,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T18" s="1" t="str">
+        <f aca="false">IF(NOT(D18="1X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c"),IF(E18="landmark",CONCATENATE(A18,"_k"),IF(E18="house",CONCATENATE(A18,"_h"),A18))))</f>
+        <v>none</v>
+      </c>
+      <c r="U18" s="1" t="str">
+        <f aca="false">IF(D18="1X1","none",IF(E18="skyscraper",CONCATENATE(A18,"_c_north"),IF(E18="landmark",CONCATENATE(A18,"_k_north"),IF(E18="house",CONCATENATE(A18,"_h_north"),CONCATENATE(A18,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V18" s="1" t="str">
+        <f aca="false">IF(OR(D18="1X1",D18="2X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_east"),IF(E18="landmark",CONCATENATE(A18,"_k_east"),CONCATENATE(A18,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W18" s="1" t="str">
+        <f aca="false">IF(OR(D18="1X1",D18="1X2"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_west"),IF(E18="landmark",CONCATENATE(A18,"_k_west"),CONCATENATE(A18,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X18" s="1" t="str">
+        <f aca="false">IF(NOT(D18="2X2"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_south"),IF(E18="landmark",CONCATENATE(A18,"_k_south"),CONCATENATE(A18,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y16" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
+      <c r="Y18" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -1895,15 +2084,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L16" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L18" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P16" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P18" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S16" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S18" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1937,15 +2126,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -1953,7 +2142,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -1961,7 +2150,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -1969,7 +2158,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3</v>
@@ -1977,7 +2166,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
@@ -1985,7 +2174,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
@@ -1993,7 +2182,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -2001,7 +2190,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>7</v>
@@ -2009,7 +2198,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>8</v>
@@ -2017,7 +2206,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>9</v>
@@ -2025,7 +2214,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10</v>
@@ -2033,7 +2222,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>11</v>
@@ -2041,7 +2230,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>12</v>
@@ -2049,7 +2238,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>13</v>
@@ -2057,7 +2246,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>14</v>
@@ -2065,7 +2254,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>15</v>
@@ -2097,16 +2286,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,11 +2338,11 @@
       </c>
       <c r="B4" s="1" t="str">
         <f aca="false">IF(C4="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A4,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">MAX(IF(C4="ID not in use",0,IF(C4="1X1",1,IF(C4="2X2",4,2)))-1,0)</f>
@@ -5719,15 +5908,15 @@
       </c>
       <c r="B214" s="1" t="str">
         <f aca="false">IF(C214="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C214" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A214,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>2X2</v>
       </c>
       <c r="D214" s="1" t="n">
         <f aca="false">IF(C214="Multi-tile",D213-1,MAX(IF(C214="ID not in use",0,IF(C214="1X1",1,IF(C214="2X2",4,2)))-1,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6477,10 +6666,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6495,25 +6684,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6530,10 +6719,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -6550,13 +6739,13 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>108</v>
+      <c r="F3" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>59</v>
@@ -6573,13 +6762,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>109</v>
+      <c r="F4" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>69</v>
@@ -6587,13 +6776,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>110</v>
+      <c r="F5" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6603,16 +6792,35 @@
       <c r="E6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>111</v>
+      <c r="F6" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>112</v>
+      <c r="F9" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -6641,40 +6849,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
@@ -6682,24 +6890,24 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: shrine_prohibition formerly shrine_01
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="151">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -296,6 +296,15 @@
     <t xml:space="preserve">NAME_SHIRO</t>
   </si>
   <si>
+    <t xml:space="preserve">shrine_prohibition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_SHRINE_PROHIBITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
     <t xml:space="preserve">stadium</t>
   </si>
   <si>
@@ -309,9 +318,6 @@
   </si>
   <si>
     <t xml:space="preserve">NAME_TEMPLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
   </si>
   <si>
     <t xml:space="preserve">colour</t>
@@ -579,16 +585,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.55"/>
@@ -598,7 +607,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="14.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="17.15"/>
@@ -2288,10 +2297,10 @@
         <v>90</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>77</v>
@@ -2300,13 +2309,13 @@
         <v>91</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>39</v>
@@ -2315,52 +2324,52 @@
         <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="M21" s="2" t="str">
         <f aca="false">VLOOKUP(L21,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O21" s="1" t="n">
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O21" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R21" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="T21" s="1" t="str">
         <f aca="false">IF(NOT(D21="1X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c"),IF(E21="landmark",CONCATENATE(A21,"_k"),IF(E21="house",CONCATENATE(A21,"_h"),A21))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U21" s="1" t="str">
         <f aca="false">IF(D21="1X1","none",IF(E21="skyscraper",CONCATENATE(A21,"_c_north"),IF(E21="landmark",CONCATENATE(A21,"_k_north"),IF(E21="house",CONCATENATE(A21,"_h_north"),CONCATENATE(A21,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V21" s="1" t="str">
         <f aca="false">IF(OR(D21="1X1",D21="2X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_east"),IF(E21="landmark",CONCATENATE(A21,"_k_east"),CONCATENATE(A21,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W21" s="1" t="str">
         <f aca="false">IF(OR(D21="1X1",D21="1X2"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_west"),IF(E21="landmark",CONCATENATE(A21,"_k_west"),CONCATENATE(A21,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X21" s="1" t="str">
         <f aca="false">IF(NOT(D21="2X2"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_south"),IF(E21="landmark",CONCATENATE(A21,"_k_south"),CONCATENATE(A21,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,7 +2380,7 @@
         <v>93</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>65</v>
@@ -2383,13 +2392,13 @@
         <v>94</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>39</v>
@@ -2398,11 +2407,11 @@
         <v>20</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="M22" s="2" t="str">
         <f aca="false">VLOOKUP(L22,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N22" s="1" t="n">
         <v>20</v>
@@ -2411,16 +2420,16 @@
         <v>3</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R22" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="T22" s="1" t="str">
         <f aca="false">IF(NOT(D22="1X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c"),IF(E22="landmark",CONCATENATE(A22,"_k"),IF(E22="house",CONCATENATE(A22,"_h"),A22))))</f>
@@ -2428,33 +2437,116 @@
       </c>
       <c r="U22" s="1" t="str">
         <f aca="false">IF(D22="1X1","none",IF(E22="skyscraper",CONCATENATE(A22,"_c_north"),IF(E22="landmark",CONCATENATE(A22,"_k_north"),IF(E22="house",CONCATENATE(A22,"_h_north"),CONCATENATE(A22,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>stadium_k_north</v>
       </c>
       <c r="V22" s="1" t="str">
         <f aca="false">IF(OR(D22="1X1",D22="2X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_east"),IF(E22="landmark",CONCATENATE(A22,"_k_east"),CONCATENATE(A22,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>stadium_k_east</v>
       </c>
       <c r="W22" s="1" t="str">
         <f aca="false">IF(OR(D22="1X1",D22="1X2"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_west"),IF(E22="landmark",CONCATENATE(A22,"_k_west"),CONCATENATE(A22,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>stadium_k_west</v>
       </c>
       <c r="X22" s="1" t="str">
         <f aca="false">IF(NOT(D22="2X2"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_south"),IF(E22="landmark",CONCATENATE(A22,"_k_south"),CONCATENATE(A22,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M23" s="2" t="str">
+        <f aca="false">VLOOKUP(L23,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q23" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="T23" s="1" t="str">
+        <f aca="false">IF(NOT(D23="1X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c"),IF(E23="landmark",CONCATENATE(A23,"_k"),IF(E23="house",CONCATENATE(A23,"_h"),A23))))</f>
+        <v>none</v>
+      </c>
+      <c r="U23" s="1" t="str">
+        <f aca="false">IF(D23="1X1","none",IF(E23="skyscraper",CONCATENATE(A23,"_c_north"),IF(E23="landmark",CONCATENATE(A23,"_k_north"),IF(E23="house",CONCATENATE(A23,"_h_north"),CONCATENATE(A23,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V23" s="1" t="str">
+        <f aca="false">IF(OR(D23="1X1",D23="2X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_east"),IF(E23="landmark",CONCATENATE(A23,"_k_east"),CONCATENATE(A23,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W23" s="1" t="str">
+        <f aca="false">IF(OR(D23="1X1",D23="1X2"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_west"),IF(E23="landmark",CONCATENATE(A23,"_k_west"),CONCATENATE(A23,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X23" s="1" t="str">
+        <f aca="false">IF(NOT(D23="2X2"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_south"),IF(E23="landmark",CONCATENATE(A23,"_k_south"),CONCATENATE(A23,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y22" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="D23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="S23" s="2"/>
+      <c r="Y23" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="D24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="S24" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2462,15 +2554,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L23" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L24" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P23" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P24" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S23" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S24" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2504,15 +2596,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -2520,7 +2612,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -2528,7 +2620,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -2536,7 +2628,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3</v>
@@ -2544,7 +2636,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
@@ -2552,7 +2644,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
@@ -2560,7 +2652,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -2568,7 +2660,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>7</v>
@@ -2576,7 +2668,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>8</v>
@@ -2584,7 +2676,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>9</v>
@@ -2592,7 +2684,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10</v>
@@ -2600,7 +2692,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>11</v>
@@ -2608,7 +2700,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>12</v>
@@ -2616,7 +2708,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>13</v>
@@ -2624,7 +2716,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>14</v>
@@ -2632,7 +2724,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>15</v>
@@ -2664,16 +2756,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4603,11 +4695,11 @@
       </c>
       <c r="B115" s="1" t="str">
         <f aca="false">IF(C115="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C115" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A115,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D115" s="1" t="n">
         <f aca="false">IF(C115="Multi-tile",D114-1,MAX(IF(C115="ID not in use",0,IF(C115="1X1",1,IF(C115="2X2",4,2)))-1,0))</f>
@@ -7062,25 +7154,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7094,13 +7186,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -7123,7 +7215,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>59</v>
@@ -7146,7 +7238,7 @@
         <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>69</v>
@@ -7154,13 +7246,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7171,7 +7263,7 @@
         <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7182,7 +7274,7 @@
         <v>81</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7193,15 +7285,15 @@
         <v>73</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7209,7 +7301,7 @@
         <v>68</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -7238,40 +7330,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
@@ -7279,24 +7371,24 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: shrine & enterprise_tower
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="156">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -206,6 +206,15 @@
     <t xml:space="preserve">bitmask(HOUSE_FLAG_NOT_SLOPED,HOUSE_FLAG_PROTECTED)</t>
   </si>
   <si>
+    <t xml:space="preserve">enterprise_tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_ENTERPRISE_TOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PASS, 8],[MAIL, 4],[GOOD, 4]</t>
+  </si>
+  <si>
     <t xml:space="preserve">tsuno_building</t>
   </si>
   <si>
@@ -215,9 +224,6 @@
     <t xml:space="preserve">NAME_TSUNO_BUILDING</t>
   </si>
   <si>
-    <t xml:space="preserve">[PASS, 8],[MAIL, 4],[GOOD, 4]</t>
-  </si>
-  <si>
     <t xml:space="preserve">farm</t>
   </si>
   <si>
@@ -296,13 +302,22 @@
     <t xml:space="preserve">NAME_SHIRO</t>
   </si>
   <si>
+    <t xml:space="preserve">shrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_SHRINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PASS, 4]</t>
+  </si>
+  <si>
     <t xml:space="preserve">shrine_prohibition</t>
   </si>
   <si>
     <t xml:space="preserve">NAME_SHRINE_PROHIBITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
   </si>
   <si>
     <t xml:space="preserve">stadium</t>
@@ -585,14 +600,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,25 +1648,25 @@
         <v>60</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>2006</v>
+        <v>1990</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>39</v>
@@ -1667,7 +1682,7 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O13" s="1" t="n">
         <v>5</v>
@@ -1682,19 +1697,19 @@
         <v>10</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T13" s="1" t="str">
         <f aca="false">IF(NOT(D13="1X1"),"none",IF(E13="skyscraper",CONCATENATE(A13,"_c"),IF(E13="landmark",CONCATENATE(A13,"_k"),IF(E13="house",CONCATENATE(A13,"_h"),A13))))</f>
-        <v>none</v>
+        <v>enterprise_tower_c</v>
       </c>
       <c r="U13" s="1" t="str">
         <f aca="false">IF(D13="1X1","none",IF(E13="skyscraper",CONCATENATE(A13,"_c_north"),IF(E13="landmark",CONCATENATE(A13,"_k_north"),IF(E13="house",CONCATENATE(A13,"_h_north"),CONCATENATE(A13,"_north")))))</f>
-        <v>tsuno_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V13" s="1" t="str">
         <f aca="false">IF(OR(D13="1X1",D13="2X1"),"none",IF(E13="skyscraper",CONCATENATE(A13,"_c_east"),IF(E13="landmark",CONCATENATE(A13,"_k_east"),CONCATENATE(A13,"_east"))))</f>
-        <v>tsuno_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W13" s="1" t="str">
         <f aca="false">IF(OR(D13="1X1",D13="1X2"),"none",IF(E13="skyscraper",CONCATENATE(A13,"_c_west"),IF(E13="landmark",CONCATENATE(A13,"_k_west"),CONCATENATE(A13,"_west"))))</f>
@@ -1710,62 +1725,62 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G14" s="1" t="n">
-        <v>15</v>
+        <v>255</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>1700</v>
+        <v>2006</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="M14" s="2" t="str">
         <f aca="false">VLOOKUP(L14,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="R14" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="T14" s="1" t="str">
         <f aca="false">IF(NOT(D14="1X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c"),IF(E14="landmark",CONCATENATE(A14,"_k"),IF(E14="house",CONCATENATE(A14,"_h"),A14))))</f>
@@ -1773,173 +1788,173 @@
       </c>
       <c r="U14" s="1" t="str">
         <f aca="false">IF(D14="1X1","none",IF(E14="skyscraper",CONCATENATE(A14,"_c_north"),IF(E14="landmark",CONCATENATE(A14,"_k_north"),IF(E14="house",CONCATENATE(A14,"_h_north"),CONCATENATE(A14,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>tsuno_building_c_north</v>
       </c>
       <c r="V14" s="1" t="str">
-        <f aca="false">IF(OR(D14="1X1",D14="2X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_east"),IF(E14="landmark",CONCATENATE(A14,"_k_east"),IF(E14="house",CONCATENATE(A14,"_h_east"),CONCATENATE(A14,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D14="1X1",D14="2X1"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_east"),IF(E14="landmark",CONCATENATE(A14,"_k_east"),CONCATENATE(A14,"_east"))))</f>
+        <v>tsuno_building_c_east</v>
       </c>
       <c r="W14" s="1" t="str">
-        <f aca="false">IF(OR(D14="1X1",D14="1X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_west"),IF(E14="landmark",CONCATENATE(A14,"_k_west"),IF(E14="house",CONCATENATE(A14,"_h_west"),CONCATENATE(A14,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D14="1X1",D14="1X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_west"),IF(E14="landmark",CONCATENATE(A14,"_k_west"),CONCATENATE(A14,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X14" s="1" t="str">
-        <f aca="false">IF(NOT(D14="2X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_south"),IF(E14="landmark",CONCATENATE(A14,"_k_south"),IF(E14="house",CONCATENATE(A14,"_h_south"),CONCATENATE(A14,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D14="2X2"),"none",IF(E14="skyscraper",CONCATENATE(A14,"_c_south"),IF(E14="landmark",CONCATENATE(A14,"_k_south"),CONCATENATE(A14,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>1870</v>
+        <v>1700</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M15" s="2" t="str">
         <f aca="false">VLOOKUP(L15,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O15" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="O15" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="P15" s="2" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="Q15" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="R15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R15" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="T15" s="1" t="str">
         <f aca="false">IF(NOT(D15="1X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c"),IF(E15="landmark",CONCATENATE(A15,"_k"),IF(E15="house",CONCATENATE(A15,"_h"),A15))))</f>
-        <v>naganuma_h</v>
+        <v>none</v>
       </c>
       <c r="U15" s="1" t="str">
         <f aca="false">IF(D15="1X1","none",IF(E15="skyscraper",CONCATENATE(A15,"_c_north"),IF(E15="landmark",CONCATENATE(A15,"_k_north"),IF(E15="house",CONCATENATE(A15,"_h_north"),CONCATENATE(A15,"_north")))))</f>
-        <v>none</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V15" s="1" t="str">
         <f aca="false">IF(OR(D15="1X1",D15="2X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_east"),IF(E15="landmark",CONCATENATE(A15,"_k_east"),IF(E15="house",CONCATENATE(A15,"_h_east"),CONCATENATE(A15,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W15" s="1" t="str">
         <f aca="false">IF(OR(D15="1X1",D15="1X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_west"),IF(E15="landmark",CONCATENATE(A15,"_k_west"),IF(E15="house",CONCATENATE(A15,"_h_west"),CONCATENATE(A15,"_west")))))</f>
-        <v>none</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X15" s="1" t="str">
         <f aca="false">IF(NOT(D15="2X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_south"),IF(E15="landmark",CONCATENATE(A15,"_k_south"),IF(E15="house",CONCATENATE(A15,"_h_south"),CONCATENATE(A15,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M16" s="2" t="str">
         <f aca="false">VLOOKUP(L16,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R16" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="T16" s="1" t="str">
         <f aca="false">IF(NOT(D16="1X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c"),IF(E16="landmark",CONCATENATE(A16,"_k"),IF(E16="house",CONCATENATE(A16,"_h"),A16))))</f>
-        <v>none</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U16" s="1" t="str">
         <f aca="false">IF(D16="1X1","none",IF(E16="skyscraper",CONCATENATE(A16,"_c_north"),IF(E16="landmark",CONCATENATE(A16,"_k_north"),IF(E16="house",CONCATENATE(A16,"_h_north"),CONCATENATE(A16,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V16" s="1" t="str">
         <f aca="false">IF(OR(D16="1X1",D16="2X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_east"),IF(E16="landmark",CONCATENATE(A16,"_k_east"),IF(E16="house",CONCATENATE(A16,"_h_east"),CONCATENATE(A16,"_east")))))</f>
@@ -1947,37 +1962,37 @@
       </c>
       <c r="W16" s="1" t="str">
         <f aca="false">IF(OR(D16="1X1",D16="1X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_west"),IF(E16="landmark",CONCATENATE(A16,"_k_west"),IF(E16="house",CONCATENATE(A16,"_h_west"),CONCATENATE(A16,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>none</v>
       </c>
       <c r="X16" s="1" t="str">
         <f aca="false">IF(NOT(D16="2X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_south"),IF(E16="landmark",CONCATENATE(A16,"_k_south"),IF(E16="house",CONCATENATE(A16,"_h_south"),CONCATENATE(A16,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>80</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>3</v>
@@ -1992,29 +2007,29 @@
         <v>20</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M17" s="2" t="str">
         <f aca="false">VLOOKUP(L17,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="O17" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q17" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="T17" s="1" t="str">
         <f aca="false">IF(NOT(D17="1X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c"),IF(E17="landmark",CONCATENATE(A17,"_k"),IF(E17="house",CONCATENATE(A17,"_h"),A17))))</f>
@@ -2022,177 +2037,177 @@
       </c>
       <c r="U17" s="1" t="str">
         <f aca="false">IF(D17="1X1","none",IF(E17="skyscraper",CONCATENATE(A17,"_c_north"),IF(E17="landmark",CONCATENATE(A17,"_k_north"),IF(E17="house",CONCATENATE(A17,"_h_north"),CONCATENATE(A17,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V17" s="1" t="str">
-        <f aca="false">IF(OR(D17="1X1",D17="2X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_east"),IF(E17="landmark",CONCATENATE(A17,"_k_east"),CONCATENATE(A17,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D17="1X1",D17="2X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_east"),IF(E17="landmark",CONCATENATE(A17,"_k_east"),IF(E17="house",CONCATENATE(A17,"_h_east"),CONCATENATE(A17,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W17" s="1" t="str">
-        <f aca="false">IF(OR(D17="1X1",D17="1X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_west"),IF(E17="landmark",CONCATENATE(A17,"_k_west"),CONCATENATE(A17,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D17="1X1",D17="1X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_west"),IF(E17="landmark",CONCATENATE(A17,"_k_west"),IF(E17="house",CONCATENATE(A17,"_h_west"),CONCATENATE(A17,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X17" s="1" t="str">
-        <f aca="false">IF(NOT(D17="2X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_south"),IF(E17="landmark",CONCATENATE(A17,"_k_south"),CONCATENATE(A17,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D17="2X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_south"),IF(E17="landmark",CONCATENATE(A17,"_k_south"),IF(E17="house",CONCATENATE(A17,"_h_south"),CONCATENATE(A17,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="M18" s="2" t="str">
         <f aca="false">VLOOKUP(L18,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O18" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R18" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T18" s="1" t="str">
         <f aca="false">IF(NOT(D18="1X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c"),IF(E18="landmark",CONCATENATE(A18,"_k"),IF(E18="house",CONCATENATE(A18,"_h"),A18))))</f>
-        <v>pachinko_k</v>
+        <v>none</v>
       </c>
       <c r="U18" s="1" t="str">
         <f aca="false">IF(D18="1X1","none",IF(E18="skyscraper",CONCATENATE(A18,"_c_north"),IF(E18="landmark",CONCATENATE(A18,"_k_north"),IF(E18="house",CONCATENATE(A18,"_h_north"),CONCATENATE(A18,"_north")))))</f>
-        <v>none</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V18" s="1" t="str">
         <f aca="false">IF(OR(D18="1X1",D18="2X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_east"),IF(E18="landmark",CONCATENATE(A18,"_k_east"),CONCATENATE(A18,"_east"))))</f>
-        <v>none</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W18" s="1" t="str">
         <f aca="false">IF(OR(D18="1X1",D18="1X2"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_west"),IF(E18="landmark",CONCATENATE(A18,"_k_west"),CONCATENATE(A18,"_west"))))</f>
-        <v>none</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X18" s="1" t="str">
         <f aca="false">IF(NOT(D18="2X2"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_south"),IF(E18="landmark",CONCATENATE(A18,"_k_south"),CONCATENATE(A18,"_south"))))</f>
-        <v>none</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="G19" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="M19" s="2" t="str">
         <f aca="false">VLOOKUP(L19,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="O19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="T19" s="1" t="str">
         <f aca="false">IF(NOT(D19="1X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c"),IF(E19="landmark",CONCATENATE(A19,"_k"),IF(E19="house",CONCATENATE(A19,"_h"),A19))))</f>
-        <v>none</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U19" s="1" t="str">
         <f aca="false">IF(D19="1X1","none",IF(E19="skyscraper",CONCATENATE(A19,"_c_north"),IF(E19="landmark",CONCATENATE(A19,"_k_north"),IF(E19="house",CONCATENATE(A19,"_h_north"),CONCATENATE(A19,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V19" s="1" t="str">
         <f aca="false">IF(OR(D19="1X1",D19="2X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_east"),IF(E19="landmark",CONCATENATE(A19,"_k_east"),CONCATENATE(A19,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>none</v>
       </c>
       <c r="W19" s="1" t="str">
         <f aca="false">IF(OR(D19="1X1",D19="1X2"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_west"),IF(E19="landmark",CONCATENATE(A19,"_k_west"),CONCATENATE(A19,"_west"))))</f>
@@ -2203,7 +2218,7 @@
         <v>none</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,25 +2229,25 @@
         <v>88</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H20" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>39</v>
@@ -2241,20 +2256,20 @@
         <v>20</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M20" s="2" t="str">
         <f aca="false">VLOOKUP(L20,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N20" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O20" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O20" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>10</v>
@@ -2263,7 +2278,7 @@
         <v>2</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="T20" s="1" t="str">
         <f aca="false">IF(NOT(D20="1X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c"),IF(E20="landmark",CONCATENATE(A20,"_k"),IF(E20="house",CONCATENATE(A20,"_h"),A20))))</f>
@@ -2271,19 +2286,19 @@
       </c>
       <c r="U20" s="1" t="str">
         <f aca="false">IF(D20="1X1","none",IF(E20="skyscraper",CONCATENATE(A20,"_c_north"),IF(E20="landmark",CONCATENATE(A20,"_k_north"),IF(E20="house",CONCATENATE(A20,"_h_north"),CONCATENATE(A20,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V20" s="1" t="str">
         <f aca="false">IF(OR(D20="1X1",D20="2X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_east"),IF(E20="landmark",CONCATENATE(A20,"_k_east"),CONCATENATE(A20,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W20" s="1" t="str">
         <f aca="false">IF(OR(D20="1X1",D20="1X2"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_west"),IF(E20="landmark",CONCATENATE(A20,"_k_west"),CONCATENATE(A20,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>none</v>
       </c>
       <c r="X20" s="1" t="str">
         <f aca="false">IF(NOT(D20="2X2"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_south"),IF(E20="landmark",CONCATENATE(A20,"_k_south"),CONCATENATE(A20,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y20" s="1" t="s">
         <v>88</v>
@@ -2297,25 +2312,25 @@
         <v>90</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>91</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>39</v>
@@ -2324,14 +2339,14 @@
         <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="M21" s="2" t="str">
         <f aca="false">VLOOKUP(L21,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O21" s="0" t="n">
         <v>3</v>
@@ -2340,33 +2355,33 @@
         <v>59</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R21" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="T21" s="1" t="str">
         <f aca="false">IF(NOT(D21="1X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c"),IF(E21="landmark",CONCATENATE(A21,"_k"),IF(E21="house",CONCATENATE(A21,"_h"),A21))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>none</v>
       </c>
       <c r="U21" s="1" t="str">
         <f aca="false">IF(D21="1X1","none",IF(E21="skyscraper",CONCATENATE(A21,"_c_north"),IF(E21="landmark",CONCATENATE(A21,"_k_north"),IF(E21="house",CONCATENATE(A21,"_h_north"),CONCATENATE(A21,"_north")))))</f>
-        <v>none</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V21" s="1" t="str">
         <f aca="false">IF(OR(D21="1X1",D21="2X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_east"),IF(E21="landmark",CONCATENATE(A21,"_k_east"),CONCATENATE(A21,"_east"))))</f>
-        <v>none</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W21" s="1" t="str">
         <f aca="false">IF(OR(D21="1X1",D21="1X2"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_west"),IF(E21="landmark",CONCATENATE(A21,"_k_west"),CONCATENATE(A21,"_west"))))</f>
-        <v>none</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X21" s="1" t="str">
         <f aca="false">IF(NOT(D21="2X2"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_south"),IF(E21="landmark",CONCATENATE(A21,"_k_south"),CONCATENATE(A21,"_south"))))</f>
-        <v>none</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>90</v>
@@ -2374,31 +2389,31 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="G22" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>39</v>
@@ -2407,52 +2422,52 @@
         <v>20</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="M22" s="2" t="str">
         <f aca="false">VLOOKUP(L22,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O22" s="1" t="n">
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O22" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R22" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>95</v>
       </c>
       <c r="T22" s="1" t="str">
         <f aca="false">IF(NOT(D22="1X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c"),IF(E22="landmark",CONCATENATE(A22,"_k"),IF(E22="house",CONCATENATE(A22,"_h"),A22))))</f>
-        <v>none</v>
+        <v>shrine_k</v>
       </c>
       <c r="U22" s="1" t="str">
         <f aca="false">IF(D22="1X1","none",IF(E22="skyscraper",CONCATENATE(A22,"_c_north"),IF(E22="landmark",CONCATENATE(A22,"_k_north"),IF(E22="house",CONCATENATE(A22,"_h_north"),CONCATENATE(A22,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V22" s="1" t="str">
         <f aca="false">IF(OR(D22="1X1",D22="2X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_east"),IF(E22="landmark",CONCATENATE(A22,"_k_east"),CONCATENATE(A22,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W22" s="1" t="str">
         <f aca="false">IF(OR(D22="1X1",D22="1X2"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_west"),IF(E22="landmark",CONCATENATE(A22,"_k_west"),CONCATENATE(A22,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X22" s="1" t="str">
         <f aca="false">IF(NOT(D22="2X2"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_south"),IF(E22="landmark",CONCATENATE(A22,"_k_south"),CONCATENATE(A22,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,25 +2478,25 @@
         <v>96</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>208</v>
+        <v>113</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>97</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>39</v>
@@ -2490,63 +2505,229 @@
         <v>20</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M23" s="2" t="str">
         <f aca="false">VLOOKUP(L23,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
-      <c r="N23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O23" s="1" t="n">
+      <c r="N23" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O23" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>59</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R23" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="T23" s="1" t="str">
         <f aca="false">IF(NOT(D23="1X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c"),IF(E23="landmark",CONCATENATE(A23,"_k"),IF(E23="house",CONCATENATE(A23,"_h"),A23))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U23" s="1" t="str">
         <f aca="false">IF(D23="1X1","none",IF(E23="skyscraper",CONCATENATE(A23,"_c_north"),IF(E23="landmark",CONCATENATE(A23,"_k_north"),IF(E23="house",CONCATENATE(A23,"_h_north"),CONCATENATE(A23,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>none</v>
       </c>
       <c r="V23" s="1" t="str">
         <f aca="false">IF(OR(D23="1X1",D23="2X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_east"),IF(E23="landmark",CONCATENATE(A23,"_k_east"),CONCATENATE(A23,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>none</v>
       </c>
       <c r="W23" s="1" t="str">
         <f aca="false">IF(OR(D23="1X1",D23="1X2"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_west"),IF(E23="landmark",CONCATENATE(A23,"_k_west"),CONCATENATE(A23,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X23" s="1" t="str">
         <f aca="false">IF(NOT(D23="2X2"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_south"),IF(E23="landmark",CONCATENATE(A23,"_k_south"),CONCATENATE(A23,"_south"))))</f>
-        <v>temple_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y23" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="D24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="S24" s="2"/>
+      <c r="A24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M24" s="2" t="str">
+        <f aca="false">VLOOKUP(L24,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q24" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R24" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="T24" s="1" t="str">
+        <f aca="false">IF(NOT(D24="1X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c"),IF(E24="landmark",CONCATENATE(A24,"_k"),IF(E24="house",CONCATENATE(A24,"_h"),A24))))</f>
+        <v>none</v>
+      </c>
+      <c r="U24" s="1" t="str">
+        <f aca="false">IF(D24="1X1","none",IF(E24="skyscraper",CONCATENATE(A24,"_c_north"),IF(E24="landmark",CONCATENATE(A24,"_k_north"),IF(E24="house",CONCATENATE(A24,"_h_north"),CONCATENATE(A24,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V24" s="1" t="str">
+        <f aca="false">IF(OR(D24="1X1",D24="2X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c_east"),IF(E24="landmark",CONCATENATE(A24,"_k_east"),CONCATENATE(A24,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W24" s="1" t="str">
+        <f aca="false">IF(OR(D24="1X1",D24="1X2"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c_west"),IF(E24="landmark",CONCATENATE(A24,"_k_west"),CONCATENATE(A24,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X24" s="1" t="str">
+        <f aca="false">IF(NOT(D24="2X2"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c_south"),IF(E24="landmark",CONCATENATE(A24,"_k_south"),CONCATENATE(A24,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M25" s="2" t="str">
+        <f aca="false">VLOOKUP(L25,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="T25" s="1" t="str">
+        <f aca="false">IF(NOT(D25="1X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c"),IF(E25="landmark",CONCATENATE(A25,"_k"),IF(E25="house",CONCATENATE(A25,"_h"),A25))))</f>
+        <v>none</v>
+      </c>
+      <c r="U25" s="1" t="str">
+        <f aca="false">IF(D25="1X1","none",IF(E25="skyscraper",CONCATENATE(A25,"_c_north"),IF(E25="landmark",CONCATENATE(A25,"_k_north"),IF(E25="house",CONCATENATE(A25,"_h_north"),CONCATENATE(A25,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V25" s="1" t="str">
+        <f aca="false">IF(OR(D25="1X1",D25="2X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c_east"),IF(E25="landmark",CONCATENATE(A25,"_k_east"),CONCATENATE(A25,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W25" s="1" t="str">
+        <f aca="false">IF(OR(D25="1X1",D25="1X2"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c_west"),IF(E25="landmark",CONCATENATE(A25,"_k_west"),CONCATENATE(A25,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X25" s="1" t="str">
+        <f aca="false">IF(NOT(D25="2X2"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c_south"),IF(E25="landmark",CONCATENATE(A25,"_k_south"),CONCATENATE(A25,"_south"))))</f>
+        <v>temple_k_south</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="D26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2554,15 +2735,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L24" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L26" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P24" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P26" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S24" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S26" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2596,15 +2777,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -2612,7 +2793,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -2620,7 +2801,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -2628,7 +2809,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3</v>
@@ -2636,7 +2817,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
@@ -2644,7 +2825,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
@@ -2652,7 +2833,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -2660,7 +2841,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>7</v>
@@ -2668,7 +2849,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>8</v>
@@ -2676,7 +2857,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>9</v>
@@ -2684,7 +2865,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10</v>
@@ -2692,7 +2873,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>11</v>
@@ -2700,7 +2881,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>12</v>
@@ -2708,7 +2889,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>13</v>
@@ -2716,7 +2897,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>14</v>
@@ -2724,7 +2905,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>15</v>
@@ -2756,16 +2937,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4151,11 +4332,11 @@
       </c>
       <c r="B83" s="1" t="str">
         <f aca="false">IF(C83="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C83" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A83,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D83" s="1" t="n">
         <f aca="false">IF(C83="Multi-tile",D82-1,MAX(IF(C83="ID not in use",0,IF(C83="1X1",1,IF(C83="2X2",4,2)))-1,0))</f>
@@ -4712,11 +4893,11 @@
       </c>
       <c r="B116" s="1" t="str">
         <f aca="false">IF(C116="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C116" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A116,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D116" s="1" t="n">
         <f aca="false">IF(C116="Multi-tile",D115-1,MAX(IF(C116="ID not in use",0,IF(C116="1X1",1,IF(C116="2X2",4,2)))-1,0))</f>
@@ -7139,7 +7320,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7154,25 +7335,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7186,13 +7367,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -7215,7 +7396,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>59</v>
@@ -7232,76 +7413,79 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -7330,40 +7514,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
@@ -7371,24 +7555,24 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: kuroi_tower & mitsui_tower
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="162">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -219,6 +219,18 @@
   </si>
   <si>
     <t xml:space="preserve">NAME_INSURANCE_TOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuroi_tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_KUROI_TOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mitsui_tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_MITSUI_TOWER</t>
   </si>
   <si>
     <t xml:space="preserve">tsuno_building</t>
@@ -606,14 +618,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q34" activeCellId="0" sqref="Q34"/>
+      <selection pane="bottomRight" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1595,7 +1607,7 @@
         <v>39</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>58</v>
@@ -1678,7 +1690,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>58</v>
@@ -1761,7 +1773,7 @@
         <v>39</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>58</v>
@@ -1820,31 +1832,31 @@
         <v>65</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>58</v>
@@ -1854,7 +1866,7 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>5</v>
@@ -1873,15 +1885,15 @@
       </c>
       <c r="T15" s="1" t="str">
         <f aca="false">IF(NOT(D15="1X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c"),IF(E15="landmark",CONCATENATE(A15,"_k"),IF(E15="house",CONCATENATE(A15,"_h"),A15))))</f>
-        <v>none</v>
+        <v>kuroi_tower_c</v>
       </c>
       <c r="U15" s="1" t="str">
         <f aca="false">IF(D15="1X1","none",IF(E15="skyscraper",CONCATENATE(A15,"_c_north"),IF(E15="landmark",CONCATENATE(A15,"_k_north"),IF(E15="house",CONCATENATE(A15,"_h_north"),CONCATENATE(A15,"_north")))))</f>
-        <v>tsuno_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V15" s="1" t="str">
         <f aca="false">IF(OR(D15="1X1",D15="2X1"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_east"),IF(E15="landmark",CONCATENATE(A15,"_k_east"),CONCATENATE(A15,"_east"))))</f>
-        <v>tsuno_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W15" s="1" t="str">
         <f aca="false">IF(OR(D15="1X1",D15="1X2"),"none",IF(E15="skyscraper",CONCATENATE(A15,"_c_west"),IF(E15="landmark",CONCATENATE(A15,"_k_west"),CONCATENATE(A15,"_west"))))</f>
@@ -1897,228 +1909,228 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="G16" s="1" t="n">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="M16" s="2" t="str">
         <f aca="false">VLOOKUP(L16,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="R16" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="T16" s="1" t="str">
         <f aca="false">IF(NOT(D16="1X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c"),IF(E16="landmark",CONCATENATE(A16,"_k"),IF(E16="house",CONCATENATE(A16,"_h"),A16))))</f>
-        <v>none</v>
+        <v>mitsui_tower_c</v>
       </c>
       <c r="U16" s="1" t="str">
         <f aca="false">IF(D16="1X1","none",IF(E16="skyscraper",CONCATENATE(A16,"_c_north"),IF(E16="landmark",CONCATENATE(A16,"_k_north"),IF(E16="house",CONCATENATE(A16,"_h_north"),CONCATENATE(A16,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>none</v>
       </c>
       <c r="V16" s="1" t="str">
-        <f aca="false">IF(OR(D16="1X1",D16="2X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_east"),IF(E16="landmark",CONCATENATE(A16,"_k_east"),IF(E16="house",CONCATENATE(A16,"_h_east"),CONCATENATE(A16,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D16="1X1",D16="2X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_east"),IF(E16="landmark",CONCATENATE(A16,"_k_east"),CONCATENATE(A16,"_east"))))</f>
+        <v>none</v>
       </c>
       <c r="W16" s="1" t="str">
-        <f aca="false">IF(OR(D16="1X1",D16="1X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_west"),IF(E16="landmark",CONCATENATE(A16,"_k_west"),IF(E16="house",CONCATENATE(A16,"_h_west"),CONCATENATE(A16,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D16="1X1",D16="1X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_west"),IF(E16="landmark",CONCATENATE(A16,"_k_west"),CONCATENATE(A16,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X16" s="1" t="str">
-        <f aca="false">IF(NOT(D16="2X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_south"),IF(E16="landmark",CONCATENATE(A16,"_k_south"),IF(E16="house",CONCATENATE(A16,"_h_south"),CONCATENATE(A16,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D16="2X2"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c_south"),IF(E16="landmark",CONCATENATE(A16,"_k_south"),CONCATENATE(A16,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>20</v>
+        <v>255</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>1870</v>
+        <v>2006</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="M17" s="2" t="str">
         <f aca="false">VLOOKUP(L17,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="T17" s="1" t="str">
         <f aca="false">IF(NOT(D17="1X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c"),IF(E17="landmark",CONCATENATE(A17,"_k"),IF(E17="house",CONCATENATE(A17,"_h"),A17))))</f>
-        <v>naganuma_h</v>
+        <v>none</v>
       </c>
       <c r="U17" s="1" t="str">
         <f aca="false">IF(D17="1X1","none",IF(E17="skyscraper",CONCATENATE(A17,"_c_north"),IF(E17="landmark",CONCATENATE(A17,"_k_north"),IF(E17="house",CONCATENATE(A17,"_h_north"),CONCATENATE(A17,"_north")))))</f>
-        <v>none</v>
+        <v>tsuno_building_c_north</v>
       </c>
       <c r="V17" s="1" t="str">
-        <f aca="false">IF(OR(D17="1X1",D17="2X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_east"),IF(E17="landmark",CONCATENATE(A17,"_k_east"),IF(E17="house",CONCATENATE(A17,"_h_east"),CONCATENATE(A17,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D17="1X1",D17="2X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_east"),IF(E17="landmark",CONCATENATE(A17,"_k_east"),CONCATENATE(A17,"_east"))))</f>
+        <v>tsuno_building_c_east</v>
       </c>
       <c r="W17" s="1" t="str">
-        <f aca="false">IF(OR(D17="1X1",D17="1X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_west"),IF(E17="landmark",CONCATENATE(A17,"_k_west"),IF(E17="house",CONCATENATE(A17,"_h_west"),CONCATENATE(A17,"_west")))))</f>
+        <f aca="false">IF(OR(D17="1X1",D17="1X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_west"),IF(E17="landmark",CONCATENATE(A17,"_k_west"),CONCATENATE(A17,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X17" s="1" t="str">
-        <f aca="false">IF(NOT(D17="2X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_south"),IF(E17="landmark",CONCATENATE(A17,"_k_south"),IF(E17="house",CONCATENATE(A17,"_h_south"),CONCATENATE(A17,"_south")))))</f>
+        <f aca="false">IF(NOT(D17="2X2"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c_south"),IF(E17="landmark",CONCATENATE(A17,"_k_south"),CONCATENATE(A17,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M18" s="2" t="str">
         <f aca="false">VLOOKUP(L18,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="T18" s="1" t="str">
         <f aca="false">IF(NOT(D18="1X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c"),IF(E18="landmark",CONCATENATE(A18,"_k"),IF(E18="house",CONCATENATE(A18,"_h"),A18))))</f>
@@ -2126,211 +2138,211 @@
       </c>
       <c r="U18" s="1" t="str">
         <f aca="false">IF(D18="1X1","none",IF(E18="skyscraper",CONCATENATE(A18,"_c_north"),IF(E18="landmark",CONCATENATE(A18,"_k_north"),IF(E18="house",CONCATENATE(A18,"_h_north"),CONCATENATE(A18,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V18" s="1" t="str">
         <f aca="false">IF(OR(D18="1X1",D18="2X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_east"),IF(E18="landmark",CONCATENATE(A18,"_k_east"),IF(E18="house",CONCATENATE(A18,"_h_east"),CONCATENATE(A18,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W18" s="1" t="str">
         <f aca="false">IF(OR(D18="1X1",D18="1X2"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_west"),IF(E18="landmark",CONCATENATE(A18,"_k_west"),IF(E18="house",CONCATENATE(A18,"_h_west"),CONCATENATE(A18,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X18" s="1" t="str">
         <f aca="false">IF(NOT(D18="2X2"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c_south"),IF(E18="landmark",CONCATENATE(A18,"_k_south"),IF(E18="house",CONCATENATE(A18,"_h_south"),CONCATENATE(A18,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="M19" s="2" t="str">
         <f aca="false">VLOOKUP(L19,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="T19" s="1" t="str">
         <f aca="false">IF(NOT(D19="1X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c"),IF(E19="landmark",CONCATENATE(A19,"_k"),IF(E19="house",CONCATENATE(A19,"_h"),A19))))</f>
-        <v>none</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U19" s="1" t="str">
         <f aca="false">IF(D19="1X1","none",IF(E19="skyscraper",CONCATENATE(A19,"_c_north"),IF(E19="landmark",CONCATENATE(A19,"_k_north"),IF(E19="house",CONCATENATE(A19,"_h_north"),CONCATENATE(A19,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>none</v>
       </c>
       <c r="V19" s="1" t="str">
-        <f aca="false">IF(OR(D19="1X1",D19="2X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_east"),IF(E19="landmark",CONCATENATE(A19,"_k_east"),CONCATENATE(A19,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D19="1X1",D19="2X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_east"),IF(E19="landmark",CONCATENATE(A19,"_k_east"),IF(E19="house",CONCATENATE(A19,"_h_east"),CONCATENATE(A19,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W19" s="1" t="str">
-        <f aca="false">IF(OR(D19="1X1",D19="1X2"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_west"),IF(E19="landmark",CONCATENATE(A19,"_k_west"),CONCATENATE(A19,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D19="1X1",D19="1X2"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_west"),IF(E19="landmark",CONCATENATE(A19,"_k_west"),IF(E19="house",CONCATENATE(A19,"_h_west"),CONCATENATE(A19,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X19" s="1" t="str">
-        <f aca="false">IF(NOT(D19="2X2"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_south"),IF(E19="landmark",CONCATENATE(A19,"_k_south"),CONCATENATE(A19,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D19="2X2"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c_south"),IF(E19="landmark",CONCATENATE(A19,"_k_south"),IF(E19="house",CONCATENATE(A19,"_h_south"),CONCATENATE(A19,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="M20" s="2" t="str">
         <f aca="false">VLOOKUP(L20,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R20" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="T20" s="1" t="str">
         <f aca="false">IF(NOT(D20="1X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c"),IF(E20="landmark",CONCATENATE(A20,"_k"),IF(E20="house",CONCATENATE(A20,"_h"),A20))))</f>
-        <v>pachinko_k</v>
+        <v>none</v>
       </c>
       <c r="U20" s="1" t="str">
         <f aca="false">IF(D20="1X1","none",IF(E20="skyscraper",CONCATENATE(A20,"_c_north"),IF(E20="landmark",CONCATENATE(A20,"_k_north"),IF(E20="house",CONCATENATE(A20,"_h_north"),CONCATENATE(A20,"_north")))))</f>
-        <v>none</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V20" s="1" t="str">
-        <f aca="false">IF(OR(D20="1X1",D20="2X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_east"),IF(E20="landmark",CONCATENATE(A20,"_k_east"),CONCATENATE(A20,"_east"))))</f>
+        <f aca="false">IF(OR(D20="1X1",D20="2X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_east"),IF(E20="landmark",CONCATENATE(A20,"_k_east"),IF(E20="house",CONCATENATE(A20,"_h_east"),CONCATENATE(A20,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W20" s="1" t="str">
-        <f aca="false">IF(OR(D20="1X1",D20="1X2"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_west"),IF(E20="landmark",CONCATENATE(A20,"_k_west"),CONCATENATE(A20,"_west"))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D20="1X1",D20="1X2"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_west"),IF(E20="landmark",CONCATENATE(A20,"_k_west"),IF(E20="house",CONCATENATE(A20,"_h_west"),CONCATENATE(A20,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X20" s="1" t="str">
-        <f aca="false">IF(NOT(D20="2X2"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_south"),IF(E20="landmark",CONCATENATE(A20,"_k_south"),CONCATENATE(A20,"_south"))))</f>
+        <f aca="false">IF(NOT(D20="2X2"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c_south"),IF(E20="landmark",CONCATENATE(A20,"_k_south"),IF(E20="house",CONCATENATE(A20,"_h_south"),CONCATENATE(A20,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>3</v>
@@ -2345,29 +2357,29 @@
         <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="M21" s="2" t="str">
         <f aca="false">VLOOKUP(L21,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O21" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="Q21" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R21" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="T21" s="1" t="str">
         <f aca="false">IF(NOT(D21="1X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c"),IF(E21="landmark",CONCATENATE(A21,"_k"),IF(E21="house",CONCATENATE(A21,"_h"),A21))))</f>
@@ -2375,105 +2387,105 @@
       </c>
       <c r="U21" s="1" t="str">
         <f aca="false">IF(D21="1X1","none",IF(E21="skyscraper",CONCATENATE(A21,"_c_north"),IF(E21="landmark",CONCATENATE(A21,"_k_north"),IF(E21="house",CONCATENATE(A21,"_h_north"),CONCATENATE(A21,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V21" s="1" t="str">
         <f aca="false">IF(OR(D21="1X1",D21="2X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_east"),IF(E21="landmark",CONCATENATE(A21,"_k_east"),CONCATENATE(A21,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W21" s="1" t="str">
         <f aca="false">IF(OR(D21="1X1",D21="1X2"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_west"),IF(E21="landmark",CONCATENATE(A21,"_k_west"),CONCATENATE(A21,"_west"))))</f>
-        <v>none</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X21" s="1" t="str">
         <f aca="false">IF(NOT(D21="2X2"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c_south"),IF(E21="landmark",CONCATENATE(A21,"_k_south"),CONCATENATE(A21,"_south"))))</f>
-        <v>none</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="G22" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H22" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>1700</v>
+        <v>1980</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="M22" s="2" t="str">
         <f aca="false">VLOOKUP(L22,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N22" s="0" t="n">
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N22" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O22" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="O22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q22" s="1" t="n">
-        <v>10</v>
-      </c>
       <c r="R22" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="T22" s="1" t="str">
         <f aca="false">IF(NOT(D22="1X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c"),IF(E22="landmark",CONCATENATE(A22,"_k"),IF(E22="house",CONCATENATE(A22,"_h"),A22))))</f>
-        <v>none</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U22" s="1" t="str">
         <f aca="false">IF(D22="1X1","none",IF(E22="skyscraper",CONCATENATE(A22,"_c_north"),IF(E22="landmark",CONCATENATE(A22,"_k_north"),IF(E22="house",CONCATENATE(A22,"_h_north"),CONCATENATE(A22,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>none</v>
       </c>
       <c r="V22" s="1" t="str">
         <f aca="false">IF(OR(D22="1X1",D22="2X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_east"),IF(E22="landmark",CONCATENATE(A22,"_k_east"),CONCATENATE(A22,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>none</v>
       </c>
       <c r="W22" s="1" t="str">
         <f aca="false">IF(OR(D22="1X1",D22="1X2"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_west"),IF(E22="landmark",CONCATENATE(A22,"_k_west"),CONCATENATE(A22,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>none</v>
       </c>
       <c r="X22" s="1" t="str">
         <f aca="false">IF(NOT(D22="2X2"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c_south"),IF(E22="landmark",CONCATENATE(A22,"_k_south"),CONCATENATE(A22,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,25 +2496,25 @@
         <v>94</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>95</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>0</v>
+        <v>1970</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>39</v>
@@ -2511,41 +2523,41 @@
         <v>20</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="M23" s="2" t="str">
         <f aca="false">VLOOKUP(L23,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N23" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O23" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N23" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O23" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="T23" s="1" t="str">
         <f aca="false">IF(NOT(D23="1X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c"),IF(E23="landmark",CONCATENATE(A23,"_k"),IF(E23="house",CONCATENATE(A23,"_h"),A23))))</f>
-        <v>shrine_k</v>
+        <v>none</v>
       </c>
       <c r="U23" s="1" t="str">
         <f aca="false">IF(D23="1X1","none",IF(E23="skyscraper",CONCATENATE(A23,"_c_north"),IF(E23="landmark",CONCATENATE(A23,"_k_north"),IF(E23="house",CONCATENATE(A23,"_h_north"),CONCATENATE(A23,"_north")))))</f>
-        <v>none</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V23" s="1" t="str">
         <f aca="false">IF(OR(D23="1X1",D23="2X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_east"),IF(E23="landmark",CONCATENATE(A23,"_k_east"),CONCATENATE(A23,"_east"))))</f>
-        <v>none</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W23" s="1" t="str">
         <f aca="false">IF(OR(D23="1X1",D23="1X2"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c_west"),IF(E23="landmark",CONCATENATE(A23,"_k_west"),CONCATENATE(A23,"_west"))))</f>
@@ -2561,31 +2573,31 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>39</v>
@@ -2594,14 +2606,14 @@
         <v>20</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="M24" s="2" t="str">
         <f aca="false">VLOOKUP(L24,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O24" s="0" t="n">
         <v>3</v>
@@ -2610,65 +2622,65 @@
         <v>59</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R24" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="T24" s="1" t="str">
         <f aca="false">IF(NOT(D24="1X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c"),IF(E24="landmark",CONCATENATE(A24,"_k"),IF(E24="house",CONCATENATE(A24,"_h"),A24))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>none</v>
       </c>
       <c r="U24" s="1" t="str">
         <f aca="false">IF(D24="1X1","none",IF(E24="skyscraper",CONCATENATE(A24,"_c_north"),IF(E24="landmark",CONCATENATE(A24,"_k_north"),IF(E24="house",CONCATENATE(A24,"_h_north"),CONCATENATE(A24,"_north")))))</f>
-        <v>none</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V24" s="1" t="str">
         <f aca="false">IF(OR(D24="1X1",D24="2X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c_east"),IF(E24="landmark",CONCATENATE(A24,"_k_east"),CONCATENATE(A24,"_east"))))</f>
-        <v>none</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W24" s="1" t="str">
         <f aca="false">IF(OR(D24="1X1",D24="1X2"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c_west"),IF(E24="landmark",CONCATENATE(A24,"_k_west"),CONCATENATE(A24,"_west"))))</f>
-        <v>none</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X24" s="1" t="str">
         <f aca="false">IF(NOT(D24="2X2"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c_south"),IF(E24="landmark",CONCATENATE(A24,"_k_south"),CONCATENATE(A24,"_south"))))</f>
-        <v>none</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>39</v>
@@ -2677,81 +2689,81 @@
         <v>20</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="M25" s="2" t="str">
         <f aca="false">VLOOKUP(L25,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O25" s="1" t="n">
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O25" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R25" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T25" s="1" t="str">
         <f aca="false">IF(NOT(D25="1X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c"),IF(E25="landmark",CONCATENATE(A25,"_k"),IF(E25="house",CONCATENATE(A25,"_h"),A25))))</f>
-        <v>none</v>
+        <v>shrine_k</v>
       </c>
       <c r="U25" s="1" t="str">
         <f aca="false">IF(D25="1X1","none",IF(E25="skyscraper",CONCATENATE(A25,"_c_north"),IF(E25="landmark",CONCATENATE(A25,"_k_north"),IF(E25="house",CONCATENATE(A25,"_h_north"),CONCATENATE(A25,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V25" s="1" t="str">
         <f aca="false">IF(OR(D25="1X1",D25="2X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c_east"),IF(E25="landmark",CONCATENATE(A25,"_k_east"),CONCATENATE(A25,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W25" s="1" t="str">
         <f aca="false">IF(OR(D25="1X1",D25="1X2"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c_west"),IF(E25="landmark",CONCATENATE(A25,"_k_west"),CONCATENATE(A25,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X25" s="1" t="str">
         <f aca="false">IF(NOT(D25="2X2"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c_south"),IF(E25="landmark",CONCATENATE(A25,"_k_south"),CONCATENATE(A25,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="G26" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>39</v>
@@ -2760,63 +2772,229 @@
         <v>20</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M26" s="2" t="str">
         <f aca="false">VLOOKUP(L26,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
-      <c r="N26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O26" s="1" t="n">
+      <c r="N26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O26" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>59</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R26" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="T26" s="1" t="str">
         <f aca="false">IF(NOT(D26="1X1"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c"),IF(E26="landmark",CONCATENATE(A26,"_k"),IF(E26="house",CONCATENATE(A26,"_h"),A26))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U26" s="1" t="str">
         <f aca="false">IF(D26="1X1","none",IF(E26="skyscraper",CONCATENATE(A26,"_c_north"),IF(E26="landmark",CONCATENATE(A26,"_k_north"),IF(E26="house",CONCATENATE(A26,"_h_north"),CONCATENATE(A26,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>none</v>
       </c>
       <c r="V26" s="1" t="str">
         <f aca="false">IF(OR(D26="1X1",D26="2X1"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c_east"),IF(E26="landmark",CONCATENATE(A26,"_k_east"),CONCATENATE(A26,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>none</v>
       </c>
       <c r="W26" s="1" t="str">
         <f aca="false">IF(OR(D26="1X1",D26="1X2"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c_west"),IF(E26="landmark",CONCATENATE(A26,"_k_west"),CONCATENATE(A26,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X26" s="1" t="str">
         <f aca="false">IF(NOT(D26="2X2"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c_south"),IF(E26="landmark",CONCATENATE(A26,"_k_south"),CONCATENATE(A26,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M27" s="2" t="str">
+        <f aca="false">VLOOKUP(L27,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R27" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T27" s="1" t="str">
+        <f aca="false">IF(NOT(D27="1X1"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c"),IF(E27="landmark",CONCATENATE(A27,"_k"),IF(E27="house",CONCATENATE(A27,"_h"),A27))))</f>
+        <v>none</v>
+      </c>
+      <c r="U27" s="1" t="str">
+        <f aca="false">IF(D27="1X1","none",IF(E27="skyscraper",CONCATENATE(A27,"_c_north"),IF(E27="landmark",CONCATENATE(A27,"_k_north"),IF(E27="house",CONCATENATE(A27,"_h_north"),CONCATENATE(A27,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V27" s="1" t="str">
+        <f aca="false">IF(OR(D27="1X1",D27="2X1"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c_east"),IF(E27="landmark",CONCATENATE(A27,"_k_east"),CONCATENATE(A27,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W27" s="1" t="str">
+        <f aca="false">IF(OR(D27="1X1",D27="1X2"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c_west"),IF(E27="landmark",CONCATENATE(A27,"_k_west"),CONCATENATE(A27,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X27" s="1" t="str">
+        <f aca="false">IF(NOT(D27="2X2"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c_south"),IF(E27="landmark",CONCATENATE(A27,"_k_south"),CONCATENATE(A27,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M28" s="2" t="str">
+        <f aca="false">VLOOKUP(L28,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="T28" s="1" t="str">
+        <f aca="false">IF(NOT(D28="1X1"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c"),IF(E28="landmark",CONCATENATE(A28,"_k"),IF(E28="house",CONCATENATE(A28,"_h"),A28))))</f>
+        <v>none</v>
+      </c>
+      <c r="U28" s="1" t="str">
+        <f aca="false">IF(D28="1X1","none",IF(E28="skyscraper",CONCATENATE(A28,"_c_north"),IF(E28="landmark",CONCATENATE(A28,"_k_north"),IF(E28="house",CONCATENATE(A28,"_h_north"),CONCATENATE(A28,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V28" s="1" t="str">
+        <f aca="false">IF(OR(D28="1X1",D28="2X1"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c_east"),IF(E28="landmark",CONCATENATE(A28,"_k_east"),CONCATENATE(A28,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W28" s="1" t="str">
+        <f aca="false">IF(OR(D28="1X1",D28="1X2"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c_west"),IF(E28="landmark",CONCATENATE(A28,"_k_west"),CONCATENATE(A28,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X28" s="1" t="str">
+        <f aca="false">IF(NOT(D28="2X2"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c_south"),IF(E28="landmark",CONCATENATE(A28,"_k_south"),CONCATENATE(A28,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y26" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="D27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="S27" s="2"/>
+      <c r="Y28" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="D29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="S29" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2824,15 +3002,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L27" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L29" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P27" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P29" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S27" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S29" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2866,15 +3044,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -2882,7 +3060,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -2890,7 +3068,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -2898,7 +3076,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3</v>
@@ -2906,7 +3084,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
@@ -2914,7 +3092,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
@@ -2922,7 +3100,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -2930,7 +3108,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>7</v>
@@ -2938,7 +3116,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>8</v>
@@ -2946,7 +3124,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>9</v>
@@ -2954,7 +3132,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10</v>
@@ -2962,7 +3140,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>11</v>
@@ -2970,7 +3148,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>12</v>
@@ -2978,7 +3156,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>13</v>
@@ -2986,7 +3164,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>14</v>
@@ -2994,7 +3172,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>15</v>
@@ -3018,7 +3196,7 @@
   </sheetPr>
   <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A234" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H194" activeCellId="0" sqref="H194"/>
     </sheetView>
   </sheetViews>
@@ -3026,16 +3204,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3367,11 +3545,11 @@
       </c>
       <c r="B21" s="1" t="str">
         <f aca="false">IF(C21="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C21" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A21,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D21" s="1" t="n">
         <f aca="false">MAX(IF(C21="ID not in use",0,IF(C21="1X1",1,IF(C21="2X2",4,2)))-1,0)</f>
@@ -3690,11 +3868,11 @@
       </c>
       <c r="B40" s="1" t="str">
         <f aca="false">IF(C40="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C40" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A40,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">IF(C40="Multi-tile",D39-1,MAX(IF(C40="ID not in use",0,IF(C40="1X1",1,IF(C40="2X2",4,2)))-1,0))</f>
@@ -7424,25 +7602,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7456,13 +7634,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -7485,7 +7663,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>59</v>
@@ -7502,49 +7680,49 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7552,29 +7730,29 @@
         <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -7603,40 +7781,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
@@ -7644,24 +7822,24 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: yamashiro, yamashita & onsen
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="192">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -308,6 +308,18 @@
     <t xml:space="preserve">NAME_YAMAGUCHI_OFFICE</t>
   </si>
   <si>
+    <t xml:space="preserve">yamashiro_office_building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_YAMASHIRO_OFFICE_BUILDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yamashita_building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_YAMASHITA_BUILDING</t>
+  </si>
+  <si>
     <t xml:space="preserve">farm</t>
   </si>
   <si>
@@ -341,15 +353,24 @@
     <t xml:space="preserve">single_house</t>
   </si>
   <si>
+    <t xml:space="preserve">onsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_ONSEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">fire_station</t>
   </si>
   <si>
     <t xml:space="preserve">2X1</t>
   </si>
   <si>
-    <t xml:space="preserve">landmark</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME_FIRE_STATION</t>
   </si>
   <si>
@@ -522,6 +543,9 @@
   </si>
   <si>
     <t xml:space="preserve">bitmask(TOWNZONE_CENTRE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</t>
   </si>
   <si>
     <t xml:space="preserve">bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</t>
@@ -694,14 +718,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -725,8 +749,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="23.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="29.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="28.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="17.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="17.7"/>
@@ -3086,56 +3110,56 @@
         <v>94</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G29" s="1" t="n">
-        <v>15</v>
+        <v>255</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>1700</v>
+        <v>1990</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="M29" s="2" t="str">
         <f aca="false">VLOOKUP(L29,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="R29" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="T29" s="1" t="str">
         <f aca="false">IF(NOT(D29="1X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c"),IF(E29="landmark",CONCATENATE(A29,"_k"),IF(E29="house",CONCATENATE(A29,"_h"),A29))))</f>
@@ -3143,165 +3167,165 @@
       </c>
       <c r="U29" s="1" t="str">
         <f aca="false">IF(D29="1X1","none",IF(E29="skyscraper",CONCATENATE(A29,"_c_north"),IF(E29="landmark",CONCATENATE(A29,"_k_north"),IF(E29="house",CONCATENATE(A29,"_h_north"),CONCATENATE(A29,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>yamashiro_office_building_c_north</v>
       </c>
       <c r="V29" s="1" t="str">
-        <f aca="false">IF(OR(D29="1X1",D29="2X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c_east"),IF(E29="landmark",CONCATENATE(A29,"_k_east"),IF(E29="house",CONCATENATE(A29,"_h_east"),CONCATENATE(A29,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D29="1X1",D29="2X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c_east"),IF(E29="landmark",CONCATENATE(A29,"_k_east"),CONCATENATE(A29,"_east"))))</f>
+        <v>yamashiro_office_building_c_east</v>
       </c>
       <c r="W29" s="1" t="str">
-        <f aca="false">IF(OR(D29="1X1",D29="1X2"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c_west"),IF(E29="landmark",CONCATENATE(A29,"_k_west"),IF(E29="house",CONCATENATE(A29,"_h_west"),CONCATENATE(A29,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D29="1X1",D29="1X2"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c_west"),IF(E29="landmark",CONCATENATE(A29,"_k_west"),CONCATENATE(A29,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X29" s="1" t="str">
-        <f aca="false">IF(NOT(D29="2X2"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c_south"),IF(E29="landmark",CONCATENATE(A29,"_k_south"),IF(E29="house",CONCATENATE(A29,"_h_south"),CONCATENATE(A29,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D29="2X2"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c_south"),IF(E29="landmark",CONCATENATE(A29,"_k_south"),CONCATENATE(A29,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>1870</v>
+        <v>2000</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="M30" s="2" t="str">
         <f aca="false">VLOOKUP(L30,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="R30" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="T30" s="1" t="str">
         <f aca="false">IF(NOT(D30="1X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c"),IF(E30="landmark",CONCATENATE(A30,"_k"),IF(E30="house",CONCATENATE(A30,"_h"),A30))))</f>
-        <v>naganuma_h</v>
+        <v>yamashita_building_c</v>
       </c>
       <c r="U30" s="1" t="str">
         <f aca="false">IF(D30="1X1","none",IF(E30="skyscraper",CONCATENATE(A30,"_c_north"),IF(E30="landmark",CONCATENATE(A30,"_k_north"),IF(E30="house",CONCATENATE(A30,"_h_north"),CONCATENATE(A30,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V30" s="1" t="str">
-        <f aca="false">IF(OR(D30="1X1",D30="2X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_east"),IF(E30="landmark",CONCATENATE(A30,"_k_east"),IF(E30="house",CONCATENATE(A30,"_h_east"),CONCATENATE(A30,"_east")))))</f>
+        <f aca="false">IF(OR(D30="1X1",D30="2X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_east"),IF(E30="landmark",CONCATENATE(A30,"_k_east"),CONCATENATE(A30,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W30" s="1" t="str">
-        <f aca="false">IF(OR(D30="1X1",D30="1X2"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_west"),IF(E30="landmark",CONCATENATE(A30,"_k_west"),IF(E30="house",CONCATENATE(A30,"_h_west"),CONCATENATE(A30,"_west")))))</f>
+        <f aca="false">IF(OR(D30="1X1",D30="1X2"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_west"),IF(E30="landmark",CONCATENATE(A30,"_k_west"),CONCATENATE(A30,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X30" s="1" t="str">
-        <f aca="false">IF(NOT(D30="2X2"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_south"),IF(E30="landmark",CONCATENATE(A30,"_k_south"),IF(E30="house",CONCATENATE(A30,"_h_south"),CONCATENATE(A30,"_south")))))</f>
+        <f aca="false">IF(NOT(D30="2X2"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_south"),IF(E30="landmark",CONCATENATE(A30,"_k_south"),CONCATENATE(A30,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M31" s="2" t="str">
         <f aca="false">VLOOKUP(L31,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R31" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="T31" s="1" t="str">
         <f aca="false">IF(NOT(D31="1X1"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c"),IF(E31="landmark",CONCATENATE(A31,"_k"),IF(E31="house",CONCATENATE(A31,"_h"),A31))))</f>
@@ -3309,134 +3333,134 @@
       </c>
       <c r="U31" s="1" t="str">
         <f aca="false">IF(D31="1X1","none",IF(E31="skyscraper",CONCATENATE(A31,"_c_north"),IF(E31="landmark",CONCATENATE(A31,"_k_north"),IF(E31="house",CONCATENATE(A31,"_h_north"),CONCATENATE(A31,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V31" s="1" t="str">
         <f aca="false">IF(OR(D31="1X1",D31="2X1"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c_east"),IF(E31="landmark",CONCATENATE(A31,"_k_east"),IF(E31="house",CONCATENATE(A31,"_h_east"),CONCATENATE(A31,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W31" s="1" t="str">
         <f aca="false">IF(OR(D31="1X1",D31="1X2"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c_west"),IF(E31="landmark",CONCATENATE(A31,"_k_west"),IF(E31="house",CONCATENATE(A31,"_h_west"),CONCATENATE(A31,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X31" s="1" t="str">
         <f aca="false">IF(NOT(D31="2X2"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c_south"),IF(E31="landmark",CONCATENATE(A31,"_k_south"),IF(E31="house",CONCATENATE(A31,"_h_south"),CONCATENATE(A31,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M32" s="2" t="str">
         <f aca="false">VLOOKUP(L32,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R32" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="T32" s="1" t="str">
         <f aca="false">IF(NOT(D32="1X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c"),IF(E32="landmark",CONCATENATE(A32,"_k"),IF(E32="house",CONCATENATE(A32,"_h"),A32))))</f>
-        <v>none</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U32" s="1" t="str">
         <f aca="false">IF(D32="1X1","none",IF(E32="skyscraper",CONCATENATE(A32,"_c_north"),IF(E32="landmark",CONCATENATE(A32,"_k_north"),IF(E32="house",CONCATENATE(A32,"_h_north"),CONCATENATE(A32,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>none</v>
       </c>
       <c r="V32" s="1" t="str">
-        <f aca="false">IF(OR(D32="1X1",D32="2X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_east"),IF(E32="landmark",CONCATENATE(A32,"_k_east"),CONCATENATE(A32,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D32="1X1",D32="2X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_east"),IF(E32="landmark",CONCATENATE(A32,"_k_east"),IF(E32="house",CONCATENATE(A32,"_h_east"),CONCATENATE(A32,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W32" s="1" t="str">
-        <f aca="false">IF(OR(D32="1X1",D32="1X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_west"),IF(E32="landmark",CONCATENATE(A32,"_k_west"),CONCATENATE(A32,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D32="1X1",D32="1X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_west"),IF(E32="landmark",CONCATENATE(A32,"_k_west"),IF(E32="house",CONCATENATE(A32,"_h_west"),CONCATENATE(A32,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X32" s="1" t="str">
-        <f aca="false">IF(NOT(D32="2X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_south"),IF(E32="landmark",CONCATENATE(A32,"_k_south"),CONCATENATE(A32,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D32="2X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_south"),IF(E32="landmark",CONCATENATE(A32,"_k_south"),IF(E32="house",CONCATENATE(A32,"_h_south"),CONCATENATE(A32,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>1980</v>
+        <v>1870</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>39</v>
@@ -3445,11 +3469,11 @@
         <v>10</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="M33" s="2" t="str">
         <f aca="false">VLOOKUP(L33,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
       <c r="N33" s="1" t="n">
         <v>29</v>
@@ -3458,59 +3482,59 @@
         <v>3</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="T33" s="1" t="str">
         <f aca="false">IF(NOT(D33="1X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c"),IF(E33="landmark",CONCATENATE(A33,"_k"),IF(E33="house",CONCATENATE(A33,"_h"),A33))))</f>
-        <v>pachinko_k</v>
+        <v>onsen_k</v>
       </c>
       <c r="U33" s="1" t="str">
         <f aca="false">IF(D33="1X1","none",IF(E33="skyscraper",CONCATENATE(A33,"_c_north"),IF(E33="landmark",CONCATENATE(A33,"_k_north"),IF(E33="house",CONCATENATE(A33,"_h_north"),CONCATENATE(A33,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V33" s="1" t="str">
-        <f aca="false">IF(OR(D33="1X1",D33="2X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_east"),IF(E33="landmark",CONCATENATE(A33,"_k_east"),CONCATENATE(A33,"_east"))))</f>
+        <f aca="false">IF(OR(D33="1X1",D33="2X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_east"),IF(E33="landmark",CONCATENATE(A33,"_k_east"),IF(E33="house",CONCATENATE(A33,"_h_east"),CONCATENATE(A33,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W33" s="1" t="str">
-        <f aca="false">IF(OR(D33="1X1",D33="1X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_west"),IF(E33="landmark",CONCATENATE(A33,"_k_west"),CONCATENATE(A33,"_west"))))</f>
+        <f aca="false">IF(OR(D33="1X1",D33="1X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_west"),IF(E33="landmark",CONCATENATE(A33,"_k_west"),IF(E33="house",CONCATENATE(A33,"_h_west"),CONCATENATE(A33,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X33" s="1" t="str">
-        <f aca="false">IF(NOT(D33="2X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_south"),IF(E33="landmark",CONCATENATE(A33,"_k_south"),CONCATENATE(A33,"_south"))))</f>
+        <f aca="false">IF(NOT(D33="2X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_south"),IF(E33="landmark",CONCATENATE(A33,"_k_south"),IF(E33="house",CONCATENATE(A33,"_h_south"),CONCATENATE(A33,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>80</v>
@@ -3528,20 +3552,20 @@
         <v>20</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="M34" s="2" t="str">
         <f aca="false">VLOOKUP(L34,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="O34" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="Q34" s="1" t="n">
         <v>10</v>
@@ -3550,7 +3574,7 @@
         <v>2</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="T34" s="1" t="str">
         <f aca="false">IF(NOT(D34="1X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c"),IF(E34="landmark",CONCATENATE(A34,"_k"),IF(E34="house",CONCATENATE(A34,"_h"),A34))))</f>
@@ -3558,51 +3582,51 @@
       </c>
       <c r="U34" s="1" t="str">
         <f aca="false">IF(D34="1X1","none",IF(E34="skyscraper",CONCATENATE(A34,"_c_north"),IF(E34="landmark",CONCATENATE(A34,"_k_north"),IF(E34="house",CONCATENATE(A34,"_h_north"),CONCATENATE(A34,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V34" s="1" t="str">
-        <f aca="false">IF(OR(D34="1X1",D34="2X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_east"),IF(E34="landmark",CONCATENATE(A34,"_k_east"),CONCATENATE(A34,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <f aca="false">IF(OR(D34="1X1",D34="2X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_east"),IF(E34="landmark",CONCATENATE(A34,"_k_east"),IF(E34="house",CONCATENATE(A34,"_h_east"),CONCATENATE(A34,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W34" s="1" t="str">
-        <f aca="false">IF(OR(D34="1X1",D34="1X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_west"),IF(E34="landmark",CONCATENATE(A34,"_k_west"),CONCATENATE(A34,"_west"))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D34="1X1",D34="1X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_west"),IF(E34="landmark",CONCATENATE(A34,"_k_west"),IF(E34="house",CONCATENATE(A34,"_h_west"),CONCATENATE(A34,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X34" s="1" t="str">
-        <f aca="false">IF(NOT(D34="2X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_south"),IF(E34="landmark",CONCATENATE(A34,"_k_south"),CONCATENATE(A34,"_south"))))</f>
+        <f aca="false">IF(NOT(D34="2X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_south"),IF(E34="landmark",CONCATENATE(A34,"_k_south"),IF(E34="house",CONCATENATE(A34,"_h_south"),CONCATENATE(A34,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H35" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>39</v>
@@ -3611,29 +3635,29 @@
         <v>20</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="M35" s="2" t="str">
         <f aca="false">VLOOKUP(L35,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
-      <c r="N35" s="0" t="n">
+      <c r="N35" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="O35" s="0" t="n">
+      <c r="O35" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R35" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="T35" s="1" t="str">
         <f aca="false">IF(NOT(D35="1X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c"),IF(E35="landmark",CONCATENATE(A35,"_k"),IF(E35="house",CONCATENATE(A35,"_h"),A35))))</f>
@@ -3641,22 +3665,22 @@
       </c>
       <c r="U35" s="1" t="str">
         <f aca="false">IF(D35="1X1","none",IF(E35="skyscraper",CONCATENATE(A35,"_c_north"),IF(E35="landmark",CONCATENATE(A35,"_k_north"),IF(E35="house",CONCATENATE(A35,"_h_north"),CONCATENATE(A35,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V35" s="1" t="str">
         <f aca="false">IF(OR(D35="1X1",D35="2X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_east"),IF(E35="landmark",CONCATENATE(A35,"_k_east"),CONCATENATE(A35,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W35" s="1" t="str">
         <f aca="false">IF(OR(D35="1X1",D35="1X2"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_west"),IF(E35="landmark",CONCATENATE(A35,"_k_west"),CONCATENATE(A35,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X35" s="1" t="str">
         <f aca="false">IF(NOT(D35="2X2"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_south"),IF(E35="landmark",CONCATENATE(A35,"_k_south"),CONCATENATE(A35,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3667,60 +3691,60 @@
         <v>120</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H36" s="0" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>0</v>
+        <v>1980</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="M36" s="2" t="str">
         <f aca="false">VLOOKUP(L36,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N36" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O36" s="0" t="n">
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="Q36" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R36" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T36" s="1" t="str">
         <f aca="false">IF(NOT(D36="1X1"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c"),IF(E36="landmark",CONCATENATE(A36,"_k"),IF(E36="house",CONCATENATE(A36,"_h"),A36))))</f>
-        <v>shrine_k</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U36" s="1" t="str">
         <f aca="false">IF(D36="1X1","none",IF(E36="skyscraper",CONCATENATE(A36,"_c_north"),IF(E36="landmark",CONCATENATE(A36,"_k_north"),IF(E36="house",CONCATENATE(A36,"_h_north"),CONCATENATE(A36,"_north")))))</f>
@@ -3744,31 +3768,31 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="G37" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <v>5</v>
+        <v>80</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>0</v>
+        <v>1970</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>39</v>
@@ -3777,41 +3801,41 @@
         <v>20</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="M37" s="2" t="str">
         <f aca="false">VLOOKUP(L37,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N37" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O37" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O37" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="Q37" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R37" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="T37" s="1" t="str">
         <f aca="false">IF(NOT(D37="1X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c"),IF(E37="landmark",CONCATENATE(A37,"_k"),IF(E37="house",CONCATENATE(A37,"_h"),A37))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>none</v>
       </c>
       <c r="U37" s="1" t="str">
         <f aca="false">IF(D37="1X1","none",IF(E37="skyscraper",CONCATENATE(A37,"_c_north"),IF(E37="landmark",CONCATENATE(A37,"_k_north"),IF(E37="house",CONCATENATE(A37,"_h_north"),CONCATENATE(A37,"_north")))))</f>
-        <v>none</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V37" s="1" t="str">
         <f aca="false">IF(OR(D37="1X1",D37="2X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c_east"),IF(E37="landmark",CONCATENATE(A37,"_k_east"),CONCATENATE(A37,"_east"))))</f>
-        <v>none</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W37" s="1" t="str">
         <f aca="false">IF(OR(D37="1X1",D37="1X2"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c_west"),IF(E37="landmark",CONCATENATE(A37,"_k_west"),CONCATENATE(A37,"_west"))))</f>
@@ -3822,36 +3846,36 @@
         <v>none</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="G38" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H38" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>39</v>
@@ -3860,29 +3884,29 @@
         <v>20</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="M38" s="2" t="str">
         <f aca="false">VLOOKUP(L38,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
-      <c r="N38" s="1" t="n">
+      <c r="N38" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O38" s="1" t="n">
+      <c r="O38" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="Q38" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R38" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="T38" s="1" t="str">
         <f aca="false">IF(NOT(D38="1X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c"),IF(E38="landmark",CONCATENATE(A38,"_k"),IF(E38="house",CONCATENATE(A38,"_h"),A38))))</f>
@@ -3890,51 +3914,51 @@
       </c>
       <c r="U38" s="1" t="str">
         <f aca="false">IF(D38="1X1","none",IF(E38="skyscraper",CONCATENATE(A38,"_c_north"),IF(E38="landmark",CONCATENATE(A38,"_k_north"),IF(E38="house",CONCATENATE(A38,"_h_north"),CONCATENATE(A38,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V38" s="1" t="str">
         <f aca="false">IF(OR(D38="1X1",D38="2X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_east"),IF(E38="landmark",CONCATENATE(A38,"_k_east"),CONCATENATE(A38,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W38" s="1" t="str">
         <f aca="false">IF(OR(D38="1X1",D38="1X2"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_west"),IF(E38="landmark",CONCATENATE(A38,"_k_west"),CONCATENATE(A38,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X38" s="1" t="str">
         <f aca="false">IF(NOT(D38="2X2"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_south"),IF(E38="landmark",CONCATENATE(A38,"_k_south"),CONCATENATE(A38,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>208</v>
+        <v>114</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>39</v>
@@ -3943,63 +3967,312 @@
         <v>20</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="M39" s="2" t="str">
         <f aca="false">VLOOKUP(L39,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
-      <c r="N39" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O39" s="1" t="n">
+      <c r="N39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O39" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P39" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Q39" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R39" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="T39" s="1" t="str">
         <f aca="false">IF(NOT(D39="1X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c"),IF(E39="landmark",CONCATENATE(A39,"_k"),IF(E39="house",CONCATENATE(A39,"_h"),A39))))</f>
-        <v>none</v>
+        <v>shrine_k</v>
       </c>
       <c r="U39" s="1" t="str">
         <f aca="false">IF(D39="1X1","none",IF(E39="skyscraper",CONCATENATE(A39,"_c_north"),IF(E39="landmark",CONCATENATE(A39,"_k_north"),IF(E39="house",CONCATENATE(A39,"_h_north"),CONCATENATE(A39,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>none</v>
       </c>
       <c r="V39" s="1" t="str">
         <f aca="false">IF(OR(D39="1X1",D39="2X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_east"),IF(E39="landmark",CONCATENATE(A39,"_k_east"),CONCATENATE(A39,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>none</v>
       </c>
       <c r="W39" s="1" t="str">
         <f aca="false">IF(OR(D39="1X1",D39="1X2"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_west"),IF(E39="landmark",CONCATENATE(A39,"_k_west"),CONCATENATE(A39,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X39" s="1" t="str">
         <f aca="false">IF(NOT(D39="2X2"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_south"),IF(E39="landmark",CONCATENATE(A39,"_k_south"),CONCATENATE(A39,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y39" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M40" s="2" t="str">
+        <f aca="false">VLOOKUP(L40,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="T40" s="1" t="str">
+        <f aca="false">IF(NOT(D40="1X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c"),IF(E40="landmark",CONCATENATE(A40,"_k"),IF(E40="house",CONCATENATE(A40,"_h"),A40))))</f>
+        <v>shrine_prohibition_k</v>
+      </c>
+      <c r="U40" s="1" t="str">
+        <f aca="false">IF(D40="1X1","none",IF(E40="skyscraper",CONCATENATE(A40,"_c_north"),IF(E40="landmark",CONCATENATE(A40,"_k_north"),IF(E40="house",CONCATENATE(A40,"_h_north"),CONCATENATE(A40,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V40" s="1" t="str">
+        <f aca="false">IF(OR(D40="1X1",D40="2X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_east"),IF(E40="landmark",CONCATENATE(A40,"_k_east"),CONCATENATE(A40,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W40" s="1" t="str">
+        <f aca="false">IF(OR(D40="1X1",D40="1X2"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_west"),IF(E40="landmark",CONCATENATE(A40,"_k_west"),CONCATENATE(A40,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X40" s="1" t="str">
+        <f aca="false">IF(NOT(D40="2X2"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_south"),IF(E40="landmark",CONCATENATE(A40,"_k_south"),CONCATENATE(A40,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y40" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M41" s="2" t="str">
+        <f aca="false">VLOOKUP(L41,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R41" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T41" s="1" t="str">
+        <f aca="false">IF(NOT(D41="1X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c"),IF(E41="landmark",CONCATENATE(A41,"_k"),IF(E41="house",CONCATENATE(A41,"_h"),A41))))</f>
+        <v>none</v>
+      </c>
+      <c r="U41" s="1" t="str">
+        <f aca="false">IF(D41="1X1","none",IF(E41="skyscraper",CONCATENATE(A41,"_c_north"),IF(E41="landmark",CONCATENATE(A41,"_k_north"),IF(E41="house",CONCATENATE(A41,"_h_north"),CONCATENATE(A41,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V41" s="1" t="str">
+        <f aca="false">IF(OR(D41="1X1",D41="2X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_east"),IF(E41="landmark",CONCATENATE(A41,"_k_east"),CONCATENATE(A41,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W41" s="1" t="str">
+        <f aca="false">IF(OR(D41="1X1",D41="1X2"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_west"),IF(E41="landmark",CONCATENATE(A41,"_k_west"),CONCATENATE(A41,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X41" s="1" t="str">
+        <f aca="false">IF(NOT(D41="2X2"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_south"),IF(E41="landmark",CONCATENATE(A41,"_k_south"),CONCATENATE(A41,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y41" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M42" s="2" t="str">
+        <f aca="false">VLOOKUP(L42,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O42" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q42" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R42" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="T42" s="1" t="str">
+        <f aca="false">IF(NOT(D42="1X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c"),IF(E42="landmark",CONCATENATE(A42,"_k"),IF(E42="house",CONCATENATE(A42,"_h"),A42))))</f>
+        <v>none</v>
+      </c>
+      <c r="U42" s="1" t="str">
+        <f aca="false">IF(D42="1X1","none",IF(E42="skyscraper",CONCATENATE(A42,"_c_north"),IF(E42="landmark",CONCATENATE(A42,"_k_north"),IF(E42="house",CONCATENATE(A42,"_h_north"),CONCATENATE(A42,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V42" s="1" t="str">
+        <f aca="false">IF(OR(D42="1X1",D42="2X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_east"),IF(E42="landmark",CONCATENATE(A42,"_k_east"),CONCATENATE(A42,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W42" s="1" t="str">
+        <f aca="false">IF(OR(D42="1X1",D42="1X2"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_west"),IF(E42="landmark",CONCATENATE(A42,"_k_west"),CONCATENATE(A42,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X42" s="1" t="str">
+        <f aca="false">IF(NOT(D42="2X2"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_south"),IF(E42="landmark",CONCATENATE(A42,"_k_south"),CONCATENATE(A42,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y39" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="D40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="S40" s="2"/>
+      <c r="Y42" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="D43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="S43" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
@@ -4010,15 +4283,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L40" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L43" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P40" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P43" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S40" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S43" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4052,15 +4325,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -4068,7 +4341,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -4076,7 +4349,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -4084,7 +4357,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3</v>
@@ -4092,7 +4365,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
@@ -4100,7 +4373,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
@@ -4108,7 +4381,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -4116,7 +4389,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>7</v>
@@ -4124,7 +4397,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>8</v>
@@ -4132,7 +4405,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>9</v>
@@ -4140,7 +4413,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10</v>
@@ -4148,7 +4421,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>11</v>
@@ -4156,7 +4429,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>12</v>
@@ -4164,7 +4437,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>13</v>
@@ -4172,7 +4445,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>14</v>
@@ -4180,7 +4453,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>15</v>
@@ -4212,16 +4485,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5029,11 +5302,11 @@
       </c>
       <c r="B49" s="1" t="str">
         <f aca="false">IF(C49="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C49" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A49,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D49" s="1" t="n">
         <f aca="false">IF(C49="Multi-tile",D48-1,MAX(IF(C49="ID not in use",0,IF(C49="1X1",1,IF(C49="2X2",4,2)))-1,0))</f>
@@ -5811,11 +6084,11 @@
       </c>
       <c r="B95" s="1" t="str">
         <f aca="false">IF(C95="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C95" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A95,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D95" s="1" t="n">
         <f aca="false">IF(C95="Multi-tile",D94-1,MAX(IF(C95="ID not in use",0,IF(C95="1X1",1,IF(C95="2X2",4,2)))-1,0))</f>
@@ -5947,15 +6220,15 @@
       </c>
       <c r="B103" s="1" t="str">
         <f aca="false">IF(C103="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C103" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A103,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X2</v>
       </c>
       <c r="D103" s="1" t="n">
         <f aca="false">IF(C103="Multi-tile",D102-1,MAX(IF(C103="ID not in use",0,IF(C103="1X1",1,IF(C103="2X2",4,2)))-1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8592,10 +8865,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8604,31 +8877,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="81.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="83.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="59.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8642,13 +8915,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -8671,7 +8944,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>67</v>
@@ -8688,49 +8961,49 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8738,29 +9011,37 @@
         <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>168</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -8789,40 +9070,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>64</v>
@@ -8830,24 +9111,24 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: okada_office_tower & old_office_building
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="175">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -213,6 +213,39 @@
     <t xml:space="preserve">murakami_m</t>
   </si>
   <si>
+    <t xml:space="preserve">okada_office_tower_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okada_office_tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_OKADA_OFFICE_TOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okada_office_tower_l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okada_office_tower_x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old_office_building_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old_office_building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_OLD_OFFICE_BUILDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old_office_building_l</t>
+  </si>
+  <si>
     <t xml:space="preserve">yano_m</t>
   </si>
   <si>
@@ -226,9 +259,6 @@
   </si>
   <si>
     <t xml:space="preserve">NAME_BANK_BUILDING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 only</t>
   </si>
   <si>
     <t xml:space="preserve">bitmask(HOUSE_FLAG_NOT_SLOPED,HOUSE_FLAG_PROTECTED)</t>
@@ -643,14 +673,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y45"/>
+  <dimension ref="A1:Y50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1953,10 +1983,10 @@
         <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>27</v>
@@ -1965,7 +1995,7 @@
         <v>28</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>100</v>
@@ -1974,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>1970</v>
+        <v>1955</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>39</v>
@@ -1999,9 +2029,11 @@
         <v>31</v>
       </c>
       <c r="Q16" s="1" t="n">
+        <f aca="false">VLOOKUP(E16,dropdowns!A:C,2,0)</f>
         <v>10</v>
       </c>
       <c r="R16" s="1" t="n">
+        <f aca="false">VLOOKUP(E16,dropdowns!A:C,3,0)</f>
         <v>4</v>
       </c>
       <c r="S16" s="3" t="s">
@@ -2009,7 +2041,7 @@
       </c>
       <c r="T16" s="1" t="str">
         <f aca="false">IF(NOT(D16="1X1"),"none",IF(E16="skyscraper",CONCATENATE(A16,"_c"),IF(E16="landmark",CONCATENATE(A16,"_k"),IF(E16="house",CONCATENATE(A16,"_h"),A16))))</f>
-        <v>yano_m</v>
+        <v>okada_office_tower_m</v>
       </c>
       <c r="U16" s="1" t="str">
         <f aca="false">IF(D16="1X1","none",IF(E16="skyscraper",CONCATENATE(A16,"_c_north"),IF(E16="landmark",CONCATENATE(A16,"_k_north"),IF(E16="house",CONCATENATE(A16,"_h_north"),CONCATENATE(A16,"_north")))))</f>
@@ -2033,66 +2065,66 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>66</v>
+      <c r="E17" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>220</v>
+        <v>125</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>1980</v>
+        <v>1955</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="M17" s="3" t="str">
         <f aca="false">VLOOKUP(L17,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="O17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R17" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q17" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="R17" s="1" t="n">
-        <v>6</v>
       </c>
       <c r="S17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="T17" s="1" t="str">
         <f aca="false">IF(NOT(D17="1X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c"),IF(E17="landmark",CONCATENATE(A17,"_k"),IF(E17="house",CONCATENATE(A17,"_h"),A17))))</f>
-        <v>bank_building_c</v>
+        <v>okada_office_tower_l</v>
       </c>
       <c r="U17" s="1" t="str">
         <f aca="false">IF(D17="1X1","none",IF(E17="skyscraper",CONCATENATE(A17,"_c_north"),IF(E17="landmark",CONCATENATE(A17,"_k_north"),IF(E17="house",CONCATENATE(A17,"_h_north"),CONCATENATE(A17,"_north")))))</f>
@@ -2116,66 +2148,66 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>66</v>
+      <c r="E18" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>1990</v>
+        <v>1955</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M18" s="3" t="str">
         <f aca="false">VLOOKUP(L18,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N18" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O18" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O18" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P18" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R18" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="T18" s="1" t="str">
         <f aca="false">IF(NOT(D18="1X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c"),IF(E18="landmark",CONCATENATE(A18,"_k"),IF(E18="house",CONCATENATE(A18,"_h"),A18))))</f>
-        <v>enterprise_tower_c</v>
+        <v>okada_office_tower_x</v>
       </c>
       <c r="U18" s="1" t="str">
         <f aca="false">IF(D18="1X1","none",IF(E18="skyscraper",CONCATENATE(A18,"_c_north"),IF(E18="landmark",CONCATENATE(A18,"_k_north"),IF(E18="house",CONCATENATE(A18,"_h_north"),CONCATENATE(A18,"_north")))))</f>
@@ -2199,66 +2231,66 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>66</v>
+      <c r="E19" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>1960</v>
+        <v>1945</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="M19" s="3" t="str">
         <f aca="false">VLOOKUP(L19,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N19" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O19" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O19" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P19" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="T19" s="1" t="str">
         <f aca="false">IF(NOT(D19="1X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c"),IF(E19="landmark",CONCATENATE(A19,"_k"),IF(E19="house",CONCATENATE(A19,"_h"),A19))))</f>
-        <v>insurance_tower_c</v>
+        <v>old_office_building_m</v>
       </c>
       <c r="U19" s="1" t="str">
         <f aca="false">IF(D19="1X1","none",IF(E19="skyscraper",CONCATENATE(A19,"_c_north"),IF(E19="landmark",CONCATENATE(A19,"_k_north"),IF(E19="house",CONCATENATE(A19,"_h_north"),CONCATENATE(A19,"_north")))))</f>
@@ -2282,66 +2314,66 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>66</v>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>220</v>
+        <v>125</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>2000</v>
+        <v>1945</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="M20" s="3" t="str">
         <f aca="false">VLOOKUP(L20,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N20" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O20" s="1" t="n">
+      <c r="P20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R20" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="P20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q20" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="R20" s="1" t="n">
-        <v>10</v>
-      </c>
       <c r="S20" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="T20" s="1" t="str">
         <f aca="false">IF(NOT(D20="1X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c"),IF(E20="landmark",CONCATENATE(A20,"_k"),IF(E20="house",CONCATENATE(A20,"_h"),A20))))</f>
-        <v>kuroi_tower_c</v>
+        <v>old_office_building_l</v>
       </c>
       <c r="U20" s="1" t="str">
         <f aca="false">IF(D20="1X1","none",IF(E20="skyscraper",CONCATENATE(A20,"_c_north"),IF(E20="landmark",CONCATENATE(A20,"_k_north"),IF(E20="house",CONCATENATE(A20,"_h_north"),CONCATENATE(A20,"_north")))))</f>
@@ -2365,66 +2397,66 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>66</v>
+      <c r="E21" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>2000</v>
+        <v>1970</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="M21" s="3" t="str">
         <f aca="false">VLOOKUP(L21,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N21" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O21" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P21" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="R21" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="T21" s="1" t="str">
         <f aca="false">IF(NOT(D21="1X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c"),IF(E21="landmark",CONCATENATE(A21,"_k"),IF(E21="house",CONCATENATE(A21,"_h"),A21))))</f>
-        <v>mitsui_tower_c</v>
+        <v>yano_m</v>
       </c>
       <c r="U21" s="1" t="str">
         <f aca="false">IF(D21="1X1","none",IF(E21="skyscraper",CONCATENATE(A21,"_c_north"),IF(E21="landmark",CONCATENATE(A21,"_k_north"),IF(E21="house",CONCATENATE(A21,"_h_north"),CONCATENATE(A21,"_north")))))</f>
@@ -2448,22 +2480,22 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>220</v>
@@ -2472,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>2000</v>
+        <v>1980</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>39</v>
@@ -2481,33 +2513,33 @@
         <v>25</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M22" s="3" t="str">
         <f aca="false">VLOOKUP(L22,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="O22" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R22" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="T22" s="1" t="str">
         <f aca="false">IF(NOT(D22="1X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c"),IF(E22="landmark",CONCATENATE(A22,"_k"),IF(E22="house",CONCATENATE(A22,"_h"),A22))))</f>
-        <v>modern_office_tower_c</v>
+        <v>bank_building_c</v>
       </c>
       <c r="U22" s="1" t="str">
         <f aca="false">IF(D22="1X1","none",IF(E22="skyscraper",CONCATENATE(A22,"_c_north"),IF(E22="landmark",CONCATENATE(A22,"_k_north"),IF(E22="house",CONCATENATE(A22,"_h_north"),CONCATENATE(A22,"_north")))))</f>
@@ -2531,22 +2563,22 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="n">
         <v>81</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G23" s="1" t="n">
         <v>220</v>
@@ -2564,7 +2596,7 @@
         <v>25</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M23" s="3" t="str">
         <f aca="false">VLOOKUP(L23,dropdowns!E:F,2,0)</f>
@@ -2577,7 +2609,7 @@
         <v>5</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q23" s="1" t="n">
         <v>24</v>
@@ -2586,11 +2618,11 @@
         <v>10</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T23" s="1" t="str">
         <f aca="false">IF(NOT(D23="1X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c"),IF(E23="landmark",CONCATENATE(A23,"_k"),IF(E23="house",CONCATENATE(A23,"_h"),A23))))</f>
-        <v>multimedia_offices_c</v>
+        <v>enterprise_tower_c</v>
       </c>
       <c r="U23" s="1" t="str">
         <f aca="false">IF(D23="1X1","none",IF(E23="skyscraper",CONCATENATE(A23,"_c_north"),IF(E23="landmark",CONCATENATE(A23,"_k_north"),IF(E23="house",CONCATENATE(A23,"_h_north"),CONCATENATE(A23,"_north")))))</f>
@@ -2620,25 +2652,25 @@
         <v>83</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>84</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>2000</v>
+        <v>1960</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>39</v>
@@ -2647,7 +2679,7 @@
         <v>25</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M24" s="3" t="str">
         <f aca="false">VLOOKUP(L24,dropdowns!E:F,2,0)</f>
@@ -2660,7 +2692,7 @@
         <v>5</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q24" s="1" t="n">
         <v>24</v>
@@ -2669,11 +2701,11 @@
         <v>10</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T24" s="1" t="str">
         <f aca="false">IF(NOT(D24="1X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c"),IF(E24="landmark",CONCATENATE(A24,"_k"),IF(E24="house",CONCATENATE(A24,"_h"),A24))))</f>
-        <v>office_tower_c</v>
+        <v>insurance_tower_c</v>
       </c>
       <c r="U24" s="1" t="str">
         <f aca="false">IF(D24="1X1","none",IF(E24="skyscraper",CONCATENATE(A24,"_c_north"),IF(E24="landmark",CONCATENATE(A24,"_k_north"),IF(E24="house",CONCATENATE(A24,"_h_north"),CONCATENATE(A24,"_north")))))</f>
@@ -2703,25 +2735,25 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>1960</v>
+        <v>2000</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>39</v>
@@ -2730,7 +2762,7 @@
         <v>25</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M25" s="3" t="str">
         <f aca="false">VLOOKUP(L25,dropdowns!E:F,2,0)</f>
@@ -2743,7 +2775,7 @@
         <v>5</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q25" s="1" t="n">
         <v>24</v>
@@ -2752,11 +2784,11 @@
         <v>10</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T25" s="1" t="str">
         <f aca="false">IF(NOT(D25="1X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c"),IF(E25="landmark",CONCATENATE(A25,"_k"),IF(E25="house",CONCATENATE(A25,"_h"),A25))))</f>
-        <v>sato_building_c</v>
+        <v>kuroi_tower_c</v>
       </c>
       <c r="U25" s="1" t="str">
         <f aca="false">IF(D25="1X1","none",IF(E25="skyscraper",CONCATENATE(A25,"_c_north"),IF(E25="landmark",CONCATENATE(A25,"_k_north"),IF(E25="house",CONCATENATE(A25,"_h_north"),CONCATENATE(A25,"_north")))))</f>
@@ -2786,25 +2818,25 @@
         <v>87</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>88</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>39</v>
@@ -2813,7 +2845,7 @@
         <v>25</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M26" s="3" t="str">
         <f aca="false">VLOOKUP(L26,dropdowns!E:F,2,0)</f>
@@ -2826,7 +2858,7 @@
         <v>5</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q26" s="1" t="n">
         <v>24</v>
@@ -2835,11 +2867,11 @@
         <v>10</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T26" s="1" t="str">
         <f aca="false">IF(NOT(D26="1X1"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c"),IF(E26="landmark",CONCATENATE(A26,"_k"),IF(E26="house",CONCATENATE(A26,"_h"),A26))))</f>
-        <v>sugiyama_office_building_c</v>
+        <v>mitsui_tower_c</v>
       </c>
       <c r="U26" s="1" t="str">
         <f aca="false">IF(D26="1X1","none",IF(E26="skyscraper",CONCATENATE(A26,"_c_north"),IF(E26="landmark",CONCATENATE(A26,"_k_north"),IF(E26="house",CONCATENATE(A26,"_h_north"),CONCATENATE(A26,"_north")))))</f>
@@ -2869,25 +2901,25 @@
         <v>89</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G27" s="1" t="n">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>39</v>
@@ -2896,20 +2928,20 @@
         <v>25</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M27" s="3" t="str">
         <f aca="false">VLOOKUP(L27,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q27" s="1" t="n">
         <v>24</v>
@@ -2918,19 +2950,19 @@
         <v>10</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T27" s="1" t="str">
         <f aca="false">IF(NOT(D27="1X1"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c"),IF(E27="landmark",CONCATENATE(A27,"_k"),IF(E27="house",CONCATENATE(A27,"_h"),A27))))</f>
-        <v>none</v>
+        <v>modern_office_tower_c</v>
       </c>
       <c r="U27" s="1" t="str">
         <f aca="false">IF(D27="1X1","none",IF(E27="skyscraper",CONCATENATE(A27,"_c_north"),IF(E27="landmark",CONCATENATE(A27,"_k_north"),IF(E27="house",CONCATENATE(A27,"_h_north"),CONCATENATE(A27,"_north")))))</f>
-        <v>tsuno_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V27" s="1" t="str">
         <f aca="false">IF(OR(D27="1X1",D27="2X1"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c_east"),IF(E27="landmark",CONCATENATE(A27,"_k_east"),CONCATENATE(A27,"_east"))))</f>
-        <v>tsuno_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W27" s="1" t="str">
         <f aca="false">IF(OR(D27="1X1",D27="1X2"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c_west"),IF(E27="landmark",CONCATENATE(A27,"_k_west"),CONCATENATE(A27,"_west"))))</f>
@@ -2946,40 +2978,40 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>1955</v>
-      </c>
-      <c r="J28" s="4" t="n">
-        <v>1989</v>
+        <v>1990</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>25</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M28" s="3" t="str">
         <f aca="false">VLOOKUP(L28,dropdowns!E:F,2,0)</f>
@@ -2992,7 +3024,7 @@
         <v>5</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q28" s="1" t="n">
         <v>24</v>
@@ -3001,11 +3033,11 @@
         <v>10</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T28" s="1" t="str">
         <f aca="false">IF(NOT(D28="1X1"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c"),IF(E28="landmark",CONCATENATE(A28,"_k"),IF(E28="house",CONCATENATE(A28,"_h"),A28))))</f>
-        <v>ueda_office_block_c</v>
+        <v>multimedia_offices_c</v>
       </c>
       <c r="U28" s="1" t="str">
         <f aca="false">IF(D28="1X1","none",IF(E28="skyscraper",CONCATENATE(A28,"_c_north"),IF(E28="landmark",CONCATENATE(A28,"_k_north"),IF(E28="house",CONCATENATE(A28,"_h_north"),CONCATENATE(A28,"_north")))))</f>
@@ -3029,31 +3061,31 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>1965</v>
+        <v>2000</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>39</v>
@@ -3062,7 +3094,7 @@
         <v>25</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M29" s="3" t="str">
         <f aca="false">VLOOKUP(L29,dropdowns!E:F,2,0)</f>
@@ -3075,20 +3107,20 @@
         <v>5</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R29" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T29" s="1" t="str">
         <f aca="false">IF(NOT(D29="1X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c"),IF(E29="landmark",CONCATENATE(A29,"_k"),IF(E29="house",CONCATENATE(A29,"_h"),A29))))</f>
-        <v>yamaguchi_office_c</v>
+        <v>office_tower_c</v>
       </c>
       <c r="U29" s="1" t="str">
         <f aca="false">IF(D29="1X1","none",IF(E29="skyscraper",CONCATENATE(A29,"_c_north"),IF(E29="landmark",CONCATENATE(A29,"_k_north"),IF(E29="house",CONCATENATE(A29,"_h_north"),CONCATENATE(A29,"_north")))))</f>
@@ -3112,31 +3144,31 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>84</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G30" s="1" t="n">
-        <v>255</v>
+        <v>200</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>39</v>
@@ -3145,20 +3177,20 @@
         <v>25</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M30" s="3" t="str">
         <f aca="false">VLOOKUP(L30,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O30" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q30" s="1" t="n">
         <v>24</v>
@@ -3167,19 +3199,19 @@
         <v>10</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T30" s="1" t="str">
         <f aca="false">IF(NOT(D30="1X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c"),IF(E30="landmark",CONCATENATE(A30,"_k"),IF(E30="house",CONCATENATE(A30,"_h"),A30))))</f>
-        <v>none</v>
+        <v>sato_building_c</v>
       </c>
       <c r="U30" s="1" t="str">
         <f aca="false">IF(D30="1X1","none",IF(E30="skyscraper",CONCATENATE(A30,"_c_north"),IF(E30="landmark",CONCATENATE(A30,"_k_north"),IF(E30="house",CONCATENATE(A30,"_h_north"),CONCATENATE(A30,"_north")))))</f>
-        <v>yamashiro_office_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V30" s="1" t="str">
         <f aca="false">IF(OR(D30="1X1",D30="2X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_east"),IF(E30="landmark",CONCATENATE(A30,"_k_east"),CONCATENATE(A30,"_east"))))</f>
-        <v>yamashiro_office_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W30" s="1" t="str">
         <f aca="false">IF(OR(D30="1X1",D30="1X2"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c_west"),IF(E30="landmark",CONCATENATE(A30,"_k_west"),CONCATENATE(A30,"_west"))))</f>
@@ -3195,31 +3227,31 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>39</v>
@@ -3228,7 +3260,7 @@
         <v>25</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M31" s="3" t="str">
         <f aca="false">VLOOKUP(L31,dropdowns!E:F,2,0)</f>
@@ -3241,7 +3273,7 @@
         <v>5</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q31" s="1" t="n">
         <v>24</v>
@@ -3250,11 +3282,11 @@
         <v>10</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T31" s="1" t="str">
         <f aca="false">IF(NOT(D31="1X1"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c"),IF(E31="landmark",CONCATENATE(A31,"_k"),IF(E31="house",CONCATENATE(A31,"_h"),A31))))</f>
-        <v>yamashita_building_c</v>
+        <v>sugiyama_office_building_c</v>
       </c>
       <c r="U31" s="1" t="str">
         <f aca="false">IF(D31="1X1","none",IF(E31="skyscraper",CONCATENATE(A31,"_c_north"),IF(E31="landmark",CONCATENATE(A31,"_k_north"),IF(E31="house",CONCATENATE(A31,"_h_north"),CONCATENATE(A31,"_north")))))</f>
@@ -3278,62 +3310,62 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="2" t="n">
-        <v>212</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="G32" s="1" t="n">
-        <v>15</v>
+        <v>255</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>1700</v>
+        <v>2006</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="M32" s="3" t="str">
         <f aca="false">VLOOKUP(L32,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="R32" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="T32" s="1" t="str">
         <f aca="false">IF(NOT(D32="1X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c"),IF(E32="landmark",CONCATENATE(A32,"_k"),IF(E32="house",CONCATENATE(A32,"_h"),A32))))</f>
@@ -3341,248 +3373,248 @@
       </c>
       <c r="U32" s="1" t="str">
         <f aca="false">IF(D32="1X1","none",IF(E32="skyscraper",CONCATENATE(A32,"_c_north"),IF(E32="landmark",CONCATENATE(A32,"_k_north"),IF(E32="house",CONCATENATE(A32,"_h_north"),CONCATENATE(A32,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>tsuno_building_c_north</v>
       </c>
       <c r="V32" s="1" t="str">
-        <f aca="false">IF(OR(D32="1X1",D32="2X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_east"),IF(E32="landmark",CONCATENATE(A32,"_k_east"),IF(E32="house",CONCATENATE(A32,"_h_east"),CONCATENATE(A32,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D32="1X1",D32="2X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_east"),IF(E32="landmark",CONCATENATE(A32,"_k_east"),CONCATENATE(A32,"_east"))))</f>
+        <v>tsuno_building_c_east</v>
       </c>
       <c r="W32" s="1" t="str">
-        <f aca="false">IF(OR(D32="1X1",D32="1X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_west"),IF(E32="landmark",CONCATENATE(A32,"_k_west"),IF(E32="house",CONCATENATE(A32,"_h_west"),CONCATENATE(A32,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D32="1X1",D32="1X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_west"),IF(E32="landmark",CONCATENATE(A32,"_k_west"),CONCATENATE(A32,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X32" s="1" t="str">
-        <f aca="false">IF(NOT(D32="2X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_south"),IF(E32="landmark",CONCATENATE(A32,"_k_south"),IF(E32="house",CONCATENATE(A32,"_h_south"),CONCATENATE(A32,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D32="2X2"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c_south"),IF(E32="landmark",CONCATENATE(A32,"_k_south"),CONCATENATE(A32,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>1870</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>39</v>
+        <v>1955</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>1989</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="M33" s="3" t="str">
         <f aca="false">VLOOKUP(L33,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O33" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="T33" s="1" t="str">
         <f aca="false">IF(NOT(D33="1X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c"),IF(E33="landmark",CONCATENATE(A33,"_k"),IF(E33="house",CONCATENATE(A33,"_h"),A33))))</f>
-        <v>naganuma_h</v>
+        <v>ueda_office_block_c</v>
       </c>
       <c r="U33" s="1" t="str">
         <f aca="false">IF(D33="1X1","none",IF(E33="skyscraper",CONCATENATE(A33,"_c_north"),IF(E33="landmark",CONCATENATE(A33,"_k_north"),IF(E33="house",CONCATENATE(A33,"_h_north"),CONCATENATE(A33,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V33" s="1" t="str">
-        <f aca="false">IF(OR(D33="1X1",D33="2X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_east"),IF(E33="landmark",CONCATENATE(A33,"_k_east"),IF(E33="house",CONCATENATE(A33,"_h_east"),CONCATENATE(A33,"_east")))))</f>
+        <f aca="false">IF(OR(D33="1X1",D33="2X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_east"),IF(E33="landmark",CONCATENATE(A33,"_k_east"),CONCATENATE(A33,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W33" s="1" t="str">
-        <f aca="false">IF(OR(D33="1X1",D33="1X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_west"),IF(E33="landmark",CONCATENATE(A33,"_k_west"),IF(E33="house",CONCATENATE(A33,"_h_west"),CONCATENATE(A33,"_west")))))</f>
+        <f aca="false">IF(OR(D33="1X1",D33="1X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_west"),IF(E33="landmark",CONCATENATE(A33,"_k_west"),CONCATENATE(A33,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X33" s="1" t="str">
-        <f aca="false">IF(NOT(D33="2X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_south"),IF(E33="landmark",CONCATENATE(A33,"_k_south"),IF(E33="house",CONCATENATE(A33,"_h_south"),CONCATENATE(A33,"_south")))))</f>
+        <f aca="false">IF(NOT(D33="2X2"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c_south"),IF(E33="landmark",CONCATENATE(A33,"_k_south"),CONCATENATE(A33,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>95</v>
+      <c r="A34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>36</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H34" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="0" t="n">
-        <v>1950</v>
+      <c r="I34" s="1" t="n">
+        <v>1965</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="0" t="n">
-        <v>5</v>
+      <c r="K34" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="M34" s="3" t="str">
         <f aca="false">VLOOKUP(L34,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N34" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O34" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
+      </c>
+      <c r="N34" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O34" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q34" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="Q34" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R34" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="R34" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="S34" s="3" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="T34" s="1" t="str">
         <f aca="false">IF(NOT(D34="1X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c"),IF(E34="landmark",CONCATENATE(A34,"_k"),IF(E34="house",CONCATENATE(A34,"_h"),A34))))</f>
-        <v>convini_k</v>
+        <v>yamaguchi_office_c</v>
       </c>
       <c r="U34" s="1" t="str">
         <f aca="false">IF(D34="1X1","none",IF(E34="skyscraper",CONCATENATE(A34,"_c_north"),IF(E34="landmark",CONCATENATE(A34,"_k_north"),IF(E34="house",CONCATENATE(A34,"_h_north"),CONCATENATE(A34,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V34" s="1" t="str">
-        <f aca="false">IF(OR(D34="1X1",D34="2X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_east"),IF(E34="landmark",CONCATENATE(A34,"_k_east"),IF(E34="house",CONCATENATE(A34,"_h_east"),CONCATENATE(A34,"_east")))))</f>
+        <f aca="false">IF(OR(D34="1X1",D34="2X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_east"),IF(E34="landmark",CONCATENATE(A34,"_k_east"),CONCATENATE(A34,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W34" s="1" t="str">
-        <f aca="false">IF(OR(D34="1X1",D34="1X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_west"),IF(E34="landmark",CONCATENATE(A34,"_k_west"),IF(E34="house",CONCATENATE(A34,"_h_west"),CONCATENATE(A34,"_west")))))</f>
+        <f aca="false">IF(OR(D34="1X1",D34="1X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_west"),IF(E34="landmark",CONCATENATE(A34,"_k_west"),CONCATENATE(A34,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X34" s="1" t="str">
-        <f aca="false">IF(NOT(D34="2X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_south"),IF(E34="landmark",CONCATENATE(A34,"_k_south"),IF(E34="house",CONCATENATE(A34,"_h_south"),CONCATENATE(A34,"_south")))))</f>
-        <v>none</v>
-      </c>
-      <c r="Y34" s="0" t="s">
-        <v>116</v>
+        <f aca="false">IF(NOT(D34="2X2"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c_south"),IF(E34="landmark",CONCATENATE(A34,"_k_south"),CONCATENATE(A34,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C35" s="2" t="n">
+        <v>101</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="G35" s="1" t="n">
-        <v>80</v>
+        <v>255</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="M35" s="3" t="str">
         <f aca="false">VLOOKUP(L35,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="Q35" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R35" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="R35" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="S35" s="3" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="T35" s="1" t="str">
         <f aca="false">IF(NOT(D35="1X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c"),IF(E35="landmark",CONCATENATE(A35,"_k"),IF(E35="house",CONCATENATE(A35,"_h"),A35))))</f>
@@ -3590,199 +3622,199 @@
       </c>
       <c r="U35" s="1" t="str">
         <f aca="false">IF(D35="1X1","none",IF(E35="skyscraper",CONCATENATE(A35,"_c_north"),IF(E35="landmark",CONCATENATE(A35,"_k_north"),IF(E35="house",CONCATENATE(A35,"_h_north"),CONCATENATE(A35,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>yamashiro_office_building_c_north</v>
       </c>
       <c r="V35" s="1" t="str">
-        <f aca="false">IF(OR(D35="1X1",D35="2X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_east"),IF(E35="landmark",CONCATENATE(A35,"_k_east"),IF(E35="house",CONCATENATE(A35,"_h_east"),CONCATENATE(A35,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D35="1X1",D35="2X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_east"),IF(E35="landmark",CONCATENATE(A35,"_k_east"),CONCATENATE(A35,"_east"))))</f>
+        <v>yamashiro_office_building_c_east</v>
       </c>
       <c r="W35" s="1" t="str">
-        <f aca="false">IF(OR(D35="1X1",D35="1X2"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_west"),IF(E35="landmark",CONCATENATE(A35,"_k_west"),IF(E35="house",CONCATENATE(A35,"_h_west"),CONCATENATE(A35,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <f aca="false">IF(OR(D35="1X1",D35="1X2"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_west"),IF(E35="landmark",CONCATENATE(A35,"_k_west"),CONCATENATE(A35,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X35" s="1" t="str">
-        <f aca="false">IF(NOT(D35="2X2"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_south"),IF(E35="landmark",CONCATENATE(A35,"_k_south"),IF(E35="house",CONCATENATE(A35,"_h_south"),CONCATENATE(A35,"_south")))))</f>
+        <f aca="false">IF(NOT(D35="2X2"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c_south"),IF(E35="landmark",CONCATENATE(A35,"_k_south"),CONCATENATE(A35,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>200</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>1970</v>
+        <v>2000</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="M36" s="3" t="str">
         <f aca="false">VLOOKUP(L36,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N36" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O36" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="Q36" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R36" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="R36" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="S36" s="3" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="T36" s="1" t="str">
         <f aca="false">IF(NOT(D36="1X1"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c"),IF(E36="landmark",CONCATENATE(A36,"_k"),IF(E36="house",CONCATENATE(A36,"_h"),A36))))</f>
-        <v>none</v>
+        <v>yamashita_building_c</v>
       </c>
       <c r="U36" s="1" t="str">
         <f aca="false">IF(D36="1X1","none",IF(E36="skyscraper",CONCATENATE(A36,"_c_north"),IF(E36="landmark",CONCATENATE(A36,"_k_north"),IF(E36="house",CONCATENATE(A36,"_h_north"),CONCATENATE(A36,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>none</v>
       </c>
       <c r="V36" s="1" t="str">
         <f aca="false">IF(OR(D36="1X1",D36="2X1"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c_east"),IF(E36="landmark",CONCATENATE(A36,"_k_east"),CONCATENATE(A36,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <v>none</v>
       </c>
       <c r="W36" s="1" t="str">
         <f aca="false">IF(OR(D36="1X1",D36="1X2"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c_west"),IF(E36="landmark",CONCATENATE(A36,"_k_west"),CONCATENATE(A36,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <v>none</v>
       </c>
       <c r="X36" s="1" t="str">
         <f aca="false">IF(NOT(D36="2X2"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c_south"),IF(E36="landmark",CONCATENATE(A36,"_k_south"),CONCATENATE(A36,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>1870</v>
+        <v>1700</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>114</v>
       </c>
       <c r="M37" s="3" t="str">
         <f aca="false">VLOOKUP(L37,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N37" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O37" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Q37" s="1" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="R37" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="T37" s="1" t="str">
         <f aca="false">IF(NOT(D37="1X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c"),IF(E37="landmark",CONCATENATE(A37,"_k"),IF(E37="house",CONCATENATE(A37,"_h"),A37))))</f>
-        <v>onsen_k</v>
+        <v>none</v>
       </c>
       <c r="U37" s="1" t="str">
         <f aca="false">IF(D37="1X1","none",IF(E37="skyscraper",CONCATENATE(A37,"_c_north"),IF(E37="landmark",CONCATENATE(A37,"_k_north"),IF(E37="house",CONCATENATE(A37,"_h_north"),CONCATENATE(A37,"_north")))))</f>
-        <v>none</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V37" s="1" t="str">
         <f aca="false">IF(OR(D37="1X1",D37="2X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c_east"),IF(E37="landmark",CONCATENATE(A37,"_k_east"),IF(E37="house",CONCATENATE(A37,"_h_east"),CONCATENATE(A37,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W37" s="1" t="str">
         <f aca="false">IF(OR(D37="1X1",D37="1X2"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c_west"),IF(E37="landmark",CONCATENATE(A37,"_k_west"),IF(E37="house",CONCATENATE(A37,"_h_west"),CONCATENATE(A37,"_west")))))</f>
-        <v>none</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X37" s="1" t="str">
         <f aca="false">IF(NOT(D37="2X2"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c_south"),IF(E37="landmark",CONCATENATE(A37,"_k_south"),IF(E37="house",CONCATENATE(A37,"_h_south"),CONCATENATE(A37,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>27</v>
@@ -3791,182 +3823,182 @@
         <v>112</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>1980</v>
+        <v>1870</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="M38" s="3" t="str">
         <f aca="false">VLOOKUP(L38,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N38" s="1" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="O38" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="Q38" s="1" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="R38" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="T38" s="1" t="str">
         <f aca="false">IF(NOT(D38="1X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c"),IF(E38="landmark",CONCATENATE(A38,"_k"),IF(E38="house",CONCATENATE(A38,"_h"),A38))))</f>
-        <v>pachinko_k</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U38" s="1" t="str">
         <f aca="false">IF(D38="1X1","none",IF(E38="skyscraper",CONCATENATE(A38,"_c_north"),IF(E38="landmark",CONCATENATE(A38,"_k_north"),IF(E38="house",CONCATENATE(A38,"_h_north"),CONCATENATE(A38,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V38" s="1" t="str">
-        <f aca="false">IF(OR(D38="1X1",D38="2X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_east"),IF(E38="landmark",CONCATENATE(A38,"_k_east"),CONCATENATE(A38,"_east"))))</f>
+        <f aca="false">IF(OR(D38="1X1",D38="2X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_east"),IF(E38="landmark",CONCATENATE(A38,"_k_east"),IF(E38="house",CONCATENATE(A38,"_h_east"),CONCATENATE(A38,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W38" s="1" t="str">
-        <f aca="false">IF(OR(D38="1X1",D38="1X2"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_west"),IF(E38="landmark",CONCATENATE(A38,"_k_west"),CONCATENATE(A38,"_west"))))</f>
+        <f aca="false">IF(OR(D38="1X1",D38="1X2"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_west"),IF(E38="landmark",CONCATENATE(A38,"_k_west"),IF(E38="house",CONCATENATE(A38,"_h_west"),CONCATENATE(A38,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X38" s="1" t="str">
-        <f aca="false">IF(NOT(D38="2X2"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_south"),IF(E38="landmark",CONCATENATE(A38,"_k_south"),CONCATENATE(A38,"_south"))))</f>
+        <f aca="false">IF(NOT(D38="2X2"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c_south"),IF(E38="landmark",CONCATENATE(A38,"_k_south"),IF(E38="house",CONCATENATE(A38,"_h_south"),CONCATENATE(A38,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>105</v>
+      <c r="A39" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>95</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I39" s="1" t="n">
-        <v>1970</v>
+        <v>123</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>1950</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K39" s="1" t="n">
-        <v>20</v>
+      <c r="K39" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="M39" s="3" t="str">
         <f aca="false">VLOOKUP(L39,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
-      </c>
-      <c r="N39" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="O39" s="1" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="O39" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q39" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="R39" s="1" t="n">
-        <v>2</v>
+        <v>115</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="T39" s="1" t="str">
         <f aca="false">IF(NOT(D39="1X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c"),IF(E39="landmark",CONCATENATE(A39,"_k"),IF(E39="house",CONCATENATE(A39,"_h"),A39))))</f>
-        <v>none</v>
+        <v>convini_k</v>
       </c>
       <c r="U39" s="1" t="str">
         <f aca="false">IF(D39="1X1","none",IF(E39="skyscraper",CONCATENATE(A39,"_c_north"),IF(E39="landmark",CONCATENATE(A39,"_k_north"),IF(E39="house",CONCATENATE(A39,"_h_north"),CONCATENATE(A39,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V39" s="1" t="str">
-        <f aca="false">IF(OR(D39="1X1",D39="2X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_east"),IF(E39="landmark",CONCATENATE(A39,"_k_east"),CONCATENATE(A39,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <f aca="false">IF(OR(D39="1X1",D39="2X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_east"),IF(E39="landmark",CONCATENATE(A39,"_k_east"),IF(E39="house",CONCATENATE(A39,"_h_east"),CONCATENATE(A39,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W39" s="1" t="str">
-        <f aca="false">IF(OR(D39="1X1",D39="1X2"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_west"),IF(E39="landmark",CONCATENATE(A39,"_k_west"),CONCATENATE(A39,"_west"))))</f>
+        <f aca="false">IF(OR(D39="1X1",D39="1X2"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_west"),IF(E39="landmark",CONCATENATE(A39,"_k_west"),IF(E39="house",CONCATENATE(A39,"_h_west"),CONCATENATE(A39,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X39" s="1" t="str">
-        <f aca="false">IF(NOT(D39="2X2"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_south"),IF(E39="landmark",CONCATENATE(A39,"_k_south"),CONCATENATE(A39,"_south"))))</f>
-        <v>none</v>
-      </c>
-      <c r="Y39" s="1" t="s">
-        <v>128</v>
+        <f aca="false">IF(NOT(D39="2X2"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c_south"),IF(E39="landmark",CONCATENATE(A39,"_k_south"),IF(E39="house",CONCATENATE(A39,"_h_south"),CONCATENATE(A39,"_south")))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y39" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>216</v>
+        <v>107</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H40" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>39</v>
@@ -3975,20 +4007,20 @@
         <v>20</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M40" s="3" t="str">
         <f aca="false">VLOOKUP(L40,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N40" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O40" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N40" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="O40" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="Q40" s="1" t="n">
         <v>10</v>
@@ -3997,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="T40" s="1" t="str">
         <f aca="false">IF(NOT(D40="1X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c"),IF(E40="landmark",CONCATENATE(A40,"_k"),IF(E40="house",CONCATENATE(A40,"_h"),A40))))</f>
@@ -4005,51 +4037,51 @@
       </c>
       <c r="U40" s="1" t="str">
         <f aca="false">IF(D40="1X1","none",IF(E40="skyscraper",CONCATENATE(A40,"_c_north"),IF(E40="landmark",CONCATENATE(A40,"_k_north"),IF(E40="house",CONCATENATE(A40,"_h_north"),CONCATENATE(A40,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V40" s="1" t="str">
-        <f aca="false">IF(OR(D40="1X1",D40="2X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_east"),IF(E40="landmark",CONCATENATE(A40,"_k_east"),CONCATENATE(A40,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <f aca="false">IF(OR(D40="1X1",D40="2X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_east"),IF(E40="landmark",CONCATENATE(A40,"_k_east"),IF(E40="house",CONCATENATE(A40,"_h_east"),CONCATENATE(A40,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W40" s="1" t="str">
-        <f aca="false">IF(OR(D40="1X1",D40="1X2"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_west"),IF(E40="landmark",CONCATENATE(A40,"_k_west"),CONCATENATE(A40,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <f aca="false">IF(OR(D40="1X1",D40="1X2"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_west"),IF(E40="landmark",CONCATENATE(A40,"_k_west"),IF(E40="house",CONCATENATE(A40,"_h_west"),CONCATENATE(A40,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X40" s="1" t="str">
-        <f aca="false">IF(NOT(D40="2X2"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_south"),IF(E40="landmark",CONCATENATE(A40,"_k_south"),CONCATENATE(A40,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <f aca="false">IF(NOT(D40="2X2"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c_south"),IF(E40="landmark",CONCATENATE(A40,"_k_south"),IF(E40="house",CONCATENATE(A40,"_h_south"),CONCATENATE(A40,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>114</v>
+        <v>200</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G41" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H41" s="0" t="n">
-        <v>1</v>
+        <v>150</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>0</v>
+        <v>1970</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>39</v>
@@ -4058,247 +4090,247 @@
         <v>20</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M41" s="3" t="str">
         <f aca="false">VLOOKUP(L41,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N41" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O41" s="0" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O41" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="Q41" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R41" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T41" s="1" t="str">
         <f aca="false">IF(NOT(D41="1X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c"),IF(E41="landmark",CONCATENATE(A41,"_k"),IF(E41="house",CONCATENATE(A41,"_h"),A41))))</f>
-        <v>shrine_k</v>
+        <v>none</v>
       </c>
       <c r="U41" s="1" t="str">
         <f aca="false">IF(D41="1X1","none",IF(E41="skyscraper",CONCATENATE(A41,"_c_north"),IF(E41="landmark",CONCATENATE(A41,"_k_north"),IF(E41="house",CONCATENATE(A41,"_h_north"),CONCATENATE(A41,"_north")))))</f>
-        <v>none</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V41" s="1" t="str">
         <f aca="false">IF(OR(D41="1X1",D41="2X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_east"),IF(E41="landmark",CONCATENATE(A41,"_k_east"),CONCATENATE(A41,"_east"))))</f>
-        <v>none</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W41" s="1" t="str">
         <f aca="false">IF(OR(D41="1X1",D41="1X2"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_west"),IF(E41="landmark",CONCATENATE(A41,"_k_west"),CONCATENATE(A41,"_west"))))</f>
-        <v>none</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X41" s="1" t="str">
         <f aca="false">IF(NOT(D41="2X2"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_south"),IF(E41="landmark",CONCATENATE(A41,"_k_south"),CONCATENATE(A41,"_south"))))</f>
-        <v>none</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y41" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H42" s="0" t="n">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>0</v>
+        <v>1870</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K42" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="M42" s="3" t="str">
         <f aca="false">VLOOKUP(L42,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N42" s="0" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O42" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q42" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R42" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="O42" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q42" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R42" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="S42" s="3" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="T42" s="1" t="str">
         <f aca="false">IF(NOT(D42="1X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c"),IF(E42="landmark",CONCATENATE(A42,"_k"),IF(E42="house",CONCATENATE(A42,"_h"),A42))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>onsen_k</v>
       </c>
       <c r="U42" s="1" t="str">
         <f aca="false">IF(D42="1X1","none",IF(E42="skyscraper",CONCATENATE(A42,"_c_north"),IF(E42="landmark",CONCATENATE(A42,"_k_north"),IF(E42="house",CONCATENATE(A42,"_h_north"),CONCATENATE(A42,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V42" s="1" t="str">
-        <f aca="false">IF(OR(D42="1X1",D42="2X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_east"),IF(E42="landmark",CONCATENATE(A42,"_k_east"),CONCATENATE(A42,"_east"))))</f>
+        <f aca="false">IF(OR(D42="1X1",D42="2X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_east"),IF(E42="landmark",CONCATENATE(A42,"_k_east"),IF(E42="house",CONCATENATE(A42,"_h_east"),CONCATENATE(A42,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W42" s="1" t="str">
-        <f aca="false">IF(OR(D42="1X1",D42="1X2"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_west"),IF(E42="landmark",CONCATENATE(A42,"_k_west"),CONCATENATE(A42,"_west"))))</f>
+        <f aca="false">IF(OR(D42="1X1",D42="1X2"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_west"),IF(E42="landmark",CONCATENATE(A42,"_k_west"),IF(E42="house",CONCATENATE(A42,"_h_west"),CONCATENATE(A42,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X42" s="1" t="str">
-        <f aca="false">IF(NOT(D42="2X2"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_south"),IF(E42="landmark",CONCATENATE(A42,"_k_south"),CONCATENATE(A42,"_south"))))</f>
+        <f aca="false">IF(NOT(D42="2X2"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c_south"),IF(E42="landmark",CONCATENATE(A42,"_k_south"),IF(E42="house",CONCATENATE(A42,"_h_south"),CONCATENATE(A42,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>204</v>
+        <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="M43" s="3" t="str">
         <f aca="false">VLOOKUP(L43,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="O43" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Q43" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="R43" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="T43" s="1" t="str">
         <f aca="false">IF(NOT(D43="1X1"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c"),IF(E43="landmark",CONCATENATE(A43,"_k"),IF(E43="house",CONCATENATE(A43,"_h"),A43))))</f>
-        <v>none</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U43" s="1" t="str">
         <f aca="false">IF(D43="1X1","none",IF(E43="skyscraper",CONCATENATE(A43,"_c_north"),IF(E43="landmark",CONCATENATE(A43,"_k_north"),IF(E43="house",CONCATENATE(A43,"_h_north"),CONCATENATE(A43,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V43" s="1" t="str">
         <f aca="false">IF(OR(D43="1X1",D43="2X1"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c_east"),IF(E43="landmark",CONCATENATE(A43,"_k_east"),CONCATENATE(A43,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W43" s="1" t="str">
         <f aca="false">IF(OR(D43="1X1",D43="1X2"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c_west"),IF(E43="landmark",CONCATENATE(A43,"_k_west"),CONCATENATE(A43,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X43" s="1" t="str">
         <f aca="false">IF(NOT(D43="2X2"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c_south"),IF(E43="landmark",CONCATENATE(A43,"_k_south"),CONCATENATE(A43,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y43" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>208</v>
+        <v>105</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G44" s="1" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H44" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>39</v>
@@ -4307,20 +4339,20 @@
         <v>20</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="M44" s="3" t="str">
         <f aca="false">VLOOKUP(L44,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N44" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O44" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="Q44" s="1" t="n">
         <v>10</v>
@@ -4329,7 +4361,7 @@
         <v>2</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="T44" s="1" t="str">
         <f aca="false">IF(NOT(D44="1X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c"),IF(E44="landmark",CONCATENATE(A44,"_k"),IF(E44="house",CONCATENATE(A44,"_h"),A44))))</f>
@@ -4337,52 +4369,467 @@
       </c>
       <c r="U44" s="1" t="str">
         <f aca="false">IF(D44="1X1","none",IF(E44="skyscraper",CONCATENATE(A44,"_c_north"),IF(E44="landmark",CONCATENATE(A44,"_k_north"),IF(E44="house",CONCATENATE(A44,"_h_north"),CONCATENATE(A44,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V44" s="1" t="str">
         <f aca="false">IF(OR(D44="1X1",D44="2X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_east"),IF(E44="landmark",CONCATENATE(A44,"_k_east"),CONCATENATE(A44,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W44" s="1" t="str">
         <f aca="false">IF(OR(D44="1X1",D44="1X2"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_west"),IF(E44="landmark",CONCATENATE(A44,"_k_west"),CONCATENATE(A44,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X44" s="1" t="str">
         <f aca="false">IF(NOT(D44="2X2"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_south"),IF(E44="landmark",CONCATENATE(A44,"_k_south"),CONCATENATE(A44,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M45" s="3" t="str">
+        <f aca="false">VLOOKUP(L45,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q45" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T45" s="1" t="str">
+        <f aca="false">IF(NOT(D45="1X1"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c"),IF(E45="landmark",CONCATENATE(A45,"_k"),IF(E45="house",CONCATENATE(A45,"_h"),A45))))</f>
+        <v>none</v>
+      </c>
+      <c r="U45" s="1" t="str">
+        <f aca="false">IF(D45="1X1","none",IF(E45="skyscraper",CONCATENATE(A45,"_c_north"),IF(E45="landmark",CONCATENATE(A45,"_k_north"),IF(E45="house",CONCATENATE(A45,"_h_north"),CONCATENATE(A45,"_north")))))</f>
+        <v>shiro_k_north</v>
+      </c>
+      <c r="V45" s="1" t="str">
+        <f aca="false">IF(OR(D45="1X1",D45="2X1"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c_east"),IF(E45="landmark",CONCATENATE(A45,"_k_east"),CONCATENATE(A45,"_east"))))</f>
+        <v>shiro_k_east</v>
+      </c>
+      <c r="W45" s="1" t="str">
+        <f aca="false">IF(OR(D45="1X1",D45="1X2"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c_west"),IF(E45="landmark",CONCATENATE(A45,"_k_west"),CONCATENATE(A45,"_west"))))</f>
+        <v>shiro_k_west</v>
+      </c>
+      <c r="X45" s="1" t="str">
+        <f aca="false">IF(NOT(D45="2X2"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c_south"),IF(E45="landmark",CONCATENATE(A45,"_k_south"),CONCATENATE(A45,"_south"))))</f>
+        <v>shiro_k_south</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="M46" s="3" t="str">
+        <f aca="false">VLOOKUP(L46,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="T46" s="1" t="str">
+        <f aca="false">IF(NOT(D46="1X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c"),IF(E46="landmark",CONCATENATE(A46,"_k"),IF(E46="house",CONCATENATE(A46,"_h"),A46))))</f>
+        <v>shrine_k</v>
+      </c>
+      <c r="U46" s="1" t="str">
+        <f aca="false">IF(D46="1X1","none",IF(E46="skyscraper",CONCATENATE(A46,"_c_north"),IF(E46="landmark",CONCATENATE(A46,"_k_north"),IF(E46="house",CONCATENATE(A46,"_h_north"),CONCATENATE(A46,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V46" s="1" t="str">
+        <f aca="false">IF(OR(D46="1X1",D46="2X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_east"),IF(E46="landmark",CONCATENATE(A46,"_k_east"),CONCATENATE(A46,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W46" s="1" t="str">
+        <f aca="false">IF(OR(D46="1X1",D46="1X2"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_west"),IF(E46="landmark",CONCATENATE(A46,"_k_west"),CONCATENATE(A46,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X46" s="1" t="str">
+        <f aca="false">IF(NOT(D46="2X2"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_south"),IF(E46="landmark",CONCATENATE(A46,"_k_south"),CONCATENATE(A46,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="M47" s="3" t="str">
+        <f aca="false">VLOOKUP(L47,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S47" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="T47" s="1" t="str">
+        <f aca="false">IF(NOT(D47="1X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c"),IF(E47="landmark",CONCATENATE(A47,"_k"),IF(E47="house",CONCATENATE(A47,"_h"),A47))))</f>
+        <v>shrine_prohibition_k</v>
+      </c>
+      <c r="U47" s="1" t="str">
+        <f aca="false">IF(D47="1X1","none",IF(E47="skyscraper",CONCATENATE(A47,"_c_north"),IF(E47="landmark",CONCATENATE(A47,"_k_north"),IF(E47="house",CONCATENATE(A47,"_h_north"),CONCATENATE(A47,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V47" s="1" t="str">
+        <f aca="false">IF(OR(D47="1X1",D47="2X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_east"),IF(E47="landmark",CONCATENATE(A47,"_k_east"),CONCATENATE(A47,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W47" s="1" t="str">
+        <f aca="false">IF(OR(D47="1X1",D47="1X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_west"),IF(E47="landmark",CONCATENATE(A47,"_k_west"),CONCATENATE(A47,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X47" s="1" t="str">
+        <f aca="false">IF(NOT(D47="2X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_south"),IF(E47="landmark",CONCATENATE(A47,"_k_south"),CONCATENATE(A47,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M48" s="3" t="str">
+        <f aca="false">VLOOKUP(L48,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N48" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O48" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q48" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R48" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T48" s="1" t="str">
+        <f aca="false">IF(NOT(D48="1X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c"),IF(E48="landmark",CONCATENATE(A48,"_k"),IF(E48="house",CONCATENATE(A48,"_h"),A48))))</f>
+        <v>none</v>
+      </c>
+      <c r="U48" s="1" t="str">
+        <f aca="false">IF(D48="1X1","none",IF(E48="skyscraper",CONCATENATE(A48,"_c_north"),IF(E48="landmark",CONCATENATE(A48,"_k_north"),IF(E48="house",CONCATENATE(A48,"_h_north"),CONCATENATE(A48,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V48" s="1" t="str">
+        <f aca="false">IF(OR(D48="1X1",D48="2X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_east"),IF(E48="landmark",CONCATENATE(A48,"_k_east"),CONCATENATE(A48,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W48" s="1" t="str">
+        <f aca="false">IF(OR(D48="1X1",D48="1X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_west"),IF(E48="landmark",CONCATENATE(A48,"_k_west"),CONCATENATE(A48,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X48" s="1" t="str">
+        <f aca="false">IF(NOT(D48="2X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_south"),IF(E48="landmark",CONCATENATE(A48,"_k_south"),CONCATENATE(A48,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y48" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="M49" s="3" t="str">
+        <f aca="false">VLOOKUP(L49,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N49" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O49" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q49" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T49" s="1" t="str">
+        <f aca="false">IF(NOT(D49="1X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c"),IF(E49="landmark",CONCATENATE(A49,"_k"),IF(E49="house",CONCATENATE(A49,"_h"),A49))))</f>
+        <v>none</v>
+      </c>
+      <c r="U49" s="1" t="str">
+        <f aca="false">IF(D49="1X1","none",IF(E49="skyscraper",CONCATENATE(A49,"_c_north"),IF(E49="landmark",CONCATENATE(A49,"_k_north"),IF(E49="house",CONCATENATE(A49,"_h_north"),CONCATENATE(A49,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V49" s="1" t="str">
+        <f aca="false">IF(OR(D49="1X1",D49="2X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_east"),IF(E49="landmark",CONCATENATE(A49,"_k_east"),CONCATENATE(A49,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W49" s="1" t="str">
+        <f aca="false">IF(OR(D49="1X1",D49="1X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_west"),IF(E49="landmark",CONCATENATE(A49,"_k_west"),CONCATENATE(A49,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X49" s="1" t="str">
+        <f aca="false">IF(NOT(D49="2X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_south"),IF(E49="landmark",CONCATENATE(A49,"_k_south"),CONCATENATE(A49,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y44" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="D45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="S45" s="3"/>
+      <c r="Y49" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="D50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="S50" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C33 C35:C1048576">
+  <conditionalFormatting sqref="C1:C38 C40:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E16" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E21" type="list">
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L45" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L50" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P45" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P50" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S45" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S50" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4404,7 +4851,7 @@
   </sheetPr>
   <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H194" activeCellId="0" sqref="H194"/>
     </sheetView>
   </sheetViews>
@@ -4412,16 +4859,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6385,11 +6832,11 @@
       </c>
       <c r="B117" s="1" t="str">
         <f aca="false">IF(C117="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C117" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A117,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D117" s="1" t="n">
         <f aca="false">IF(C117="Multi-tile",D116-1,MAX(IF(C117="ID not in use",0,IF(C117="1X1",1,IF(C117="2X2",4,2)))-1,0))</f>
@@ -6402,11 +6849,11 @@
       </c>
       <c r="B118" s="1" t="str">
         <f aca="false">IF(C118="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C118" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A118,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D118" s="1" t="n">
         <f aca="false">IF(C118="Multi-tile",D117-1,MAX(IF(C118="ID not in use",0,IF(C118="1X1",1,IF(C118="2X2",4,2)))-1,0))</f>
@@ -6470,11 +6917,11 @@
       </c>
       <c r="B122" s="1" t="str">
         <f aca="false">IF(C122="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C122" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A122,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D122" s="1" t="n">
         <f aca="false">IF(C122="Multi-tile",D121-1,MAX(IF(C122="ID not in use",0,IF(C122="1X1",1,IF(C122="2X2",4,2)))-1,0))</f>
@@ -6487,11 +6934,11 @@
       </c>
       <c r="B123" s="1" t="str">
         <f aca="false">IF(C123="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C123" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A123,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D123" s="1" t="n">
         <f aca="false">IF(C123="Multi-tile",D122-1,MAX(IF(C123="ID not in use",0,IF(C123="1X1",1,IF(C123="2X2",4,2)))-1,0))</f>
@@ -6504,11 +6951,11 @@
       </c>
       <c r="B124" s="1" t="str">
         <f aca="false">IF(C124="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C124" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A124,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D124" s="1" t="n">
         <f aca="false">IF(C124="Multi-tile",D123-1,MAX(IF(C124="ID not in use",0,IF(C124="1X1",1,IF(C124="2X2",4,2)))-1,0))</f>
@@ -8795,7 +9242,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8810,25 +9257,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8842,13 +9289,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -8871,10 +9318,10 @@
         <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8888,87 +9335,90 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: imai & kaneko
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="199">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -220,6 +220,27 @@
   </si>
   <si>
     <t xml:space="preserve">hirata_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imai_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_IMAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaneko_l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaneko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_KANEKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaneko_x</t>
   </si>
   <si>
     <t xml:space="preserve">kimura_s</t>
@@ -729,14 +750,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y59"/>
+  <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2121,38 +2142,38 @@
         <v>67</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>1950</v>
+        <v>1965</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="M17" s="5" t="str">
         <f aca="false">VLOOKUP(L17,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N17" s="1" t="n">
         <v>27</v>
@@ -2165,18 +2186,18 @@
       </c>
       <c r="Q17" s="1" t="n">
         <f aca="false">VLOOKUP(E17,dropdowns!A:C,2,0)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R17" s="1" t="n">
         <f aca="false">VLOOKUP(E17,dropdowns!A:C,3,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T17" s="1" t="str">
         <f aca="false">IF(NOT(D17="1X1"),"none",IF(E17="skyscraper",CONCATENATE(A17,"_c"),IF(E17="landmark",CONCATENATE(A17,"_k"),IF(E17="house",CONCATENATE(A17,"_h"),A17))))</f>
-        <v>kimura_s</v>
+        <v>imai_m</v>
       </c>
       <c r="U17" s="1" t="str">
         <f aca="false">IF(D17="1X1","none",IF(E17="skyscraper",CONCATENATE(A17,"_c_north"),IF(E17="landmark",CONCATENATE(A17,"_k_north"),IF(E17="house",CONCATENATE(A17,"_h_north"),CONCATENATE(A17,"_north")))))</f>
@@ -2203,41 +2224,41 @@
         <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="M18" s="5" t="str">
         <f aca="false">VLOOKUP(L18,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N18" s="1" t="n">
         <v>27</v>
@@ -2249,19 +2270,17 @@
         <v>32</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <f aca="false">VLOOKUP(E18,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R18" s="1" t="n">
-        <f aca="false">VLOOKUP(E18,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T18" s="1" t="str">
         <f aca="false">IF(NOT(D18="1X1"),"none",IF(E18="skyscraper",CONCATENATE(A18,"_c"),IF(E18="landmark",CONCATENATE(A18,"_k"),IF(E18="house",CONCATENATE(A18,"_h"),A18))))</f>
-        <v>kimura_m</v>
+        <v>kaneko_l</v>
       </c>
       <c r="U18" s="1" t="str">
         <f aca="false">IF(D18="1X1","none",IF(E18="skyscraper",CONCATENATE(A18,"_c_north"),IF(E18="landmark",CONCATENATE(A18,"_k_north"),IF(E18="house",CONCATENATE(A18,"_h_north"),CONCATENATE(A18,"_north")))))</f>
@@ -2285,44 +2304,44 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C19" s="2" t="n">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>1945</v>
+        <v>2000</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="M19" s="5" t="str">
         <f aca="false">VLOOKUP(L19,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N19" s="1" t="n">
         <v>27</v>
@@ -2334,19 +2353,17 @@
         <v>32</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <f aca="false">VLOOKUP(E19,dropdowns!A:C,2,0)</f>
+        <v>16</v>
+      </c>
+      <c r="R19" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="R19" s="1" t="n">
-        <f aca="false">VLOOKUP(E19,dropdowns!A:C,3,0)</f>
-        <v>2</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T19" s="1" t="str">
         <f aca="false">IF(NOT(D19="1X1"),"none",IF(E19="skyscraper",CONCATENATE(A19,"_c"),IF(E19="landmark",CONCATENATE(A19,"_k"),IF(E19="house",CONCATENATE(A19,"_h"),A19))))</f>
-        <v>murakami_s</v>
+        <v>kaneko_x</v>
       </c>
       <c r="U19" s="1" t="str">
         <f aca="false">IF(D19="1X1","none",IF(E19="skyscraper",CONCATENATE(A19,"_c_north"),IF(E19="landmark",CONCATENATE(A19,"_k_north"),IF(E19="house",CONCATENATE(A19,"_h_north"),CONCATENATE(A19,"_north")))))</f>
@@ -2373,41 +2390,41 @@
         <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>1945</v>
+        <v>1950</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="M20" s="5" t="str">
         <f aca="false">VLOOKUP(L20,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N20" s="1" t="n">
         <v>27</v>
@@ -2420,18 +2437,18 @@
       </c>
       <c r="Q20" s="1" t="n">
         <f aca="false">VLOOKUP(E20,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R20" s="1" t="n">
         <f aca="false">VLOOKUP(E20,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T20" s="1" t="str">
         <f aca="false">IF(NOT(D20="1X1"),"none",IF(E20="skyscraper",CONCATENATE(A20,"_c"),IF(E20="landmark",CONCATENATE(A20,"_k"),IF(E20="house",CONCATENATE(A20,"_h"),A20))))</f>
-        <v>murakami_m</v>
+        <v>kimura_s</v>
       </c>
       <c r="U20" s="1" t="str">
         <f aca="false">IF(D20="1X1","none",IF(E20="skyscraper",CONCATENATE(A20,"_c_north"),IF(E20="landmark",CONCATENATE(A20,"_k_north"),IF(E20="house",CONCATENATE(A20,"_h_north"),CONCATENATE(A20,"_north")))))</f>
@@ -2455,13 +2472,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C21" s="2" t="n">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>27</v>
@@ -2470,7 +2487,7 @@
         <v>28</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G21" s="1" t="n">
         <v>100</v>
@@ -2516,7 +2533,7 @@
       </c>
       <c r="T21" s="1" t="str">
         <f aca="false">IF(NOT(D21="1X1"),"none",IF(E21="skyscraper",CONCATENATE(A21,"_c"),IF(E21="landmark",CONCATENATE(A21,"_k"),IF(E21="house",CONCATENATE(A21,"_h"),A21))))</f>
-        <v>nakayama_m</v>
+        <v>kimura_m</v>
       </c>
       <c r="U21" s="1" t="str">
         <f aca="false">IF(D21="1X1","none",IF(E21="skyscraper",CONCATENATE(A21,"_c_north"),IF(E21="landmark",CONCATENATE(A21,"_k_north"),IF(E21="house",CONCATENATE(A21,"_h_north"),CONCATENATE(A21,"_north")))))</f>
@@ -2546,38 +2563,38 @@
         <v>78</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="M22" s="5" t="str">
         <f aca="false">VLOOKUP(L22,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N22" s="1" t="n">
         <v>27</v>
@@ -2590,18 +2607,18 @@
       </c>
       <c r="Q22" s="1" t="n">
         <f aca="false">VLOOKUP(E22,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R22" s="1" t="n">
         <f aca="false">VLOOKUP(E22,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T22" s="1" t="str">
         <f aca="false">IF(NOT(D22="1X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c"),IF(E22="landmark",CONCATENATE(A22,"_k"),IF(E22="house",CONCATENATE(A22,"_h"),A22))))</f>
-        <v>okada_office_tower_m</v>
+        <v>murakami_s</v>
       </c>
       <c r="U22" s="1" t="str">
         <f aca="false">IF(D22="1X1","none",IF(E22="skyscraper",CONCATENATE(A22,"_c_north"),IF(E22="landmark",CONCATENATE(A22,"_k_north"),IF(E22="house",CONCATENATE(A22,"_h_north"),CONCATENATE(A22,"_north")))))</f>
@@ -2631,38 +2648,38 @@
         <v>78</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M23" s="5" t="str">
         <f aca="false">VLOOKUP(L23,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N23" s="1" t="n">
         <v>27</v>
@@ -2674,17 +2691,19 @@
         <v>32</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>14</v>
+        <f aca="false">VLOOKUP(E23,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R23" s="1" t="n">
-        <v>5</v>
+        <f aca="false">VLOOKUP(E23,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T23" s="1" t="str">
         <f aca="false">IF(NOT(D23="1X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c"),IF(E23="landmark",CONCATENATE(A23,"_k"),IF(E23="house",CONCATENATE(A23,"_h"),A23))))</f>
-        <v>okada_office_tower_l</v>
+        <v>murakami_m</v>
       </c>
       <c r="U23" s="1" t="str">
         <f aca="false">IF(D23="1X1","none",IF(E23="skyscraper",CONCATENATE(A23,"_c_north"),IF(E23="landmark",CONCATENATE(A23,"_k_north"),IF(E23="house",CONCATENATE(A23,"_h_north"),CONCATENATE(A23,"_north")))))</f>
@@ -2711,41 +2730,41 @@
         <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M24" s="5" t="str">
         <f aca="false">VLOOKUP(L24,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N24" s="1" t="n">
         <v>27</v>
@@ -2757,17 +2776,19 @@
         <v>32</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>16</v>
+        <f aca="false">VLOOKUP(E24,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R24" s="1" t="n">
-        <v>6</v>
+        <f aca="false">VLOOKUP(E24,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T24" s="1" t="str">
         <f aca="false">IF(NOT(D24="1X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c"),IF(E24="landmark",CONCATENATE(A24,"_k"),IF(E24="house",CONCATENATE(A24,"_h"),A24))))</f>
-        <v>okada_office_tower_x</v>
+        <v>nakayama_m</v>
       </c>
       <c r="U24" s="1" t="str">
         <f aca="false">IF(D24="1X1","none",IF(E24="skyscraper",CONCATENATE(A24,"_c_north"),IF(E24="landmark",CONCATENATE(A24,"_k_north"),IF(E24="house",CONCATENATE(A24,"_h_north"),CONCATENATE(A24,"_north")))))</f>
@@ -2791,13 +2812,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
@@ -2806,7 +2827,7 @@
         <v>28</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>100</v>
@@ -2815,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>1945</v>
+        <v>1955</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>30</v>
@@ -2840,9 +2861,11 @@
         <v>32</v>
       </c>
       <c r="Q25" s="1" t="n">
+        <f aca="false">VLOOKUP(E25,dropdowns!A:C,2,0)</f>
         <v>10</v>
       </c>
       <c r="R25" s="1" t="n">
+        <f aca="false">VLOOKUP(E25,dropdowns!A:C,3,0)</f>
         <v>4</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -2850,7 +2873,7 @@
       </c>
       <c r="T25" s="1" t="str">
         <f aca="false">IF(NOT(D25="1X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c"),IF(E25="landmark",CONCATENATE(A25,"_k"),IF(E25="house",CONCATENATE(A25,"_h"),A25))))</f>
-        <v>old_office_building_m</v>
+        <v>okada_office_tower_m</v>
       </c>
       <c r="U25" s="1" t="str">
         <f aca="false">IF(D25="1X1","none",IF(E25="skyscraper",CONCATENATE(A25,"_c_north"),IF(E25="landmark",CONCATENATE(A25,"_k_north"),IF(E25="house",CONCATENATE(A25,"_h_north"),CONCATENATE(A25,"_north")))))</f>
@@ -2874,13 +2897,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C26" s="2" t="n">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
@@ -2889,7 +2912,7 @@
         <v>35</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>125</v>
@@ -2898,7 +2921,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>1945</v>
+        <v>1955</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>30</v>
@@ -2933,7 +2956,7 @@
       </c>
       <c r="T26" s="1" t="str">
         <f aca="false">IF(NOT(D26="1X1"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c"),IF(E26="landmark",CONCATENATE(A26,"_k"),IF(E26="house",CONCATENATE(A26,"_h"),A26))))</f>
-        <v>old_office_building_l</v>
+        <v>okada_office_tower_l</v>
       </c>
       <c r="U26" s="1" t="str">
         <f aca="false">IF(D26="1X1","none",IF(E26="skyscraper",CONCATENATE(A26,"_c_north"),IF(E26="landmark",CONCATENATE(A26,"_k_north"),IF(E26="house",CONCATENATE(A26,"_h_north"),CONCATENATE(A26,"_north")))))</f>
@@ -2957,44 +2980,44 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>1970</v>
+        <v>1955</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M27" s="5" t="str">
         <f aca="false">VLOOKUP(L27,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N27" s="1" t="n">
         <v>27</v>
@@ -3006,19 +3029,17 @@
         <v>32</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <f aca="false">VLOOKUP(E27,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="R27" s="1" t="n">
-        <f aca="false">VLOOKUP(E27,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T27" s="1" t="str">
         <f aca="false">IF(NOT(D27="1X1"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c"),IF(E27="landmark",CONCATENATE(A27,"_k"),IF(E27="house",CONCATENATE(A27,"_h"),A27))))</f>
-        <v>yamada_electronics_centre_m</v>
+        <v>okada_office_tower_x</v>
       </c>
       <c r="U27" s="1" t="str">
         <f aca="false">IF(D27="1X1","none",IF(E27="skyscraper",CONCATENATE(A27,"_c_north"),IF(E27="landmark",CONCATENATE(A27,"_k_north"),IF(E27="house",CONCATENATE(A27,"_h_north"),CONCATENATE(A27,"_north")))))</f>
@@ -3045,41 +3066,41 @@
         <v>89</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>1970</v>
+        <v>1945</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M28" s="5" t="str">
         <f aca="false">VLOOKUP(L28,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N28" s="1" t="n">
         <v>27</v>
@@ -3091,17 +3112,17 @@
         <v>32</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R28" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T28" s="1" t="str">
         <f aca="false">IF(NOT(D28="1X1"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c"),IF(E28="landmark",CONCATENATE(A28,"_k"),IF(E28="house",CONCATENATE(A28,"_h"),A28))))</f>
-        <v>yamada_electronics_centre_l</v>
+        <v>old_office_building_m</v>
       </c>
       <c r="U28" s="1" t="str">
         <f aca="false">IF(D28="1X1","none",IF(E28="skyscraper",CONCATENATE(A28,"_c_north"),IF(E28="landmark",CONCATENATE(A28,"_k_north"),IF(E28="house",CONCATENATE(A28,"_h_north"),CONCATENATE(A28,"_north")))))</f>
@@ -3125,44 +3146,44 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="C29" s="2" t="n">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>1970</v>
+        <v>1945</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M29" s="5" t="str">
         <f aca="false">VLOOKUP(L29,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N29" s="1" t="n">
         <v>27</v>
@@ -3174,17 +3195,17 @@
         <v>32</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R29" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T29" s="1" t="str">
         <f aca="false">IF(NOT(D29="1X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c"),IF(E29="landmark",CONCATENATE(A29,"_k"),IF(E29="house",CONCATENATE(A29,"_h"),A29))))</f>
-        <v>yamada_electronics_centre_x</v>
+        <v>old_office_building_l</v>
       </c>
       <c r="U29" s="1" t="str">
         <f aca="false">IF(D29="1X1","none",IF(E29="skyscraper",CONCATENATE(A29,"_c_north"),IF(E29="landmark",CONCATENATE(A29,"_k_north"),IF(E29="house",CONCATENATE(A29,"_h_north"),CONCATENATE(A29,"_north")))))</f>
@@ -3208,13 +3229,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
@@ -3223,7 +3244,7 @@
         <v>28</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>100</v>
@@ -3257,9 +3278,11 @@
         <v>32</v>
       </c>
       <c r="Q30" s="1" t="n">
+        <f aca="false">VLOOKUP(E30,dropdowns!A:C,2,0)</f>
         <v>10</v>
       </c>
       <c r="R30" s="1" t="n">
+        <f aca="false">VLOOKUP(E30,dropdowns!A:C,3,0)</f>
         <v>4</v>
       </c>
       <c r="S30" s="3" t="s">
@@ -3267,7 +3290,7 @@
       </c>
       <c r="T30" s="1" t="str">
         <f aca="false">IF(NOT(D30="1X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c"),IF(E30="landmark",CONCATENATE(A30,"_k"),IF(E30="house",CONCATENATE(A30,"_h"),A30))))</f>
-        <v>yano_m</v>
+        <v>yamada_electronics_centre_m</v>
       </c>
       <c r="U30" s="1" t="str">
         <f aca="false">IF(D30="1X1","none",IF(E30="skyscraper",CONCATENATE(A30,"_c_north"),IF(E30="landmark",CONCATENATE(A30,"_k_north"),IF(E30="house",CONCATENATE(A30,"_h_north"),CONCATENATE(A30,"_north")))))</f>
@@ -3291,66 +3314,66 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>94</v>
+      <c r="E31" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>95</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>220</v>
+        <v>125</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M31" s="5" t="str">
         <f aca="false">VLOOKUP(L31,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="O31" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R31" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q31" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="R31" s="1" t="n">
-        <v>6</v>
       </c>
       <c r="S31" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T31" s="1" t="str">
         <f aca="false">IF(NOT(D31="1X1"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c"),IF(E31="landmark",CONCATENATE(A31,"_k"),IF(E31="house",CONCATENATE(A31,"_h"),A31))))</f>
-        <v>bank_building_c</v>
+        <v>yamada_electronics_centre_l</v>
       </c>
       <c r="U31" s="1" t="str">
         <f aca="false">IF(D31="1X1","none",IF(E31="skyscraper",CONCATENATE(A31,"_c_north"),IF(E31="landmark",CONCATENATE(A31,"_k_north"),IF(E31="house",CONCATENATE(A31,"_h_north"),CONCATENATE(A31,"_north")))))</f>
@@ -3377,34 +3400,34 @@
         <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>94</v>
+      <c r="E32" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>1990</v>
+        <v>1970</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>39</v>
@@ -3414,26 +3437,26 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N32" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O32" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O32" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P32" s="3" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R32" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="T32" s="1" t="str">
         <f aca="false">IF(NOT(D32="1X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c"),IF(E32="landmark",CONCATENATE(A32,"_k"),IF(E32="house",CONCATENATE(A32,"_h"),A32))))</f>
-        <v>enterprise_tower_c</v>
+        <v>yamada_electronics_centre_x</v>
       </c>
       <c r="U32" s="1" t="str">
         <f aca="false">IF(D32="1X1","none",IF(E32="skyscraper",CONCATENATE(A32,"_c_north"),IF(E32="landmark",CONCATENATE(A32,"_k_north"),IF(E32="house",CONCATENATE(A32,"_h_north"),CONCATENATE(A32,"_north")))))</f>
@@ -3457,66 +3480,66 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>94</v>
+      <c r="E33" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>1960</v>
+        <v>1970</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M33" s="5" t="str">
         <f aca="false">VLOOKUP(L33,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N33" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O33" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O33" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P33" s="3" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="T33" s="1" t="str">
         <f aca="false">IF(NOT(D33="1X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c"),IF(E33="landmark",CONCATENATE(A33,"_k"),IF(E33="house",CONCATENATE(A33,"_h"),A33))))</f>
-        <v>insurance_tower_c</v>
+        <v>yano_m</v>
       </c>
       <c r="U33" s="1" t="str">
         <f aca="false">IF(D33="1X1","none",IF(E33="skyscraper",CONCATENATE(A33,"_c_north"),IF(E33="landmark",CONCATENATE(A33,"_k_north"),IF(E33="house",CONCATENATE(A33,"_h_north"),CONCATENATE(A33,"_north")))))</f>
@@ -3540,22 +3563,22 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>220</v>
@@ -3564,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>2000</v>
+        <v>1980</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>30</v>
@@ -3580,26 +3603,26 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="O34" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R34" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="T34" s="1" t="str">
         <f aca="false">IF(NOT(D34="1X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c"),IF(E34="landmark",CONCATENATE(A34,"_k"),IF(E34="house",CONCATENATE(A34,"_h"),A34))))</f>
-        <v>kuroi_tower_c</v>
+        <v>bank_building_c</v>
       </c>
       <c r="U34" s="1" t="str">
         <f aca="false">IF(D34="1X1","none",IF(E34="skyscraper",CONCATENATE(A34,"_c_north"),IF(E34="landmark",CONCATENATE(A34,"_k_north"),IF(E34="house",CONCATENATE(A34,"_h_north"),CONCATENATE(A34,"_north")))))</f>
@@ -3629,13 +3652,13 @@
         <v>104</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>105</v>
@@ -3647,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>30</v>
@@ -3669,7 +3692,7 @@
         <v>5</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>24</v>
@@ -3678,11 +3701,11 @@
         <v>10</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T35" s="1" t="str">
         <f aca="false">IF(NOT(D35="1X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c"),IF(E35="landmark",CONCATENATE(A35,"_k"),IF(E35="house",CONCATENATE(A35,"_h"),A35))))</f>
-        <v>mitsui_tower_c</v>
+        <v>enterprise_tower_c</v>
       </c>
       <c r="U35" s="1" t="str">
         <f aca="false">IF(D35="1X1","none",IF(E35="skyscraper",CONCATENATE(A35,"_c_north"),IF(E35="landmark",CONCATENATE(A35,"_k_north"),IF(E35="house",CONCATENATE(A35,"_h_north"),CONCATENATE(A35,"_north")))))</f>
@@ -3706,31 +3729,31 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>2000</v>
+        <v>1960</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>30</v>
@@ -3752,7 +3775,7 @@
         <v>5</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q36" s="1" t="n">
         <v>24</v>
@@ -3761,11 +3784,11 @@
         <v>10</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T36" s="1" t="str">
         <f aca="false">IF(NOT(D36="1X1"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c"),IF(E36="landmark",CONCATENATE(A36,"_k"),IF(E36="house",CONCATENATE(A36,"_h"),A36))))</f>
-        <v>modern_office_tower_c</v>
+        <v>insurance_tower_c</v>
       </c>
       <c r="U36" s="1" t="str">
         <f aca="false">IF(D36="1X1","none",IF(E36="skyscraper",CONCATENATE(A36,"_c_north"),IF(E36="landmark",CONCATENATE(A36,"_k_north"),IF(E36="house",CONCATENATE(A36,"_h_north"),CONCATENATE(A36,"_north")))))</f>
@@ -3789,22 +3812,22 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>220</v>
@@ -3813,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>30</v>
@@ -3835,7 +3858,7 @@
         <v>5</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q37" s="1" t="n">
         <v>24</v>
@@ -3844,11 +3867,11 @@
         <v>10</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T37" s="1" t="str">
         <f aca="false">IF(NOT(D37="1X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c"),IF(E37="landmark",CONCATENATE(A37,"_k"),IF(E37="house",CONCATENATE(A37,"_h"),A37))))</f>
-        <v>multimedia_offices_c</v>
+        <v>kuroi_tower_c</v>
       </c>
       <c r="U37" s="1" t="str">
         <f aca="false">IF(D37="1X1","none",IF(E37="skyscraper",CONCATENATE(A37,"_c_north"),IF(E37="landmark",CONCATENATE(A37,"_k_north"),IF(E37="house",CONCATENATE(A37,"_h_north"),CONCATENATE(A37,"_north")))))</f>
@@ -3872,22 +3895,22 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>220</v>
@@ -3918,7 +3941,7 @@
         <v>5</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q38" s="1" t="n">
         <v>24</v>
@@ -3927,11 +3950,11 @@
         <v>10</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T38" s="1" t="str">
         <f aca="false">IF(NOT(D38="1X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c"),IF(E38="landmark",CONCATENATE(A38,"_k"),IF(E38="house",CONCATENATE(A38,"_h"),A38))))</f>
-        <v>office_tower_c</v>
+        <v>mitsui_tower_c</v>
       </c>
       <c r="U38" s="1" t="str">
         <f aca="false">IF(D38="1X1","none",IF(E38="skyscraper",CONCATENATE(A38,"_c_north"),IF(E38="landmark",CONCATENATE(A38,"_k_north"),IF(E38="house",CONCATENATE(A38,"_h_north"),CONCATENATE(A38,"_north")))))</f>
@@ -3955,31 +3978,31 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>1960</v>
+        <v>2000</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>30</v>
@@ -4001,7 +4024,7 @@
         <v>5</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q39" s="1" t="n">
         <v>24</v>
@@ -4010,11 +4033,11 @@
         <v>10</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T39" s="1" t="str">
         <f aca="false">IF(NOT(D39="1X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c"),IF(E39="landmark",CONCATENATE(A39,"_k"),IF(E39="house",CONCATENATE(A39,"_h"),A39))))</f>
-        <v>sato_building_c</v>
+        <v>modern_office_tower_c</v>
       </c>
       <c r="U39" s="1" t="str">
         <f aca="false">IF(D39="1X1","none",IF(E39="skyscraper",CONCATENATE(A39,"_c_north"),IF(E39="landmark",CONCATENATE(A39,"_k_north"),IF(E39="house",CONCATENATE(A39,"_h_north"),CONCATENATE(A39,"_north")))))</f>
@@ -4038,25 +4061,25 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H40" s="1" t="n">
         <v>1</v>
@@ -4084,7 +4107,7 @@
         <v>5</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q40" s="1" t="n">
         <v>24</v>
@@ -4093,11 +4116,11 @@
         <v>10</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T40" s="1" t="str">
         <f aca="false">IF(NOT(D40="1X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c"),IF(E40="landmark",CONCATENATE(A40,"_k"),IF(E40="house",CONCATENATE(A40,"_h"),A40))))</f>
-        <v>sugiyama_office_building_c</v>
+        <v>multimedia_offices_c</v>
       </c>
       <c r="U40" s="1" t="str">
         <f aca="false">IF(D40="1X1","none",IF(E40="skyscraper",CONCATENATE(A40,"_c_north"),IF(E40="landmark",CONCATENATE(A40,"_k_north"),IF(E40="house",CONCATENATE(A40,"_h_north"),CONCATENATE(A40,"_north")))))</f>
@@ -4121,31 +4144,31 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>118</v>
       </c>
       <c r="G41" s="1" t="n">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>30</v>
@@ -4161,13 +4184,13 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O41" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q41" s="1" t="n">
         <v>24</v>
@@ -4176,19 +4199,19 @@
         <v>10</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T41" s="1" t="str">
         <f aca="false">IF(NOT(D41="1X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c"),IF(E41="landmark",CONCATENATE(A41,"_k"),IF(E41="house",CONCATENATE(A41,"_h"),A41))))</f>
-        <v>none</v>
+        <v>office_tower_c</v>
       </c>
       <c r="U41" s="1" t="str">
         <f aca="false">IF(D41="1X1","none",IF(E41="skyscraper",CONCATENATE(A41,"_c_north"),IF(E41="landmark",CONCATENATE(A41,"_k_north"),IF(E41="house",CONCATENATE(A41,"_h_north"),CONCATENATE(A41,"_north")))))</f>
-        <v>tsuno_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V41" s="1" t="str">
         <f aca="false">IF(OR(D41="1X1",D41="2X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_east"),IF(E41="landmark",CONCATENATE(A41,"_k_east"),CONCATENATE(A41,"_east"))))</f>
-        <v>tsuno_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W41" s="1" t="str">
         <f aca="false">IF(OR(D41="1X1",D41="1X2"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c_west"),IF(E41="landmark",CONCATENATE(A41,"_k_west"),CONCATENATE(A41,"_west"))))</f>
@@ -4210,13 +4233,13 @@
         <v>119</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>120</v>
@@ -4228,10 +4251,10 @@
         <v>1</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>1955</v>
-      </c>
-      <c r="J42" s="4" t="n">
-        <v>1989</v>
+        <v>1960</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="K42" s="1" t="n">
         <v>25</v>
@@ -4250,7 +4273,7 @@
         <v>5</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q42" s="1" t="n">
         <v>24</v>
@@ -4259,11 +4282,11 @@
         <v>10</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T42" s="1" t="str">
         <f aca="false">IF(NOT(D42="1X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c"),IF(E42="landmark",CONCATENATE(A42,"_k"),IF(E42="house",CONCATENATE(A42,"_h"),A42))))</f>
-        <v>ueda_office_block_c</v>
+        <v>sato_building_c</v>
       </c>
       <c r="U42" s="1" t="str">
         <f aca="false">IF(D42="1X1","none",IF(E42="skyscraper",CONCATENATE(A42,"_c_north"),IF(E42="landmark",CONCATENATE(A42,"_k_north"),IF(E42="house",CONCATENATE(A42,"_h_north"),CONCATENATE(A42,"_north")))))</f>
@@ -4293,25 +4316,25 @@
         <v>121</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>1965</v>
+        <v>1990</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>30</v>
@@ -4333,20 +4356,20 @@
         <v>5</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q43" s="1" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R43" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T43" s="1" t="str">
         <f aca="false">IF(NOT(D43="1X1"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c"),IF(E43="landmark",CONCATENATE(A43,"_k"),IF(E43="house",CONCATENATE(A43,"_h"),A43))))</f>
-        <v>yamaguchi_office_c</v>
+        <v>sugiyama_office_building_c</v>
       </c>
       <c r="U43" s="1" t="str">
         <f aca="false">IF(D43="1X1","none",IF(E43="skyscraper",CONCATENATE(A43,"_c_north"),IF(E43="landmark",CONCATENATE(A43,"_k_north"),IF(E43="house",CONCATENATE(A43,"_h_north"),CONCATENATE(A43,"_north")))))</f>
@@ -4376,16 +4399,16 @@
         <v>123</v>
       </c>
       <c r="C44" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>255</v>
@@ -4394,7 +4417,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>1990</v>
+        <v>2006</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>30</v>
@@ -4416,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q44" s="1" t="n">
         <v>24</v>
@@ -4425,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T44" s="1" t="str">
         <f aca="false">IF(NOT(D44="1X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c"),IF(E44="landmark",CONCATENATE(A44,"_k"),IF(E44="house",CONCATENATE(A44,"_h"),A44))))</f>
@@ -4433,11 +4456,11 @@
       </c>
       <c r="U44" s="1" t="str">
         <f aca="false">IF(D44="1X1","none",IF(E44="skyscraper",CONCATENATE(A44,"_c_north"),IF(E44="landmark",CONCATENATE(A44,"_k_north"),IF(E44="house",CONCATENATE(A44,"_h_north"),CONCATENATE(A44,"_north")))))</f>
-        <v>yamashiro_office_building_c_north</v>
+        <v>tsuno_building_c_north</v>
       </c>
       <c r="V44" s="1" t="str">
         <f aca="false">IF(OR(D44="1X1",D44="2X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_east"),IF(E44="landmark",CONCATENATE(A44,"_k_east"),CONCATENATE(A44,"_east"))))</f>
-        <v>yamashiro_office_building_c_east</v>
+        <v>tsuno_building_c_east</v>
       </c>
       <c r="W44" s="1" t="str">
         <f aca="false">IF(OR(D44="1X1",D44="1X2"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_west"),IF(E44="landmark",CONCATENATE(A44,"_k_west"),CONCATENATE(A44,"_west"))))</f>
@@ -4453,34 +4476,34 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G45" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>30</v>
+        <v>1955</v>
+      </c>
+      <c r="J45" s="4" t="n">
+        <v>1989</v>
       </c>
       <c r="K45" s="1" t="n">
         <v>25</v>
@@ -4499,7 +4522,7 @@
         <v>5</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q45" s="1" t="n">
         <v>24</v>
@@ -4508,11 +4531,11 @@
         <v>10</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T45" s="1" t="str">
         <f aca="false">IF(NOT(D45="1X1"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c"),IF(E45="landmark",CONCATENATE(A45,"_k"),IF(E45="house",CONCATENATE(A45,"_h"),A45))))</f>
-        <v>yamashita_building_c</v>
+        <v>ueda_office_block_c</v>
       </c>
       <c r="U45" s="1" t="str">
         <f aca="false">IF(D45="1X1","none",IF(E45="skyscraper",CONCATENATE(A45,"_c_north"),IF(E45="landmark",CONCATENATE(A45,"_k_north"),IF(E45="house",CONCATENATE(A45,"_h_north"),CONCATENATE(A45,"_north")))))</f>
@@ -4536,311 +4559,311 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="G46" s="1" t="n">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>1700</v>
+        <v>1965</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K46" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="M46" s="5" t="str">
         <f aca="false">VLOOKUP(L46,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N46" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O46" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="Q46" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="R46" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="T46" s="1" t="str">
         <f aca="false">IF(NOT(D46="1X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c"),IF(E46="landmark",CONCATENATE(A46,"_k"),IF(E46="house",CONCATENATE(A46,"_h"),A46))))</f>
-        <v>none</v>
+        <v>yamaguchi_office_c</v>
       </c>
       <c r="U46" s="1" t="str">
         <f aca="false">IF(D46="1X1","none",IF(E46="skyscraper",CONCATENATE(A46,"_c_north"),IF(E46="landmark",CONCATENATE(A46,"_k_north"),IF(E46="house",CONCATENATE(A46,"_h_north"),CONCATENATE(A46,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>none</v>
       </c>
       <c r="V46" s="1" t="str">
-        <f aca="false">IF(OR(D46="1X1",D46="2X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_east"),IF(E46="landmark",CONCATENATE(A46,"_k_east"),IF(E46="house",CONCATENATE(A46,"_h_east"),CONCATENATE(A46,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D46="1X1",D46="2X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_east"),IF(E46="landmark",CONCATENATE(A46,"_k_east"),CONCATENATE(A46,"_east"))))</f>
+        <v>none</v>
       </c>
       <c r="W46" s="1" t="str">
-        <f aca="false">IF(OR(D46="1X1",D46="1X2"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_west"),IF(E46="landmark",CONCATENATE(A46,"_k_west"),IF(E46="house",CONCATENATE(A46,"_h_west"),CONCATENATE(A46,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D46="1X1",D46="1X2"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_west"),IF(E46="landmark",CONCATENATE(A46,"_k_west"),CONCATENATE(A46,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X46" s="1" t="str">
-        <f aca="false">IF(NOT(D46="2X2"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_south"),IF(E46="landmark",CONCATENATE(A46,"_k_south"),IF(E46="house",CONCATENATE(A46,"_h_south"),CONCATENATE(A46,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D46="2X2"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c_south"),IF(E46="landmark",CONCATENATE(A46,"_k_south"),CONCATENATE(A46,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y46" s="1" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>20</v>
+        <v>255</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I47" s="1" t="n">
-        <v>1870</v>
+        <v>1990</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K47" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>136</v>
+        <v>39</v>
       </c>
       <c r="M47" s="5" t="str">
         <f aca="false">VLOOKUP(L47,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N47" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O47" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="Q47" s="1" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="R47" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="T47" s="1" t="str">
         <f aca="false">IF(NOT(D47="1X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c"),IF(E47="landmark",CONCATENATE(A47,"_k"),IF(E47="house",CONCATENATE(A47,"_h"),A47))))</f>
-        <v>naganuma_h</v>
+        <v>none</v>
       </c>
       <c r="U47" s="1" t="str">
         <f aca="false">IF(D47="1X1","none",IF(E47="skyscraper",CONCATENATE(A47,"_c_north"),IF(E47="landmark",CONCATENATE(A47,"_k_north"),IF(E47="house",CONCATENATE(A47,"_h_north"),CONCATENATE(A47,"_north")))))</f>
-        <v>none</v>
+        <v>yamashiro_office_building_c_north</v>
       </c>
       <c r="V47" s="1" t="str">
-        <f aca="false">IF(OR(D47="1X1",D47="2X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_east"),IF(E47="landmark",CONCATENATE(A47,"_k_east"),IF(E47="house",CONCATENATE(A47,"_h_east"),CONCATENATE(A47,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D47="1X1",D47="2X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_east"),IF(E47="landmark",CONCATENATE(A47,"_k_east"),CONCATENATE(A47,"_east"))))</f>
+        <v>yamashiro_office_building_c_east</v>
       </c>
       <c r="W47" s="1" t="str">
-        <f aca="false">IF(OR(D47="1X1",D47="1X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_west"),IF(E47="landmark",CONCATENATE(A47,"_k_west"),IF(E47="house",CONCATENATE(A47,"_h_west"),CONCATENATE(A47,"_west")))))</f>
+        <f aca="false">IF(OR(D47="1X1",D47="1X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_west"),IF(E47="landmark",CONCATENATE(A47,"_k_west"),CONCATENATE(A47,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X47" s="1" t="str">
-        <f aca="false">IF(NOT(D47="2X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_south"),IF(E47="landmark",CONCATENATE(A47,"_k_south"),IF(E47="house",CONCATENATE(A47,"_h_south"),CONCATENATE(A47,"_south")))))</f>
+        <f aca="false">IF(NOT(D47="2X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_south"),IF(E47="landmark",CONCATENATE(A47,"_k_south"),CONCATENATE(A47,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y47" s="1" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="6" t="n">
-        <v>95</v>
+      <c r="A48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G48" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H48" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="H48" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I48" s="0" t="n">
-        <v>1950</v>
+      <c r="I48" s="1" t="n">
+        <v>2000</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K48" s="0" t="n">
-        <v>5</v>
+      <c r="K48" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="M48" s="5" t="str">
         <f aca="false">VLOOKUP(L48,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N48" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O48" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
+      </c>
+      <c r="N48" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O48" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q48" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R48" s="0" t="n">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="Q48" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R48" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="T48" s="1" t="str">
         <f aca="false">IF(NOT(D48="1X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c"),IF(E48="landmark",CONCATENATE(A48,"_k"),IF(E48="house",CONCATENATE(A48,"_h"),A48))))</f>
-        <v>convini_k</v>
+        <v>yamashita_building_c</v>
       </c>
       <c r="U48" s="1" t="str">
         <f aca="false">IF(D48="1X1","none",IF(E48="skyscraper",CONCATENATE(A48,"_c_north"),IF(E48="landmark",CONCATENATE(A48,"_k_north"),IF(E48="house",CONCATENATE(A48,"_h_north"),CONCATENATE(A48,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V48" s="1" t="str">
-        <f aca="false">IF(OR(D48="1X1",D48="2X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_east"),IF(E48="landmark",CONCATENATE(A48,"_k_east"),IF(E48="house",CONCATENATE(A48,"_h_east"),CONCATENATE(A48,"_east")))))</f>
+        <f aca="false">IF(OR(D48="1X1",D48="2X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_east"),IF(E48="landmark",CONCATENATE(A48,"_k_east"),CONCATENATE(A48,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W48" s="1" t="str">
-        <f aca="false">IF(OR(D48="1X1",D48="1X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_west"),IF(E48="landmark",CONCATENATE(A48,"_k_west"),IF(E48="house",CONCATENATE(A48,"_h_west"),CONCATENATE(A48,"_west")))))</f>
+        <f aca="false">IF(OR(D48="1X1",D48="1X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_west"),IF(E48="landmark",CONCATENATE(A48,"_k_west"),CONCATENATE(A48,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X48" s="1" t="str">
-        <f aca="false">IF(NOT(D48="2X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_south"),IF(E48="landmark",CONCATENATE(A48,"_k_south"),IF(E48="house",CONCATENATE(A48,"_h_south"),CONCATENATE(A48,"_south")))))</f>
-        <v>none</v>
-      </c>
-      <c r="Y48" s="0" t="s">
-        <v>143</v>
+        <f aca="false">IF(NOT(D48="2X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_south"),IF(E48="landmark",CONCATENATE(A48,"_k_south"),CONCATENATE(A48,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y48" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K49" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="M49" s="5" t="str">
         <f aca="false">VLOOKUP(L49,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N49" s="1" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="O49" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="Q49" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R49" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>33</v>
+        <v>140</v>
       </c>
       <c r="T49" s="1" t="str">
         <f aca="false">IF(NOT(D49="1X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c"),IF(E49="landmark",CONCATENATE(A49,"_k"),IF(E49="house",CONCATENATE(A49,"_h"),A49))))</f>
@@ -4848,169 +4871,169 @@
       </c>
       <c r="U49" s="1" t="str">
         <f aca="false">IF(D49="1X1","none",IF(E49="skyscraper",CONCATENATE(A49,"_c_north"),IF(E49="landmark",CONCATENATE(A49,"_k_north"),IF(E49="house",CONCATENATE(A49,"_h_north"),CONCATENATE(A49,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V49" s="1" t="str">
         <f aca="false">IF(OR(D49="1X1",D49="2X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_east"),IF(E49="landmark",CONCATENATE(A49,"_k_east"),IF(E49="house",CONCATENATE(A49,"_h_east"),CONCATENATE(A49,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W49" s="1" t="str">
         <f aca="false">IF(OR(D49="1X1",D49="1X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_west"),IF(E49="landmark",CONCATENATE(A49,"_k_west"),IF(E49="house",CONCATENATE(A49,"_h_west"),CONCATENATE(A49,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X49" s="1" t="str">
         <f aca="false">IF(NOT(D49="2X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_south"),IF(E49="landmark",CONCATENATE(A49,"_k_south"),IF(E49="house",CONCATENATE(A49,"_h_south"),CONCATENATE(A49,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G50" s="1" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K50" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="M50" s="5" t="str">
         <f aca="false">VLOOKUP(L50,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N50" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O50" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="Q50" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R50" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="T50" s="1" t="str">
         <f aca="false">IF(NOT(D50="1X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c"),IF(E50="landmark",CONCATENATE(A50,"_k"),IF(E50="house",CONCATENATE(A50,"_h"),A50))))</f>
-        <v>none</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U50" s="1" t="str">
         <f aca="false">IF(D50="1X1","none",IF(E50="skyscraper",CONCATENATE(A50,"_c_north"),IF(E50="landmark",CONCATENATE(A50,"_k_north"),IF(E50="house",CONCATENATE(A50,"_h_north"),CONCATENATE(A50,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>none</v>
       </c>
       <c r="V50" s="1" t="str">
-        <f aca="false">IF(OR(D50="1X1",D50="2X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_east"),IF(E50="landmark",CONCATENATE(A50,"_k_east"),CONCATENATE(A50,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D50="1X1",D50="2X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_east"),IF(E50="landmark",CONCATENATE(A50,"_k_east"),IF(E50="house",CONCATENATE(A50,"_h_east"),CONCATENATE(A50,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W50" s="1" t="str">
-        <f aca="false">IF(OR(D50="1X1",D50="1X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_west"),IF(E50="landmark",CONCATENATE(A50,"_k_west"),CONCATENATE(A50,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D50="1X1",D50="1X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_west"),IF(E50="landmark",CONCATENATE(A50,"_k_west"),IF(E50="house",CONCATENATE(A50,"_h_west"),CONCATENATE(A50,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X50" s="1" t="str">
-        <f aca="false">IF(NOT(D50="2X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_south"),IF(E50="landmark",CONCATENATE(A50,"_k_south"),CONCATENATE(A50,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D50="2X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_south"),IF(E50="landmark",CONCATENATE(A50,"_k_south"),IF(E50="house",CONCATENATE(A50,"_h_south"),CONCATENATE(A50,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="2" t="n">
-        <v>93</v>
+      <c r="A51" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="6" t="n">
+        <v>95</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G51" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H51" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H51" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I51" s="1" t="n">
-        <v>1870</v>
+      <c r="I51" s="0" t="n">
+        <v>1950</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K51" s="1" t="n">
-        <v>10</v>
+      <c r="K51" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="M51" s="5" t="str">
         <f aca="false">VLOOKUP(L51,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
-      <c r="N51" s="1" t="n">
+      <c r="N51" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="O51" s="1" t="n">
+      <c r="O51" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q51" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="R51" s="1" t="n">
-        <v>6</v>
+        <v>139</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R51" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="T51" s="1" t="str">
         <f aca="false">IF(NOT(D51="1X1"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c"),IF(E51="landmark",CONCATENATE(A51,"_k"),IF(E51="house",CONCATENATE(A51,"_h"),A51))))</f>
-        <v>onsen_k</v>
+        <v>convini_k</v>
       </c>
       <c r="U51" s="1" t="str">
         <f aca="false">IF(D51="1X1","none",IF(E51="skyscraper",CONCATENATE(A51,"_c_north"),IF(E51="landmark",CONCATENATE(A51,"_k_north"),IF(E51="house",CONCATENATE(A51,"_h_north"),CONCATENATE(A51,"_north")))))</f>
@@ -5028,114 +5051,114 @@
         <f aca="false">IF(NOT(D51="2X2"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_south"),IF(E51="landmark",CONCATENATE(A51,"_k_south"),IF(E51="house",CONCATENATE(A51,"_h_south"),CONCATENATE(A51,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y51" s="1" t="s">
-        <v>143</v>
+      <c r="Y51" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C52" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>153</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H52" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K52" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="M52" s="5" t="str">
         <f aca="false">VLOOKUP(L52,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N52" s="1" t="n">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="O52" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="Q52" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R52" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>154</v>
+        <v>33</v>
       </c>
       <c r="T52" s="1" t="str">
         <f aca="false">IF(NOT(D52="1X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c"),IF(E52="landmark",CONCATENATE(A52,"_k"),IF(E52="house",CONCATENATE(A52,"_h"),A52))))</f>
-        <v>pachinko_k</v>
+        <v>none</v>
       </c>
       <c r="U52" s="1" t="str">
         <f aca="false">IF(D52="1X1","none",IF(E52="skyscraper",CONCATENATE(A52,"_c_north"),IF(E52="landmark",CONCATENATE(A52,"_k_north"),IF(E52="house",CONCATENATE(A52,"_h_north"),CONCATENATE(A52,"_north")))))</f>
-        <v>none</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V52" s="1" t="str">
-        <f aca="false">IF(OR(D52="1X1",D52="2X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_east"),IF(E52="landmark",CONCATENATE(A52,"_k_east"),CONCATENATE(A52,"_east"))))</f>
+        <f aca="false">IF(OR(D52="1X1",D52="2X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_east"),IF(E52="landmark",CONCATENATE(A52,"_k_east"),IF(E52="house",CONCATENATE(A52,"_h_east"),CONCATENATE(A52,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W52" s="1" t="str">
-        <f aca="false">IF(OR(D52="1X1",D52="1X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_west"),IF(E52="landmark",CONCATENATE(A52,"_k_west"),CONCATENATE(A52,"_west"))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D52="1X1",D52="1X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_west"),IF(E52="landmark",CONCATENATE(A52,"_k_west"),IF(E52="house",CONCATENATE(A52,"_h_west"),CONCATENATE(A52,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X52" s="1" t="str">
-        <f aca="false">IF(NOT(D52="2X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_south"),IF(E52="landmark",CONCATENATE(A52,"_k_south"),CONCATENATE(A52,"_south"))))</f>
+        <f aca="false">IF(NOT(D52="2X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_south"),IF(E52="landmark",CONCATENATE(A52,"_k_south"),IF(E52="house",CONCATENATE(A52,"_h_south"),CONCATENATE(A52,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y52" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="G53" s="1" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="H53" s="1" t="n">
         <v>3</v>
@@ -5150,29 +5173,29 @@
         <v>20</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="M53" s="5" t="str">
         <f aca="false">VLOOKUP(L53,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N53" s="1" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O53" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="Q53" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R53" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="T53" s="1" t="str">
         <f aca="false">IF(NOT(D53="1X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c"),IF(E53="landmark",CONCATENATE(A53,"_k"),IF(E53="house",CONCATENATE(A53,"_h"),A53))))</f>
@@ -5180,39 +5203,39 @@
       </c>
       <c r="U53" s="1" t="str">
         <f aca="false">IF(D53="1X1","none",IF(E53="skyscraper",CONCATENATE(A53,"_c_north"),IF(E53="landmark",CONCATENATE(A53,"_k_north"),IF(E53="house",CONCATENATE(A53,"_h_north"),CONCATENATE(A53,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V53" s="1" t="str">
         <f aca="false">IF(OR(D53="1X1",D53="2X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_east"),IF(E53="landmark",CONCATENATE(A53,"_k_east"),CONCATENATE(A53,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W53" s="1" t="str">
         <f aca="false">IF(OR(D53="1X1",D53="1X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_west"),IF(E53="landmark",CONCATENATE(A53,"_k_west"),CONCATENATE(A53,"_west"))))</f>
-        <v>none</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X53" s="1" t="str">
         <f aca="false">IF(NOT(D53="2X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_south"),IF(E53="landmark",CONCATENATE(A53,"_k_south"),CONCATENATE(A53,"_south"))))</f>
-        <v>none</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y53" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>216</v>
+        <v>93</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>158</v>
@@ -5220,65 +5243,65 @@
       <c r="G54" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H54" s="0" t="n">
-        <v>3</v>
+      <c r="H54" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I54" s="1" t="n">
-        <v>1700</v>
+        <v>1870</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M54" s="5" t="str">
         <f aca="false">VLOOKUP(L54,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N54" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O54" s="0" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N54" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O54" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="Q54" s="1" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="R54" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>154</v>
+        <v>33</v>
       </c>
       <c r="T54" s="1" t="str">
         <f aca="false">IF(NOT(D54="1X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c"),IF(E54="landmark",CONCATENATE(A54,"_k"),IF(E54="house",CONCATENATE(A54,"_h"),A54))))</f>
-        <v>none</v>
+        <v>onsen_k</v>
       </c>
       <c r="U54" s="1" t="str">
         <f aca="false">IF(D54="1X1","none",IF(E54="skyscraper",CONCATENATE(A54,"_c_north"),IF(E54="landmark",CONCATENATE(A54,"_k_north"),IF(E54="house",CONCATENATE(A54,"_h_north"),CONCATENATE(A54,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>none</v>
       </c>
       <c r="V54" s="1" t="str">
-        <f aca="false">IF(OR(D54="1X1",D54="2X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_east"),IF(E54="landmark",CONCATENATE(A54,"_k_east"),CONCATENATE(A54,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <f aca="false">IF(OR(D54="1X1",D54="2X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_east"),IF(E54="landmark",CONCATENATE(A54,"_k_east"),IF(E54="house",CONCATENATE(A54,"_h_east"),CONCATENATE(A54,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W54" s="1" t="str">
-        <f aca="false">IF(OR(D54="1X1",D54="1X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_west"),IF(E54="landmark",CONCATENATE(A54,"_k_west"),CONCATENATE(A54,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <f aca="false">IF(OR(D54="1X1",D54="1X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_west"),IF(E54="landmark",CONCATENATE(A54,"_k_west"),IF(E54="house",CONCATENATE(A54,"_h_west"),CONCATENATE(A54,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X54" s="1" t="str">
-        <f aca="false">IF(NOT(D54="2X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_south"),IF(E54="landmark",CONCATENATE(A54,"_k_south"),CONCATENATE(A54,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <f aca="false">IF(NOT(D54="2X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_south"),IF(E54="landmark",CONCATENATE(A54,"_k_south"),IF(E54="house",CONCATENATE(A54,"_h_south"),CONCATENATE(A54,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,60 +5312,60 @@
         <v>159</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>160</v>
       </c>
       <c r="G55" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I55" s="1" t="n">
-        <v>0</v>
+        <v>1980</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K55" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>161</v>
+        <v>56</v>
       </c>
       <c r="M55" s="5" t="str">
         <f aca="false">VLOOKUP(L55,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N55" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O55" s="0" t="n">
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N55" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O55" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="Q55" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R55" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T55" s="1" t="str">
         <f aca="false">IF(NOT(D55="1X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c"),IF(E55="landmark",CONCATENATE(A55,"_k"),IF(E55="house",CONCATENATE(A55,"_h"),A55))))</f>
-        <v>shrine_k</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U55" s="1" t="str">
         <f aca="false">IF(D55="1X1","none",IF(E55="skyscraper",CONCATENATE(A55,"_c_north"),IF(E55="landmark",CONCATENATE(A55,"_k_north"),IF(E55="house",CONCATENATE(A55,"_h_north"),CONCATENATE(A55,"_north")))))</f>
@@ -5366,31 +5389,31 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" s="2" t="n">
-        <v>113</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G56" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <v>5</v>
+        <v>80</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I56" s="1" t="n">
-        <v>0</v>
+        <v>1970</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>30</v>
@@ -5399,41 +5422,41 @@
         <v>20</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="M56" s="5" t="str">
         <f aca="false">VLOOKUP(L56,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N56" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O56" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N56" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O56" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="Q56" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R56" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="T56" s="1" t="str">
         <f aca="false">IF(NOT(D56="1X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c"),IF(E56="landmark",CONCATENATE(A56,"_k"),IF(E56="house",CONCATENATE(A56,"_h"),A56))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>none</v>
       </c>
       <c r="U56" s="1" t="str">
         <f aca="false">IF(D56="1X1","none",IF(E56="skyscraper",CONCATENATE(A56,"_c_north"),IF(E56="landmark",CONCATENATE(A56,"_k_north"),IF(E56="house",CONCATENATE(A56,"_h_north"),CONCATENATE(A56,"_north")))))</f>
-        <v>none</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V56" s="1" t="str">
         <f aca="false">IF(OR(D56="1X1",D56="2X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_east"),IF(E56="landmark",CONCATENATE(A56,"_k_east"),CONCATENATE(A56,"_east"))))</f>
-        <v>none</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W56" s="1" t="str">
         <f aca="false">IF(OR(D56="1X1",D56="1X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_west"),IF(E56="landmark",CONCATENATE(A56,"_k_west"),CONCATENATE(A56,"_west"))))</f>
@@ -5444,36 +5467,36 @@
         <v>none</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" s="2" t="n">
-        <v>204</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="G57" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H57" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H57" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>30</v>
@@ -5482,29 +5505,29 @@
         <v>20</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="M57" s="5" t="str">
         <f aca="false">VLOOKUP(L57,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
-      <c r="N57" s="1" t="n">
+      <c r="N57" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O57" s="1" t="n">
+      <c r="O57" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="Q57" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R57" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="T57" s="1" t="str">
         <f aca="false">IF(NOT(D57="1X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c"),IF(E57="landmark",CONCATENATE(A57,"_k"),IF(E57="house",CONCATENATE(A57,"_h"),A57))))</f>
@@ -5512,51 +5535,51 @@
       </c>
       <c r="U57" s="1" t="str">
         <f aca="false">IF(D57="1X1","none",IF(E57="skyscraper",CONCATENATE(A57,"_c_north"),IF(E57="landmark",CONCATENATE(A57,"_k_north"),IF(E57="house",CONCATENATE(A57,"_h_north"),CONCATENATE(A57,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V57" s="1" t="str">
         <f aca="false">IF(OR(D57="1X1",D57="2X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_east"),IF(E57="landmark",CONCATENATE(A57,"_k_east"),CONCATENATE(A57,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W57" s="1" t="str">
         <f aca="false">IF(OR(D57="1X1",D57="1X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_west"),IF(E57="landmark",CONCATENATE(A57,"_k_west"),CONCATENATE(A57,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X57" s="1" t="str">
         <f aca="false">IF(NOT(D57="2X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_south"),IF(E57="landmark",CONCATENATE(A57,"_k_south"),CONCATENATE(A57,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y57" s="1" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C58" s="2" t="n">
-        <v>208</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="G58" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H58" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I58" s="1" t="n">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>30</v>
@@ -5565,82 +5588,331 @@
         <v>20</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="M58" s="5" t="str">
         <f aca="false">VLOOKUP(L58,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
-      <c r="N58" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O58" s="1" t="n">
+      <c r="N58" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O58" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q58" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R58" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="T58" s="1" t="str">
         <f aca="false">IF(NOT(D58="1X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c"),IF(E58="landmark",CONCATENATE(A58,"_k"),IF(E58="house",CONCATENATE(A58,"_h"),A58))))</f>
-        <v>none</v>
+        <v>shrine_k</v>
       </c>
       <c r="U58" s="1" t="str">
         <f aca="false">IF(D58="1X1","none",IF(E58="skyscraper",CONCATENATE(A58,"_c_north"),IF(E58="landmark",CONCATENATE(A58,"_k_north"),IF(E58="house",CONCATENATE(A58,"_h_north"),CONCATENATE(A58,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>none</v>
       </c>
       <c r="V58" s="1" t="str">
         <f aca="false">IF(OR(D58="1X1",D58="2X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_east"),IF(E58="landmark",CONCATENATE(A58,"_k_east"),CONCATENATE(A58,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>none</v>
       </c>
       <c r="W58" s="1" t="str">
         <f aca="false">IF(OR(D58="1X1",D58="1X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_west"),IF(E58="landmark",CONCATENATE(A58,"_k_west"),CONCATENATE(A58,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X58" s="1" t="str">
         <f aca="false">IF(NOT(D58="2X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_south"),IF(E58="landmark",CONCATENATE(A58,"_k_south"),CONCATENATE(A58,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y58" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K59" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="M59" s="5" t="str">
+        <f aca="false">VLOOKUP(L59,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="T59" s="1" t="str">
+        <f aca="false">IF(NOT(D59="1X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c"),IF(E59="landmark",CONCATENATE(A59,"_k"),IF(E59="house",CONCATENATE(A59,"_h"),A59))))</f>
+        <v>shrine_prohibition_k</v>
+      </c>
+      <c r="U59" s="1" t="str">
+        <f aca="false">IF(D59="1X1","none",IF(E59="skyscraper",CONCATENATE(A59,"_c_north"),IF(E59="landmark",CONCATENATE(A59,"_k_north"),IF(E59="house",CONCATENATE(A59,"_h_north"),CONCATENATE(A59,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V59" s="1" t="str">
+        <f aca="false">IF(OR(D59="1X1",D59="2X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_east"),IF(E59="landmark",CONCATENATE(A59,"_k_east"),CONCATENATE(A59,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W59" s="1" t="str">
+        <f aca="false">IF(OR(D59="1X1",D59="1X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_west"),IF(E59="landmark",CONCATENATE(A59,"_k_west"),CONCATENATE(A59,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X59" s="1" t="str">
+        <f aca="false">IF(NOT(D59="2X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_south"),IF(E59="landmark",CONCATENATE(A59,"_k_south"),CONCATENATE(A59,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H60" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I60" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="M60" s="5" t="str">
+        <f aca="false">VLOOKUP(L60,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N60" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O60" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P60" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q60" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R60" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S60" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="T60" s="1" t="str">
+        <f aca="false">IF(NOT(D60="1X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c"),IF(E60="landmark",CONCATENATE(A60,"_k"),IF(E60="house",CONCATENATE(A60,"_h"),A60))))</f>
+        <v>none</v>
+      </c>
+      <c r="U60" s="1" t="str">
+        <f aca="false">IF(D60="1X1","none",IF(E60="skyscraper",CONCATENATE(A60,"_c_north"),IF(E60="landmark",CONCATENATE(A60,"_k_north"),IF(E60="house",CONCATENATE(A60,"_h_north"),CONCATENATE(A60,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V60" s="1" t="str">
+        <f aca="false">IF(OR(D60="1X1",D60="2X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_east"),IF(E60="landmark",CONCATENATE(A60,"_k_east"),CONCATENATE(A60,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W60" s="1" t="str">
+        <f aca="false">IF(OR(D60="1X1",D60="1X2"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_west"),IF(E60="landmark",CONCATENATE(A60,"_k_west"),CONCATENATE(A60,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X60" s="1" t="str">
+        <f aca="false">IF(NOT(D60="2X2"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_south"),IF(E60="landmark",CONCATENATE(A60,"_k_south"),CONCATENATE(A60,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y60" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K61" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="M61" s="5" t="str">
+        <f aca="false">VLOOKUP(L61,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N61" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O61" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P61" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q61" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R61" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S61" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="T61" s="1" t="str">
+        <f aca="false">IF(NOT(D61="1X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c"),IF(E61="landmark",CONCATENATE(A61,"_k"),IF(E61="house",CONCATENATE(A61,"_h"),A61))))</f>
+        <v>none</v>
+      </c>
+      <c r="U61" s="1" t="str">
+        <f aca="false">IF(D61="1X1","none",IF(E61="skyscraper",CONCATENATE(A61,"_c_north"),IF(E61="landmark",CONCATENATE(A61,"_k_north"),IF(E61="house",CONCATENATE(A61,"_h_north"),CONCATENATE(A61,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V61" s="1" t="str">
+        <f aca="false">IF(OR(D61="1X1",D61="2X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_east"),IF(E61="landmark",CONCATENATE(A61,"_k_east"),CONCATENATE(A61,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W61" s="1" t="str">
+        <f aca="false">IF(OR(D61="1X1",D61="1X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_west"),IF(E61="landmark",CONCATENATE(A61,"_k_west"),CONCATENATE(A61,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X61" s="1" t="str">
+        <f aca="false">IF(NOT(D61="2X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_south"),IF(E61="landmark",CONCATENATE(A61,"_k_south"),CONCATENATE(A61,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y58" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0"/>
-      <c r="D59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="5"/>
-      <c r="P59" s="3"/>
-      <c r="S59" s="3"/>
+      <c r="Y61" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0"/>
+      <c r="D62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="5"/>
+      <c r="P62" s="3"/>
+      <c r="S62" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C47 C49:C1048576">
+  <conditionalFormatting sqref="C1:C50 C52:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E30" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E33" type="list">
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L59" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L62" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P59" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P62" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S59" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S62" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5670,16 +5942,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6436,11 +6708,11 @@
       </c>
       <c r="B46" s="1" t="str">
         <f aca="false">IF(C46="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C46" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A46,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D46" s="1" t="n">
         <f aca="false">IF(C46="Multi-tile",D45-1,MAX(IF(C46="ID not in use",0,IF(C46="1X1",1,IF(C46="2X2",4,2)))-1,0))</f>
@@ -6521,11 +6793,11 @@
       </c>
       <c r="B51" s="1" t="str">
         <f aca="false">IF(C51="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C51" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A51,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D51" s="1" t="n">
         <f aca="false">IF(C51="Multi-tile",D50-1,MAX(IF(C51="ID not in use",0,IF(C51="1X1",1,IF(C51="2X2",4,2)))-1,0))</f>
@@ -6640,11 +6912,11 @@
       </c>
       <c r="B58" s="1" t="str">
         <f aca="false">IF(C58="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C58" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A58,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D58" s="1" t="n">
         <f aca="false">IF(C58="Multi-tile",D57-1,MAX(IF(C58="ID not in use",0,IF(C58="1X1",1,IF(C58="2X2",4,2)))-1,0))</f>
@@ -10068,25 +10340,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10100,13 +10372,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -10129,10 +10401,10 @@
         <v>56</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10146,16 +10418,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10163,73 +10435,73 @@
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode kono & mori
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="207">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -253,6 +253,30 @@
   </si>
   <si>
     <t xml:space="preserve">kimura_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kono_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_KONO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kono_l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mori_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_MORI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mori_m</t>
   </si>
   <si>
     <t xml:space="preserve">murakami_s</t>
@@ -750,14 +774,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y62"/>
+  <dimension ref="A1:Y66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2563,38 +2587,38 @@
         <v>78</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>1945</v>
+        <v>1980</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5" t="str">
         <f aca="false">VLOOKUP(L22,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N22" s="1" t="n">
         <v>27</v>
@@ -2607,18 +2631,18 @@
       </c>
       <c r="Q22" s="1" t="n">
         <f aca="false">VLOOKUP(E22,dropdowns!A:C,2,0)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R22" s="1" t="n">
         <f aca="false">VLOOKUP(E22,dropdowns!A:C,3,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T22" s="1" t="str">
         <f aca="false">IF(NOT(D22="1X1"),"none",IF(E22="skyscraper",CONCATENATE(A22,"_c"),IF(E22="landmark",CONCATENATE(A22,"_k"),IF(E22="house",CONCATENATE(A22,"_h"),A22))))</f>
-        <v>murakami_s</v>
+        <v>kono_m</v>
       </c>
       <c r="U22" s="1" t="str">
         <f aca="false">IF(D22="1X1","none",IF(E22="skyscraper",CONCATENATE(A22,"_c_north"),IF(E22="landmark",CONCATENATE(A22,"_k_north"),IF(E22="house",CONCATENATE(A22,"_h_north"),CONCATENATE(A22,"_north")))))</f>
@@ -2648,38 +2672,38 @@
         <v>78</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>1945</v>
+        <v>1980</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="M23" s="5" t="str">
         <f aca="false">VLOOKUP(L23,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N23" s="1" t="n">
         <v>27</v>
@@ -2691,19 +2715,17 @@
         <v>32</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <f aca="false">VLOOKUP(E23,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R23" s="1" t="n">
-        <f aca="false">VLOOKUP(E23,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T23" s="1" t="str">
         <f aca="false">IF(NOT(D23="1X1"),"none",IF(E23="skyscraper",CONCATENATE(A23,"_c"),IF(E23="landmark",CONCATENATE(A23,"_k"),IF(E23="house",CONCATENATE(A23,"_h"),A23))))</f>
-        <v>murakami_m</v>
+        <v>kono_l</v>
       </c>
       <c r="U23" s="1" t="str">
         <f aca="false">IF(D23="1X1","none",IF(E23="skyscraper",CONCATENATE(A23,"_c_north"),IF(E23="landmark",CONCATENATE(A23,"_k_north"),IF(E23="house",CONCATENATE(A23,"_h_north"),CONCATENATE(A23,"_north")))))</f>
@@ -2733,19 +2755,19 @@
         <v>82</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>83</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>1</v>
@@ -2757,14 +2779,14 @@
         <v>30</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="M24" s="5" t="str">
         <f aca="false">VLOOKUP(L24,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N24" s="1" t="n">
         <v>27</v>
@@ -2777,18 +2799,18 @@
       </c>
       <c r="Q24" s="1" t="n">
         <f aca="false">VLOOKUP(E24,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R24" s="1" t="n">
         <f aca="false">VLOOKUP(E24,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T24" s="1" t="str">
         <f aca="false">IF(NOT(D24="1X1"),"none",IF(E24="skyscraper",CONCATENATE(A24,"_c"),IF(E24="landmark",CONCATENATE(A24,"_k"),IF(E24="house",CONCATENATE(A24,"_h"),A24))))</f>
-        <v>nakayama_m</v>
+        <v>mori_s</v>
       </c>
       <c r="U24" s="1" t="str">
         <f aca="false">IF(D24="1X1","none",IF(E24="skyscraper",CONCATENATE(A24,"_c_north"),IF(E24="landmark",CONCATENATE(A24,"_k_north"),IF(E24="house",CONCATENATE(A24,"_h_north"),CONCATENATE(A24,"_north")))))</f>
@@ -2815,10 +2837,10 @@
         <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
@@ -2827,7 +2849,7 @@
         <v>28</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>100</v>
@@ -2836,7 +2858,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>30</v>
@@ -2873,7 +2895,7 @@
       </c>
       <c r="T25" s="1" t="str">
         <f aca="false">IF(NOT(D25="1X1"),"none",IF(E25="skyscraper",CONCATENATE(A25,"_c"),IF(E25="landmark",CONCATENATE(A25,"_k"),IF(E25="house",CONCATENATE(A25,"_h"),A25))))</f>
-        <v>okada_office_tower_m</v>
+        <v>mori_m</v>
       </c>
       <c r="U25" s="1" t="str">
         <f aca="false">IF(D25="1X1","none",IF(E25="skyscraper",CONCATENATE(A25,"_c_north"),IF(E25="landmark",CONCATENATE(A25,"_k_north"),IF(E25="house",CONCATENATE(A25,"_h_north"),CONCATENATE(A25,"_north")))))</f>
@@ -2897,44 +2919,44 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K26" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="M26" s="5" t="str">
         <f aca="false">VLOOKUP(L26,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N26" s="1" t="n">
         <v>27</v>
@@ -2946,17 +2968,19 @@
         <v>32</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>14</v>
+        <f aca="false">VLOOKUP(E26,dropdowns!A:C,2,0)</f>
+        <v>6</v>
       </c>
       <c r="R26" s="1" t="n">
-        <v>5</v>
+        <f aca="false">VLOOKUP(E26,dropdowns!A:C,3,0)</f>
+        <v>2</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T26" s="1" t="str">
         <f aca="false">IF(NOT(D26="1X1"),"none",IF(E26="skyscraper",CONCATENATE(A26,"_c"),IF(E26="landmark",CONCATENATE(A26,"_k"),IF(E26="house",CONCATENATE(A26,"_h"),A26))))</f>
-        <v>okada_office_tower_l</v>
+        <v>murakami_s</v>
       </c>
       <c r="U26" s="1" t="str">
         <f aca="false">IF(D26="1X1","none",IF(E26="skyscraper",CONCATENATE(A26,"_c_north"),IF(E26="landmark",CONCATENATE(A26,"_k_north"),IF(E26="house",CONCATENATE(A26,"_h_north"),CONCATENATE(A26,"_north")))))</f>
@@ -2983,41 +3007,41 @@
         <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>122</v>
+        <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M27" s="5" t="str">
         <f aca="false">VLOOKUP(L27,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N27" s="1" t="n">
         <v>27</v>
@@ -3029,17 +3053,19 @@
         <v>32</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>16</v>
+        <f aca="false">VLOOKUP(E27,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R27" s="1" t="n">
-        <v>6</v>
+        <f aca="false">VLOOKUP(E27,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T27" s="1" t="str">
         <f aca="false">IF(NOT(D27="1X1"),"none",IF(E27="skyscraper",CONCATENATE(A27,"_c"),IF(E27="landmark",CONCATENATE(A27,"_k"),IF(E27="house",CONCATENATE(A27,"_h"),A27))))</f>
-        <v>okada_office_tower_x</v>
+        <v>murakami_m</v>
       </c>
       <c r="U27" s="1" t="str">
         <f aca="false">IF(D27="1X1","none",IF(E27="skyscraper",CONCATENATE(A27,"_c_north"),IF(E27="landmark",CONCATENATE(A27,"_k_north"),IF(E27="house",CONCATENATE(A27,"_h_north"),CONCATENATE(A27,"_north")))))</f>
@@ -3069,7 +3095,7 @@
         <v>90</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -3087,7 +3113,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>1945</v>
+        <v>1950</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>30</v>
@@ -3112,9 +3138,11 @@
         <v>32</v>
       </c>
       <c r="Q28" s="1" t="n">
+        <f aca="false">VLOOKUP(E28,dropdowns!A:C,2,0)</f>
         <v>10</v>
       </c>
       <c r="R28" s="1" t="n">
+        <f aca="false">VLOOKUP(E28,dropdowns!A:C,3,0)</f>
         <v>4</v>
       </c>
       <c r="S28" s="3" t="s">
@@ -3122,7 +3150,7 @@
       </c>
       <c r="T28" s="1" t="str">
         <f aca="false">IF(NOT(D28="1X1"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c"),IF(E28="landmark",CONCATENATE(A28,"_k"),IF(E28="house",CONCATENATE(A28,"_h"),A28))))</f>
-        <v>old_office_building_m</v>
+        <v>nakayama_m</v>
       </c>
       <c r="U28" s="1" t="str">
         <f aca="false">IF(D28="1X1","none",IF(E28="skyscraper",CONCATENATE(A28,"_c_north"),IF(E28="landmark",CONCATENATE(A28,"_k_north"),IF(E28="house",CONCATENATE(A28,"_h_north"),CONCATENATE(A28,"_north")))))</f>
@@ -3149,41 +3177,41 @@
         <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>1945</v>
+        <v>1955</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M29" s="5" t="str">
         <f aca="false">VLOOKUP(L29,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N29" s="1" t="n">
         <v>27</v>
@@ -3195,17 +3223,19 @@
         <v>32</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>14</v>
+        <f aca="false">VLOOKUP(E29,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R29" s="1" t="n">
-        <v>5</v>
+        <f aca="false">VLOOKUP(E29,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T29" s="1" t="str">
         <f aca="false">IF(NOT(D29="1X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c"),IF(E29="landmark",CONCATENATE(A29,"_k"),IF(E29="house",CONCATENATE(A29,"_h"),A29))))</f>
-        <v>old_office_building_l</v>
+        <v>okada_office_tower_m</v>
       </c>
       <c r="U29" s="1" t="str">
         <f aca="false">IF(D29="1X1","none",IF(E29="skyscraper",CONCATENATE(A29,"_c_north"),IF(E29="landmark",CONCATENATE(A29,"_k_north"),IF(E29="house",CONCATENATE(A29,"_h_north"),CONCATENATE(A29,"_north")))))</f>
@@ -3229,44 +3259,44 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C30" s="2" t="n">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>1970</v>
+        <v>1955</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="M30" s="5" t="str">
         <f aca="false">VLOOKUP(L30,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N30" s="1" t="n">
         <v>27</v>
@@ -3278,19 +3308,17 @@
         <v>32</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <f aca="false">VLOOKUP(E30,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R30" s="1" t="n">
-        <f aca="false">VLOOKUP(E30,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T30" s="1" t="str">
         <f aca="false">IF(NOT(D30="1X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c"),IF(E30="landmark",CONCATENATE(A30,"_k"),IF(E30="house",CONCATENATE(A30,"_h"),A30))))</f>
-        <v>yamada_electronics_centre_m</v>
+        <v>okada_office_tower_l</v>
       </c>
       <c r="U30" s="1" t="str">
         <f aca="false">IF(D30="1X1","none",IF(E30="skyscraper",CONCATENATE(A30,"_c_north"),IF(E30="landmark",CONCATENATE(A30,"_k_north"),IF(E30="house",CONCATENATE(A30,"_h_north"),CONCATENATE(A30,"_north")))))</f>
@@ -3317,41 +3345,41 @@
         <v>96</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>1970</v>
+        <v>1955</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M31" s="5" t="str">
         <f aca="false">VLOOKUP(L31,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N31" s="1" t="n">
         <v>27</v>
@@ -3363,17 +3391,17 @@
         <v>32</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="R31" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S31" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T31" s="1" t="str">
         <f aca="false">IF(NOT(D31="1X1"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c"),IF(E31="landmark",CONCATENATE(A31,"_k"),IF(E31="house",CONCATENATE(A31,"_h"),A31))))</f>
-        <v>yamada_electronics_centre_l</v>
+        <v>okada_office_tower_x</v>
       </c>
       <c r="U31" s="1" t="str">
         <f aca="false">IF(D31="1X1","none",IF(E31="skyscraper",CONCATENATE(A31,"_c_north"),IF(E31="landmark",CONCATENATE(A31,"_k_north"),IF(E31="house",CONCATENATE(A31,"_h_north"),CONCATENATE(A31,"_north")))))</f>
@@ -3400,41 +3428,41 @@
         <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>1970</v>
+        <v>1945</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M32" s="5" t="str">
         <f aca="false">VLOOKUP(L32,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N32" s="1" t="n">
         <v>27</v>
@@ -3446,17 +3474,17 @@
         <v>32</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="R32" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T32" s="1" t="str">
         <f aca="false">IF(NOT(D32="1X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c"),IF(E32="landmark",CONCATENATE(A32,"_k"),IF(E32="house",CONCATENATE(A32,"_h"),A32))))</f>
-        <v>yamada_electronics_centre_x</v>
+        <v>old_office_building_m</v>
       </c>
       <c r="U32" s="1" t="str">
         <f aca="false">IF(D32="1X1","none",IF(E32="skyscraper",CONCATENATE(A32,"_c_north"),IF(E32="landmark",CONCATENATE(A32,"_k_north"),IF(E32="house",CONCATENATE(A32,"_h_north"),CONCATENATE(A32,"_north")))))</f>
@@ -3480,44 +3508,44 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>99</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>1970</v>
+        <v>1945</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="M33" s="5" t="str">
         <f aca="false">VLOOKUP(L33,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N33" s="1" t="n">
         <v>27</v>
@@ -3529,17 +3557,17 @@
         <v>32</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S33" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T33" s="1" t="str">
         <f aca="false">IF(NOT(D33="1X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c"),IF(E33="landmark",CONCATENATE(A33,"_k"),IF(E33="house",CONCATENATE(A33,"_h"),A33))))</f>
-        <v>yano_m</v>
+        <v>old_office_building_l</v>
       </c>
       <c r="U33" s="1" t="str">
         <f aca="false">IF(D33="1X1","none",IF(E33="skyscraper",CONCATENATE(A33,"_c_north"),IF(E33="landmark",CONCATENATE(A33,"_k_north"),IF(E33="house",CONCATENATE(A33,"_h_north"),CONCATENATE(A33,"_north")))))</f>
@@ -3563,66 +3591,68 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>101</v>
+      <c r="E34" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M34" s="5" t="str">
         <f aca="false">VLOOKUP(L34,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="O34" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>16</v>
+        <f aca="false">VLOOKUP(E34,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R34" s="1" t="n">
-        <v>6</v>
+        <f aca="false">VLOOKUP(E34,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T34" s="1" t="str">
         <f aca="false">IF(NOT(D34="1X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c"),IF(E34="landmark",CONCATENATE(A34,"_k"),IF(E34="house",CONCATENATE(A34,"_h"),A34))))</f>
-        <v>bank_building_c</v>
+        <v>yamada_electronics_centre_m</v>
       </c>
       <c r="U34" s="1" t="str">
         <f aca="false">IF(D34="1X1","none",IF(E34="skyscraper",CONCATENATE(A34,"_c_north"),IF(E34="landmark",CONCATENATE(A34,"_k_north"),IF(E34="house",CONCATENATE(A34,"_h_north"),CONCATENATE(A34,"_north")))))</f>
@@ -3649,63 +3679,63 @@
         <v>104</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>101</v>
+      <c r="E35" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>220</v>
+        <v>125</v>
       </c>
       <c r="H35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>1990</v>
+        <v>1970</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M35" s="5" t="str">
         <f aca="false">VLOOKUP(L35,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N35" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O35" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O35" s="1" t="n">
+      <c r="P35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R35" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="P35" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q35" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="R35" s="1" t="n">
-        <v>10</v>
-      </c>
       <c r="S35" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T35" s="1" t="str">
         <f aca="false">IF(NOT(D35="1X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c"),IF(E35="landmark",CONCATENATE(A35,"_k"),IF(E35="house",CONCATENATE(A35,"_h"),A35))))</f>
-        <v>enterprise_tower_c</v>
+        <v>yamada_electronics_centre_l</v>
       </c>
       <c r="U35" s="1" t="str">
         <f aca="false">IF(D35="1X1","none",IF(E35="skyscraper",CONCATENATE(A35,"_c_north"),IF(E35="landmark",CONCATENATE(A35,"_k_north"),IF(E35="house",CONCATENATE(A35,"_h_north"),CONCATENATE(A35,"_north")))))</f>
@@ -3729,37 +3759,37 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>101</v>
+      <c r="E36" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>1960</v>
+        <v>1970</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>39</v>
@@ -3769,26 +3799,26 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N36" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O36" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O36" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P36" s="3" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="Q36" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R36" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T36" s="1" t="str">
         <f aca="false">IF(NOT(D36="1X1"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c"),IF(E36="landmark",CONCATENATE(A36,"_k"),IF(E36="house",CONCATENATE(A36,"_h"),A36))))</f>
-        <v>insurance_tower_c</v>
+        <v>yamada_electronics_centre_x</v>
       </c>
       <c r="U36" s="1" t="str">
         <f aca="false">IF(D36="1X1","none",IF(E36="skyscraper",CONCATENATE(A36,"_c_north"),IF(E36="landmark",CONCATENATE(A36,"_k_north"),IF(E36="house",CONCATENATE(A36,"_h_north"),CONCATENATE(A36,"_north")))))</f>
@@ -3812,66 +3842,66 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>101</v>
+      <c r="E37" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="H37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>2000</v>
+        <v>1970</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M37" s="5" t="str">
         <f aca="false">VLOOKUP(L37,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N37" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O37" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O37" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P37" s="3" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="Q37" s="1" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="R37" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T37" s="1" t="str">
         <f aca="false">IF(NOT(D37="1X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c"),IF(E37="landmark",CONCATENATE(A37,"_k"),IF(E37="house",CONCATENATE(A37,"_h"),A37))))</f>
-        <v>kuroi_tower_c</v>
+        <v>yano_m</v>
       </c>
       <c r="U37" s="1" t="str">
         <f aca="false">IF(D37="1X1","none",IF(E37="skyscraper",CONCATENATE(A37,"_c_north"),IF(E37="landmark",CONCATENATE(A37,"_k_north"),IF(E37="house",CONCATENATE(A37,"_h_north"),CONCATENATE(A37,"_north")))))</f>
@@ -3895,22 +3925,22 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>220</v>
@@ -3919,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>2000</v>
+        <v>1980</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>30</v>
@@ -3935,26 +3965,26 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N38" s="1" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="O38" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q38" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R38" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T38" s="1" t="str">
         <f aca="false">IF(NOT(D38="1X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c"),IF(E38="landmark",CONCATENATE(A38,"_k"),IF(E38="house",CONCATENATE(A38,"_h"),A38))))</f>
-        <v>mitsui_tower_c</v>
+        <v>bank_building_c</v>
       </c>
       <c r="U38" s="1" t="str">
         <f aca="false">IF(D38="1X1","none",IF(E38="skyscraper",CONCATENATE(A38,"_c_north"),IF(E38="landmark",CONCATENATE(A38,"_k_north"),IF(E38="house",CONCATENATE(A38,"_h_north"),CONCATENATE(A38,"_north")))))</f>
@@ -3978,22 +4008,22 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>220</v>
@@ -4002,7 +4032,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>30</v>
@@ -4024,7 +4054,7 @@
         <v>5</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q39" s="1" t="n">
         <v>24</v>
@@ -4033,11 +4063,11 @@
         <v>10</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T39" s="1" t="str">
         <f aca="false">IF(NOT(D39="1X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c"),IF(E39="landmark",CONCATENATE(A39,"_k"),IF(E39="house",CONCATENATE(A39,"_h"),A39))))</f>
-        <v>modern_office_tower_c</v>
+        <v>enterprise_tower_c</v>
       </c>
       <c r="U39" s="1" t="str">
         <f aca="false">IF(D39="1X1","none",IF(E39="skyscraper",CONCATENATE(A39,"_c_north"),IF(E39="landmark",CONCATENATE(A39,"_k_north"),IF(E39="house",CONCATENATE(A39,"_h_north"),CONCATENATE(A39,"_north")))))</f>
@@ -4067,25 +4097,25 @@
         <v>115</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>116</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>30</v>
@@ -4107,7 +4137,7 @@
         <v>5</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q40" s="1" t="n">
         <v>24</v>
@@ -4116,11 +4146,11 @@
         <v>10</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T40" s="1" t="str">
         <f aca="false">IF(NOT(D40="1X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c"),IF(E40="landmark",CONCATENATE(A40,"_k"),IF(E40="house",CONCATENATE(A40,"_h"),A40))))</f>
-        <v>multimedia_offices_c</v>
+        <v>insurance_tower_c</v>
       </c>
       <c r="U40" s="1" t="str">
         <f aca="false">IF(D40="1X1","none",IF(E40="skyscraper",CONCATENATE(A40,"_c_north"),IF(E40="landmark",CONCATENATE(A40,"_k_north"),IF(E40="house",CONCATENATE(A40,"_h_north"),CONCATENATE(A40,"_north")))))</f>
@@ -4150,13 +4180,13 @@
         <v>117</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>118</v>
@@ -4190,7 +4220,7 @@
         <v>5</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q41" s="1" t="n">
         <v>24</v>
@@ -4199,11 +4229,11 @@
         <v>10</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T41" s="1" t="str">
         <f aca="false">IF(NOT(D41="1X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c"),IF(E41="landmark",CONCATENATE(A41,"_k"),IF(E41="house",CONCATENATE(A41,"_h"),A41))))</f>
-        <v>office_tower_c</v>
+        <v>kuroi_tower_c</v>
       </c>
       <c r="U41" s="1" t="str">
         <f aca="false">IF(D41="1X1","none",IF(E41="skyscraper",CONCATENATE(A41,"_c_north"),IF(E41="landmark",CONCATENATE(A41,"_k_north"),IF(E41="house",CONCATENATE(A41,"_h_north"),CONCATENATE(A41,"_north")))))</f>
@@ -4233,25 +4263,25 @@
         <v>119</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>1960</v>
+        <v>2000</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>30</v>
@@ -4273,7 +4303,7 @@
         <v>5</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q42" s="1" t="n">
         <v>24</v>
@@ -4282,11 +4312,11 @@
         <v>10</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T42" s="1" t="str">
         <f aca="false">IF(NOT(D42="1X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c"),IF(E42="landmark",CONCATENATE(A42,"_k"),IF(E42="house",CONCATENATE(A42,"_h"),A42))))</f>
-        <v>sato_building_c</v>
+        <v>mitsui_tower_c</v>
       </c>
       <c r="U42" s="1" t="str">
         <f aca="false">IF(D42="1X1","none",IF(E42="skyscraper",CONCATENATE(A42,"_c_north"),IF(E42="landmark",CONCATENATE(A42,"_k_north"),IF(E42="house",CONCATENATE(A42,"_h_north"),CONCATENATE(A42,"_north")))))</f>
@@ -4316,25 +4346,25 @@
         <v>121</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>30</v>
@@ -4356,7 +4386,7 @@
         <v>5</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q43" s="1" t="n">
         <v>24</v>
@@ -4365,11 +4395,11 @@
         <v>10</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T43" s="1" t="str">
         <f aca="false">IF(NOT(D43="1X1"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c"),IF(E43="landmark",CONCATENATE(A43,"_k"),IF(E43="house",CONCATENATE(A43,"_h"),A43))))</f>
-        <v>sugiyama_office_building_c</v>
+        <v>modern_office_tower_c</v>
       </c>
       <c r="U43" s="1" t="str">
         <f aca="false">IF(D43="1X1","none",IF(E43="skyscraper",CONCATENATE(A43,"_c_north"),IF(E43="landmark",CONCATENATE(A43,"_k_north"),IF(E43="house",CONCATENATE(A43,"_h_north"),CONCATENATE(A43,"_north")))))</f>
@@ -4399,25 +4429,25 @@
         <v>123</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="G44" s="1" t="n">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>2006</v>
+        <v>1990</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>30</v>
@@ -4433,13 +4463,13 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N44" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O44" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q44" s="1" t="n">
         <v>24</v>
@@ -4448,19 +4478,19 @@
         <v>10</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T44" s="1" t="str">
         <f aca="false">IF(NOT(D44="1X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c"),IF(E44="landmark",CONCATENATE(A44,"_k"),IF(E44="house",CONCATENATE(A44,"_h"),A44))))</f>
-        <v>none</v>
+        <v>multimedia_offices_c</v>
       </c>
       <c r="U44" s="1" t="str">
         <f aca="false">IF(D44="1X1","none",IF(E44="skyscraper",CONCATENATE(A44,"_c_north"),IF(E44="landmark",CONCATENATE(A44,"_k_north"),IF(E44="house",CONCATENATE(A44,"_h_north"),CONCATENATE(A44,"_north")))))</f>
-        <v>tsuno_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V44" s="1" t="str">
         <f aca="false">IF(OR(D44="1X1",D44="2X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_east"),IF(E44="landmark",CONCATENATE(A44,"_k_east"),CONCATENATE(A44,"_east"))))</f>
-        <v>tsuno_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W44" s="1" t="str">
         <f aca="false">IF(OR(D44="1X1",D44="1X2"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c_west"),IF(E44="landmark",CONCATENATE(A44,"_k_west"),CONCATENATE(A44,"_west"))))</f>
@@ -4476,34 +4506,34 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G45" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>1955</v>
-      </c>
-      <c r="J45" s="4" t="n">
-        <v>1989</v>
+        <v>2000</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="K45" s="1" t="n">
         <v>25</v>
@@ -4522,7 +4552,7 @@
         <v>5</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q45" s="1" t="n">
         <v>24</v>
@@ -4531,11 +4561,11 @@
         <v>10</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T45" s="1" t="str">
         <f aca="false">IF(NOT(D45="1X1"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c"),IF(E45="landmark",CONCATENATE(A45,"_k"),IF(E45="house",CONCATENATE(A45,"_h"),A45))))</f>
-        <v>ueda_office_block_c</v>
+        <v>office_tower_c</v>
       </c>
       <c r="U45" s="1" t="str">
         <f aca="false">IF(D45="1X1","none",IF(E45="skyscraper",CONCATENATE(A45,"_c_north"),IF(E45="landmark",CONCATENATE(A45,"_k_north"),IF(E45="house",CONCATENATE(A45,"_h_north"),CONCATENATE(A45,"_north")))))</f>
@@ -4559,31 +4589,31 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G46" s="1" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="H46" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>1965</v>
+        <v>1960</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>30</v>
@@ -4605,20 +4635,20 @@
         <v>5</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q46" s="1" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R46" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T46" s="1" t="str">
         <f aca="false">IF(NOT(D46="1X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c"),IF(E46="landmark",CONCATENATE(A46,"_k"),IF(E46="house",CONCATENATE(A46,"_h"),A46))))</f>
-        <v>yamaguchi_office_c</v>
+        <v>sato_building_c</v>
       </c>
       <c r="U46" s="1" t="str">
         <f aca="false">IF(D46="1X1","none",IF(E46="skyscraper",CONCATENATE(A46,"_c_north"),IF(E46="landmark",CONCATENATE(A46,"_k_north"),IF(E46="house",CONCATENATE(A46,"_h_north"),CONCATENATE(A46,"_north")))))</f>
@@ -4642,25 +4672,25 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="G47" s="1" t="n">
-        <v>255</v>
+        <v>200</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>1</v>
@@ -4682,13 +4712,13 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N47" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O47" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q47" s="1" t="n">
         <v>24</v>
@@ -4697,19 +4727,19 @@
         <v>10</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T47" s="1" t="str">
         <f aca="false">IF(NOT(D47="1X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c"),IF(E47="landmark",CONCATENATE(A47,"_k"),IF(E47="house",CONCATENATE(A47,"_h"),A47))))</f>
-        <v>none</v>
+        <v>sugiyama_office_building_c</v>
       </c>
       <c r="U47" s="1" t="str">
         <f aca="false">IF(D47="1X1","none",IF(E47="skyscraper",CONCATENATE(A47,"_c_north"),IF(E47="landmark",CONCATENATE(A47,"_k_north"),IF(E47="house",CONCATENATE(A47,"_h_north"),CONCATENATE(A47,"_north")))))</f>
-        <v>yamashiro_office_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V47" s="1" t="str">
         <f aca="false">IF(OR(D47="1X1",D47="2X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_east"),IF(E47="landmark",CONCATENATE(A47,"_k_east"),CONCATENATE(A47,"_east"))))</f>
-        <v>yamashiro_office_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W47" s="1" t="str">
         <f aca="false">IF(OR(D47="1X1",D47="1X2"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c_west"),IF(E47="landmark",CONCATENATE(A47,"_k_west"),CONCATENATE(A47,"_west"))))</f>
@@ -4725,31 +4755,31 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="2" t="n">
-        <v>47</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="H48" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>30</v>
@@ -4765,13 +4795,13 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N48" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O48" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q48" s="1" t="n">
         <v>24</v>
@@ -4780,19 +4810,19 @@
         <v>10</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="T48" s="1" t="str">
         <f aca="false">IF(NOT(D48="1X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c"),IF(E48="landmark",CONCATENATE(A48,"_k"),IF(E48="house",CONCATENATE(A48,"_h"),A48))))</f>
-        <v>yamashita_building_c</v>
+        <v>none</v>
       </c>
       <c r="U48" s="1" t="str">
         <f aca="false">IF(D48="1X1","none",IF(E48="skyscraper",CONCATENATE(A48,"_c_north"),IF(E48="landmark",CONCATENATE(A48,"_k_north"),IF(E48="house",CONCATENATE(A48,"_h_north"),CONCATENATE(A48,"_north")))))</f>
-        <v>none</v>
+        <v>tsuno_building_c_north</v>
       </c>
       <c r="V48" s="1" t="str">
         <f aca="false">IF(OR(D48="1X1",D48="2X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_east"),IF(E48="landmark",CONCATENATE(A48,"_k_east"),CONCATENATE(A48,"_east"))))</f>
-        <v>none</v>
+        <v>tsuno_building_c_east</v>
       </c>
       <c r="W48" s="1" t="str">
         <f aca="false">IF(OR(D48="1X1",D48="1X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_west"),IF(E48="landmark",CONCATENATE(A48,"_k_west"),CONCATENATE(A48,"_west"))))</f>
@@ -4814,388 +4844,388 @@
         <v>134</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>212</v>
+        <v>89</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="G49" s="1" t="n">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>1700</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>30</v>
+        <v>1955</v>
+      </c>
+      <c r="J49" s="4" t="n">
+        <v>1989</v>
       </c>
       <c r="K49" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="M49" s="5" t="str">
         <f aca="false">VLOOKUP(L49,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N49" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O49" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="Q49" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="R49" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="T49" s="1" t="str">
         <f aca="false">IF(NOT(D49="1X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c"),IF(E49="landmark",CONCATENATE(A49,"_k"),IF(E49="house",CONCATENATE(A49,"_h"),A49))))</f>
-        <v>none</v>
+        <v>ueda_office_block_c</v>
       </c>
       <c r="U49" s="1" t="str">
         <f aca="false">IF(D49="1X1","none",IF(E49="skyscraper",CONCATENATE(A49,"_c_north"),IF(E49="landmark",CONCATENATE(A49,"_k_north"),IF(E49="house",CONCATENATE(A49,"_h_north"),CONCATENATE(A49,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>none</v>
       </c>
       <c r="V49" s="1" t="str">
-        <f aca="false">IF(OR(D49="1X1",D49="2X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_east"),IF(E49="landmark",CONCATENATE(A49,"_k_east"),IF(E49="house",CONCATENATE(A49,"_h_east"),CONCATENATE(A49,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D49="1X1",D49="2X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_east"),IF(E49="landmark",CONCATENATE(A49,"_k_east"),CONCATENATE(A49,"_east"))))</f>
+        <v>none</v>
       </c>
       <c r="W49" s="1" t="str">
-        <f aca="false">IF(OR(D49="1X1",D49="1X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_west"),IF(E49="landmark",CONCATENATE(A49,"_k_west"),IF(E49="house",CONCATENATE(A49,"_h_west"),CONCATENATE(A49,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D49="1X1",D49="1X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_west"),IF(E49="landmark",CONCATENATE(A49,"_k_west"),CONCATENATE(A49,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X49" s="1" t="str">
-        <f aca="false">IF(NOT(D49="2X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_south"),IF(E49="landmark",CONCATENATE(A49,"_k_south"),IF(E49="house",CONCATENATE(A49,"_h_south"),CONCATENATE(A49,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D49="2X2"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c_south"),IF(E49="landmark",CONCATENATE(A49,"_k_south"),CONCATENATE(A49,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>134</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G50" s="1" t="n">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>1870</v>
+        <v>1965</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K50" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="M50" s="5" t="str">
         <f aca="false">VLOOKUP(L50,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N50" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O50" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="Q50" s="1" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="R50" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="T50" s="1" t="str">
         <f aca="false">IF(NOT(D50="1X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c"),IF(E50="landmark",CONCATENATE(A50,"_k"),IF(E50="house",CONCATENATE(A50,"_h"),A50))))</f>
-        <v>naganuma_h</v>
+        <v>yamaguchi_office_c</v>
       </c>
       <c r="U50" s="1" t="str">
         <f aca="false">IF(D50="1X1","none",IF(E50="skyscraper",CONCATENATE(A50,"_c_north"),IF(E50="landmark",CONCATENATE(A50,"_k_north"),IF(E50="house",CONCATENATE(A50,"_h_north"),CONCATENATE(A50,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V50" s="1" t="str">
-        <f aca="false">IF(OR(D50="1X1",D50="2X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_east"),IF(E50="landmark",CONCATENATE(A50,"_k_east"),IF(E50="house",CONCATENATE(A50,"_h_east"),CONCATENATE(A50,"_east")))))</f>
+        <f aca="false">IF(OR(D50="1X1",D50="2X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_east"),IF(E50="landmark",CONCATENATE(A50,"_k_east"),CONCATENATE(A50,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W50" s="1" t="str">
-        <f aca="false">IF(OR(D50="1X1",D50="1X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_west"),IF(E50="landmark",CONCATENATE(A50,"_k_west"),IF(E50="house",CONCATENATE(A50,"_h_west"),CONCATENATE(A50,"_west")))))</f>
+        <f aca="false">IF(OR(D50="1X1",D50="1X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_west"),IF(E50="landmark",CONCATENATE(A50,"_k_west"),CONCATENATE(A50,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X50" s="1" t="str">
-        <f aca="false">IF(NOT(D50="2X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_south"),IF(E50="landmark",CONCATENATE(A50,"_k_south"),IF(E50="house",CONCATENATE(A50,"_h_south"),CONCATENATE(A50,"_south")))))</f>
+        <f aca="false">IF(NOT(D50="2X2"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c_south"),IF(E50="landmark",CONCATENATE(A50,"_k_south"),CONCATENATE(A50,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="6" t="n">
-        <v>95</v>
+      <c r="A51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>101</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G51" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H51" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="G51" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="H51" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I51" s="0" t="n">
-        <v>1950</v>
+      <c r="I51" s="1" t="n">
+        <v>1990</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K51" s="0" t="n">
-        <v>5</v>
+      <c r="K51" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="M51" s="5" t="str">
         <f aca="false">VLOOKUP(L51,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N51" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O51" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
+      </c>
+      <c r="N51" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O51" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q51" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R51" s="0" t="n">
-        <v>3</v>
+        <v>111</v>
+      </c>
+      <c r="Q51" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R51" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="T51" s="1" t="str">
         <f aca="false">IF(NOT(D51="1X1"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c"),IF(E51="landmark",CONCATENATE(A51,"_k"),IF(E51="house",CONCATENATE(A51,"_h"),A51))))</f>
-        <v>convini_k</v>
+        <v>none</v>
       </c>
       <c r="U51" s="1" t="str">
         <f aca="false">IF(D51="1X1","none",IF(E51="skyscraper",CONCATENATE(A51,"_c_north"),IF(E51="landmark",CONCATENATE(A51,"_k_north"),IF(E51="house",CONCATENATE(A51,"_h_north"),CONCATENATE(A51,"_north")))))</f>
-        <v>none</v>
+        <v>yamashiro_office_building_c_north</v>
       </c>
       <c r="V51" s="1" t="str">
-        <f aca="false">IF(OR(D51="1X1",D51="2X1"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_east"),IF(E51="landmark",CONCATENATE(A51,"_k_east"),IF(E51="house",CONCATENATE(A51,"_h_east"),CONCATENATE(A51,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D51="1X1",D51="2X1"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_east"),IF(E51="landmark",CONCATENATE(A51,"_k_east"),CONCATENATE(A51,"_east"))))</f>
+        <v>yamashiro_office_building_c_east</v>
       </c>
       <c r="W51" s="1" t="str">
-        <f aca="false">IF(OR(D51="1X1",D51="1X2"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_west"),IF(E51="landmark",CONCATENATE(A51,"_k_west"),IF(E51="house",CONCATENATE(A51,"_h_west"),CONCATENATE(A51,"_west")))))</f>
+        <f aca="false">IF(OR(D51="1X1",D51="1X2"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_west"),IF(E51="landmark",CONCATENATE(A51,"_k_west"),CONCATENATE(A51,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X51" s="1" t="str">
-        <f aca="false">IF(NOT(D51="2X2"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_south"),IF(E51="landmark",CONCATENATE(A51,"_k_south"),IF(E51="house",CONCATENATE(A51,"_h_south"),CONCATENATE(A51,"_south")))))</f>
-        <v>none</v>
-      </c>
-      <c r="Y51" s="0" t="s">
-        <v>150</v>
+        <f aca="false">IF(NOT(D51="2X2"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_south"),IF(E51="landmark",CONCATENATE(A51,"_k_south"),CONCATENATE(A51,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>80</v>
+        <v>220</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>1970</v>
+        <v>2000</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K52" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="M52" s="5" t="str">
         <f aca="false">VLOOKUP(L52,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N52" s="1" t="n">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="O52" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="Q52" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R52" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="R52" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="S52" s="3" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="T52" s="1" t="str">
         <f aca="false">IF(NOT(D52="1X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c"),IF(E52="landmark",CONCATENATE(A52,"_k"),IF(E52="house",CONCATENATE(A52,"_h"),A52))))</f>
-        <v>none</v>
+        <v>yamashita_building_c</v>
       </c>
       <c r="U52" s="1" t="str">
         <f aca="false">IF(D52="1X1","none",IF(E52="skyscraper",CONCATENATE(A52,"_c_north"),IF(E52="landmark",CONCATENATE(A52,"_k_north"),IF(E52="house",CONCATENATE(A52,"_h_north"),CONCATENATE(A52,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V52" s="1" t="str">
-        <f aca="false">IF(OR(D52="1X1",D52="2X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_east"),IF(E52="landmark",CONCATENATE(A52,"_k_east"),IF(E52="house",CONCATENATE(A52,"_h_east"),CONCATENATE(A52,"_east")))))</f>
+        <f aca="false">IF(OR(D52="1X1",D52="2X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_east"),IF(E52="landmark",CONCATENATE(A52,"_k_east"),CONCATENATE(A52,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W52" s="1" t="str">
-        <f aca="false">IF(OR(D52="1X1",D52="1X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_west"),IF(E52="landmark",CONCATENATE(A52,"_k_west"),IF(E52="house",CONCATENATE(A52,"_h_west"),CONCATENATE(A52,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <f aca="false">IF(OR(D52="1X1",D52="1X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_west"),IF(E52="landmark",CONCATENATE(A52,"_k_west"),CONCATENATE(A52,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X52" s="1" t="str">
-        <f aca="false">IF(NOT(D52="2X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_south"),IF(E52="landmark",CONCATENATE(A52,"_k_south"),IF(E52="house",CONCATENATE(A52,"_h_south"),CONCATENATE(A52,"_south")))))</f>
+        <f aca="false">IF(NOT(D52="2X2"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c_south"),IF(E52="landmark",CONCATENATE(A52,"_k_south"),CONCATENATE(A52,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y52" s="1" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="G53" s="1" t="n">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I53" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K53" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="M53" s="5" t="str">
         <f aca="false">VLOOKUP(L53,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N53" s="1" t="n">
         <v>20</v>
       </c>
       <c r="O53" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="Q53" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R53" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="T53" s="1" t="str">
         <f aca="false">IF(NOT(D53="1X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c"),IF(E53="landmark",CONCATENATE(A53,"_k"),IF(E53="house",CONCATENATE(A53,"_h"),A53))))</f>
@@ -5203,48 +5233,48 @@
       </c>
       <c r="U53" s="1" t="str">
         <f aca="false">IF(D53="1X1","none",IF(E53="skyscraper",CONCATENATE(A53,"_c_north"),IF(E53="landmark",CONCATENATE(A53,"_k_north"),IF(E53="house",CONCATENATE(A53,"_h_north"),CONCATENATE(A53,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V53" s="1" t="str">
-        <f aca="false">IF(OR(D53="1X1",D53="2X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_east"),IF(E53="landmark",CONCATENATE(A53,"_k_east"),CONCATENATE(A53,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D53="1X1",D53="2X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_east"),IF(E53="landmark",CONCATENATE(A53,"_k_east"),IF(E53="house",CONCATENATE(A53,"_h_east"),CONCATENATE(A53,"_east")))))</f>
+        <v>farm_h_east</v>
       </c>
       <c r="W53" s="1" t="str">
-        <f aca="false">IF(OR(D53="1X1",D53="1X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_west"),IF(E53="landmark",CONCATENATE(A53,"_k_west"),CONCATENATE(A53,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D53="1X1",D53="1X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_west"),IF(E53="landmark",CONCATENATE(A53,"_k_west"),IF(E53="house",CONCATENATE(A53,"_h_west"),CONCATENATE(A53,"_west")))))</f>
+        <v>farm_h_west</v>
       </c>
       <c r="X53" s="1" t="str">
-        <f aca="false">IF(NOT(D53="2X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_south"),IF(E53="landmark",CONCATENATE(A53,"_k_south"),CONCATENATE(A53,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D53="2X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_south"),IF(E53="landmark",CONCATENATE(A53,"_k_south"),IF(E53="house",CONCATENATE(A53,"_h_south"),CONCATENATE(A53,"_south")))))</f>
+        <v>farm_h_south</v>
       </c>
       <c r="Y53" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="G54" s="1" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I54" s="1" t="n">
         <v>1870</v>
@@ -5253,36 +5283,36 @@
         <v>30</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="M54" s="5" t="str">
         <f aca="false">VLOOKUP(L54,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N54" s="1" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="O54" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="Q54" s="1" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="R54" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S54" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T54" s="1" t="str">
         <f aca="false">IF(NOT(D54="1X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c"),IF(E54="landmark",CONCATENATE(A54,"_k"),IF(E54="house",CONCATENATE(A54,"_h"),A54))))</f>
-        <v>onsen_k</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U54" s="1" t="str">
         <f aca="false">IF(D54="1X1","none",IF(E54="skyscraper",CONCATENATE(A54,"_c_north"),IF(E54="landmark",CONCATENATE(A54,"_k_north"),IF(E54="house",CONCATENATE(A54,"_h_north"),CONCATENATE(A54,"_north")))))</f>
@@ -5301,110 +5331,110 @@
         <v>none</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="2" t="n">
-        <v>11</v>
+      <c r="A55" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="6" t="n">
+        <v>95</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G55" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="G55" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="H55" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I55" s="1" t="n">
-        <v>1980</v>
+      <c r="H55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>1950</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="1" t="n">
-        <v>10</v>
+      <c r="K55" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="M55" s="5" t="str">
         <f aca="false">VLOOKUP(L55,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
-      </c>
-      <c r="N55" s="1" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N55" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="O55" s="1" t="n">
+      <c r="O55" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q55" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="R55" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="Q55" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="R55" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="S55" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="T55" s="1" t="str">
         <f aca="false">IF(NOT(D55="1X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c"),IF(E55="landmark",CONCATENATE(A55,"_k"),IF(E55="house",CONCATENATE(A55,"_h"),A55))))</f>
-        <v>pachinko_k</v>
+        <v>convini_k</v>
       </c>
       <c r="U55" s="1" t="str">
         <f aca="false">IF(D55="1X1","none",IF(E55="skyscraper",CONCATENATE(A55,"_c_north"),IF(E55="landmark",CONCATENATE(A55,"_k_north"),IF(E55="house",CONCATENATE(A55,"_h_north"),CONCATENATE(A55,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V55" s="1" t="str">
-        <f aca="false">IF(OR(D55="1X1",D55="2X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_east"),IF(E55="landmark",CONCATENATE(A55,"_k_east"),CONCATENATE(A55,"_east"))))</f>
+        <f aca="false">IF(OR(D55="1X1",D55="2X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_east"),IF(E55="landmark",CONCATENATE(A55,"_k_east"),IF(E55="house",CONCATENATE(A55,"_h_east"),CONCATENATE(A55,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W55" s="1" t="str">
-        <f aca="false">IF(OR(D55="1X1",D55="1X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_west"),IF(E55="landmark",CONCATENATE(A55,"_k_west"),CONCATENATE(A55,"_west"))))</f>
+        <f aca="false">IF(OR(D55="1X1",D55="1X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_west"),IF(E55="landmark",CONCATENATE(A55,"_k_west"),IF(E55="house",CONCATENATE(A55,"_h_west"),CONCATENATE(A55,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X55" s="1" t="str">
-        <f aca="false">IF(NOT(D55="2X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_south"),IF(E55="landmark",CONCATENATE(A55,"_k_south"),CONCATENATE(A55,"_south"))))</f>
-        <v>none</v>
-      </c>
-      <c r="Y55" s="1" t="s">
-        <v>159</v>
+        <f aca="false">IF(NOT(D55="2X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_south"),IF(E55="landmark",CONCATENATE(A55,"_k_south"),IF(E55="house",CONCATENATE(A55,"_h_south"),CONCATENATE(A55,"_south")))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y55" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G56" s="1" t="n">
         <v>80</v>
@@ -5422,20 +5452,20 @@
         <v>20</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="M56" s="5" t="str">
         <f aca="false">VLOOKUP(L56,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N56" s="1" t="n">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="O56" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="Q56" s="1" t="n">
         <v>10</v>
@@ -5444,7 +5474,7 @@
         <v>2</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T56" s="1" t="str">
         <f aca="false">IF(NOT(D56="1X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c"),IF(E56="landmark",CONCATENATE(A56,"_k"),IF(E56="house",CONCATENATE(A56,"_h"),A56))))</f>
@@ -5452,51 +5482,51 @@
       </c>
       <c r="U56" s="1" t="str">
         <f aca="false">IF(D56="1X1","none",IF(E56="skyscraper",CONCATENATE(A56,"_c_north"),IF(E56="landmark",CONCATENATE(A56,"_k_north"),IF(E56="house",CONCATENATE(A56,"_h_north"),CONCATENATE(A56,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V56" s="1" t="str">
-        <f aca="false">IF(OR(D56="1X1",D56="2X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_east"),IF(E56="landmark",CONCATENATE(A56,"_k_east"),CONCATENATE(A56,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <f aca="false">IF(OR(D56="1X1",D56="2X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_east"),IF(E56="landmark",CONCATENATE(A56,"_k_east"),IF(E56="house",CONCATENATE(A56,"_h_east"),CONCATENATE(A56,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W56" s="1" t="str">
-        <f aca="false">IF(OR(D56="1X1",D56="1X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_west"),IF(E56="landmark",CONCATENATE(A56,"_k_west"),CONCATENATE(A56,"_west"))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D56="1X1",D56="1X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_west"),IF(E56="landmark",CONCATENATE(A56,"_k_west"),IF(E56="house",CONCATENATE(A56,"_h_west"),CONCATENATE(A56,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X56" s="1" t="str">
-        <f aca="false">IF(NOT(D56="2X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_south"),IF(E56="landmark",CONCATENATE(A56,"_k_south"),CONCATENATE(A56,"_south"))))</f>
+        <f aca="false">IF(NOT(D56="2X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_south"),IF(E56="landmark",CONCATENATE(A56,"_k_south"),IF(E56="house",CONCATENATE(A56,"_h_south"),CONCATENATE(A56,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G57" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H57" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="H57" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>30</v>
@@ -5505,29 +5535,29 @@
         <v>20</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="M57" s="5" t="str">
         <f aca="false">VLOOKUP(L57,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
-      <c r="N57" s="0" t="n">
+      <c r="N57" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="O57" s="0" t="n">
+      <c r="O57" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="Q57" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R57" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="T57" s="1" t="str">
         <f aca="false">IF(NOT(D57="1X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c"),IF(E57="landmark",CONCATENATE(A57,"_k"),IF(E57="house",CONCATENATE(A57,"_h"),A57))))</f>
@@ -5535,169 +5565,169 @@
       </c>
       <c r="U57" s="1" t="str">
         <f aca="false">IF(D57="1X1","none",IF(E57="skyscraper",CONCATENATE(A57,"_c_north"),IF(E57="landmark",CONCATENATE(A57,"_k_north"),IF(E57="house",CONCATENATE(A57,"_h_north"),CONCATENATE(A57,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V57" s="1" t="str">
         <f aca="false">IF(OR(D57="1X1",D57="2X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_east"),IF(E57="landmark",CONCATENATE(A57,"_k_east"),CONCATENATE(A57,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W57" s="1" t="str">
         <f aca="false">IF(OR(D57="1X1",D57="1X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_west"),IF(E57="landmark",CONCATENATE(A57,"_k_west"),CONCATENATE(A57,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X57" s="1" t="str">
         <f aca="false">IF(NOT(D57="2X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_south"),IF(E57="landmark",CONCATENATE(A57,"_k_south"),CONCATENATE(A57,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y57" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G58" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H58" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="H58" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I58" s="1" t="n">
-        <v>0</v>
+        <v>1870</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K58" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="M58" s="5" t="str">
         <f aca="false">VLOOKUP(L58,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N58" s="0" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N58" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O58" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q58" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R58" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="O58" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q58" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R58" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="S58" s="3" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="T58" s="1" t="str">
         <f aca="false">IF(NOT(D58="1X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c"),IF(E58="landmark",CONCATENATE(A58,"_k"),IF(E58="house",CONCATENATE(A58,"_h"),A58))))</f>
-        <v>shrine_k</v>
+        <v>onsen_k</v>
       </c>
       <c r="U58" s="1" t="str">
         <f aca="false">IF(D58="1X1","none",IF(E58="skyscraper",CONCATENATE(A58,"_c_north"),IF(E58="landmark",CONCATENATE(A58,"_k_north"),IF(E58="house",CONCATENATE(A58,"_h_north"),CONCATENATE(A58,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V58" s="1" t="str">
-        <f aca="false">IF(OR(D58="1X1",D58="2X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_east"),IF(E58="landmark",CONCATENATE(A58,"_k_east"),CONCATENATE(A58,"_east"))))</f>
+        <f aca="false">IF(OR(D58="1X1",D58="2X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_east"),IF(E58="landmark",CONCATENATE(A58,"_k_east"),IF(E58="house",CONCATENATE(A58,"_h_east"),CONCATENATE(A58,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W58" s="1" t="str">
-        <f aca="false">IF(OR(D58="1X1",D58="1X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_west"),IF(E58="landmark",CONCATENATE(A58,"_k_west"),CONCATENATE(A58,"_west"))))</f>
+        <f aca="false">IF(OR(D58="1X1",D58="1X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_west"),IF(E58="landmark",CONCATENATE(A58,"_k_west"),IF(E58="house",CONCATENATE(A58,"_h_west"),CONCATENATE(A58,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X58" s="1" t="str">
-        <f aca="false">IF(NOT(D58="2X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_south"),IF(E58="landmark",CONCATENATE(A58,"_k_south"),CONCATENATE(A58,"_south"))))</f>
+        <f aca="false">IF(NOT(D58="2X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_south"),IF(E58="landmark",CONCATENATE(A58,"_k_south"),IF(E58="house",CONCATENATE(A58,"_h_south"),CONCATENATE(A58,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y58" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G59" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H59" s="0" t="n">
-        <v>5</v>
+        <v>50</v>
+      </c>
+      <c r="H59" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I59" s="1" t="n">
-        <v>0</v>
+        <v>1980</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>168</v>
+        <v>56</v>
       </c>
       <c r="M59" s="5" t="str">
         <f aca="false">VLOOKUP(L59,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N59" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O59" s="0" t="n">
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N59" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O59" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R59" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S59" s="3" t="s">
         <v>169</v>
       </c>
       <c r="T59" s="1" t="str">
         <f aca="false">IF(NOT(D59="1X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c"),IF(E59="landmark",CONCATENATE(A59,"_k"),IF(E59="house",CONCATENATE(A59,"_h"),A59))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U59" s="1" t="str">
         <f aca="false">IF(D59="1X1","none",IF(E59="skyscraper",CONCATENATE(A59,"_c_north"),IF(E59="landmark",CONCATENATE(A59,"_k_north"),IF(E59="house",CONCATENATE(A59,"_h_north"),CONCATENATE(A59,"_north")))))</f>
@@ -5716,30 +5746,30 @@
         <v>none</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G60" s="1" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="H60" s="1" t="n">
         <v>3</v>
@@ -5754,29 +5784,29 @@
         <v>20</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="M60" s="5" t="str">
         <f aca="false">VLOOKUP(L60,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N60" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O60" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="Q60" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R60" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="T60" s="1" t="str">
         <f aca="false">IF(NOT(D60="1X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c"),IF(E60="landmark",CONCATENATE(A60,"_k"),IF(E60="house",CONCATENATE(A60,"_h"),A60))))</f>
@@ -5784,47 +5814,47 @@
       </c>
       <c r="U60" s="1" t="str">
         <f aca="false">IF(D60="1X1","none",IF(E60="skyscraper",CONCATENATE(A60,"_c_north"),IF(E60="landmark",CONCATENATE(A60,"_k_north"),IF(E60="house",CONCATENATE(A60,"_h_north"),CONCATENATE(A60,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V60" s="1" t="str">
         <f aca="false">IF(OR(D60="1X1",D60="2X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_east"),IF(E60="landmark",CONCATENATE(A60,"_k_east"),CONCATENATE(A60,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W60" s="1" t="str">
         <f aca="false">IF(OR(D60="1X1",D60="1X2"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_west"),IF(E60="landmark",CONCATENATE(A60,"_k_west"),CONCATENATE(A60,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X60" s="1" t="str">
         <f aca="false">IF(NOT(D60="2X2"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_south"),IF(E60="landmark",CONCATENATE(A60,"_k_south"),CONCATENATE(A60,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y60" s="1" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G61" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H61" s="1" t="n">
+      <c r="H61" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I61" s="1" t="n">
@@ -5837,20 +5867,20 @@
         <v>20</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M61" s="5" t="str">
         <f aca="false">VLOOKUP(L61,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N61" s="1" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N61" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O61" s="1" t="n">
+      <c r="O61" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q61" s="1" t="n">
         <v>10</v>
@@ -5859,7 +5889,7 @@
         <v>2</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="T61" s="1" t="str">
         <f aca="false">IF(NOT(D61="1X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c"),IF(E61="landmark",CONCATENATE(A61,"_k"),IF(E61="house",CONCATENATE(A61,"_h"),A61))))</f>
@@ -5867,52 +5897,384 @@
       </c>
       <c r="U61" s="1" t="str">
         <f aca="false">IF(D61="1X1","none",IF(E61="skyscraper",CONCATENATE(A61,"_c_north"),IF(E61="landmark",CONCATENATE(A61,"_k_north"),IF(E61="house",CONCATENATE(A61,"_h_north"),CONCATENATE(A61,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V61" s="1" t="str">
         <f aca="false">IF(OR(D61="1X1",D61="2X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_east"),IF(E61="landmark",CONCATENATE(A61,"_k_east"),CONCATENATE(A61,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W61" s="1" t="str">
         <f aca="false">IF(OR(D61="1X1",D61="1X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_west"),IF(E61="landmark",CONCATENATE(A61,"_k_west"),CONCATENATE(A61,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X61" s="1" t="str">
         <f aca="false">IF(NOT(D61="2X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_south"),IF(E61="landmark",CONCATENATE(A61,"_k_south"),CONCATENATE(A61,"_south"))))</f>
+        <v>shiro_k_south</v>
+      </c>
+      <c r="Y61" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K62" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M62" s="5" t="str">
+        <f aca="false">VLOOKUP(L62,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S62" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="T62" s="1" t="str">
+        <f aca="false">IF(NOT(D62="1X1"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c"),IF(E62="landmark",CONCATENATE(A62,"_k"),IF(E62="house",CONCATENATE(A62,"_h"),A62))))</f>
+        <v>shrine_k</v>
+      </c>
+      <c r="U62" s="1" t="str">
+        <f aca="false">IF(D62="1X1","none",IF(E62="skyscraper",CONCATENATE(A62,"_c_north"),IF(E62="landmark",CONCATENATE(A62,"_k_north"),IF(E62="house",CONCATENATE(A62,"_h_north"),CONCATENATE(A62,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V62" s="1" t="str">
+        <f aca="false">IF(OR(D62="1X1",D62="2X1"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c_east"),IF(E62="landmark",CONCATENATE(A62,"_k_east"),CONCATENATE(A62,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W62" s="1" t="str">
+        <f aca="false">IF(OR(D62="1X1",D62="1X2"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c_west"),IF(E62="landmark",CONCATENATE(A62,"_k_west"),CONCATENATE(A62,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X62" s="1" t="str">
+        <f aca="false">IF(NOT(D62="2X2"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c_south"),IF(E62="landmark",CONCATENATE(A62,"_k_south"),CONCATENATE(A62,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G63" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K63" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M63" s="5" t="str">
+        <f aca="false">VLOOKUP(L63,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N63" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S63" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="T63" s="1" t="str">
+        <f aca="false">IF(NOT(D63="1X1"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c"),IF(E63="landmark",CONCATENATE(A63,"_k"),IF(E63="house",CONCATENATE(A63,"_h"),A63))))</f>
+        <v>shrine_prohibition_k</v>
+      </c>
+      <c r="U63" s="1" t="str">
+        <f aca="false">IF(D63="1X1","none",IF(E63="skyscraper",CONCATENATE(A63,"_c_north"),IF(E63="landmark",CONCATENATE(A63,"_k_north"),IF(E63="house",CONCATENATE(A63,"_h_north"),CONCATENATE(A63,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V63" s="1" t="str">
+        <f aca="false">IF(OR(D63="1X1",D63="2X1"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c_east"),IF(E63="landmark",CONCATENATE(A63,"_k_east"),CONCATENATE(A63,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W63" s="1" t="str">
+        <f aca="false">IF(OR(D63="1X1",D63="1X2"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c_west"),IF(E63="landmark",CONCATENATE(A63,"_k_west"),CONCATENATE(A63,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X63" s="1" t="str">
+        <f aca="false">IF(NOT(D63="2X2"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c_south"),IF(E63="landmark",CONCATENATE(A63,"_k_south"),CONCATENATE(A63,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y63" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G64" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H64" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K64" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="M64" s="5" t="str">
+        <f aca="false">VLOOKUP(L64,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N64" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O64" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q64" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R64" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S64" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="T64" s="1" t="str">
+        <f aca="false">IF(NOT(D64="1X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c"),IF(E64="landmark",CONCATENATE(A64,"_k"),IF(E64="house",CONCATENATE(A64,"_h"),A64))))</f>
+        <v>none</v>
+      </c>
+      <c r="U64" s="1" t="str">
+        <f aca="false">IF(D64="1X1","none",IF(E64="skyscraper",CONCATENATE(A64,"_c_north"),IF(E64="landmark",CONCATENATE(A64,"_k_north"),IF(E64="house",CONCATENATE(A64,"_h_north"),CONCATENATE(A64,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V64" s="1" t="str">
+        <f aca="false">IF(OR(D64="1X1",D64="2X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_east"),IF(E64="landmark",CONCATENATE(A64,"_k_east"),CONCATENATE(A64,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W64" s="1" t="str">
+        <f aca="false">IF(OR(D64="1X1",D64="1X2"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_west"),IF(E64="landmark",CONCATENATE(A64,"_k_west"),CONCATENATE(A64,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X64" s="1" t="str">
+        <f aca="false">IF(NOT(D64="2X2"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_south"),IF(E64="landmark",CONCATENATE(A64,"_k_south"),CONCATENATE(A64,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y64" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M65" s="5" t="str">
+        <f aca="false">VLOOKUP(L65,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O65" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P65" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S65" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="T65" s="1" t="str">
+        <f aca="false">IF(NOT(D65="1X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c"),IF(E65="landmark",CONCATENATE(A65,"_k"),IF(E65="house",CONCATENATE(A65,"_h"),A65))))</f>
+        <v>none</v>
+      </c>
+      <c r="U65" s="1" t="str">
+        <f aca="false">IF(D65="1X1","none",IF(E65="skyscraper",CONCATENATE(A65,"_c_north"),IF(E65="landmark",CONCATENATE(A65,"_k_north"),IF(E65="house",CONCATENATE(A65,"_h_north"),CONCATENATE(A65,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V65" s="1" t="str">
+        <f aca="false">IF(OR(D65="1X1",D65="2X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_east"),IF(E65="landmark",CONCATENATE(A65,"_k_east"),CONCATENATE(A65,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W65" s="1" t="str">
+        <f aca="false">IF(OR(D65="1X1",D65="1X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_west"),IF(E65="landmark",CONCATENATE(A65,"_k_west"),CONCATENATE(A65,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X65" s="1" t="str">
+        <f aca="false">IF(NOT(D65="2X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_south"),IF(E65="landmark",CONCATENATE(A65,"_k_south"),CONCATENATE(A65,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y61" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0"/>
-      <c r="D62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="5"/>
-      <c r="P62" s="3"/>
-      <c r="S62" s="3"/>
+      <c r="Y65" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0"/>
+      <c r="D66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="5"/>
+      <c r="P66" s="3"/>
+      <c r="S66" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C50 C52:C1048576">
+  <conditionalFormatting sqref="C1:C54 C56:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E33" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E37" type="list">
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L62" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L66" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P62" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P66" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S62" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S66" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5942,16 +6304,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6640,11 +7002,11 @@
       </c>
       <c r="B42" s="1" t="str">
         <f aca="false">IF(C42="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C42" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A42,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D42" s="1" t="n">
         <f aca="false">IF(C42="Multi-tile",D41-1,MAX(IF(C42="ID not in use",0,IF(C42="1X1",1,IF(C42="2X2",4,2)))-1,0))</f>
@@ -6657,11 +7019,11 @@
       </c>
       <c r="B43" s="1" t="str">
         <f aca="false">IF(C43="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C43" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A43,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D43" s="1" t="n">
         <f aca="false">IF(C43="Multi-tile",D42-1,MAX(IF(C43="ID not in use",0,IF(C43="1X1",1,IF(C43="2X2",4,2)))-1,0))</f>
@@ -7218,11 +7580,11 @@
       </c>
       <c r="B76" s="1" t="str">
         <f aca="false">IF(C76="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C76" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A76,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D76" s="1" t="n">
         <f aca="false">IF(C76="Multi-tile",D75-1,MAX(IF(C76="ID not in use",0,IF(C76="1X1",1,IF(C76="2X2",4,2)))-1,0))</f>
@@ -7235,11 +7597,11 @@
       </c>
       <c r="B77" s="1" t="str">
         <f aca="false">IF(C77="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C77" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A77,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D77" s="1" t="n">
         <f aca="false">IF(C77="Multi-tile",D76-1,MAX(IF(C77="ID not in use",0,IF(C77="1X1",1,IF(C77="2X2",4,2)))-1,0))</f>
@@ -10340,25 +10702,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10372,13 +10734,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -10401,10 +10763,10 @@
         <v>56</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10418,16 +10780,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10435,73 +10797,73 @@
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: nagoya & nakamura
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="214">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -289,6 +289,27 @@
   </si>
   <si>
     <t xml:space="preserve">murakami_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nagoya_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nagoya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_NAGOYA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nakamura_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nakamura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_NAKAMURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nakamura_m</t>
   </si>
   <si>
     <t xml:space="preserve">nakayama_m</t>
@@ -774,14 +795,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y66"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3095,7 +3116,7 @@
         <v>90</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -3113,7 +3134,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>1950</v>
+        <v>1960</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>30</v>
@@ -3150,7 +3171,7 @@
       </c>
       <c r="T28" s="1" t="str">
         <f aca="false">IF(NOT(D28="1X1"),"none",IF(E28="skyscraper",CONCATENATE(A28,"_c"),IF(E28="landmark",CONCATENATE(A28,"_k"),IF(E28="house",CONCATENATE(A28,"_h"),A28))))</f>
-        <v>nakayama_m</v>
+        <v>nagoya_m</v>
       </c>
       <c r="U28" s="1" t="str">
         <f aca="false">IF(D28="1X1","none",IF(E28="skyscraper",CONCATENATE(A28,"_c_north"),IF(E28="landmark",CONCATENATE(A28,"_k_north"),IF(E28="house",CONCATENATE(A28,"_h_north"),CONCATENATE(A28,"_north")))))</f>
@@ -3180,38 +3201,38 @@
         <v>93</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="M29" s="5" t="str">
         <f aca="false">VLOOKUP(L29,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N29" s="1" t="n">
         <v>27</v>
@@ -3224,18 +3245,18 @@
       </c>
       <c r="Q29" s="1" t="n">
         <f aca="false">VLOOKUP(E29,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R29" s="1" t="n">
         <f aca="false">VLOOKUP(E29,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T29" s="1" t="str">
         <f aca="false">IF(NOT(D29="1X1"),"none",IF(E29="skyscraper",CONCATENATE(A29,"_c"),IF(E29="landmark",CONCATENATE(A29,"_k"),IF(E29="house",CONCATENATE(A29,"_h"),A29))))</f>
-        <v>okada_office_tower_m</v>
+        <v>nakamura_s</v>
       </c>
       <c r="U29" s="1" t="str">
         <f aca="false">IF(D29="1X1","none",IF(E29="skyscraper",CONCATENATE(A29,"_c_north"),IF(E29="landmark",CONCATENATE(A29,"_k_north"),IF(E29="house",CONCATENATE(A29,"_h_north"),CONCATENATE(A29,"_north")))))</f>
@@ -3265,38 +3286,38 @@
         <v>93</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>94</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M30" s="5" t="str">
         <f aca="false">VLOOKUP(L30,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N30" s="1" t="n">
         <v>27</v>
@@ -3308,17 +3329,19 @@
         <v>32</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>14</v>
+        <f aca="false">VLOOKUP(E30,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R30" s="1" t="n">
-        <v>5</v>
+        <f aca="false">VLOOKUP(E30,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T30" s="1" t="str">
         <f aca="false">IF(NOT(D30="1X1"),"none",IF(E30="skyscraper",CONCATENATE(A30,"_c"),IF(E30="landmark",CONCATENATE(A30,"_k"),IF(E30="house",CONCATENATE(A30,"_h"),A30))))</f>
-        <v>okada_office_tower_l</v>
+        <v>nakamura_m</v>
       </c>
       <c r="U30" s="1" t="str">
         <f aca="false">IF(D30="1X1","none",IF(E30="skyscraper",CONCATENATE(A30,"_c_north"),IF(E30="landmark",CONCATENATE(A30,"_k_north"),IF(E30="house",CONCATENATE(A30,"_h_north"),CONCATENATE(A30,"_north")))))</f>
@@ -3345,41 +3368,41 @@
         <v>96</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M31" s="5" t="str">
         <f aca="false">VLOOKUP(L31,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N31" s="1" t="n">
         <v>27</v>
@@ -3391,17 +3414,19 @@
         <v>32</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>16</v>
+        <f aca="false">VLOOKUP(E31,dropdowns!A:C,2,0)</f>
+        <v>10</v>
       </c>
       <c r="R31" s="1" t="n">
-        <v>6</v>
+        <f aca="false">VLOOKUP(E31,dropdowns!A:C,3,0)</f>
+        <v>4</v>
       </c>
       <c r="S31" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T31" s="1" t="str">
         <f aca="false">IF(NOT(D31="1X1"),"none",IF(E31="skyscraper",CONCATENATE(A31,"_c"),IF(E31="landmark",CONCATENATE(A31,"_k"),IF(E31="house",CONCATENATE(A31,"_h"),A31))))</f>
-        <v>okada_office_tower_x</v>
+        <v>nakayama_m</v>
       </c>
       <c r="U31" s="1" t="str">
         <f aca="false">IF(D31="1X1","none",IF(E31="skyscraper",CONCATENATE(A31,"_c_north"),IF(E31="landmark",CONCATENATE(A31,"_k_north"),IF(E31="house",CONCATENATE(A31,"_h_north"),CONCATENATE(A31,"_north")))))</f>
@@ -3425,13 +3450,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
@@ -3440,7 +3465,7 @@
         <v>28</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>100</v>
@@ -3449,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>1945</v>
+        <v>1955</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>30</v>
@@ -3474,9 +3499,11 @@
         <v>32</v>
       </c>
       <c r="Q32" s="1" t="n">
+        <f aca="false">VLOOKUP(E32,dropdowns!A:C,2,0)</f>
         <v>10</v>
       </c>
       <c r="R32" s="1" t="n">
+        <f aca="false">VLOOKUP(E32,dropdowns!A:C,3,0)</f>
         <v>4</v>
       </c>
       <c r="S32" s="3" t="s">
@@ -3484,7 +3511,7 @@
       </c>
       <c r="T32" s="1" t="str">
         <f aca="false">IF(NOT(D32="1X1"),"none",IF(E32="skyscraper",CONCATENATE(A32,"_c"),IF(E32="landmark",CONCATENATE(A32,"_k"),IF(E32="house",CONCATENATE(A32,"_h"),A32))))</f>
-        <v>old_office_building_m</v>
+        <v>okada_office_tower_m</v>
       </c>
       <c r="U32" s="1" t="str">
         <f aca="false">IF(D32="1X1","none",IF(E32="skyscraper",CONCATENATE(A32,"_c_north"),IF(E32="landmark",CONCATENATE(A32,"_k_north"),IF(E32="house",CONCATENATE(A32,"_h_north"),CONCATENATE(A32,"_north")))))</f>
@@ -3508,13 +3535,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C33" s="2" t="n">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
@@ -3523,7 +3550,7 @@
         <v>35</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>125</v>
@@ -3532,7 +3559,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>1945</v>
+        <v>1955</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>30</v>
@@ -3567,7 +3594,7 @@
       </c>
       <c r="T33" s="1" t="str">
         <f aca="false">IF(NOT(D33="1X1"),"none",IF(E33="skyscraper",CONCATENATE(A33,"_c"),IF(E33="landmark",CONCATENATE(A33,"_k"),IF(E33="house",CONCATENATE(A33,"_h"),A33))))</f>
-        <v>old_office_building_l</v>
+        <v>okada_office_tower_l</v>
       </c>
       <c r="U33" s="1" t="str">
         <f aca="false">IF(D33="1X1","none",IF(E33="skyscraper",CONCATENATE(A33,"_c_north"),IF(E33="landmark",CONCATENATE(A33,"_k_north"),IF(E33="house",CONCATENATE(A33,"_h_north"),CONCATENATE(A33,"_north")))))</f>
@@ -3591,44 +3618,44 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>1970</v>
+        <v>1955</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M34" s="5" t="str">
         <f aca="false">VLOOKUP(L34,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N34" s="1" t="n">
         <v>27</v>
@@ -3640,19 +3667,17 @@
         <v>32</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <f aca="false">VLOOKUP(E34,dropdowns!A:C,2,0)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="R34" s="1" t="n">
-        <f aca="false">VLOOKUP(E34,dropdowns!A:C,3,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T34" s="1" t="str">
         <f aca="false">IF(NOT(D34="1X1"),"none",IF(E34="skyscraper",CONCATENATE(A34,"_c"),IF(E34="landmark",CONCATENATE(A34,"_k"),IF(E34="house",CONCATENATE(A34,"_h"),A34))))</f>
-        <v>yamada_electronics_centre_m</v>
+        <v>okada_office_tower_x</v>
       </c>
       <c r="U34" s="1" t="str">
         <f aca="false">IF(D34="1X1","none",IF(E34="skyscraper",CONCATENATE(A34,"_c_north"),IF(E34="landmark",CONCATENATE(A34,"_k_north"),IF(E34="house",CONCATENATE(A34,"_h_north"),CONCATENATE(A34,"_north")))))</f>
@@ -3679,41 +3704,41 @@
         <v>104</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="H35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>1970</v>
+        <v>1945</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M35" s="5" t="str">
         <f aca="false">VLOOKUP(L35,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N35" s="1" t="n">
         <v>27</v>
@@ -3725,17 +3750,17 @@
         <v>32</v>
       </c>
       <c r="Q35" s="1" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R35" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T35" s="1" t="str">
         <f aca="false">IF(NOT(D35="1X1"),"none",IF(E35="skyscraper",CONCATENATE(A35,"_c"),IF(E35="landmark",CONCATENATE(A35,"_k"),IF(E35="house",CONCATENATE(A35,"_h"),A35))))</f>
-        <v>yamada_electronics_centre_l</v>
+        <v>old_office_building_m</v>
       </c>
       <c r="U35" s="1" t="str">
         <f aca="false">IF(D35="1X1","none",IF(E35="skyscraper",CONCATENATE(A35,"_c_north"),IF(E35="landmark",CONCATENATE(A35,"_k_north"),IF(E35="house",CONCATENATE(A35,"_h_north"),CONCATENATE(A35,"_north")))))</f>
@@ -3759,44 +3784,44 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C36" s="2" t="n">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>1970</v>
+        <v>1945</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M36" s="5" t="str">
         <f aca="false">VLOOKUP(L36,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N36" s="1" t="n">
         <v>27</v>
@@ -3808,17 +3833,17 @@
         <v>32</v>
       </c>
       <c r="Q36" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R36" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T36" s="1" t="str">
         <f aca="false">IF(NOT(D36="1X1"),"none",IF(E36="skyscraper",CONCATENATE(A36,"_c"),IF(E36="landmark",CONCATENATE(A36,"_k"),IF(E36="house",CONCATENATE(A36,"_h"),A36))))</f>
-        <v>yamada_electronics_centre_x</v>
+        <v>old_office_building_l</v>
       </c>
       <c r="U36" s="1" t="str">
         <f aca="false">IF(D36="1X1","none",IF(E36="skyscraper",CONCATENATE(A36,"_c_north"),IF(E36="landmark",CONCATENATE(A36,"_k_north"),IF(E36="house",CONCATENATE(A36,"_h_north"),CONCATENATE(A36,"_north")))))</f>
@@ -3842,13 +3867,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
@@ -3857,7 +3882,7 @@
         <v>28</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>100</v>
@@ -3891,9 +3916,11 @@
         <v>32</v>
       </c>
       <c r="Q37" s="1" t="n">
+        <f aca="false">VLOOKUP(E37,dropdowns!A:C,2,0)</f>
         <v>10</v>
       </c>
       <c r="R37" s="1" t="n">
+        <f aca="false">VLOOKUP(E37,dropdowns!A:C,3,0)</f>
         <v>4</v>
       </c>
       <c r="S37" s="3" t="s">
@@ -3901,7 +3928,7 @@
       </c>
       <c r="T37" s="1" t="str">
         <f aca="false">IF(NOT(D37="1X1"),"none",IF(E37="skyscraper",CONCATENATE(A37,"_c"),IF(E37="landmark",CONCATENATE(A37,"_k"),IF(E37="house",CONCATENATE(A37,"_h"),A37))))</f>
-        <v>yano_m</v>
+        <v>yamada_electronics_centre_m</v>
       </c>
       <c r="U37" s="1" t="str">
         <f aca="false">IF(D37="1X1","none",IF(E37="skyscraper",CONCATENATE(A37,"_c_north"),IF(E37="landmark",CONCATENATE(A37,"_k_north"),IF(E37="house",CONCATENATE(A37,"_h_north"),CONCATENATE(A37,"_north")))))</f>
@@ -3925,66 +3952,66 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>109</v>
+      <c r="E38" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>220</v>
+        <v>125</v>
       </c>
       <c r="H38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M38" s="5" t="str">
         <f aca="false">VLOOKUP(L38,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N38" s="1" t="n">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="O38" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R38" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="P38" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q38" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="R38" s="1" t="n">
-        <v>6</v>
       </c>
       <c r="S38" s="3" t="s">
         <v>33</v>
       </c>
       <c r="T38" s="1" t="str">
         <f aca="false">IF(NOT(D38="1X1"),"none",IF(E38="skyscraper",CONCATENATE(A38,"_c"),IF(E38="landmark",CONCATENATE(A38,"_k"),IF(E38="house",CONCATENATE(A38,"_h"),A38))))</f>
-        <v>bank_building_c</v>
+        <v>yamada_electronics_centre_l</v>
       </c>
       <c r="U38" s="1" t="str">
         <f aca="false">IF(D38="1X1","none",IF(E38="skyscraper",CONCATENATE(A38,"_c_north"),IF(E38="landmark",CONCATENATE(A38,"_k_north"),IF(E38="house",CONCATENATE(A38,"_h_north"),CONCATENATE(A38,"_north")))))</f>
@@ -4011,34 +4038,34 @@
         <v>112</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>109</v>
+      <c r="E39" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="H39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>1990</v>
+        <v>1970</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>39</v>
@@ -4048,26 +4075,26 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N39" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O39" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O39" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P39" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="Q39" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R39" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="T39" s="1" t="str">
         <f aca="false">IF(NOT(D39="1X1"),"none",IF(E39="skyscraper",CONCATENATE(A39,"_c"),IF(E39="landmark",CONCATENATE(A39,"_k"),IF(E39="house",CONCATENATE(A39,"_h"),A39))))</f>
-        <v>enterprise_tower_c</v>
+        <v>yamada_electronics_centre_x</v>
       </c>
       <c r="U39" s="1" t="str">
         <f aca="false">IF(D39="1X1","none",IF(E39="skyscraper",CONCATENATE(A39,"_c_north"),IF(E39="landmark",CONCATENATE(A39,"_k_north"),IF(E39="house",CONCATENATE(A39,"_h_north"),CONCATENATE(A39,"_north")))))</f>
@@ -4091,66 +4118,66 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>109</v>
+      <c r="E40" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>1960</v>
+        <v>1970</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M40" s="5" t="str">
         <f aca="false">VLOOKUP(L40,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE)</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N40" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="O40" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O40" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="P40" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="Q40" s="1" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="R40" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="T40" s="1" t="str">
         <f aca="false">IF(NOT(D40="1X1"),"none",IF(E40="skyscraper",CONCATENATE(A40,"_c"),IF(E40="landmark",CONCATENATE(A40,"_k"),IF(E40="house",CONCATENATE(A40,"_h"),A40))))</f>
-        <v>insurance_tower_c</v>
+        <v>yano_m</v>
       </c>
       <c r="U40" s="1" t="str">
         <f aca="false">IF(D40="1X1","none",IF(E40="skyscraper",CONCATENATE(A40,"_c_north"),IF(E40="landmark",CONCATENATE(A40,"_k_north"),IF(E40="house",CONCATENATE(A40,"_h_north"),CONCATENATE(A40,"_north")))))</f>
@@ -4174,22 +4201,22 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>220</v>
@@ -4198,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>2000</v>
+        <v>1980</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>30</v>
@@ -4214,26 +4241,26 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="O41" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q41" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="R41" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="T41" s="1" t="str">
         <f aca="false">IF(NOT(D41="1X1"),"none",IF(E41="skyscraper",CONCATENATE(A41,"_c"),IF(E41="landmark",CONCATENATE(A41,"_k"),IF(E41="house",CONCATENATE(A41,"_h"),A41))))</f>
-        <v>kuroi_tower_c</v>
+        <v>bank_building_c</v>
       </c>
       <c r="U41" s="1" t="str">
         <f aca="false">IF(D41="1X1","none",IF(E41="skyscraper",CONCATENATE(A41,"_c_north"),IF(E41="landmark",CONCATENATE(A41,"_k_north"),IF(E41="house",CONCATENATE(A41,"_h_north"),CONCATENATE(A41,"_north")))))</f>
@@ -4263,13 +4290,13 @@
         <v>119</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>120</v>
@@ -4281,7 +4308,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>30</v>
@@ -4303,7 +4330,7 @@
         <v>5</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q42" s="1" t="n">
         <v>24</v>
@@ -4312,11 +4339,11 @@
         <v>10</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T42" s="1" t="str">
         <f aca="false">IF(NOT(D42="1X1"),"none",IF(E42="skyscraper",CONCATENATE(A42,"_c"),IF(E42="landmark",CONCATENATE(A42,"_k"),IF(E42="house",CONCATENATE(A42,"_h"),A42))))</f>
-        <v>mitsui_tower_c</v>
+        <v>enterprise_tower_c</v>
       </c>
       <c r="U42" s="1" t="str">
         <f aca="false">IF(D42="1X1","none",IF(E42="skyscraper",CONCATENATE(A42,"_c_north"),IF(E42="landmark",CONCATENATE(A42,"_k_north"),IF(E42="house",CONCATENATE(A42,"_h_north"),CONCATENATE(A42,"_north")))))</f>
@@ -4340,31 +4367,31 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>2000</v>
+        <v>1960</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>30</v>
@@ -4386,7 +4413,7 @@
         <v>5</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q43" s="1" t="n">
         <v>24</v>
@@ -4395,11 +4422,11 @@
         <v>10</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T43" s="1" t="str">
         <f aca="false">IF(NOT(D43="1X1"),"none",IF(E43="skyscraper",CONCATENATE(A43,"_c"),IF(E43="landmark",CONCATENATE(A43,"_k"),IF(E43="house",CONCATENATE(A43,"_h"),A43))))</f>
-        <v>modern_office_tower_c</v>
+        <v>insurance_tower_c</v>
       </c>
       <c r="U43" s="1" t="str">
         <f aca="false">IF(D43="1X1","none",IF(E43="skyscraper",CONCATENATE(A43,"_c_north"),IF(E43="landmark",CONCATENATE(A43,"_k_north"),IF(E43="house",CONCATENATE(A43,"_h_north"),CONCATENATE(A43,"_north")))))</f>
@@ -4423,22 +4450,22 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>220</v>
@@ -4447,7 +4474,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>30</v>
@@ -4469,7 +4496,7 @@
         <v>5</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q44" s="1" t="n">
         <v>24</v>
@@ -4478,11 +4505,11 @@
         <v>10</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T44" s="1" t="str">
         <f aca="false">IF(NOT(D44="1X1"),"none",IF(E44="skyscraper",CONCATENATE(A44,"_c"),IF(E44="landmark",CONCATENATE(A44,"_k"),IF(E44="house",CONCATENATE(A44,"_h"),A44))))</f>
-        <v>multimedia_offices_c</v>
+        <v>kuroi_tower_c</v>
       </c>
       <c r="U44" s="1" t="str">
         <f aca="false">IF(D44="1X1","none",IF(E44="skyscraper",CONCATENATE(A44,"_c_north"),IF(E44="landmark",CONCATENATE(A44,"_k_north"),IF(E44="house",CONCATENATE(A44,"_h_north"),CONCATENATE(A44,"_north")))))</f>
@@ -4506,22 +4533,22 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G45" s="1" t="n">
         <v>220</v>
@@ -4552,7 +4579,7 @@
         <v>5</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q45" s="1" t="n">
         <v>24</v>
@@ -4561,11 +4588,11 @@
         <v>10</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T45" s="1" t="str">
         <f aca="false">IF(NOT(D45="1X1"),"none",IF(E45="skyscraper",CONCATENATE(A45,"_c"),IF(E45="landmark",CONCATENATE(A45,"_k"),IF(E45="house",CONCATENATE(A45,"_h"),A45))))</f>
-        <v>office_tower_c</v>
+        <v>mitsui_tower_c</v>
       </c>
       <c r="U45" s="1" t="str">
         <f aca="false">IF(D45="1X1","none",IF(E45="skyscraper",CONCATENATE(A45,"_c_north"),IF(E45="landmark",CONCATENATE(A45,"_k_north"),IF(E45="house",CONCATENATE(A45,"_h_north"),CONCATENATE(A45,"_north")))))</f>
@@ -4589,31 +4616,31 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G46" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H46" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>1960</v>
+        <v>2000</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>30</v>
@@ -4635,7 +4662,7 @@
         <v>5</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q46" s="1" t="n">
         <v>24</v>
@@ -4644,11 +4671,11 @@
         <v>10</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T46" s="1" t="str">
         <f aca="false">IF(NOT(D46="1X1"),"none",IF(E46="skyscraper",CONCATENATE(A46,"_c"),IF(E46="landmark",CONCATENATE(A46,"_k"),IF(E46="house",CONCATENATE(A46,"_h"),A46))))</f>
-        <v>sato_building_c</v>
+        <v>modern_office_tower_c</v>
       </c>
       <c r="U46" s="1" t="str">
         <f aca="false">IF(D46="1X1","none",IF(E46="skyscraper",CONCATENATE(A46,"_c_north"),IF(E46="landmark",CONCATENATE(A46,"_k_north"),IF(E46="house",CONCATENATE(A46,"_h_north"),CONCATENATE(A46,"_north")))))</f>
@@ -4672,25 +4699,25 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>1</v>
@@ -4718,7 +4745,7 @@
         <v>5</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q47" s="1" t="n">
         <v>24</v>
@@ -4727,11 +4754,11 @@
         <v>10</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T47" s="1" t="str">
         <f aca="false">IF(NOT(D47="1X1"),"none",IF(E47="skyscraper",CONCATENATE(A47,"_c"),IF(E47="landmark",CONCATENATE(A47,"_k"),IF(E47="house",CONCATENATE(A47,"_h"),A47))))</f>
-        <v>sugiyama_office_building_c</v>
+        <v>multimedia_offices_c</v>
       </c>
       <c r="U47" s="1" t="str">
         <f aca="false">IF(D47="1X1","none",IF(E47="skyscraper",CONCATENATE(A47,"_c_north"),IF(E47="landmark",CONCATENATE(A47,"_k_north"),IF(E47="house",CONCATENATE(A47,"_h_north"),CONCATENATE(A47,"_north")))))</f>
@@ -4755,31 +4782,31 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H48" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>30</v>
@@ -4795,13 +4822,13 @@
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N48" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O48" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q48" s="1" t="n">
         <v>24</v>
@@ -4810,19 +4837,19 @@
         <v>10</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T48" s="1" t="str">
         <f aca="false">IF(NOT(D48="1X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c"),IF(E48="landmark",CONCATENATE(A48,"_k"),IF(E48="house",CONCATENATE(A48,"_h"),A48))))</f>
-        <v>none</v>
+        <v>office_tower_c</v>
       </c>
       <c r="U48" s="1" t="str">
         <f aca="false">IF(D48="1X1","none",IF(E48="skyscraper",CONCATENATE(A48,"_c_north"),IF(E48="landmark",CONCATENATE(A48,"_k_north"),IF(E48="house",CONCATENATE(A48,"_h_north"),CONCATENATE(A48,"_north")))))</f>
-        <v>tsuno_building_c_north</v>
+        <v>none</v>
       </c>
       <c r="V48" s="1" t="str">
         <f aca="false">IF(OR(D48="1X1",D48="2X1"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_east"),IF(E48="landmark",CONCATENATE(A48,"_k_east"),CONCATENATE(A48,"_east"))))</f>
-        <v>tsuno_building_c_east</v>
+        <v>none</v>
       </c>
       <c r="W48" s="1" t="str">
         <f aca="false">IF(OR(D48="1X1",D48="1X2"),"none",IF(E48="skyscraper",CONCATENATE(A48,"_c_west"),IF(E48="landmark",CONCATENATE(A48,"_k_west"),CONCATENATE(A48,"_west"))))</f>
@@ -4844,13 +4871,13 @@
         <v>134</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>135</v>
@@ -4862,10 +4889,10 @@
         <v>1</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>1955</v>
-      </c>
-      <c r="J49" s="4" t="n">
-        <v>1989</v>
+        <v>1960</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="K49" s="1" t="n">
         <v>25</v>
@@ -4884,7 +4911,7 @@
         <v>5</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q49" s="1" t="n">
         <v>24</v>
@@ -4893,11 +4920,11 @@
         <v>10</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T49" s="1" t="str">
         <f aca="false">IF(NOT(D49="1X1"),"none",IF(E49="skyscraper",CONCATENATE(A49,"_c"),IF(E49="landmark",CONCATENATE(A49,"_k"),IF(E49="house",CONCATENATE(A49,"_h"),A49))))</f>
-        <v>ueda_office_block_c</v>
+        <v>sato_building_c</v>
       </c>
       <c r="U49" s="1" t="str">
         <f aca="false">IF(D49="1X1","none",IF(E49="skyscraper",CONCATENATE(A49,"_c_north"),IF(E49="landmark",CONCATENATE(A49,"_k_north"),IF(E49="house",CONCATENATE(A49,"_h_north"),CONCATENATE(A49,"_north")))))</f>
@@ -4927,25 +4954,25 @@
         <v>136</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>137</v>
       </c>
       <c r="G50" s="1" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="H50" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>1965</v>
+        <v>1990</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>30</v>
@@ -4967,20 +4994,20 @@
         <v>5</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q50" s="1" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R50" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T50" s="1" t="str">
         <f aca="false">IF(NOT(D50="1X1"),"none",IF(E50="skyscraper",CONCATENATE(A50,"_c"),IF(E50="landmark",CONCATENATE(A50,"_k"),IF(E50="house",CONCATENATE(A50,"_h"),A50))))</f>
-        <v>yamaguchi_office_c</v>
+        <v>sugiyama_office_building_c</v>
       </c>
       <c r="U50" s="1" t="str">
         <f aca="false">IF(D50="1X1","none",IF(E50="skyscraper",CONCATENATE(A50,"_c_north"),IF(E50="landmark",CONCATENATE(A50,"_k_north"),IF(E50="house",CONCATENATE(A50,"_h_north"),CONCATENATE(A50,"_north")))))</f>
@@ -5010,16 +5037,16 @@
         <v>138</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G51" s="1" t="n">
         <v>255</v>
@@ -5028,7 +5055,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="1" t="n">
-        <v>1990</v>
+        <v>2006</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>30</v>
@@ -5050,7 +5077,7 @@
         <v>5</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q51" s="1" t="n">
         <v>24</v>
@@ -5059,7 +5086,7 @@
         <v>10</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T51" s="1" t="str">
         <f aca="false">IF(NOT(D51="1X1"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c"),IF(E51="landmark",CONCATENATE(A51,"_k"),IF(E51="house",CONCATENATE(A51,"_h"),A51))))</f>
@@ -5067,11 +5094,11 @@
       </c>
       <c r="U51" s="1" t="str">
         <f aca="false">IF(D51="1X1","none",IF(E51="skyscraper",CONCATENATE(A51,"_c_north"),IF(E51="landmark",CONCATENATE(A51,"_k_north"),IF(E51="house",CONCATENATE(A51,"_h_north"),CONCATENATE(A51,"_north")))))</f>
-        <v>yamashiro_office_building_c_north</v>
+        <v>tsuno_building_c_north</v>
       </c>
       <c r="V51" s="1" t="str">
         <f aca="false">IF(OR(D51="1X1",D51="2X1"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_east"),IF(E51="landmark",CONCATENATE(A51,"_k_east"),CONCATENATE(A51,"_east"))))</f>
-        <v>yamashiro_office_building_c_east</v>
+        <v>tsuno_building_c_east</v>
       </c>
       <c r="W51" s="1" t="str">
         <f aca="false">IF(OR(D51="1X1",D51="1X2"),"none",IF(E51="skyscraper",CONCATENATE(A51,"_c_west"),IF(E51="landmark",CONCATENATE(A51,"_k_west"),CONCATENATE(A51,"_west"))))</f>
@@ -5087,34 +5114,34 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H52" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>30</v>
+        <v>1955</v>
+      </c>
+      <c r="J52" s="4" t="n">
+        <v>1989</v>
       </c>
       <c r="K52" s="1" t="n">
         <v>25</v>
@@ -5133,7 +5160,7 @@
         <v>5</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q52" s="1" t="n">
         <v>24</v>
@@ -5142,11 +5169,11 @@
         <v>10</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="T52" s="1" t="str">
         <f aca="false">IF(NOT(D52="1X1"),"none",IF(E52="skyscraper",CONCATENATE(A52,"_c"),IF(E52="landmark",CONCATENATE(A52,"_k"),IF(E52="house",CONCATENATE(A52,"_h"),A52))))</f>
-        <v>yamashita_building_c</v>
+        <v>ueda_office_block_c</v>
       </c>
       <c r="U52" s="1" t="str">
         <f aca="false">IF(D52="1X1","none",IF(E52="skyscraper",CONCATENATE(A52,"_c_north"),IF(E52="landmark",CONCATENATE(A52,"_k_north"),IF(E52="house",CONCATENATE(A52,"_h_north"),CONCATENATE(A52,"_north")))))</f>
@@ -5170,311 +5197,311 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G53" s="1" t="n">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I53" s="1" t="n">
-        <v>1700</v>
+        <v>1965</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K53" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>146</v>
+        <v>39</v>
       </c>
       <c r="M53" s="5" t="str">
         <f aca="false">VLOOKUP(L53,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N53" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O53" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="Q53" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="R53" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="T53" s="1" t="str">
         <f aca="false">IF(NOT(D53="1X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c"),IF(E53="landmark",CONCATENATE(A53,"_k"),IF(E53="house",CONCATENATE(A53,"_h"),A53))))</f>
-        <v>none</v>
+        <v>yamaguchi_office_c</v>
       </c>
       <c r="U53" s="1" t="str">
         <f aca="false">IF(D53="1X1","none",IF(E53="skyscraper",CONCATENATE(A53,"_c_north"),IF(E53="landmark",CONCATENATE(A53,"_k_north"),IF(E53="house",CONCATENATE(A53,"_h_north"),CONCATENATE(A53,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>none</v>
       </c>
       <c r="V53" s="1" t="str">
-        <f aca="false">IF(OR(D53="1X1",D53="2X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_east"),IF(E53="landmark",CONCATENATE(A53,"_k_east"),IF(E53="house",CONCATENATE(A53,"_h_east"),CONCATENATE(A53,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D53="1X1",D53="2X1"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_east"),IF(E53="landmark",CONCATENATE(A53,"_k_east"),CONCATENATE(A53,"_east"))))</f>
+        <v>none</v>
       </c>
       <c r="W53" s="1" t="str">
-        <f aca="false">IF(OR(D53="1X1",D53="1X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_west"),IF(E53="landmark",CONCATENATE(A53,"_k_west"),IF(E53="house",CONCATENATE(A53,"_h_west"),CONCATENATE(A53,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D53="1X1",D53="1X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_west"),IF(E53="landmark",CONCATENATE(A53,"_k_west"),CONCATENATE(A53,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X53" s="1" t="str">
-        <f aca="false">IF(NOT(D53="2X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_south"),IF(E53="landmark",CONCATENATE(A53,"_k_south"),IF(E53="house",CONCATENATE(A53,"_h_south"),CONCATENATE(A53,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D53="2X2"),"none",IF(E53="skyscraper",CONCATENATE(A53,"_c_south"),IF(E53="landmark",CONCATENATE(A53,"_k_south"),CONCATENATE(A53,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y53" s="1" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G54" s="1" t="n">
-        <v>20</v>
+        <v>255</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I54" s="1" t="n">
-        <v>1870</v>
+        <v>1990</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>151</v>
+        <v>39</v>
       </c>
       <c r="M54" s="5" t="str">
         <f aca="false">VLOOKUP(L54,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="N54" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O54" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="Q54" s="1" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="R54" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="T54" s="1" t="str">
         <f aca="false">IF(NOT(D54="1X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c"),IF(E54="landmark",CONCATENATE(A54,"_k"),IF(E54="house",CONCATENATE(A54,"_h"),A54))))</f>
-        <v>naganuma_h</v>
+        <v>none</v>
       </c>
       <c r="U54" s="1" t="str">
         <f aca="false">IF(D54="1X1","none",IF(E54="skyscraper",CONCATENATE(A54,"_c_north"),IF(E54="landmark",CONCATENATE(A54,"_k_north"),IF(E54="house",CONCATENATE(A54,"_h_north"),CONCATENATE(A54,"_north")))))</f>
-        <v>none</v>
+        <v>yamashiro_office_building_c_north</v>
       </c>
       <c r="V54" s="1" t="str">
-        <f aca="false">IF(OR(D54="1X1",D54="2X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_east"),IF(E54="landmark",CONCATENATE(A54,"_k_east"),IF(E54="house",CONCATENATE(A54,"_h_east"),CONCATENATE(A54,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D54="1X1",D54="2X1"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_east"),IF(E54="landmark",CONCATENATE(A54,"_k_east"),CONCATENATE(A54,"_east"))))</f>
+        <v>yamashiro_office_building_c_east</v>
       </c>
       <c r="W54" s="1" t="str">
-        <f aca="false">IF(OR(D54="1X1",D54="1X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_west"),IF(E54="landmark",CONCATENATE(A54,"_k_west"),IF(E54="house",CONCATENATE(A54,"_h_west"),CONCATENATE(A54,"_west")))))</f>
+        <f aca="false">IF(OR(D54="1X1",D54="1X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_west"),IF(E54="landmark",CONCATENATE(A54,"_k_west"),CONCATENATE(A54,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X54" s="1" t="str">
-        <f aca="false">IF(NOT(D54="2X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_south"),IF(E54="landmark",CONCATENATE(A54,"_k_south"),IF(E54="house",CONCATENATE(A54,"_h_south"),CONCATENATE(A54,"_south")))))</f>
+        <f aca="false">IF(NOT(D54="2X2"),"none",IF(E54="skyscraper",CONCATENATE(A54,"_c_south"),IF(E54="landmark",CONCATENATE(A54,"_k_south"),CONCATENATE(A54,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>152</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="C55" s="6" t="n">
-        <v>95</v>
+      <c r="A55" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>47</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G55" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H55" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="H55" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I55" s="0" t="n">
-        <v>1950</v>
+      <c r="I55" s="1" t="n">
+        <v>2000</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="0" t="n">
-        <v>5</v>
+      <c r="K55" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="M55" s="5" t="str">
         <f aca="false">VLOOKUP(L55,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N55" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O55" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
+      </c>
+      <c r="N55" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O55" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q55" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R55" s="0" t="n">
-        <v>3</v>
+        <v>118</v>
+      </c>
+      <c r="Q55" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R55" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="T55" s="1" t="str">
         <f aca="false">IF(NOT(D55="1X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c"),IF(E55="landmark",CONCATENATE(A55,"_k"),IF(E55="house",CONCATENATE(A55,"_h"),A55))))</f>
-        <v>convini_k</v>
+        <v>yamashita_building_c</v>
       </c>
       <c r="U55" s="1" t="str">
         <f aca="false">IF(D55="1X1","none",IF(E55="skyscraper",CONCATENATE(A55,"_c_north"),IF(E55="landmark",CONCATENATE(A55,"_k_north"),IF(E55="house",CONCATENATE(A55,"_h_north"),CONCATENATE(A55,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V55" s="1" t="str">
-        <f aca="false">IF(OR(D55="1X1",D55="2X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_east"),IF(E55="landmark",CONCATENATE(A55,"_k_east"),IF(E55="house",CONCATENATE(A55,"_h_east"),CONCATENATE(A55,"_east")))))</f>
+        <f aca="false">IF(OR(D55="1X1",D55="2X1"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_east"),IF(E55="landmark",CONCATENATE(A55,"_k_east"),CONCATENATE(A55,"_east"))))</f>
         <v>none</v>
       </c>
       <c r="W55" s="1" t="str">
-        <f aca="false">IF(OR(D55="1X1",D55="1X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_west"),IF(E55="landmark",CONCATENATE(A55,"_k_west"),IF(E55="house",CONCATENATE(A55,"_h_west"),CONCATENATE(A55,"_west")))))</f>
+        <f aca="false">IF(OR(D55="1X1",D55="1X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_west"),IF(E55="landmark",CONCATENATE(A55,"_k_west"),CONCATENATE(A55,"_west"))))</f>
         <v>none</v>
       </c>
       <c r="X55" s="1" t="str">
-        <f aca="false">IF(NOT(D55="2X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_south"),IF(E55="landmark",CONCATENATE(A55,"_k_south"),IF(E55="house",CONCATENATE(A55,"_h_south"),CONCATENATE(A55,"_south")))))</f>
-        <v>none</v>
-      </c>
-      <c r="Y55" s="0" t="s">
-        <v>158</v>
+        <f aca="false">IF(NOT(D55="2X2"),"none",IF(E55="skyscraper",CONCATENATE(A55,"_c_south"),IF(E55="landmark",CONCATENATE(A55,"_k_south"),CONCATENATE(A55,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G56" s="1" t="n">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I56" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K56" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="M56" s="5" t="str">
         <f aca="false">VLOOKUP(L56,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N56" s="1" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="O56" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="Q56" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R56" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="T56" s="1" t="str">
         <f aca="false">IF(NOT(D56="1X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c"),IF(E56="landmark",CONCATENATE(A56,"_k"),IF(E56="house",CONCATENATE(A56,"_h"),A56))))</f>
@@ -5482,169 +5509,169 @@
       </c>
       <c r="U56" s="1" t="str">
         <f aca="false">IF(D56="1X1","none",IF(E56="skyscraper",CONCATENATE(A56,"_c_north"),IF(E56="landmark",CONCATENATE(A56,"_k_north"),IF(E56="house",CONCATENATE(A56,"_h_north"),CONCATENATE(A56,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V56" s="1" t="str">
         <f aca="false">IF(OR(D56="1X1",D56="2X1"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_east"),IF(E56="landmark",CONCATENATE(A56,"_k_east"),IF(E56="house",CONCATENATE(A56,"_h_east"),CONCATENATE(A56,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W56" s="1" t="str">
         <f aca="false">IF(OR(D56="1X1",D56="1X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_west"),IF(E56="landmark",CONCATENATE(A56,"_k_west"),IF(E56="house",CONCATENATE(A56,"_h_west"),CONCATENATE(A56,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X56" s="1" t="str">
         <f aca="false">IF(NOT(D56="2X2"),"none",IF(E56="skyscraper",CONCATENATE(A56,"_c_south"),IF(E56="landmark",CONCATENATE(A56,"_k_south"),IF(E56="house",CONCATENATE(A56,"_h_south"),CONCATENATE(A56,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="G57" s="1" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="H57" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K57" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="M57" s="5" t="str">
         <f aca="false">VLOOKUP(L57,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N57" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O57" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="Q57" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R57" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>165</v>
+        <v>33</v>
       </c>
       <c r="T57" s="1" t="str">
         <f aca="false">IF(NOT(D57="1X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c"),IF(E57="landmark",CONCATENATE(A57,"_k"),IF(E57="house",CONCATENATE(A57,"_h"),A57))))</f>
-        <v>none</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U57" s="1" t="str">
         <f aca="false">IF(D57="1X1","none",IF(E57="skyscraper",CONCATENATE(A57,"_c_north"),IF(E57="landmark",CONCATENATE(A57,"_k_north"),IF(E57="house",CONCATENATE(A57,"_h_north"),CONCATENATE(A57,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>none</v>
       </c>
       <c r="V57" s="1" t="str">
-        <f aca="false">IF(OR(D57="1X1",D57="2X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_east"),IF(E57="landmark",CONCATENATE(A57,"_k_east"),CONCATENATE(A57,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D57="1X1",D57="2X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_east"),IF(E57="landmark",CONCATENATE(A57,"_k_east"),IF(E57="house",CONCATENATE(A57,"_h_east"),CONCATENATE(A57,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W57" s="1" t="str">
-        <f aca="false">IF(OR(D57="1X1",D57="1X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_west"),IF(E57="landmark",CONCATENATE(A57,"_k_west"),CONCATENATE(A57,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D57="1X1",D57="1X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_west"),IF(E57="landmark",CONCATENATE(A57,"_k_west"),IF(E57="house",CONCATENATE(A57,"_h_west"),CONCATENATE(A57,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X57" s="1" t="str">
-        <f aca="false">IF(NOT(D57="2X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_south"),IF(E57="landmark",CONCATENATE(A57,"_k_south"),CONCATENATE(A57,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D57="2X2"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c_south"),IF(E57="landmark",CONCATENATE(A57,"_k_south"),IF(E57="house",CONCATENATE(A57,"_h_south"),CONCATENATE(A57,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y57" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C58" s="2" t="n">
-        <v>93</v>
+      <c r="A58" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" s="6" t="n">
+        <v>95</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G58" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H58" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H58" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I58" s="1" t="n">
-        <v>1870</v>
+      <c r="I58" s="0" t="n">
+        <v>1950</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K58" s="1" t="n">
-        <v>10</v>
+      <c r="K58" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="M58" s="5" t="str">
         <f aca="false">VLOOKUP(L58,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
-      <c r="N58" s="1" t="n">
+      <c r="N58" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="O58" s="1" t="n">
+      <c r="O58" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q58" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="R58" s="1" t="n">
-        <v>6</v>
+        <v>154</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R58" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="T58" s="1" t="str">
         <f aca="false">IF(NOT(D58="1X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c"),IF(E58="landmark",CONCATENATE(A58,"_k"),IF(E58="house",CONCATENATE(A58,"_h"),A58))))</f>
-        <v>onsen_k</v>
+        <v>convini_k</v>
       </c>
       <c r="U58" s="1" t="str">
         <f aca="false">IF(D58="1X1","none",IF(E58="skyscraper",CONCATENATE(A58,"_c_north"),IF(E58="landmark",CONCATENATE(A58,"_k_north"),IF(E58="house",CONCATENATE(A58,"_h_north"),CONCATENATE(A58,"_north")))))</f>
@@ -5662,114 +5689,114 @@
         <f aca="false">IF(NOT(D58="2X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_south"),IF(E58="landmark",CONCATENATE(A58,"_k_south"),IF(E58="house",CONCATENATE(A58,"_h_south"),CONCATENATE(A58,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y58" s="1" t="s">
-        <v>158</v>
+      <c r="Y58" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G59" s="1" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H59" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I59" s="1" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="M59" s="5" t="str">
         <f aca="false">VLOOKUP(L59,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N59" s="1" t="n">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="O59" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R59" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="T59" s="1" t="str">
         <f aca="false">IF(NOT(D59="1X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c"),IF(E59="landmark",CONCATENATE(A59,"_k"),IF(E59="house",CONCATENATE(A59,"_h"),A59))))</f>
-        <v>pachinko_k</v>
+        <v>none</v>
       </c>
       <c r="U59" s="1" t="str">
         <f aca="false">IF(D59="1X1","none",IF(E59="skyscraper",CONCATENATE(A59,"_c_north"),IF(E59="landmark",CONCATENATE(A59,"_k_north"),IF(E59="house",CONCATENATE(A59,"_h_north"),CONCATENATE(A59,"_north")))))</f>
-        <v>none</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V59" s="1" t="str">
-        <f aca="false">IF(OR(D59="1X1",D59="2X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_east"),IF(E59="landmark",CONCATENATE(A59,"_k_east"),CONCATENATE(A59,"_east"))))</f>
+        <f aca="false">IF(OR(D59="1X1",D59="2X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_east"),IF(E59="landmark",CONCATENATE(A59,"_k_east"),IF(E59="house",CONCATENATE(A59,"_h_east"),CONCATENATE(A59,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W59" s="1" t="str">
-        <f aca="false">IF(OR(D59="1X1",D59="1X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_west"),IF(E59="landmark",CONCATENATE(A59,"_k_west"),CONCATENATE(A59,"_west"))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D59="1X1",D59="1X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_west"),IF(E59="landmark",CONCATENATE(A59,"_k_west"),IF(E59="house",CONCATENATE(A59,"_h_west"),CONCATENATE(A59,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X59" s="1" t="str">
-        <f aca="false">IF(NOT(D59="2X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_south"),IF(E59="landmark",CONCATENATE(A59,"_k_south"),CONCATENATE(A59,"_south"))))</f>
+        <f aca="false">IF(NOT(D59="2X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_south"),IF(E59="landmark",CONCATENATE(A59,"_k_south"),IF(E59="house",CONCATENATE(A59,"_h_south"),CONCATENATE(A59,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C60" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="G60" s="1" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="H60" s="1" t="n">
         <v>3</v>
@@ -5784,29 +5811,29 @@
         <v>20</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="M60" s="5" t="str">
         <f aca="false">VLOOKUP(L60,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N60" s="1" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O60" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="Q60" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R60" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>114</v>
+        <v>172</v>
       </c>
       <c r="T60" s="1" t="str">
         <f aca="false">IF(NOT(D60="1X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c"),IF(E60="landmark",CONCATENATE(A60,"_k"),IF(E60="house",CONCATENATE(A60,"_h"),A60))))</f>
@@ -5814,39 +5841,39 @@
       </c>
       <c r="U60" s="1" t="str">
         <f aca="false">IF(D60="1X1","none",IF(E60="skyscraper",CONCATENATE(A60,"_c_north"),IF(E60="landmark",CONCATENATE(A60,"_k_north"),IF(E60="house",CONCATENATE(A60,"_h_north"),CONCATENATE(A60,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V60" s="1" t="str">
         <f aca="false">IF(OR(D60="1X1",D60="2X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_east"),IF(E60="landmark",CONCATENATE(A60,"_k_east"),CONCATENATE(A60,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W60" s="1" t="str">
         <f aca="false">IF(OR(D60="1X1",D60="1X2"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_west"),IF(E60="landmark",CONCATENATE(A60,"_k_west"),CONCATENATE(A60,"_west"))))</f>
-        <v>none</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X60" s="1" t="str">
         <f aca="false">IF(NOT(D60="2X2"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c_south"),IF(E60="landmark",CONCATENATE(A60,"_k_south"),CONCATENATE(A60,"_south"))))</f>
-        <v>none</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y60" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>216</v>
+        <v>93</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>173</v>
@@ -5854,65 +5881,65 @@
       <c r="G61" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H61" s="0" t="n">
-        <v>3</v>
+      <c r="H61" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>1700</v>
+        <v>1870</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K61" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M61" s="5" t="str">
         <f aca="false">VLOOKUP(L61,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N61" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O61" s="0" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N61" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O61" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="Q61" s="1" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="R61" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="T61" s="1" t="str">
         <f aca="false">IF(NOT(D61="1X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c"),IF(E61="landmark",CONCATENATE(A61,"_k"),IF(E61="house",CONCATENATE(A61,"_h"),A61))))</f>
-        <v>none</v>
+        <v>onsen_k</v>
       </c>
       <c r="U61" s="1" t="str">
         <f aca="false">IF(D61="1X1","none",IF(E61="skyscraper",CONCATENATE(A61,"_c_north"),IF(E61="landmark",CONCATENATE(A61,"_k_north"),IF(E61="house",CONCATENATE(A61,"_h_north"),CONCATENATE(A61,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>none</v>
       </c>
       <c r="V61" s="1" t="str">
-        <f aca="false">IF(OR(D61="1X1",D61="2X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_east"),IF(E61="landmark",CONCATENATE(A61,"_k_east"),CONCATENATE(A61,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <f aca="false">IF(OR(D61="1X1",D61="2X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_east"),IF(E61="landmark",CONCATENATE(A61,"_k_east"),IF(E61="house",CONCATENATE(A61,"_h_east"),CONCATENATE(A61,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W61" s="1" t="str">
-        <f aca="false">IF(OR(D61="1X1",D61="1X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_west"),IF(E61="landmark",CONCATENATE(A61,"_k_west"),CONCATENATE(A61,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <f aca="false">IF(OR(D61="1X1",D61="1X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_west"),IF(E61="landmark",CONCATENATE(A61,"_k_west"),IF(E61="house",CONCATENATE(A61,"_h_west"),CONCATENATE(A61,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X61" s="1" t="str">
-        <f aca="false">IF(NOT(D61="2X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_south"),IF(E61="landmark",CONCATENATE(A61,"_k_south"),CONCATENATE(A61,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <f aca="false">IF(NOT(D61="2X2"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c_south"),IF(E61="landmark",CONCATENATE(A61,"_k_south"),IF(E61="house",CONCATENATE(A61,"_h_south"),CONCATENATE(A61,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y61" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5923,60 +5950,60 @@
         <v>174</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>175</v>
       </c>
       <c r="G62" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H62" s="0" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I62" s="1" t="n">
-        <v>0</v>
+        <v>1980</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K62" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>176</v>
+        <v>56</v>
       </c>
       <c r="M62" s="5" t="str">
         <f aca="false">VLOOKUP(L62,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N62" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O62" s="0" t="n">
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N62" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O62" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="Q62" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R62" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T62" s="1" t="str">
         <f aca="false">IF(NOT(D62="1X1"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c"),IF(E62="landmark",CONCATENATE(A62,"_k"),IF(E62="house",CONCATENATE(A62,"_h"),A62))))</f>
-        <v>shrine_k</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U62" s="1" t="str">
         <f aca="false">IF(D62="1X1","none",IF(E62="skyscraper",CONCATENATE(A62,"_c_north"),IF(E62="landmark",CONCATENATE(A62,"_k_north"),IF(E62="house",CONCATENATE(A62,"_h_north"),CONCATENATE(A62,"_north")))))</f>
@@ -6000,31 +6027,31 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C63" s="2" t="n">
-        <v>113</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="G63" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>5</v>
+        <v>80</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I63" s="1" t="n">
-        <v>0</v>
+        <v>1970</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>30</v>
@@ -6033,41 +6060,41 @@
         <v>20</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="M63" s="5" t="str">
         <f aca="false">VLOOKUP(L63,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N63" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O63" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N63" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O63" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="Q63" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R63" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="T63" s="1" t="str">
         <f aca="false">IF(NOT(D63="1X1"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c"),IF(E63="landmark",CONCATENATE(A63,"_k"),IF(E63="house",CONCATENATE(A63,"_h"),A63))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>none</v>
       </c>
       <c r="U63" s="1" t="str">
         <f aca="false">IF(D63="1X1","none",IF(E63="skyscraper",CONCATENATE(A63,"_c_north"),IF(E63="landmark",CONCATENATE(A63,"_k_north"),IF(E63="house",CONCATENATE(A63,"_h_north"),CONCATENATE(A63,"_north")))))</f>
-        <v>none</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V63" s="1" t="str">
         <f aca="false">IF(OR(D63="1X1",D63="2X1"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c_east"),IF(E63="landmark",CONCATENATE(A63,"_k_east"),CONCATENATE(A63,"_east"))))</f>
-        <v>none</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W63" s="1" t="str">
         <f aca="false">IF(OR(D63="1X1",D63="1X2"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c_west"),IF(E63="landmark",CONCATENATE(A63,"_k_west"),CONCATENATE(A63,"_west"))))</f>
@@ -6078,36 +6105,36 @@
         <v>none</v>
       </c>
       <c r="Y63" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C64" s="2" t="n">
-        <v>204</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="G64" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H64" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H64" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I64" s="1" t="n">
-        <v>1970</v>
+        <v>1700</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>30</v>
@@ -6116,29 +6143,29 @@
         <v>20</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="M64" s="5" t="str">
         <f aca="false">VLOOKUP(L64,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
-      <c r="N64" s="1" t="n">
+      <c r="N64" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O64" s="1" t="n">
+      <c r="O64" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="Q64" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R64" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="T64" s="1" t="str">
         <f aca="false">IF(NOT(D64="1X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c"),IF(E64="landmark",CONCATENATE(A64,"_k"),IF(E64="house",CONCATENATE(A64,"_h"),A64))))</f>
@@ -6146,51 +6173,51 @@
       </c>
       <c r="U64" s="1" t="str">
         <f aca="false">IF(D64="1X1","none",IF(E64="skyscraper",CONCATENATE(A64,"_c_north"),IF(E64="landmark",CONCATENATE(A64,"_k_north"),IF(E64="house",CONCATENATE(A64,"_h_north"),CONCATENATE(A64,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V64" s="1" t="str">
         <f aca="false">IF(OR(D64="1X1",D64="2X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_east"),IF(E64="landmark",CONCATENATE(A64,"_k_east"),CONCATENATE(A64,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W64" s="1" t="str">
         <f aca="false">IF(OR(D64="1X1",D64="1X2"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_west"),IF(E64="landmark",CONCATENATE(A64,"_k_west"),CONCATENATE(A64,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X64" s="1" t="str">
         <f aca="false">IF(NOT(D64="2X2"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_south"),IF(E64="landmark",CONCATENATE(A64,"_k_south"),CONCATENATE(A64,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y64" s="1" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C65" s="2" t="n">
-        <v>208</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="G65" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H65" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I65" s="1" t="n">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>30</v>
@@ -6199,82 +6226,331 @@
         <v>20</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="M65" s="5" t="str">
         <f aca="false">VLOOKUP(L65,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
-      <c r="N65" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O65" s="1" t="n">
+      <c r="N65" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O65" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="Q65" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R65" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="T65" s="1" t="str">
         <f aca="false">IF(NOT(D65="1X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c"),IF(E65="landmark",CONCATENATE(A65,"_k"),IF(E65="house",CONCATENATE(A65,"_h"),A65))))</f>
-        <v>none</v>
+        <v>shrine_k</v>
       </c>
       <c r="U65" s="1" t="str">
         <f aca="false">IF(D65="1X1","none",IF(E65="skyscraper",CONCATENATE(A65,"_c_north"),IF(E65="landmark",CONCATENATE(A65,"_k_north"),IF(E65="house",CONCATENATE(A65,"_h_north"),CONCATENATE(A65,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>none</v>
       </c>
       <c r="V65" s="1" t="str">
         <f aca="false">IF(OR(D65="1X1",D65="2X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_east"),IF(E65="landmark",CONCATENATE(A65,"_k_east"),CONCATENATE(A65,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>none</v>
       </c>
       <c r="W65" s="1" t="str">
         <f aca="false">IF(OR(D65="1X1",D65="1X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_west"),IF(E65="landmark",CONCATENATE(A65,"_k_west"),CONCATENATE(A65,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X65" s="1" t="str">
         <f aca="false">IF(NOT(D65="2X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_south"),IF(E65="landmark",CONCATENATE(A65,"_k_south"),CONCATENATE(A65,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y65" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K66" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="M66" s="5" t="str">
+        <f aca="false">VLOOKUP(L66,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N66" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O66" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P66" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="T66" s="1" t="str">
+        <f aca="false">IF(NOT(D66="1X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c"),IF(E66="landmark",CONCATENATE(A66,"_k"),IF(E66="house",CONCATENATE(A66,"_h"),A66))))</f>
+        <v>shrine_prohibition_k</v>
+      </c>
+      <c r="U66" s="1" t="str">
+        <f aca="false">IF(D66="1X1","none",IF(E66="skyscraper",CONCATENATE(A66,"_c_north"),IF(E66="landmark",CONCATENATE(A66,"_k_north"),IF(E66="house",CONCATENATE(A66,"_h_north"),CONCATENATE(A66,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V66" s="1" t="str">
+        <f aca="false">IF(OR(D66="1X1",D66="2X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_east"),IF(E66="landmark",CONCATENATE(A66,"_k_east"),CONCATENATE(A66,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W66" s="1" t="str">
+        <f aca="false">IF(OR(D66="1X1",D66="1X2"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_west"),IF(E66="landmark",CONCATENATE(A66,"_k_west"),CONCATENATE(A66,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X66" s="1" t="str">
+        <f aca="false">IF(NOT(D66="2X2"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_south"),IF(E66="landmark",CONCATENATE(A66,"_k_south"),CONCATENATE(A66,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y66" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G67" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H67" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K67" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M67" s="5" t="str">
+        <f aca="false">VLOOKUP(L67,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N67" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O67" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P67" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q67" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R67" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S67" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="T67" s="1" t="str">
+        <f aca="false">IF(NOT(D67="1X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c"),IF(E67="landmark",CONCATENATE(A67,"_k"),IF(E67="house",CONCATENATE(A67,"_h"),A67))))</f>
+        <v>none</v>
+      </c>
+      <c r="U67" s="1" t="str">
+        <f aca="false">IF(D67="1X1","none",IF(E67="skyscraper",CONCATENATE(A67,"_c_north"),IF(E67="landmark",CONCATENATE(A67,"_k_north"),IF(E67="house",CONCATENATE(A67,"_h_north"),CONCATENATE(A67,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V67" s="1" t="str">
+        <f aca="false">IF(OR(D67="1X1",D67="2X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_east"),IF(E67="landmark",CONCATENATE(A67,"_k_east"),CONCATENATE(A67,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W67" s="1" t="str">
+        <f aca="false">IF(OR(D67="1X1",D67="1X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_west"),IF(E67="landmark",CONCATENATE(A67,"_k_west"),CONCATENATE(A67,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X67" s="1" t="str">
+        <f aca="false">IF(NOT(D67="2X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_south"),IF(E67="landmark",CONCATENATE(A67,"_k_south"),CONCATENATE(A67,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y67" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G68" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H68" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="M68" s="5" t="str">
+        <f aca="false">VLOOKUP(L68,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N68" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O68" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P68" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q68" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R68" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="T68" s="1" t="str">
+        <f aca="false">IF(NOT(D68="1X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c"),IF(E68="landmark",CONCATENATE(A68,"_k"),IF(E68="house",CONCATENATE(A68,"_h"),A68))))</f>
+        <v>none</v>
+      </c>
+      <c r="U68" s="1" t="str">
+        <f aca="false">IF(D68="1X1","none",IF(E68="skyscraper",CONCATENATE(A68,"_c_north"),IF(E68="landmark",CONCATENATE(A68,"_k_north"),IF(E68="house",CONCATENATE(A68,"_h_north"),CONCATENATE(A68,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V68" s="1" t="str">
+        <f aca="false">IF(OR(D68="1X1",D68="2X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_east"),IF(E68="landmark",CONCATENATE(A68,"_k_east"),CONCATENATE(A68,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W68" s="1" t="str">
+        <f aca="false">IF(OR(D68="1X1",D68="1X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_west"),IF(E68="landmark",CONCATENATE(A68,"_k_west"),CONCATENATE(A68,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X68" s="1" t="str">
+        <f aca="false">IF(NOT(D68="2X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_south"),IF(E68="landmark",CONCATENATE(A68,"_k_south"),CONCATENATE(A68,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y65" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0"/>
-      <c r="D66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="5"/>
-      <c r="P66" s="3"/>
-      <c r="S66" s="3"/>
+      <c r="Y68" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0"/>
+      <c r="D69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="5"/>
+      <c r="P69" s="3"/>
+      <c r="S69" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C54 C56:C1048576">
+  <conditionalFormatting sqref="C1:C57 C59:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E37" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E40" type="list">
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L66" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L69" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P66" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P69" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S66" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S69" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6304,16 +6580,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7767,11 +8043,11 @@
       </c>
       <c r="B87" s="1" t="str">
         <f aca="false">IF(C87="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C87" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A87,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D87" s="1" t="n">
         <f aca="false">IF(C87="Multi-tile",D86-1,MAX(IF(C87="ID not in use",0,IF(C87="1X1",1,IF(C87="2X2",4,2)))-1,0))</f>
@@ -7869,11 +8145,11 @@
       </c>
       <c r="B93" s="1" t="str">
         <f aca="false">IF(C93="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C93" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A93,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D93" s="1" t="n">
         <f aca="false">IF(C93="Multi-tile",D92-1,MAX(IF(C93="ID not in use",0,IF(C93="1X1",1,IF(C93="2X2",4,2)))-1,0))</f>
@@ -7920,11 +8196,11 @@
       </c>
       <c r="B96" s="1" t="str">
         <f aca="false">IF(C96="ID not in use","ID not in use","Used")</f>
-        <v>ID not in use</v>
+        <v>Used</v>
       </c>
       <c r="C96" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A96,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="D96" s="1" t="n">
         <f aca="false">IF(C96="Multi-tile",D95-1,MAX(IF(C96="ID not in use",0,IF(C96="1X1",1,IF(C96="2X2",4,2)))-1,0))</f>
@@ -10702,25 +10978,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10734,13 +11010,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -10763,10 +11039,10 @@
         <v>56</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10780,16 +11056,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10797,73 +11073,73 @@
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: large_wooden_farmhouse & wooden_farmhouse
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="233">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -510,6 +510,12 @@
     <t xml:space="preserve">[PASS, 1],[MAIL, 1],[FOOD, 1]</t>
   </si>
   <si>
+    <t xml:space="preserve">large_wooden_farmhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_LARGE_WOODEN_FARMHOUSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">naganuma</t>
   </si>
   <si>
@@ -538,6 +544,12 @@
   </si>
   <si>
     <t xml:space="preserve">[PASS, 2],[MAIL, 1],[FOOD, 2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wooden_farmhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_WOODEN_FARMHOUSE</t>
   </si>
   <si>
     <t xml:space="preserve">wooden_house</t>
@@ -938,14 +950,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y74"/>
+  <dimension ref="A1:Y76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="bottomRight" activeCell="K63" activeCellId="0" sqref="K63"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5844,7 +5856,7 @@
         <v>162</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>27</v>
@@ -5859,23 +5871,23 @@
         <v>20</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I59" s="4" t="n">
-        <v>1870</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>30</v>
+        <v>1700</v>
+      </c>
+      <c r="J59" s="6" t="n">
+        <v>1944</v>
       </c>
       <c r="K59" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="M59" s="8" t="str">
         <f aca="false">VLOOKUP(L59,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N59" s="1" t="n">
         <v>6</v>
@@ -5887,7 +5899,7 @@
         <v>32</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R59" s="1" t="n">
         <v>1</v>
@@ -5897,7 +5909,7 @@
       </c>
       <c r="T59" s="1" t="str">
         <f aca="false">IF(NOT(D59="1X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c"),IF(E59="landmark",CONCATENATE(A59,"_k"),IF(E59="house",CONCATENATE(A59,"_h"),A59))))</f>
-        <v>naganuma_h</v>
+        <v>large_wooden_farmhouse_h</v>
       </c>
       <c r="U59" s="1" t="str">
         <f aca="false">IF(D59="1X1","none",IF(E59="skyscraper",CONCATENATE(A59,"_c_north"),IF(E59="landmark",CONCATENATE(A59,"_k_north"),IF(E59="house",CONCATENATE(A59,"_h_north"),CONCATENATE(A59,"_north")))))</f>
@@ -5916,18 +5928,18 @@
         <v>none</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>27</v>
@@ -5936,7 +5948,7 @@
         <v>154</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G60" s="1" t="n">
         <v>20</v>
@@ -5954,7 +5966,7 @@
         <v>5</v>
       </c>
       <c r="L60" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="M60" s="8" t="str">
         <f aca="false">VLOOKUP(L60,dropdowns!E:F,2,0)</f>
@@ -5980,7 +5992,7 @@
       </c>
       <c r="T60" s="1" t="str">
         <f aca="false">IF(NOT(D60="1X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c"),IF(E60="landmark",CONCATENATE(A60,"_k"),IF(E60="house",CONCATENATE(A60,"_h"),A60))))</f>
-        <v>nishikawa_h</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U60" s="1" t="str">
         <f aca="false">IF(D60="1X1","none",IF(E60="skyscraper",CONCATENATE(A60,"_c_north"),IF(E60="landmark",CONCATENATE(A60,"_k_north"),IF(E60="house",CONCATENATE(A60,"_h_north"),CONCATENATE(A60,"_north")))))</f>
@@ -5999,7 +6011,7 @@
         <v>none</v>
       </c>
       <c r="Y60" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6010,7 +6022,7 @@
         <v>168</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>27</v>
@@ -6025,26 +6037,26 @@
         <v>20</v>
       </c>
       <c r="H61" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I61" s="4" t="n">
-        <v>1700</v>
-      </c>
-      <c r="J61" s="6" t="n">
-        <v>1944</v>
+        <v>1870</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K61" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M61" s="8" t="str">
         <f aca="false">VLOOKUP(L61,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N61" s="1" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="O61" s="1" t="n">
         <v>0</v>
@@ -6059,11 +6071,11 @@
         <v>1</v>
       </c>
       <c r="S61" s="5" t="s">
-        <v>171</v>
+        <v>33</v>
       </c>
       <c r="T61" s="1" t="str">
         <f aca="false">IF(NOT(D61="1X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c"),IF(E61="landmark",CONCATENATE(A61,"_k"),IF(E61="house",CONCATENATE(A61,"_h"),A61))))</f>
-        <v>old_villa_h</v>
+        <v>nishikawa_h</v>
       </c>
       <c r="U61" s="1" t="str">
         <f aca="false">IF(D61="1X1","none",IF(E61="skyscraper",CONCATENATE(A61,"_c_north"),IF(E61="landmark",CONCATENATE(A61,"_k_north"),IF(E61="house",CONCATENATE(A61,"_h_north"),CONCATENATE(A61,"_north")))))</f>
@@ -6082,18 +6094,18 @@
         <v>none</v>
       </c>
       <c r="Y61" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>27</v>
@@ -6102,7 +6114,7 @@
         <v>154</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G62" s="1" t="n">
         <v>20</v>
@@ -6120,14 +6132,14 @@
         <v>5</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="M62" s="8" t="str">
         <f aca="false">VLOOKUP(L62,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_EDGE )</v>
       </c>
       <c r="N62" s="1" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="O62" s="1" t="n">
         <v>0</v>
@@ -6136,17 +6148,17 @@
         <v>32</v>
       </c>
       <c r="Q62" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R62" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S62" s="5" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
       <c r="T62" s="1" t="str">
         <f aca="false">IF(NOT(D62="1X1"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c"),IF(E62="landmark",CONCATENATE(A62,"_k"),IF(E62="house",CONCATENATE(A62,"_h"),A62))))</f>
-        <v>wooden_house_h</v>
+        <v>old_villa_h</v>
       </c>
       <c r="U62" s="1" t="str">
         <f aca="false">IF(D62="1X1","none",IF(E62="skyscraper",CONCATENATE(A62,"_c_north"),IF(E62="landmark",CONCATENATE(A62,"_k_north"),IF(E62="house",CONCATENATE(A62,"_h_north"),CONCATENATE(A62,"_north")))))</f>
@@ -6169,67 +6181,67 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="3" t="n">
-        <v>95</v>
+      <c r="C63" s="2" t="n">
+        <v>9</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G63" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I63" s="3" t="n">
-        <v>1950</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K63" s="0" t="n">
+      <c r="G63" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" s="4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J63" s="6" t="n">
+        <v>1944</v>
+      </c>
+      <c r="K63" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="M63" s="8" t="str">
         <f aca="false">VLOOKUP(L63,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N63" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O63" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N63" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O63" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q63" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R63" s="0" t="n">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="Q63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R63" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="S63" s="5" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="T63" s="1" t="str">
         <f aca="false">IF(NOT(D63="1X1"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c"),IF(E63="landmark",CONCATENATE(A63,"_k"),IF(E63="house",CONCATENATE(A63,"_h"),A63))))</f>
-        <v>convini_k</v>
+        <v>wooden_farmhouse_h</v>
       </c>
       <c r="U63" s="1" t="str">
         <f aca="false">IF(D63="1X1","none",IF(E63="skyscraper",CONCATENATE(A63,"_c_north"),IF(E63="landmark",CONCATENATE(A63,"_k_north"),IF(E63="house",CONCATENATE(A63,"_h_north"),CONCATENATE(A63,"_north")))))</f>
@@ -6247,76 +6259,76 @@
         <f aca="false">IF(NOT(D63="2X2"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c_south"),IF(E63="landmark",CONCATENATE(A63,"_k_south"),IF(E63="house",CONCATENATE(A63,"_h_south"),CONCATENATE(A63,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y63" s="0" t="s">
-        <v>179</v>
+      <c r="Y63" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>181</v>
+        <v>27</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G64" s="1" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H64" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I64" s="4" t="n">
-        <v>1970</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>30</v>
+        <v>1700</v>
+      </c>
+      <c r="J64" s="6" t="n">
+        <v>1944</v>
       </c>
       <c r="K64" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="M64" s="8" t="str">
         <f aca="false">VLOOKUP(L64,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N64" s="1" t="n">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="O64" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P64" s="5" t="s">
-        <v>160</v>
+        <v>32</v>
       </c>
       <c r="Q64" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R64" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S64" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T64" s="1" t="str">
         <f aca="false">IF(NOT(D64="1X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c"),IF(E64="landmark",CONCATENATE(A64,"_k"),IF(E64="house",CONCATENATE(A64,"_h"),A64))))</f>
-        <v>none</v>
+        <v>wooden_house_h</v>
       </c>
       <c r="U64" s="1" t="str">
         <f aca="false">IF(D64="1X1","none",IF(E64="skyscraper",CONCATENATE(A64,"_c_north"),IF(E64="landmark",CONCATENATE(A64,"_k_north"),IF(E64="house",CONCATENATE(A64,"_h_north"),CONCATENATE(A64,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V64" s="1" t="str">
         <f aca="false">IF(OR(D64="1X1",D64="2X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_east"),IF(E64="landmark",CONCATENATE(A64,"_k_east"),IF(E64="house",CONCATENATE(A64,"_h_east"),CONCATENATE(A64,"_east")))))</f>
@@ -6324,142 +6336,142 @@
       </c>
       <c r="W64" s="1" t="str">
         <f aca="false">IF(OR(D64="1X1",D64="1X2"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_west"),IF(E64="landmark",CONCATENATE(A64,"_k_west"),IF(E64="house",CONCATENATE(A64,"_h_west"),CONCATENATE(A64,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>none</v>
       </c>
       <c r="X64" s="1" t="str">
         <f aca="false">IF(NOT(D64="2X2"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c_south"),IF(E64="landmark",CONCATENATE(A64,"_k_south"),IF(E64="house",CONCATENATE(A64,"_h_south"),CONCATENATE(A64,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y64" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C65" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C65" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G65" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H65" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I65" s="4" t="n">
-        <v>1970</v>
+      <c r="G65" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" s="3" t="n">
+        <v>1950</v>
       </c>
       <c r="J65" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K65" s="1" t="n">
-        <v>20</v>
+      <c r="K65" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M65" s="8" t="str">
         <f aca="false">VLOOKUP(L65,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N65" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O65" s="1" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N65" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="O65" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P65" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="Q65" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="R65" s="1" t="n">
-        <v>4</v>
+      <c r="Q65" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R65" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="S65" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="T65" s="1" t="str">
         <f aca="false">IF(NOT(D65="1X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c"),IF(E65="landmark",CONCATENATE(A65,"_k"),IF(E65="house",CONCATENATE(A65,"_h"),A65))))</f>
-        <v>none</v>
+        <v>convini_k</v>
       </c>
       <c r="U65" s="1" t="str">
         <f aca="false">IF(D65="1X1","none",IF(E65="skyscraper",CONCATENATE(A65,"_c_north"),IF(E65="landmark",CONCATENATE(A65,"_k_north"),IF(E65="house",CONCATENATE(A65,"_h_north"),CONCATENATE(A65,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>none</v>
       </c>
       <c r="V65" s="1" t="str">
-        <f aca="false">IF(OR(D65="1X1",D65="2X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_east"),IF(E65="landmark",CONCATENATE(A65,"_k_east"),CONCATENATE(A65,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D65="1X1",D65="2X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_east"),IF(E65="landmark",CONCATENATE(A65,"_k_east"),IF(E65="house",CONCATENATE(A65,"_h_east"),CONCATENATE(A65,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W65" s="1" t="str">
-        <f aca="false">IF(OR(D65="1X1",D65="1X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_west"),IF(E65="landmark",CONCATENATE(A65,"_k_west"),CONCATENATE(A65,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D65="1X1",D65="1X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_west"),IF(E65="landmark",CONCATENATE(A65,"_k_west"),IF(E65="house",CONCATENATE(A65,"_h_west"),CONCATENATE(A65,"_west")))))</f>
+        <v>none</v>
       </c>
       <c r="X65" s="1" t="str">
-        <f aca="false">IF(NOT(D65="2X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_south"),IF(E65="landmark",CONCATENATE(A65,"_k_south"),CONCATENATE(A65,"_south"))))</f>
-        <v>hospital_k_south</v>
-      </c>
-      <c r="Y65" s="1" t="s">
+        <f aca="false">IF(NOT(D65="2X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_south"),IF(E65="landmark",CONCATENATE(A65,"_k_south"),IF(E65="house",CONCATENATE(A65,"_h_south"),CONCATENATE(A65,"_south")))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y65" s="0" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C66" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="F66" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G66" s="1" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I66" s="4" t="n">
-        <v>1870</v>
+        <v>1970</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K66" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="M66" s="8" t="str">
         <f aca="false">VLOOKUP(L66,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N66" s="1" t="n">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="O66" s="1" t="n">
         <v>3</v>
@@ -6468,21 +6480,21 @@
         <v>160</v>
       </c>
       <c r="Q66" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="R66" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S66" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T66" s="1" t="str">
         <f aca="false">IF(NOT(D66="1X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c"),IF(E66="landmark",CONCATENATE(A66,"_k"),IF(E66="house",CONCATENATE(A66,"_h"),A66))))</f>
-        <v>onsen_k</v>
+        <v>none</v>
       </c>
       <c r="U66" s="1" t="str">
         <f aca="false">IF(D66="1X1","none",IF(E66="skyscraper",CONCATENATE(A66,"_c_north"),IF(E66="landmark",CONCATENATE(A66,"_k_north"),IF(E66="house",CONCATENATE(A66,"_h_north"),CONCATENATE(A66,"_north")))))</f>
-        <v>none</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V66" s="1" t="str">
         <f aca="false">IF(OR(D66="1X1",D66="2X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_east"),IF(E66="landmark",CONCATENATE(A66,"_k_east"),IF(E66="house",CONCATENATE(A66,"_h_east"),CONCATENATE(A66,"_east")))))</f>
@@ -6490,59 +6502,59 @@
       </c>
       <c r="W66" s="1" t="str">
         <f aca="false">IF(OR(D66="1X1",D66="1X2"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_west"),IF(E66="landmark",CONCATENATE(A66,"_k_west"),IF(E66="house",CONCATENATE(A66,"_h_west"),CONCATENATE(A66,"_west")))))</f>
-        <v>none</v>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X66" s="1" t="str">
         <f aca="false">IF(NOT(D66="2X2"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_south"),IF(E66="landmark",CONCATENATE(A66,"_k_south"),IF(E66="house",CONCATENATE(A66,"_h_south"),CONCATENATE(A66,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y66" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C67" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="G67" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I67" s="4" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="J67" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K67" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="M67" s="8" t="str">
         <f aca="false">VLOOKUP(L67,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N67" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O67" s="1" t="n">
         <v>3</v>
@@ -6551,81 +6563,81 @@
         <v>160</v>
       </c>
       <c r="Q67" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R67" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S67" s="5" t="s">
         <v>190</v>
       </c>
       <c r="T67" s="1" t="str">
         <f aca="false">IF(NOT(D67="1X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c"),IF(E67="landmark",CONCATENATE(A67,"_k"),IF(E67="house",CONCATENATE(A67,"_h"),A67))))</f>
-        <v>pachinko_k</v>
+        <v>none</v>
       </c>
       <c r="U67" s="1" t="str">
         <f aca="false">IF(D67="1X1","none",IF(E67="skyscraper",CONCATENATE(A67,"_c_north"),IF(E67="landmark",CONCATENATE(A67,"_k_north"),IF(E67="house",CONCATENATE(A67,"_h_north"),CONCATENATE(A67,"_north")))))</f>
-        <v>none</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V67" s="1" t="str">
         <f aca="false">IF(OR(D67="1X1",D67="2X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_east"),IF(E67="landmark",CONCATENATE(A67,"_k_east"),CONCATENATE(A67,"_east"))))</f>
-        <v>none</v>
+        <v>hospital_k_east</v>
       </c>
       <c r="W67" s="1" t="str">
         <f aca="false">IF(OR(D67="1X1",D67="1X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_west"),IF(E67="landmark",CONCATENATE(A67,"_k_west"),CONCATENATE(A67,"_west"))))</f>
-        <v>none</v>
+        <v>hospital_k_west</v>
       </c>
       <c r="X67" s="1" t="str">
         <f aca="false">IF(NOT(D67="2X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_south"),IF(E67="landmark",CONCATENATE(A67,"_k_south"),CONCATENATE(A67,"_south"))))</f>
-        <v>none</v>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y67" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C68" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="G68" s="1" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I68" s="4" t="n">
-        <v>1970</v>
+        <v>1870</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K68" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="M68" s="8" t="str">
         <f aca="false">VLOOKUP(L68,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
       <c r="N68" s="1" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="O68" s="1" t="n">
         <v>3</v>
@@ -6634,119 +6646,119 @@
         <v>160</v>
       </c>
       <c r="Q68" s="1" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="R68" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="T68" s="1" t="str">
         <f aca="false">IF(NOT(D68="1X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c"),IF(E68="landmark",CONCATENATE(A68,"_k"),IF(E68="house",CONCATENATE(A68,"_h"),A68))))</f>
-        <v>none</v>
+        <v>onsen_k</v>
       </c>
       <c r="U68" s="1" t="str">
         <f aca="false">IF(D68="1X1","none",IF(E68="skyscraper",CONCATENATE(A68,"_c_north"),IF(E68="landmark",CONCATENATE(A68,"_k_north"),IF(E68="house",CONCATENATE(A68,"_h_north"),CONCATENATE(A68,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V68" s="1" t="str">
-        <f aca="false">IF(OR(D68="1X1",D68="2X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_east"),IF(E68="landmark",CONCATENATE(A68,"_k_east"),CONCATENATE(A68,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <f aca="false">IF(OR(D68="1X1",D68="2X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_east"),IF(E68="landmark",CONCATENATE(A68,"_k_east"),IF(E68="house",CONCATENATE(A68,"_h_east"),CONCATENATE(A68,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W68" s="1" t="str">
-        <f aca="false">IF(OR(D68="1X1",D68="1X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_west"),IF(E68="landmark",CONCATENATE(A68,"_k_west"),CONCATENATE(A68,"_west"))))</f>
+        <f aca="false">IF(OR(D68="1X1",D68="1X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_west"),IF(E68="landmark",CONCATENATE(A68,"_k_west"),IF(E68="house",CONCATENATE(A68,"_h_west"),CONCATENATE(A68,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X68" s="1" t="str">
-        <f aca="false">IF(NOT(D68="2X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_south"),IF(E68="landmark",CONCATENATE(A68,"_k_south"),CONCATENATE(A68,"_south"))))</f>
+        <f aca="false">IF(NOT(D68="2X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_south"),IF(E68="landmark",CONCATENATE(A68,"_k_south"),IF(E68="house",CONCATENATE(A68,"_h_south"),CONCATENATE(A68,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y68" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C69" s="2" t="n">
-        <v>216</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="G69" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H69" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H69" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I69" s="4" t="n">
-        <v>1700</v>
+        <v>1980</v>
       </c>
       <c r="J69" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K69" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="M69" s="8" t="str">
         <f aca="false">VLOOKUP(L69,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N69" s="0" t="n">
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+      </c>
+      <c r="N69" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O69" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q69" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="O69" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q69" s="1" t="n">
-        <v>10</v>
-      </c>
       <c r="R69" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S69" s="5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="T69" s="1" t="str">
         <f aca="false">IF(NOT(D69="1X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c"),IF(E69="landmark",CONCATENATE(A69,"_k"),IF(E69="house",CONCATENATE(A69,"_h"),A69))))</f>
-        <v>none</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U69" s="1" t="str">
         <f aca="false">IF(D69="1X1","none",IF(E69="skyscraper",CONCATENATE(A69,"_c_north"),IF(E69="landmark",CONCATENATE(A69,"_k_north"),IF(E69="house",CONCATENATE(A69,"_h_north"),CONCATENATE(A69,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>none</v>
       </c>
       <c r="V69" s="1" t="str">
         <f aca="false">IF(OR(D69="1X1",D69="2X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_east"),IF(E69="landmark",CONCATENATE(A69,"_k_east"),CONCATENATE(A69,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>none</v>
       </c>
       <c r="W69" s="1" t="str">
         <f aca="false">IF(OR(D69="1X1",D69="1X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_west"),IF(E69="landmark",CONCATENATE(A69,"_k_west"),CONCATENATE(A69,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>none</v>
       </c>
       <c r="X69" s="1" t="str">
         <f aca="false">IF(NOT(D69="2X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_south"),IF(E69="landmark",CONCATENATE(A69,"_k_south"),CONCATENATE(A69,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y69" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6757,25 +6769,25 @@
         <v>195</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>196</v>
       </c>
       <c r="G70" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="H70" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I70" s="4" t="n">
-        <v>0</v>
+        <v>1970</v>
       </c>
       <c r="J70" s="6" t="s">
         <v>30</v>
@@ -6784,41 +6796,41 @@
         <v>20</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="M70" s="8" t="str">
         <f aca="false">VLOOKUP(L70,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
-      </c>
-      <c r="N70" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="O70" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N70" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O70" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="Q70" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R70" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S70" s="5" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
       <c r="T70" s="1" t="str">
         <f aca="false">IF(NOT(D70="1X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c"),IF(E70="landmark",CONCATENATE(A70,"_k"),IF(E70="house",CONCATENATE(A70,"_h"),A70))))</f>
-        <v>shrine_k</v>
+        <v>none</v>
       </c>
       <c r="U70" s="1" t="str">
         <f aca="false">IF(D70="1X1","none",IF(E70="skyscraper",CONCATENATE(A70,"_c_north"),IF(E70="landmark",CONCATENATE(A70,"_k_north"),IF(E70="house",CONCATENATE(A70,"_h_north"),CONCATENATE(A70,"_north")))))</f>
-        <v>none</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V70" s="1" t="str">
         <f aca="false">IF(OR(D70="1X1",D70="2X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_east"),IF(E70="landmark",CONCATENATE(A70,"_k_east"),CONCATENATE(A70,"_east"))))</f>
-        <v>none</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W70" s="1" t="str">
         <f aca="false">IF(OR(D70="1X1",D70="1X2"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_west"),IF(E70="landmark",CONCATENATE(A70,"_k_west"),CONCATENATE(A70,"_west"))))</f>
@@ -6834,31 +6846,31 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G71" s="1" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I71" s="4" t="n">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>30</v>
@@ -6867,14 +6879,14 @@
         <v>20</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="M71" s="8" t="str">
         <f aca="false">VLOOKUP(L71,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N71" s="0" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O71" s="0" t="n">
         <v>3</v>
@@ -6883,65 +6895,65 @@
         <v>122</v>
       </c>
       <c r="Q71" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R71" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="T71" s="1" t="str">
         <f aca="false">IF(NOT(D71="1X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c"),IF(E71="landmark",CONCATENATE(A71,"_k"),IF(E71="house",CONCATENATE(A71,"_h"),A71))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>none</v>
       </c>
       <c r="U71" s="1" t="str">
         <f aca="false">IF(D71="1X1","none",IF(E71="skyscraper",CONCATENATE(A71,"_c_north"),IF(E71="landmark",CONCATENATE(A71,"_k_north"),IF(E71="house",CONCATENATE(A71,"_h_north"),CONCATENATE(A71,"_north")))))</f>
-        <v>none</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V71" s="1" t="str">
         <f aca="false">IF(OR(D71="1X1",D71="2X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_east"),IF(E71="landmark",CONCATENATE(A71,"_k_east"),CONCATENATE(A71,"_east"))))</f>
-        <v>none</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W71" s="1" t="str">
         <f aca="false">IF(OR(D71="1X1",D71="1X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_west"),IF(E71="landmark",CONCATENATE(A71,"_k_west"),CONCATENATE(A71,"_west"))))</f>
-        <v>none</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X71" s="1" t="str">
         <f aca="false">IF(NOT(D71="2X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_south"),IF(E71="landmark",CONCATENATE(A71,"_k_south"),CONCATENATE(A71,"_south"))))</f>
-        <v>none</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y71" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G72" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H72" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I72" s="4" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>30</v>
@@ -6950,52 +6962,52 @@
         <v>20</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="M72" s="8" t="str">
         <f aca="false">VLOOKUP(L72,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N72" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O72" s="1" t="n">
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N72" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O72" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P72" s="5" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="Q72" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R72" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="T72" s="1" t="str">
         <f aca="false">IF(NOT(D72="1X1"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c"),IF(E72="landmark",CONCATENATE(A72,"_k"),IF(E72="house",CONCATENATE(A72,"_h"),A72))))</f>
-        <v>none</v>
+        <v>shrine_k</v>
       </c>
       <c r="U72" s="1" t="str">
         <f aca="false">IF(D72="1X1","none",IF(E72="skyscraper",CONCATENATE(A72,"_c_north"),IF(E72="landmark",CONCATENATE(A72,"_k_north"),IF(E72="house",CONCATENATE(A72,"_h_north"),CONCATENATE(A72,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V72" s="1" t="str">
         <f aca="false">IF(OR(D72="1X1",D72="2X1"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_east"),IF(E72="landmark",CONCATENATE(A72,"_k_east"),CONCATENATE(A72,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W72" s="1" t="str">
         <f aca="false">IF(OR(D72="1X1",D72="1X2"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_west"),IF(E72="landmark",CONCATENATE(A72,"_k_west"),CONCATENATE(A72,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X72" s="1" t="str">
         <f aca="false">IF(NOT(D72="2X2"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_south"),IF(E72="landmark",CONCATENATE(A72,"_k_south"),CONCATENATE(A72,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y72" s="1" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7006,25 +7018,25 @@
         <v>203</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>208</v>
+        <v>113</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>204</v>
       </c>
       <c r="G73" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H73" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="I73" s="4" t="n">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="J73" s="6" t="s">
         <v>30</v>
@@ -7033,66 +7045,232 @@
         <v>20</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M73" s="8" t="str">
         <f aca="false">VLOOKUP(L73,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
-      <c r="N73" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O73" s="1" t="n">
+      <c r="N73" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O73" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>122</v>
       </c>
       <c r="Q73" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R73" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S73" s="5" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="T73" s="1" t="str">
         <f aca="false">IF(NOT(D73="1X1"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c"),IF(E73="landmark",CONCATENATE(A73,"_k"),IF(E73="house",CONCATENATE(A73,"_h"),A73))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U73" s="1" t="str">
         <f aca="false">IF(D73="1X1","none",IF(E73="skyscraper",CONCATENATE(A73,"_c_north"),IF(E73="landmark",CONCATENATE(A73,"_k_north"),IF(E73="house",CONCATENATE(A73,"_h_north"),CONCATENATE(A73,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>none</v>
       </c>
       <c r="V73" s="1" t="str">
         <f aca="false">IF(OR(D73="1X1",D73="2X1"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c_east"),IF(E73="landmark",CONCATENATE(A73,"_k_east"),CONCATENATE(A73,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>none</v>
       </c>
       <c r="W73" s="1" t="str">
         <f aca="false">IF(OR(D73="1X1",D73="1X2"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c_west"),IF(E73="landmark",CONCATENATE(A73,"_k_west"),CONCATENATE(A73,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>none</v>
       </c>
       <c r="X73" s="1" t="str">
         <f aca="false">IF(NOT(D73="2X2"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c_south"),IF(E73="landmark",CONCATENATE(A73,"_k_south"),CONCATENATE(A73,"_south"))))</f>
-        <v>temple_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y73" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0"/>
-      <c r="D74" s="1"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="6"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="8"/>
-      <c r="P74" s="5"/>
-      <c r="S74" s="5"/>
+      <c r="A74" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G74" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H74" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I74" s="4" t="n">
+        <v>1970</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K74" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="M74" s="8" t="str">
+        <f aca="false">VLOOKUP(L74,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+      </c>
+      <c r="N74" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O74" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P74" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q74" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R74" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S74" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="T74" s="1" t="str">
+        <f aca="false">IF(NOT(D74="1X1"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c"),IF(E74="landmark",CONCATENATE(A74,"_k"),IF(E74="house",CONCATENATE(A74,"_h"),A74))))</f>
+        <v>none</v>
+      </c>
+      <c r="U74" s="1" t="str">
+        <f aca="false">IF(D74="1X1","none",IF(E74="skyscraper",CONCATENATE(A74,"_c_north"),IF(E74="landmark",CONCATENATE(A74,"_k_north"),IF(E74="house",CONCATENATE(A74,"_h_north"),CONCATENATE(A74,"_north")))))</f>
+        <v>stadium_k_north</v>
+      </c>
+      <c r="V74" s="1" t="str">
+        <f aca="false">IF(OR(D74="1X1",D74="2X1"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_east"),IF(E74="landmark",CONCATENATE(A74,"_k_east"),CONCATENATE(A74,"_east"))))</f>
+        <v>stadium_k_east</v>
+      </c>
+      <c r="W74" s="1" t="str">
+        <f aca="false">IF(OR(D74="1X1",D74="1X2"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_west"),IF(E74="landmark",CONCATENATE(A74,"_k_west"),CONCATENATE(A74,"_west"))))</f>
+        <v>stadium_k_west</v>
+      </c>
+      <c r="X74" s="1" t="str">
+        <f aca="false">IF(NOT(D74="2X2"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_south"),IF(E74="landmark",CONCATENATE(A74,"_k_south"),CONCATENATE(A74,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y74" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G75" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H75" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I75" s="4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K75" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="M75" s="8" t="str">
+        <f aca="false">VLOOKUP(L75,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N75" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O75" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P75" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q75" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R75" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S75" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="T75" s="1" t="str">
+        <f aca="false">IF(NOT(D75="1X1"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c"),IF(E75="landmark",CONCATENATE(A75,"_k"),IF(E75="house",CONCATENATE(A75,"_h"),A75))))</f>
+        <v>none</v>
+      </c>
+      <c r="U75" s="1" t="str">
+        <f aca="false">IF(D75="1X1","none",IF(E75="skyscraper",CONCATENATE(A75,"_c_north"),IF(E75="landmark",CONCATENATE(A75,"_k_north"),IF(E75="house",CONCATENATE(A75,"_h_north"),CONCATENATE(A75,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V75" s="1" t="str">
+        <f aca="false">IF(OR(D75="1X1",D75="2X1"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c_east"),IF(E75="landmark",CONCATENATE(A75,"_k_east"),CONCATENATE(A75,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W75" s="1" t="str">
+        <f aca="false">IF(OR(D75="1X1",D75="1X2"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c_west"),IF(E75="landmark",CONCATENATE(A75,"_k_west"),CONCATENATE(A75,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X75" s="1" t="str">
+        <f aca="false">IF(NOT(D75="2X2"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c_south"),IF(E75="landmark",CONCATENATE(A75,"_k_south"),CONCATENATE(A75,"_south"))))</f>
+        <v>temple_k_south</v>
+      </c>
+      <c r="Y75" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0"/>
+      <c r="D76" s="1"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="6"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="8"/>
+      <c r="P76" s="5"/>
+      <c r="S76" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C62 C64:C1048576">
+  <conditionalFormatting sqref="C1:C64 C66:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -7100,15 +7278,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L74" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L76" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P74" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P76" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S74" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S76" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7141,17 +7319,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -7369,19 +7547,19 @@
       </c>
       <c r="B11" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A11,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="false">IF(B11="2X2",4,IF(OR(B11="1X2",B11="2X1"),2,IF(B11="1X1",1,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">IF(C11&gt;0,C11,MAX(D10-1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">D11=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -7484,19 +7662,19 @@
       </c>
       <c r="B16" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A16,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="C16" s="1" t="n">
         <f aca="false">IF(B16="2X2",4,IF(OR(B16="1X2",B16="2X1"),2,IF(B16="1X1",1,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">IF(C16&gt;0,C16,MAX(D15-1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="9" t="b">
         <f aca="false">D16=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -13086,25 +13264,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13118,13 +13296,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -13147,7 +13325,7 @@
         <v>57</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>122</v>
@@ -13164,13 +13342,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>160</v>
@@ -13181,35 +13359,35 @@
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13217,21 +13395,21 @@
         <v>125</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13239,10 +13417,10 @@
         <v>161</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13250,15 +13428,15 @@
         <v>159</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: dense_townhouses (formerly townhouses_01)
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="235">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -483,10 +483,16 @@
     <t xml:space="preserve">NAME_YAMASHITA_BUILDING</t>
   </si>
   <si>
+    <t xml:space="preserve">dense_townhouses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_DENSE_TOWNHOUSES</t>
+  </si>
+  <si>
     <t xml:space="preserve">dense_wooden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">house</t>
   </si>
   <si>
     <t xml:space="preserve">NAME_DENSE_WOODEN</t>
@@ -950,14 +956,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y76"/>
+  <dimension ref="A1:Y77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="A63" activeCellId="0" sqref="A63"/>
+      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5690,7 +5696,7 @@
         <v>153</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>27</v>
@@ -5708,20 +5714,20 @@
         <v>1</v>
       </c>
       <c r="I57" s="4" t="n">
-        <v>1700</v>
-      </c>
-      <c r="J57" s="6" t="n">
-        <v>1944</v>
+        <v>1945</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K57" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L57" s="7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="M57" s="8" t="str">
         <f aca="false">VLOOKUP(L57,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N57" s="1" t="n">
         <v>6</v>
@@ -5733,7 +5739,7 @@
         <v>32</v>
       </c>
       <c r="Q57" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R57" s="1" t="n">
         <v>1</v>
@@ -5743,7 +5749,7 @@
       </c>
       <c r="T57" s="1" t="str">
         <f aca="false">IF(NOT(D57="1X1"),"none",IF(E57="skyscraper",CONCATENATE(A57,"_c"),IF(E57="landmark",CONCATENATE(A57,"_k"),IF(E57="house",CONCATENATE(A57,"_h"),A57))))</f>
-        <v>dense_wooden_h</v>
+        <v>dense_townhouses_h</v>
       </c>
       <c r="U57" s="1" t="str">
         <f aca="false">IF(D57="1X1","none",IF(E57="skyscraper",CONCATENATE(A57,"_c_north"),IF(E57="landmark",CONCATENATE(A57,"_k_north"),IF(E57="house",CONCATENATE(A57,"_h_north"),CONCATENATE(A57,"_north")))))</f>
@@ -5762,7 +5768,7 @@
         <v>none</v>
       </c>
       <c r="Y57" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5773,162 +5779,162 @@
         <v>156</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>212</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>154</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G58" s="1" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H58" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I58" s="4" t="n">
         <v>1700</v>
       </c>
-      <c r="J58" s="6" t="s">
-        <v>30</v>
+      <c r="J58" s="6" t="n">
+        <v>1944</v>
       </c>
       <c r="K58" s="1" t="n">
         <v>7</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>159</v>
+        <v>37</v>
       </c>
       <c r="M58" s="8" t="str">
         <f aca="false">VLOOKUP(L58,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
       <c r="N58" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O58" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>160</v>
+        <v>32</v>
       </c>
       <c r="Q58" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R58" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="T58" s="1" t="str">
         <f aca="false">IF(NOT(D58="1X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c"),IF(E58="landmark",CONCATENATE(A58,"_k"),IF(E58="house",CONCATENATE(A58,"_h"),A58))))</f>
-        <v>none</v>
+        <v>dense_wooden_h</v>
       </c>
       <c r="U58" s="1" t="str">
         <f aca="false">IF(D58="1X1","none",IF(E58="skyscraper",CONCATENATE(A58,"_c_north"),IF(E58="landmark",CONCATENATE(A58,"_k_north"),IF(E58="house",CONCATENATE(A58,"_h_north"),CONCATENATE(A58,"_north")))))</f>
-        <v>farm_h_north</v>
+        <v>none</v>
       </c>
       <c r="V58" s="1" t="str">
-        <f aca="false">IF(OR(D58="1X1",D58="2X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_east"),IF(E58="landmark",CONCATENATE(A58,"_k_east"),IF(E58="house",CONCATENATE(A58,"_h_east"),CONCATENATE(A58,"_east")))))</f>
-        <v>farm_h_east</v>
+        <f aca="false">IF(OR(D58="1X1",D58="2X1"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_east"),IF(E58="landmark",CONCATENATE(A58,"_k_east"),CONCATENATE(A58,"_east"))))</f>
+        <v>none</v>
       </c>
       <c r="W58" s="1" t="str">
-        <f aca="false">IF(OR(D58="1X1",D58="1X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_west"),IF(E58="landmark",CONCATENATE(A58,"_k_west"),IF(E58="house",CONCATENATE(A58,"_h_west"),CONCATENATE(A58,"_west")))))</f>
-        <v>farm_h_west</v>
+        <f aca="false">IF(OR(D58="1X1",D58="1X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_west"),IF(E58="landmark",CONCATENATE(A58,"_k_west"),CONCATENATE(A58,"_west"))))</f>
+        <v>none</v>
       </c>
       <c r="X58" s="1" t="str">
-        <f aca="false">IF(NOT(D58="2X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_south"),IF(E58="landmark",CONCATENATE(A58,"_k_south"),IF(E58="house",CONCATENATE(A58,"_h_south"),CONCATENATE(A58,"_south")))))</f>
-        <v>farm_h_south</v>
+        <f aca="false">IF(NOT(D58="2X2"),"none",IF(E58="skyscraper",CONCATENATE(A58,"_c_south"),IF(E58="landmark",CONCATENATE(A58,"_k_south"),CONCATENATE(A58,"_south"))))</f>
+        <v>none</v>
       </c>
       <c r="Y58" s="1" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>14</v>
+        <v>212</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>154</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G59" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I59" s="4" t="n">
         <v>1700</v>
       </c>
-      <c r="J59" s="6" t="n">
-        <v>1944</v>
+      <c r="J59" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M59" s="8" t="str">
         <f aca="false">VLOOKUP(L59,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N59" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O59" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="O59" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="P59" s="5" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R59" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S59" s="5" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="T59" s="1" t="str">
         <f aca="false">IF(NOT(D59="1X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c"),IF(E59="landmark",CONCATENATE(A59,"_k"),IF(E59="house",CONCATENATE(A59,"_h"),A59))))</f>
-        <v>large_wooden_farmhouse_h</v>
+        <v>none</v>
       </c>
       <c r="U59" s="1" t="str">
         <f aca="false">IF(D59="1X1","none",IF(E59="skyscraper",CONCATENATE(A59,"_c_north"),IF(E59="landmark",CONCATENATE(A59,"_k_north"),IF(E59="house",CONCATENATE(A59,"_h_north"),CONCATENATE(A59,"_north")))))</f>
-        <v>none</v>
+        <v>farm_h_north</v>
       </c>
       <c r="V59" s="1" t="str">
         <f aca="false">IF(OR(D59="1X1",D59="2X1"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_east"),IF(E59="landmark",CONCATENATE(A59,"_k_east"),IF(E59="house",CONCATENATE(A59,"_h_east"),CONCATENATE(A59,"_east")))))</f>
-        <v>none</v>
+        <v>farm_h_east</v>
       </c>
       <c r="W59" s="1" t="str">
         <f aca="false">IF(OR(D59="1X1",D59="1X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_west"),IF(E59="landmark",CONCATENATE(A59,"_k_west"),IF(E59="house",CONCATENATE(A59,"_h_west"),CONCATENATE(A59,"_west")))))</f>
-        <v>none</v>
+        <v>farm_h_west</v>
       </c>
       <c r="X59" s="1" t="str">
         <f aca="false">IF(NOT(D59="2X2"),"none",IF(E59="skyscraper",CONCATENATE(A59,"_c_south"),IF(E59="landmark",CONCATENATE(A59,"_k_south"),IF(E59="house",CONCATENATE(A59,"_h_south"),CONCATENATE(A59,"_south")))))</f>
-        <v>none</v>
+        <v>farm_h_south</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5939,7 +5945,7 @@
         <v>164</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>27</v>
@@ -5954,23 +5960,23 @@
         <v>20</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I60" s="4" t="n">
-        <v>1870</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>30</v>
+        <v>1700</v>
+      </c>
+      <c r="J60" s="6" t="n">
+        <v>1944</v>
       </c>
       <c r="K60" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L60" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="M60" s="8" t="str">
         <f aca="false">VLOOKUP(L60,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N60" s="1" t="n">
         <v>6</v>
@@ -5982,7 +5988,7 @@
         <v>32</v>
       </c>
       <c r="Q60" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R60" s="1" t="n">
         <v>1</v>
@@ -5992,7 +5998,7 @@
       </c>
       <c r="T60" s="1" t="str">
         <f aca="false">IF(NOT(D60="1X1"),"none",IF(E60="skyscraper",CONCATENATE(A60,"_c"),IF(E60="landmark",CONCATENATE(A60,"_k"),IF(E60="house",CONCATENATE(A60,"_h"),A60))))</f>
-        <v>naganuma_h</v>
+        <v>large_wooden_farmhouse_h</v>
       </c>
       <c r="U60" s="1" t="str">
         <f aca="false">IF(D60="1X1","none",IF(E60="skyscraper",CONCATENATE(A60,"_c_north"),IF(E60="landmark",CONCATENATE(A60,"_k_north"),IF(E60="house",CONCATENATE(A60,"_h_north"),CONCATENATE(A60,"_north")))))</f>
@@ -6011,18 +6017,18 @@
         <v>none</v>
       </c>
       <c r="Y60" s="1" t="s">
-        <v>167</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>27</v>
@@ -6031,7 +6037,7 @@
         <v>154</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G61" s="1" t="n">
         <v>20</v>
@@ -6049,7 +6055,7 @@
         <v>5</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="M61" s="8" t="str">
         <f aca="false">VLOOKUP(L61,dropdowns!E:F,2,0)</f>
@@ -6075,7 +6081,7 @@
       </c>
       <c r="T61" s="1" t="str">
         <f aca="false">IF(NOT(D61="1X1"),"none",IF(E61="skyscraper",CONCATENATE(A61,"_c"),IF(E61="landmark",CONCATENATE(A61,"_k"),IF(E61="house",CONCATENATE(A61,"_h"),A61))))</f>
-        <v>nishikawa_h</v>
+        <v>naganuma_h</v>
       </c>
       <c r="U61" s="1" t="str">
         <f aca="false">IF(D61="1X1","none",IF(E61="skyscraper",CONCATENATE(A61,"_c_north"),IF(E61="landmark",CONCATENATE(A61,"_k_north"),IF(E61="house",CONCATENATE(A61,"_h_north"),CONCATENATE(A61,"_north")))))</f>
@@ -6094,7 +6100,7 @@
         <v>none</v>
       </c>
       <c r="Y61" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6105,7 +6111,7 @@
         <v>170</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>27</v>
@@ -6120,26 +6126,26 @@
         <v>20</v>
       </c>
       <c r="H62" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I62" s="4" t="n">
-        <v>1700</v>
-      </c>
-      <c r="J62" s="6" t="n">
-        <v>1944</v>
+        <v>1870</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K62" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M62" s="8" t="str">
         <f aca="false">VLOOKUP(L62,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N62" s="1" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="O62" s="1" t="n">
         <v>0</v>
@@ -6154,11 +6160,11 @@
         <v>1</v>
       </c>
       <c r="S62" s="5" t="s">
-        <v>173</v>
+        <v>33</v>
       </c>
       <c r="T62" s="1" t="str">
         <f aca="false">IF(NOT(D62="1X1"),"none",IF(E62="skyscraper",CONCATENATE(A62,"_c"),IF(E62="landmark",CONCATENATE(A62,"_k"),IF(E62="house",CONCATENATE(A62,"_h"),A62))))</f>
-        <v>old_villa_h</v>
+        <v>nishikawa_h</v>
       </c>
       <c r="U62" s="1" t="str">
         <f aca="false">IF(D62="1X1","none",IF(E62="skyscraper",CONCATENATE(A62,"_c_north"),IF(E62="landmark",CONCATENATE(A62,"_k_north"),IF(E62="house",CONCATENATE(A62,"_h_north"),CONCATENATE(A62,"_north")))))</f>
@@ -6177,18 +6183,18 @@
         <v>none</v>
       </c>
       <c r="Y62" s="1" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>27</v>
@@ -6197,7 +6203,7 @@
         <v>154</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G63" s="1" t="n">
         <v>20</v>
@@ -6215,14 +6221,14 @@
         <v>5</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="M63" s="8" t="str">
         <f aca="false">VLOOKUP(L63,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_EDGE )</v>
       </c>
       <c r="N63" s="1" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="O63" s="1" t="n">
         <v>0</v>
@@ -6231,17 +6237,17 @@
         <v>32</v>
       </c>
       <c r="Q63" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R63" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S63" s="5" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
       <c r="T63" s="1" t="str">
         <f aca="false">IF(NOT(D63="1X1"),"none",IF(E63="skyscraper",CONCATENATE(A63,"_c"),IF(E63="landmark",CONCATENATE(A63,"_k"),IF(E63="house",CONCATENATE(A63,"_h"),A63))))</f>
-        <v>wooden_farmhouse_h</v>
+        <v>old_villa_h</v>
       </c>
       <c r="U63" s="1" t="str">
         <f aca="false">IF(D63="1X1","none",IF(E63="skyscraper",CONCATENATE(A63,"_c_north"),IF(E63="landmark",CONCATENATE(A63,"_k_north"),IF(E63="house",CONCATENATE(A63,"_h_north"),CONCATENATE(A63,"_north")))))</f>
@@ -6271,7 +6277,7 @@
         <v>176</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>27</v>
@@ -6298,7 +6304,7 @@
         <v>5</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M64" s="8" t="str">
         <f aca="false">VLOOKUP(L64,dropdowns!E:F,2,0)</f>
@@ -6324,7 +6330,7 @@
       </c>
       <c r="T64" s="1" t="str">
         <f aca="false">IF(NOT(D64="1X1"),"none",IF(E64="skyscraper",CONCATENATE(A64,"_c"),IF(E64="landmark",CONCATENATE(A64,"_k"),IF(E64="house",CONCATENATE(A64,"_h"),A64))))</f>
-        <v>wooden_house_h</v>
+        <v>wooden_farmhouse_h</v>
       </c>
       <c r="U64" s="1" t="str">
         <f aca="false">IF(D64="1X1","none",IF(E64="skyscraper",CONCATENATE(A64,"_c_north"),IF(E64="landmark",CONCATENATE(A64,"_k_north"),IF(E64="house",CONCATENATE(A64,"_h_north"),CONCATENATE(A64,"_north")))))</f>
@@ -6347,67 +6353,67 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="3" t="n">
-        <v>95</v>
+      <c r="C65" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I65" s="3" t="n">
-        <v>1950</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K65" s="0" t="n">
+      <c r="G65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" s="4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J65" s="6" t="n">
+        <v>1944</v>
+      </c>
+      <c r="K65" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="M65" s="8" t="str">
         <f aca="false">VLOOKUP(L65,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N65" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O65" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O65" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="P65" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q65" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R65" s="0" t="n">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="S65" s="5" t="s">
-        <v>182</v>
+        <v>33</v>
       </c>
       <c r="T65" s="1" t="str">
         <f aca="false">IF(NOT(D65="1X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c"),IF(E65="landmark",CONCATENATE(A65,"_k"),IF(E65="house",CONCATENATE(A65,"_h"),A65))))</f>
-        <v>convini_k</v>
+        <v>wooden_house_h</v>
       </c>
       <c r="U65" s="1" t="str">
         <f aca="false">IF(D65="1X1","none",IF(E65="skyscraper",CONCATENATE(A65,"_c_north"),IF(E65="landmark",CONCATENATE(A65,"_k_north"),IF(E65="house",CONCATENATE(A65,"_h_north"),CONCATENATE(A65,"_north")))))</f>
@@ -6425,76 +6431,76 @@
         <f aca="false">IF(NOT(D65="2X2"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c_south"),IF(E65="landmark",CONCATENATE(A65,"_k_south"),IF(E65="house",CONCATENATE(A65,"_h_south"),CONCATENATE(A65,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y65" s="0" t="s">
-        <v>183</v>
+      <c r="Y65" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C66" s="2" t="n">
-        <v>107</v>
+      <c r="A66" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>185</v>
+        <v>27</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G66" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="H66" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I66" s="4" t="n">
-        <v>1970</v>
+        <v>182</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" s="3" t="n">
+        <v>1950</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K66" s="1" t="n">
-        <v>20</v>
+      <c r="K66" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="M66" s="8" t="str">
         <f aca="false">VLOOKUP(L66,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
-      </c>
-      <c r="N66" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="O66" s="1" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N66" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="O66" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P66" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q66" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="R66" s="1" t="n">
-        <v>2</v>
+        <v>162</v>
+      </c>
+      <c r="Q66" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R66" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="S66" s="5" t="s">
-        <v>33</v>
+        <v>184</v>
       </c>
       <c r="T66" s="1" t="str">
         <f aca="false">IF(NOT(D66="1X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c"),IF(E66="landmark",CONCATENATE(A66,"_k"),IF(E66="house",CONCATENATE(A66,"_h"),A66))))</f>
-        <v>none</v>
+        <v>convini_k</v>
       </c>
       <c r="U66" s="1" t="str">
         <f aca="false">IF(D66="1X1","none",IF(E66="skyscraper",CONCATENATE(A66,"_c_north"),IF(E66="landmark",CONCATENATE(A66,"_k_north"),IF(E66="house",CONCATENATE(A66,"_h_north"),CONCATENATE(A66,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V66" s="1" t="str">
         <f aca="false">IF(OR(D66="1X1",D66="2X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_east"),IF(E66="landmark",CONCATENATE(A66,"_k_east"),IF(E66="house",CONCATENATE(A66,"_h_east"),CONCATENATE(A66,"_east")))))</f>
@@ -6502,37 +6508,37 @@
       </c>
       <c r="W66" s="1" t="str">
         <f aca="false">IF(OR(D66="1X1",D66="1X2"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_west"),IF(E66="landmark",CONCATENATE(A66,"_k_west"),IF(E66="house",CONCATENATE(A66,"_h_west"),CONCATENATE(A66,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>none</v>
       </c>
       <c r="X66" s="1" t="str">
         <f aca="false">IF(NOT(D66="2X2"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c_south"),IF(E66="landmark",CONCATENATE(A66,"_k_south"),IF(E66="house",CONCATENATE(A66,"_h_south"),CONCATENATE(A66,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y66" s="1" t="s">
-        <v>184</v>
+      <c r="Y66" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C67" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E67" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G67" s="1" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>3</v>
@@ -6547,29 +6553,29 @@
         <v>20</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="M67" s="8" t="str">
         <f aca="false">VLOOKUP(L67,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N67" s="1" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="O67" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="Q67" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R67" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S67" s="5" t="s">
-        <v>190</v>
+        <v>33</v>
       </c>
       <c r="T67" s="1" t="str">
         <f aca="false">IF(NOT(D67="1X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c"),IF(E67="landmark",CONCATENATE(A67,"_k"),IF(E67="house",CONCATENATE(A67,"_h"),A67))))</f>
@@ -6577,134 +6583,134 @@
       </c>
       <c r="U67" s="1" t="str">
         <f aca="false">IF(D67="1X1","none",IF(E67="skyscraper",CONCATENATE(A67,"_c_north"),IF(E67="landmark",CONCATENATE(A67,"_k_north"),IF(E67="house",CONCATENATE(A67,"_h_north"),CONCATENATE(A67,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V67" s="1" t="str">
-        <f aca="false">IF(OR(D67="1X1",D67="2X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_east"),IF(E67="landmark",CONCATENATE(A67,"_k_east"),CONCATENATE(A67,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D67="1X1",D67="2X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_east"),IF(E67="landmark",CONCATENATE(A67,"_k_east"),IF(E67="house",CONCATENATE(A67,"_h_east"),CONCATENATE(A67,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W67" s="1" t="str">
-        <f aca="false">IF(OR(D67="1X1",D67="1X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_west"),IF(E67="landmark",CONCATENATE(A67,"_k_west"),CONCATENATE(A67,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D67="1X1",D67="1X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_west"),IF(E67="landmark",CONCATENATE(A67,"_k_west"),IF(E67="house",CONCATENATE(A67,"_h_west"),CONCATENATE(A67,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X67" s="1" t="str">
-        <f aca="false">IF(NOT(D67="2X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_south"),IF(E67="landmark",CONCATENATE(A67,"_k_south"),CONCATENATE(A67,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D67="2X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_south"),IF(E67="landmark",CONCATENATE(A67,"_k_south"),IF(E67="house",CONCATENATE(A67,"_h_south"),CONCATENATE(A67,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y67" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G68" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I68" s="4" t="n">
-        <v>1870</v>
+        <v>1970</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K68" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="M68" s="8" t="str">
         <f aca="false">VLOOKUP(L68,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N68" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O68" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P68" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="Q68" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="R68" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
       <c r="T68" s="1" t="str">
         <f aca="false">IF(NOT(D68="1X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c"),IF(E68="landmark",CONCATENATE(A68,"_k"),IF(E68="house",CONCATENATE(A68,"_h"),A68))))</f>
-        <v>onsen_k</v>
+        <v>none</v>
       </c>
       <c r="U68" s="1" t="str">
         <f aca="false">IF(D68="1X1","none",IF(E68="skyscraper",CONCATENATE(A68,"_c_north"),IF(E68="landmark",CONCATENATE(A68,"_k_north"),IF(E68="house",CONCATENATE(A68,"_h_north"),CONCATENATE(A68,"_north")))))</f>
-        <v>none</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V68" s="1" t="str">
-        <f aca="false">IF(OR(D68="1X1",D68="2X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_east"),IF(E68="landmark",CONCATENATE(A68,"_k_east"),IF(E68="house",CONCATENATE(A68,"_h_east"),CONCATENATE(A68,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D68="1X1",D68="2X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_east"),IF(E68="landmark",CONCATENATE(A68,"_k_east"),CONCATENATE(A68,"_east"))))</f>
+        <v>hospital_k_east</v>
       </c>
       <c r="W68" s="1" t="str">
-        <f aca="false">IF(OR(D68="1X1",D68="1X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_west"),IF(E68="landmark",CONCATENATE(A68,"_k_west"),IF(E68="house",CONCATENATE(A68,"_h_west"),CONCATENATE(A68,"_west")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D68="1X1",D68="1X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_west"),IF(E68="landmark",CONCATENATE(A68,"_k_west"),CONCATENATE(A68,"_west"))))</f>
+        <v>hospital_k_west</v>
       </c>
       <c r="X68" s="1" t="str">
-        <f aca="false">IF(NOT(D68="2X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_south"),IF(E68="landmark",CONCATENATE(A68,"_k_south"),IF(E68="house",CONCATENATE(A68,"_h_south"),CONCATENATE(A68,"_south")))))</f>
-        <v>none</v>
+        <f aca="false">IF(NOT(D68="2X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_south"),IF(E68="landmark",CONCATENATE(A68,"_k_south"),CONCATENATE(A68,"_south"))))</f>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y68" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>193</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H69" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I69" s="4" t="n">
-        <v>1980</v>
+        <v>1870</v>
       </c>
       <c r="J69" s="6" t="s">
         <v>30</v>
@@ -6713,11 +6719,11 @@
         <v>10</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="M69" s="8" t="str">
         <f aca="false">VLOOKUP(L69,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
       <c r="N69" s="1" t="n">
         <v>29</v>
@@ -6726,111 +6732,111 @@
         <v>3</v>
       </c>
       <c r="P69" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="Q69" s="1" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="R69" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S69" s="5" t="s">
-        <v>194</v>
+        <v>33</v>
       </c>
       <c r="T69" s="1" t="str">
         <f aca="false">IF(NOT(D69="1X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c"),IF(E69="landmark",CONCATENATE(A69,"_k"),IF(E69="house",CONCATENATE(A69,"_h"),A69))))</f>
-        <v>pachinko_k</v>
+        <v>onsen_k</v>
       </c>
       <c r="U69" s="1" t="str">
         <f aca="false">IF(D69="1X1","none",IF(E69="skyscraper",CONCATENATE(A69,"_c_north"),IF(E69="landmark",CONCATENATE(A69,"_k_north"),IF(E69="house",CONCATENATE(A69,"_h_north"),CONCATENATE(A69,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V69" s="1" t="str">
-        <f aca="false">IF(OR(D69="1X1",D69="2X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_east"),IF(E69="landmark",CONCATENATE(A69,"_k_east"),CONCATENATE(A69,"_east"))))</f>
+        <f aca="false">IF(OR(D69="1X1",D69="2X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_east"),IF(E69="landmark",CONCATENATE(A69,"_k_east"),IF(E69="house",CONCATENATE(A69,"_h_east"),CONCATENATE(A69,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W69" s="1" t="str">
-        <f aca="false">IF(OR(D69="1X1",D69="1X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_west"),IF(E69="landmark",CONCATENATE(A69,"_k_west"),CONCATENATE(A69,"_west"))))</f>
+        <f aca="false">IF(OR(D69="1X1",D69="1X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_west"),IF(E69="landmark",CONCATENATE(A69,"_k_west"),IF(E69="house",CONCATENATE(A69,"_h_west"),CONCATENATE(A69,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X69" s="1" t="str">
-        <f aca="false">IF(NOT(D69="2X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_south"),IF(E69="landmark",CONCATENATE(A69,"_k_south"),CONCATENATE(A69,"_south"))))</f>
+        <f aca="false">IF(NOT(D69="2X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_south"),IF(E69="landmark",CONCATENATE(A69,"_k_south"),IF(E69="house",CONCATENATE(A69,"_h_south"),CONCATENATE(A69,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y69" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C70" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="G70" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H70" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I70" s="4" t="n">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="J70" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K70" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>166</v>
+        <v>57</v>
       </c>
       <c r="M70" s="8" t="str">
         <f aca="false">VLOOKUP(L70,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N70" s="1" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="O70" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="Q70" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="R70" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S70" s="5" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
       <c r="T70" s="1" t="str">
         <f aca="false">IF(NOT(D70="1X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c"),IF(E70="landmark",CONCATENATE(A70,"_k"),IF(E70="house",CONCATENATE(A70,"_h"),A70))))</f>
-        <v>none</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U70" s="1" t="str">
         <f aca="false">IF(D70="1X1","none",IF(E70="skyscraper",CONCATENATE(A70,"_c_north"),IF(E70="landmark",CONCATENATE(A70,"_k_north"),IF(E70="house",CONCATENATE(A70,"_h_north"),CONCATENATE(A70,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V70" s="1" t="str">
         <f aca="false">IF(OR(D70="1X1",D70="2X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_east"),IF(E70="landmark",CONCATENATE(A70,"_k_east"),CONCATENATE(A70,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>none</v>
       </c>
       <c r="W70" s="1" t="str">
         <f aca="false">IF(OR(D70="1X1",D70="1X2"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_west"),IF(E70="landmark",CONCATENATE(A70,"_k_west"),CONCATENATE(A70,"_west"))))</f>
@@ -6841,7 +6847,7 @@
         <v>none</v>
       </c>
       <c r="Y70" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6852,25 +6858,25 @@
         <v>197</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>198</v>
       </c>
       <c r="G71" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H71" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="H71" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I71" s="4" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>30</v>
@@ -6879,20 +6885,20 @@
         <v>20</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="M71" s="8" t="str">
         <f aca="false">VLOOKUP(L71,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N71" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O71" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N71" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O71" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P71" s="5" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q71" s="1" t="n">
         <v>10</v>
@@ -6901,7 +6907,7 @@
         <v>2</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="T71" s="1" t="str">
         <f aca="false">IF(NOT(D71="1X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c"),IF(E71="landmark",CONCATENATE(A71,"_k"),IF(E71="house",CONCATENATE(A71,"_h"),A71))))</f>
@@ -6909,19 +6915,19 @@
       </c>
       <c r="U71" s="1" t="str">
         <f aca="false">IF(D71="1X1","none",IF(E71="skyscraper",CONCATENATE(A71,"_c_north"),IF(E71="landmark",CONCATENATE(A71,"_k_north"),IF(E71="house",CONCATENATE(A71,"_h_north"),CONCATENATE(A71,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V71" s="1" t="str">
         <f aca="false">IF(OR(D71="1X1",D71="2X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_east"),IF(E71="landmark",CONCATENATE(A71,"_k_east"),CONCATENATE(A71,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W71" s="1" t="str">
         <f aca="false">IF(OR(D71="1X1",D71="1X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_west"),IF(E71="landmark",CONCATENATE(A71,"_k_west"),CONCATENATE(A71,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>none</v>
       </c>
       <c r="X71" s="1" t="str">
         <f aca="false">IF(NOT(D71="2X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_south"),IF(E71="landmark",CONCATENATE(A71,"_k_south"),CONCATENATE(A71,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y71" s="1" t="s">
         <v>197</v>
@@ -6935,25 +6941,25 @@
         <v>199</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>200</v>
       </c>
       <c r="G72" s="1" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I72" s="4" t="n">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>30</v>
@@ -6962,14 +6968,14 @@
         <v>20</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="M72" s="8" t="str">
         <f aca="false">VLOOKUP(L72,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N72" s="0" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O72" s="0" t="n">
         <v>3</v>
@@ -6978,33 +6984,33 @@
         <v>122</v>
       </c>
       <c r="Q72" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R72" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="T72" s="1" t="str">
         <f aca="false">IF(NOT(D72="1X1"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c"),IF(E72="landmark",CONCATENATE(A72,"_k"),IF(E72="house",CONCATENATE(A72,"_h"),A72))))</f>
-        <v>shrine_k</v>
+        <v>none</v>
       </c>
       <c r="U72" s="1" t="str">
         <f aca="false">IF(D72="1X1","none",IF(E72="skyscraper",CONCATENATE(A72,"_c_north"),IF(E72="landmark",CONCATENATE(A72,"_k_north"),IF(E72="house",CONCATENATE(A72,"_h_north"),CONCATENATE(A72,"_north")))))</f>
-        <v>none</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V72" s="1" t="str">
         <f aca="false">IF(OR(D72="1X1",D72="2X1"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_east"),IF(E72="landmark",CONCATENATE(A72,"_k_east"),CONCATENATE(A72,"_east"))))</f>
-        <v>none</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W72" s="1" t="str">
         <f aca="false">IF(OR(D72="1X1",D72="1X2"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_west"),IF(E72="landmark",CONCATENATE(A72,"_k_west"),CONCATENATE(A72,"_west"))))</f>
-        <v>none</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X72" s="1" t="str">
         <f aca="false">IF(NOT(D72="2X2"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_south"),IF(E72="landmark",CONCATENATE(A72,"_k_south"),CONCATENATE(A72,"_south"))))</f>
-        <v>none</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y72" s="1" t="s">
         <v>199</v>
@@ -7012,28 +7018,28 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G73" s="1" t="n">
         <v>5</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I73" s="4" t="n">
         <v>0</v>
@@ -7045,7 +7051,7 @@
         <v>20</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="M73" s="8" t="str">
         <f aca="false">VLOOKUP(L73,dropdowns!E:F,2,0)</f>
@@ -7067,11 +7073,11 @@
         <v>1</v>
       </c>
       <c r="S73" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="T73" s="1" t="str">
         <f aca="false">IF(NOT(D73="1X1"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c"),IF(E73="landmark",CONCATENATE(A73,"_k"),IF(E73="house",CONCATENATE(A73,"_h"),A73))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>shrine_k</v>
       </c>
       <c r="U73" s="1" t="str">
         <f aca="false">IF(D73="1X1","none",IF(E73="skyscraper",CONCATENATE(A73,"_c_north"),IF(E73="landmark",CONCATENATE(A73,"_k_north"),IF(E73="house",CONCATENATE(A73,"_h_north"),CONCATENATE(A73,"_north")))))</f>
@@ -7090,7 +7096,7 @@
         <v>none</v>
       </c>
       <c r="Y73" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7101,25 +7107,25 @@
         <v>205</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>206</v>
       </c>
       <c r="G74" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H74" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="I74" s="4" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J74" s="6" t="s">
         <v>30</v>
@@ -7128,52 +7134,52 @@
         <v>20</v>
       </c>
       <c r="L74" s="7" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="M74" s="8" t="str">
         <f aca="false">VLOOKUP(L74,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N74" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O74" s="1" t="n">
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N74" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O74" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="Q74" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R74" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S74" s="5" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="T74" s="1" t="str">
         <f aca="false">IF(NOT(D74="1X1"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c"),IF(E74="landmark",CONCATENATE(A74,"_k"),IF(E74="house",CONCATENATE(A74,"_h"),A74))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U74" s="1" t="str">
         <f aca="false">IF(D74="1X1","none",IF(E74="skyscraper",CONCATENATE(A74,"_c_north"),IF(E74="landmark",CONCATENATE(A74,"_k_north"),IF(E74="house",CONCATENATE(A74,"_h_north"),CONCATENATE(A74,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V74" s="1" t="str">
         <f aca="false">IF(OR(D74="1X1",D74="2X1"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_east"),IF(E74="landmark",CONCATENATE(A74,"_k_east"),CONCATENATE(A74,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W74" s="1" t="str">
         <f aca="false">IF(OR(D74="1X1",D74="1X2"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_west"),IF(E74="landmark",CONCATENATE(A74,"_k_west"),CONCATENATE(A74,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X74" s="1" t="str">
         <f aca="false">IF(NOT(D74="2X2"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_south"),IF(E74="landmark",CONCATENATE(A74,"_k_south"),CONCATENATE(A74,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y74" s="1" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7184,25 +7190,25 @@
         <v>207</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>208</v>
       </c>
       <c r="G75" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H75" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I75" s="4" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J75" s="6" t="s">
         <v>30</v>
@@ -7211,11 +7217,11 @@
         <v>20</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="M75" s="8" t="str">
         <f aca="false">VLOOKUP(L75,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N75" s="1" t="n">
         <v>20</v>
@@ -7224,16 +7230,16 @@
         <v>3</v>
       </c>
       <c r="P75" s="5" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q75" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R75" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="T75" s="1" t="str">
         <f aca="false">IF(NOT(D75="1X1"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c"),IF(E75="landmark",CONCATENATE(A75,"_k"),IF(E75="house",CONCATENATE(A75,"_h"),A75))))</f>
@@ -7241,36 +7247,119 @@
       </c>
       <c r="U75" s="1" t="str">
         <f aca="false">IF(D75="1X1","none",IF(E75="skyscraper",CONCATENATE(A75,"_c_north"),IF(E75="landmark",CONCATENATE(A75,"_k_north"),IF(E75="house",CONCATENATE(A75,"_h_north"),CONCATENATE(A75,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>stadium_k_north</v>
       </c>
       <c r="V75" s="1" t="str">
         <f aca="false">IF(OR(D75="1X1",D75="2X1"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c_east"),IF(E75="landmark",CONCATENATE(A75,"_k_east"),CONCATENATE(A75,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>stadium_k_east</v>
       </c>
       <c r="W75" s="1" t="str">
         <f aca="false">IF(OR(D75="1X1",D75="1X2"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c_west"),IF(E75="landmark",CONCATENATE(A75,"_k_west"),CONCATENATE(A75,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>stadium_k_west</v>
       </c>
       <c r="X75" s="1" t="str">
         <f aca="false">IF(NOT(D75="2X2"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c_south"),IF(E75="landmark",CONCATENATE(A75,"_k_south"),CONCATENATE(A75,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y75" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G76" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H76" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I76" s="4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K76" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L76" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="M76" s="8" t="str">
+        <f aca="false">VLOOKUP(L76,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N76" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O76" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P76" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q76" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R76" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="T76" s="1" t="str">
+        <f aca="false">IF(NOT(D76="1X1"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c"),IF(E76="landmark",CONCATENATE(A76,"_k"),IF(E76="house",CONCATENATE(A76,"_h"),A76))))</f>
+        <v>none</v>
+      </c>
+      <c r="U76" s="1" t="str">
+        <f aca="false">IF(D76="1X1","none",IF(E76="skyscraper",CONCATENATE(A76,"_c_north"),IF(E76="landmark",CONCATENATE(A76,"_k_north"),IF(E76="house",CONCATENATE(A76,"_h_north"),CONCATENATE(A76,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V76" s="1" t="str">
+        <f aca="false">IF(OR(D76="1X1",D76="2X1"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c_east"),IF(E76="landmark",CONCATENATE(A76,"_k_east"),CONCATENATE(A76,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W76" s="1" t="str">
+        <f aca="false">IF(OR(D76="1X1",D76="1X2"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c_west"),IF(E76="landmark",CONCATENATE(A76,"_k_west"),CONCATENATE(A76,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X76" s="1" t="str">
+        <f aca="false">IF(NOT(D76="2X2"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c_south"),IF(E76="landmark",CONCATENATE(A76,"_k_south"),CONCATENATE(A76,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y75" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0"/>
-      <c r="D76" s="1"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="6"/>
-      <c r="L76" s="7"/>
-      <c r="M76" s="8"/>
-      <c r="P76" s="5"/>
-      <c r="S76" s="5"/>
+      <c r="Y76" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0"/>
+      <c r="D77" s="1"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="6"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="P77" s="5"/>
+      <c r="S77" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C64 C66:C1048576">
+  <conditionalFormatting sqref="C1:C65 C67:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -7278,15 +7367,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L76" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L77" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P76" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P77" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S76" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S77" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7319,17 +7408,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -7478,19 +7567,19 @@
       </c>
       <c r="B8" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A8,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="C8" s="1" t="n">
         <f aca="false">IF(B8="2X2",4,IF(OR(B8="1X2",B8="2X1"),2,IF(B8="1X1",1,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">IF(C8&gt;0,C8,MAX(D7-1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="9" t="n">
         <f aca="false">D8=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -13264,25 +13353,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13296,13 +13385,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -13325,7 +13414,7 @@
         <v>57</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>122</v>
@@ -13342,16 +13431,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13359,35 +13448,35 @@
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13395,48 +13484,48 @@
         <v>125</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: townhouses (formerly townhouses_02)
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="239">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -561,6 +561,15 @@
     <t xml:space="preserve">[PASS, 4],[MAIL, 2], [GOOD, 2]</t>
   </si>
   <si>
+    <t xml:space="preserve">townhouses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_TOWNHOUSES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">wooden_farmhouse</t>
   </si>
   <si>
@@ -721,9 +730,6 @@
   </si>
   <si>
     <t xml:space="preserve">bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,1</t>
   </si>
   <si>
     <t xml:space="preserve">bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT)</t>
@@ -962,14 +968,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y78"/>
+  <dimension ref="A1:Y79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
-      <selection pane="bottomRight" activeCell="A64" activeCellId="0" sqref="A64"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6366,7 +6372,7 @@
         <v>179</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>27</v>
@@ -6384,23 +6390,23 @@
         <v>1</v>
       </c>
       <c r="I65" s="4" t="n">
-        <v>1700</v>
-      </c>
-      <c r="J65" s="6" t="n">
-        <v>1944</v>
+        <v>1945</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K65" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="M65" s="8" t="str">
         <f aca="false">VLOOKUP(L65,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT)</v>
       </c>
       <c r="N65" s="1" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="O65" s="1" t="n">
         <v>0</v>
@@ -6409,7 +6415,7 @@
         <v>32</v>
       </c>
       <c r="Q65" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R65" s="1" t="n">
         <v>1</v>
@@ -6419,7 +6425,7 @@
       </c>
       <c r="T65" s="1" t="str">
         <f aca="false">IF(NOT(D65="1X1"),"none",IF(E65="skyscraper",CONCATENATE(A65,"_c"),IF(E65="landmark",CONCATENATE(A65,"_k"),IF(E65="house",CONCATENATE(A65,"_h"),A65))))</f>
-        <v>wooden_farmhouse_h</v>
+        <v>townhouses_h</v>
       </c>
       <c r="U65" s="1" t="str">
         <f aca="false">IF(D65="1X1","none",IF(E65="skyscraper",CONCATENATE(A65,"_c_north"),IF(E65="landmark",CONCATENATE(A65,"_k_north"),IF(E65="house",CONCATENATE(A65,"_h_north"),CONCATENATE(A65,"_north")))))</f>
@@ -6438,18 +6444,18 @@
         <v>none</v>
       </c>
       <c r="Y65" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>27</v>
@@ -6458,7 +6464,7 @@
         <v>154</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G66" s="1" t="n">
         <v>20</v>
@@ -6502,7 +6508,7 @@
       </c>
       <c r="T66" s="1" t="str">
         <f aca="false">IF(NOT(D66="1X1"),"none",IF(E66="skyscraper",CONCATENATE(A66,"_c"),IF(E66="landmark",CONCATENATE(A66,"_k"),IF(E66="house",CONCATENATE(A66,"_h"),A66))))</f>
-        <v>wooden_house_h</v>
+        <v>wooden_farmhouse_h</v>
       </c>
       <c r="U66" s="1" t="str">
         <f aca="false">IF(D66="1X1","none",IF(E66="skyscraper",CONCATENATE(A66,"_c_north"),IF(E66="landmark",CONCATENATE(A66,"_k_north"),IF(E66="house",CONCATENATE(A66,"_h_north"),CONCATENATE(A66,"_north")))))</f>
@@ -6525,67 +6531,67 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="C67" s="3" t="n">
-        <v>95</v>
+      <c r="A67" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G67" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I67" s="3" t="n">
-        <v>1950</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K67" s="0" t="n">
+      <c r="G67" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H67" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" s="4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J67" s="6" t="n">
+        <v>1944</v>
+      </c>
+      <c r="K67" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="M67" s="8" t="str">
         <f aca="false">VLOOKUP(L67,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
-      </c>
-      <c r="N67" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="O67" s="0" t="n">
-        <v>3</v>
+        <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N67" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O67" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q67" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R67" s="0" t="n">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="Q67" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R67" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="S67" s="5" t="s">
-        <v>187</v>
+        <v>33</v>
       </c>
       <c r="T67" s="1" t="str">
         <f aca="false">IF(NOT(D67="1X1"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c"),IF(E67="landmark",CONCATENATE(A67,"_k"),IF(E67="house",CONCATENATE(A67,"_h"),A67))))</f>
-        <v>convini_k</v>
+        <v>wooden_house_h</v>
       </c>
       <c r="U67" s="1" t="str">
         <f aca="false">IF(D67="1X1","none",IF(E67="skyscraper",CONCATENATE(A67,"_c_north"),IF(E67="landmark",CONCATENATE(A67,"_k_north"),IF(E67="house",CONCATENATE(A67,"_h_north"),CONCATENATE(A67,"_north")))))</f>
@@ -6603,76 +6609,76 @@
         <f aca="false">IF(NOT(D67="2X2"),"none",IF(E67="skyscraper",CONCATENATE(A67,"_c_south"),IF(E67="landmark",CONCATENATE(A67,"_k_south"),IF(E67="house",CONCATENATE(A67,"_h_south"),CONCATENATE(A67,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y67" s="0" t="s">
+      <c r="Y67" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C68" s="2" t="n">
-        <v>107</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G68" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="H68" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I68" s="4" t="n">
-        <v>1970</v>
+      <c r="G68" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I68" s="3" t="n">
+        <v>1950</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K68" s="1" t="n">
-        <v>20</v>
+      <c r="K68" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="M68" s="8" t="str">
         <f aca="false">VLOOKUP(L68,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
-      </c>
-      <c r="N68" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="O68" s="1" t="n">
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N68" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="O68" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="Q68" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="R68" s="1" t="n">
-        <v>2</v>
+      <c r="Q68" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R68" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="T68" s="1" t="str">
         <f aca="false">IF(NOT(D68="1X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c"),IF(E68="landmark",CONCATENATE(A68,"_k"),IF(E68="house",CONCATENATE(A68,"_h"),A68))))</f>
-        <v>none</v>
+        <v>convini_k</v>
       </c>
       <c r="U68" s="1" t="str">
         <f aca="false">IF(D68="1X1","none",IF(E68="skyscraper",CONCATENATE(A68,"_c_north"),IF(E68="landmark",CONCATENATE(A68,"_k_north"),IF(E68="house",CONCATENATE(A68,"_h_north"),CONCATENATE(A68,"_north")))))</f>
-        <v>fire_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V68" s="1" t="str">
         <f aca="false">IF(OR(D68="1X1",D68="2X1"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_east"),IF(E68="landmark",CONCATENATE(A68,"_k_east"),IF(E68="house",CONCATENATE(A68,"_h_east"),CONCATENATE(A68,"_east")))))</f>
@@ -6680,14 +6686,14 @@
       </c>
       <c r="W68" s="1" t="str">
         <f aca="false">IF(OR(D68="1X1",D68="1X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_west"),IF(E68="landmark",CONCATENATE(A68,"_k_west"),IF(E68="house",CONCATENATE(A68,"_h_west"),CONCATENATE(A68,"_west")))))</f>
-        <v>fire_station_k_west</v>
+        <v>none</v>
       </c>
       <c r="X68" s="1" t="str">
         <f aca="false">IF(NOT(D68="2X2"),"none",IF(E68="skyscraper",CONCATENATE(A68,"_c_south"),IF(E68="landmark",CONCATENATE(A68,"_k_south"),IF(E68="house",CONCATENATE(A68,"_h_south"),CONCATENATE(A68,"_south")))))</f>
         <v>none</v>
       </c>
-      <c r="Y68" s="1" t="s">
-        <v>189</v>
+      <c r="Y68" s="0" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6698,19 +6704,19 @@
         <v>192</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>200</v>
+        <v>107</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="H69" s="1" t="n">
         <v>3</v>
@@ -6725,14 +6731,14 @@
         <v>20</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="M69" s="8" t="str">
         <f aca="false">VLOOKUP(L69,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N69" s="1" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="O69" s="1" t="n">
         <v>3</v>
@@ -6744,10 +6750,10 @@
         <v>10</v>
       </c>
       <c r="R69" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S69" s="5" t="s">
-        <v>195</v>
+        <v>33</v>
       </c>
       <c r="T69" s="1" t="str">
         <f aca="false">IF(NOT(D69="1X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c"),IF(E69="landmark",CONCATENATE(A69,"_k"),IF(E69="house",CONCATENATE(A69,"_h"),A69))))</f>
@@ -6755,19 +6761,19 @@
       </c>
       <c r="U69" s="1" t="str">
         <f aca="false">IF(D69="1X1","none",IF(E69="skyscraper",CONCATENATE(A69,"_c_north"),IF(E69="landmark",CONCATENATE(A69,"_k_north"),IF(E69="house",CONCATENATE(A69,"_h_north"),CONCATENATE(A69,"_north")))))</f>
-        <v>hospital_k_north</v>
+        <v>fire_station_k_north</v>
       </c>
       <c r="V69" s="1" t="str">
-        <f aca="false">IF(OR(D69="1X1",D69="2X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_east"),IF(E69="landmark",CONCATENATE(A69,"_k_east"),CONCATENATE(A69,"_east"))))</f>
-        <v>hospital_k_east</v>
+        <f aca="false">IF(OR(D69="1X1",D69="2X1"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_east"),IF(E69="landmark",CONCATENATE(A69,"_k_east"),IF(E69="house",CONCATENATE(A69,"_h_east"),CONCATENATE(A69,"_east")))))</f>
+        <v>none</v>
       </c>
       <c r="W69" s="1" t="str">
-        <f aca="false">IF(OR(D69="1X1",D69="1X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_west"),IF(E69="landmark",CONCATENATE(A69,"_k_west"),CONCATENATE(A69,"_west"))))</f>
-        <v>hospital_k_west</v>
+        <f aca="false">IF(OR(D69="1X1",D69="1X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_west"),IF(E69="landmark",CONCATENATE(A69,"_k_west"),IF(E69="house",CONCATENATE(A69,"_h_west"),CONCATENATE(A69,"_west")))))</f>
+        <v>fire_station_k_west</v>
       </c>
       <c r="X69" s="1" t="str">
-        <f aca="false">IF(NOT(D69="2X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_south"),IF(E69="landmark",CONCATENATE(A69,"_k_south"),CONCATENATE(A69,"_south"))))</f>
-        <v>hospital_k_south</v>
+        <f aca="false">IF(NOT(D69="2X2"),"none",IF(E69="skyscraper",CONCATENATE(A69,"_c_south"),IF(E69="landmark",CONCATENATE(A69,"_k_south"),IF(E69="house",CONCATENATE(A69,"_h_south"),CONCATENATE(A69,"_south")))))</f>
+        <v>none</v>
       </c>
       <c r="Y69" s="1" t="s">
         <v>192</v>
@@ -6775,47 +6781,47 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>196</v>
       </c>
       <c r="G70" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H70" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I70" s="4" t="n">
-        <v>1870</v>
+        <v>1970</v>
       </c>
       <c r="J70" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K70" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="M70" s="8" t="str">
         <f aca="false">VLOOKUP(L70,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N70" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O70" s="1" t="n">
         <v>3</v>
@@ -6824,65 +6830,65 @@
         <v>162</v>
       </c>
       <c r="Q70" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="R70" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S70" s="5" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="T70" s="1" t="str">
         <f aca="false">IF(NOT(D70="1X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c"),IF(E70="landmark",CONCATENATE(A70,"_k"),IF(E70="house",CONCATENATE(A70,"_h"),A70))))</f>
-        <v>onsen_k</v>
+        <v>none</v>
       </c>
       <c r="U70" s="1" t="str">
         <f aca="false">IF(D70="1X1","none",IF(E70="skyscraper",CONCATENATE(A70,"_c_north"),IF(E70="landmark",CONCATENATE(A70,"_k_north"),IF(E70="house",CONCATENATE(A70,"_h_north"),CONCATENATE(A70,"_north")))))</f>
-        <v>none</v>
+        <v>hospital_k_north</v>
       </c>
       <c r="V70" s="1" t="str">
-        <f aca="false">IF(OR(D70="1X1",D70="2X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_east"),IF(E70="landmark",CONCATENATE(A70,"_k_east"),IF(E70="house",CONCATENATE(A70,"_h_east"),CONCATENATE(A70,"_east")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D70="1X1",D70="2X1"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_east"),IF(E70="landmark",CONCATENATE(A70,"_k_east"),CONCATENATE(A70,"_east"))))</f>
+        <v>hospital_k_east</v>
       </c>
       <c r="W70" s="1" t="str">
-        <f aca="false">IF(OR(D70="1X1",D70="1X2"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_west"),IF(E70="landmark",CONCATENATE(A70,"_k_west"),IF(E70="house",CONCATENATE(A70,"_h_west"),CONCATENATE(A70,"_west")))))</f>
-        <v>none</v>
+        <f aca="false">IF(OR(D70="1X1",D70="1X2"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_west"),IF(E70="landmark",CONCATENATE(A70,"_k_west"),CONCATENATE(A70,"_west"))))</f>
+        <v>hospital_k_west</v>
       </c>
       <c r="X70" s="1" t="str">
-        <f aca="false">IF(NOT(D70="2X2"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_south"),IF(E70="landmark",CONCATENATE(A70,"_k_south"),IF(E70="house",CONCATENATE(A70,"_h_south"),CONCATENATE(A70,"_south")))))</f>
-        <v>none</v>
+        <f aca="false">IF(NOT(D70="2X2"),"none",IF(E70="skyscraper",CONCATENATE(A70,"_c_south"),IF(E70="landmark",CONCATENATE(A70,"_k_south"),CONCATENATE(A70,"_south"))))</f>
+        <v>hospital_k_south</v>
       </c>
       <c r="Y70" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G71" s="1" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H71" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I71" s="4" t="n">
-        <v>1980</v>
+        <v>1870</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>30</v>
@@ -6891,11 +6897,11 @@
         <v>10</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="M71" s="8" t="str">
         <f aca="false">VLOOKUP(L71,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
       <c r="N71" s="1" t="n">
         <v>29</v>
@@ -6907,36 +6913,36 @@
         <v>162</v>
       </c>
       <c r="Q71" s="1" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="R71" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>199</v>
+        <v>33</v>
       </c>
       <c r="T71" s="1" t="str">
         <f aca="false">IF(NOT(D71="1X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c"),IF(E71="landmark",CONCATENATE(A71,"_k"),IF(E71="house",CONCATENATE(A71,"_h"),A71))))</f>
-        <v>pachinko_k</v>
+        <v>onsen_k</v>
       </c>
       <c r="U71" s="1" t="str">
         <f aca="false">IF(D71="1X1","none",IF(E71="skyscraper",CONCATENATE(A71,"_c_north"),IF(E71="landmark",CONCATENATE(A71,"_k_north"),IF(E71="house",CONCATENATE(A71,"_h_north"),CONCATENATE(A71,"_north")))))</f>
         <v>none</v>
       </c>
       <c r="V71" s="1" t="str">
-        <f aca="false">IF(OR(D71="1X1",D71="2X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_east"),IF(E71="landmark",CONCATENATE(A71,"_k_east"),CONCATENATE(A71,"_east"))))</f>
+        <f aca="false">IF(OR(D71="1X1",D71="2X1"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_east"),IF(E71="landmark",CONCATENATE(A71,"_k_east"),IF(E71="house",CONCATENATE(A71,"_h_east"),CONCATENATE(A71,"_east")))))</f>
         <v>none</v>
       </c>
       <c r="W71" s="1" t="str">
-        <f aca="false">IF(OR(D71="1X1",D71="1X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_west"),IF(E71="landmark",CONCATENATE(A71,"_k_west"),CONCATENATE(A71,"_west"))))</f>
+        <f aca="false">IF(OR(D71="1X1",D71="1X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_west"),IF(E71="landmark",CONCATENATE(A71,"_k_west"),IF(E71="house",CONCATENATE(A71,"_h_west"),CONCATENATE(A71,"_west")))))</f>
         <v>none</v>
       </c>
       <c r="X71" s="1" t="str">
-        <f aca="false">IF(NOT(D71="2X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_south"),IF(E71="landmark",CONCATENATE(A71,"_k_south"),CONCATENATE(A71,"_south"))))</f>
+        <f aca="false">IF(NOT(D71="2X2"),"none",IF(E71="skyscraper",CONCATENATE(A71,"_c_south"),IF(E71="landmark",CONCATENATE(A71,"_k_south"),IF(E71="house",CONCATENATE(A71,"_h_south"),CONCATENATE(A71,"_south")))))</f>
         <v>none</v>
       </c>
       <c r="Y71" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6947,41 +6953,41 @@
         <v>200</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>201</v>
       </c>
       <c r="G72" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H72" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I72" s="4" t="n">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K72" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>168</v>
+        <v>57</v>
       </c>
       <c r="M72" s="8" t="str">
         <f aca="false">VLOOKUP(L72,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+        <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
       <c r="N72" s="1" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="O72" s="1" t="n">
         <v>3</v>
@@ -6990,25 +6996,25 @@
         <v>162</v>
       </c>
       <c r="Q72" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="R72" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>125</v>
+        <v>202</v>
       </c>
       <c r="T72" s="1" t="str">
         <f aca="false">IF(NOT(D72="1X1"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c"),IF(E72="landmark",CONCATENATE(A72,"_k"),IF(E72="house",CONCATENATE(A72,"_h"),A72))))</f>
-        <v>none</v>
+        <v>pachinko_k</v>
       </c>
       <c r="U72" s="1" t="str">
         <f aca="false">IF(D72="1X1","none",IF(E72="skyscraper",CONCATENATE(A72,"_c_north"),IF(E72="landmark",CONCATENATE(A72,"_k_north"),IF(E72="house",CONCATENATE(A72,"_h_north"),CONCATENATE(A72,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>none</v>
       </c>
       <c r="V72" s="1" t="str">
         <f aca="false">IF(OR(D72="1X1",D72="2X1"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_east"),IF(E72="landmark",CONCATENATE(A72,"_k_east"),CONCATENATE(A72,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>none</v>
       </c>
       <c r="W72" s="1" t="str">
         <f aca="false">IF(OR(D72="1X1",D72="1X2"),"none",IF(E72="skyscraper",CONCATENATE(A72,"_c_west"),IF(E72="landmark",CONCATENATE(A72,"_k_west"),CONCATENATE(A72,"_west"))))</f>
@@ -7024,31 +7030,31 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G73" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="H73" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="H73" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I73" s="4" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J73" s="6" t="s">
         <v>30</v>
@@ -7057,20 +7063,20 @@
         <v>20</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="M73" s="8" t="str">
         <f aca="false">VLOOKUP(L73,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N73" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O73" s="0" t="n">
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
+      </c>
+      <c r="N73" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O73" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P73" s="5" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q73" s="1" t="n">
         <v>10</v>
@@ -7079,7 +7085,7 @@
         <v>2</v>
       </c>
       <c r="S73" s="5" t="s">
-        <v>199</v>
+        <v>125</v>
       </c>
       <c r="T73" s="1" t="str">
         <f aca="false">IF(NOT(D73="1X1"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c"),IF(E73="landmark",CONCATENATE(A73,"_k"),IF(E73="house",CONCATENATE(A73,"_h"),A73))))</f>
@@ -7087,51 +7093,51 @@
       </c>
       <c r="U73" s="1" t="str">
         <f aca="false">IF(D73="1X1","none",IF(E73="skyscraper",CONCATENATE(A73,"_c_north"),IF(E73="landmark",CONCATENATE(A73,"_k_north"),IF(E73="house",CONCATENATE(A73,"_h_north"),CONCATENATE(A73,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V73" s="1" t="str">
         <f aca="false">IF(OR(D73="1X1",D73="2X1"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c_east"),IF(E73="landmark",CONCATENATE(A73,"_k_east"),CONCATENATE(A73,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W73" s="1" t="str">
         <f aca="false">IF(OR(D73="1X1",D73="1X2"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c_west"),IF(E73="landmark",CONCATENATE(A73,"_k_west"),CONCATENATE(A73,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>none</v>
       </c>
       <c r="X73" s="1" t="str">
         <f aca="false">IF(NOT(D73="2X2"),"none",IF(E73="skyscraper",CONCATENATE(A73,"_c_south"),IF(E73="landmark",CONCATENATE(A73,"_k_south"),CONCATENATE(A73,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y73" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G74" s="1" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I74" s="4" t="n">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="J74" s="6" t="s">
         <v>30</v>
@@ -7140,14 +7146,14 @@
         <v>20</v>
       </c>
       <c r="L74" s="7" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="M74" s="8" t="str">
         <f aca="false">VLOOKUP(L74,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N74" s="0" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O74" s="0" t="n">
         <v>3</v>
@@ -7156,62 +7162,62 @@
         <v>122</v>
       </c>
       <c r="Q74" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R74" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S74" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="T74" s="1" t="str">
         <f aca="false">IF(NOT(D74="1X1"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c"),IF(E74="landmark",CONCATENATE(A74,"_k"),IF(E74="house",CONCATENATE(A74,"_h"),A74))))</f>
-        <v>shrine_k</v>
+        <v>none</v>
       </c>
       <c r="U74" s="1" t="str">
         <f aca="false">IF(D74="1X1","none",IF(E74="skyscraper",CONCATENATE(A74,"_c_north"),IF(E74="landmark",CONCATENATE(A74,"_k_north"),IF(E74="house",CONCATENATE(A74,"_h_north"),CONCATENATE(A74,"_north")))))</f>
-        <v>none</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V74" s="1" t="str">
         <f aca="false">IF(OR(D74="1X1",D74="2X1"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_east"),IF(E74="landmark",CONCATENATE(A74,"_k_east"),CONCATENATE(A74,"_east"))))</f>
-        <v>none</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W74" s="1" t="str">
         <f aca="false">IF(OR(D74="1X1",D74="1X2"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_west"),IF(E74="landmark",CONCATENATE(A74,"_k_west"),CONCATENATE(A74,"_west"))))</f>
-        <v>none</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X74" s="1" t="str">
         <f aca="false">IF(NOT(D74="2X2"),"none",IF(E74="skyscraper",CONCATENATE(A74,"_c_south"),IF(E74="landmark",CONCATENATE(A74,"_k_south"),CONCATENATE(A74,"_south"))))</f>
-        <v>none</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y74" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G75" s="1" t="n">
         <v>5</v>
       </c>
       <c r="H75" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I75" s="4" t="n">
         <v>0</v>
@@ -7223,7 +7229,7 @@
         <v>20</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="M75" s="8" t="str">
         <f aca="false">VLOOKUP(L75,dropdowns!E:F,2,0)</f>
@@ -7245,11 +7251,11 @@
         <v>1</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="T75" s="1" t="str">
         <f aca="false">IF(NOT(D75="1X1"),"none",IF(E75="skyscraper",CONCATENATE(A75,"_c"),IF(E75="landmark",CONCATENATE(A75,"_k"),IF(E75="house",CONCATENATE(A75,"_h"),A75))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>shrine_k</v>
       </c>
       <c r="U75" s="1" t="str">
         <f aca="false">IF(D75="1X1","none",IF(E75="skyscraper",CONCATENATE(A75,"_c_north"),IF(E75="landmark",CONCATENATE(A75,"_k_north"),IF(E75="house",CONCATENATE(A75,"_h_north"),CONCATENATE(A75,"_north")))))</f>
@@ -7268,36 +7274,36 @@
         <v>none</v>
       </c>
       <c r="Y75" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>159</v>
+        <v>27</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G76" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="H76" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="I76" s="4" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>30</v>
@@ -7306,81 +7312,81 @@
         <v>20</v>
       </c>
       <c r="L76" s="7" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="M76" s="8" t="str">
         <f aca="false">VLOOKUP(L76,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
-      </c>
-      <c r="N76" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O76" s="1" t="n">
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O76" s="0" t="n">
         <v>3</v>
       </c>
       <c r="P76" s="5" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="Q76" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R76" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="T76" s="1" t="str">
         <f aca="false">IF(NOT(D76="1X1"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c"),IF(E76="landmark",CONCATENATE(A76,"_k"),IF(E76="house",CONCATENATE(A76,"_h"),A76))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U76" s="1" t="str">
         <f aca="false">IF(D76="1X1","none",IF(E76="skyscraper",CONCATENATE(A76,"_c_north"),IF(E76="landmark",CONCATENATE(A76,"_k_north"),IF(E76="house",CONCATENATE(A76,"_h_north"),CONCATENATE(A76,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V76" s="1" t="str">
         <f aca="false">IF(OR(D76="1X1",D76="2X1"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c_east"),IF(E76="landmark",CONCATENATE(A76,"_k_east"),CONCATENATE(A76,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W76" s="1" t="str">
         <f aca="false">IF(OR(D76="1X1",D76="1X2"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c_west"),IF(E76="landmark",CONCATENATE(A76,"_k_west"),CONCATENATE(A76,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X76" s="1" t="str">
         <f aca="false">IF(NOT(D76="2X2"),"none",IF(E76="skyscraper",CONCATENATE(A76,"_c_south"),IF(E76="landmark",CONCATENATE(A76,"_k_south"),CONCATENATE(A76,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y76" s="1" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>159</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G77" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H77" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I77" s="4" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>30</v>
@@ -7389,11 +7395,11 @@
         <v>20</v>
       </c>
       <c r="L77" s="7" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="M77" s="8" t="str">
         <f aca="false">VLOOKUP(L77,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N77" s="1" t="n">
         <v>20</v>
@@ -7402,16 +7408,16 @@
         <v>3</v>
       </c>
       <c r="P77" s="5" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q77" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R77" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="T77" s="1" t="str">
         <f aca="false">IF(NOT(D77="1X1"),"none",IF(E77="skyscraper",CONCATENATE(A77,"_c"),IF(E77="landmark",CONCATENATE(A77,"_k"),IF(E77="house",CONCATENATE(A77,"_h"),A77))))</f>
@@ -7419,36 +7425,119 @@
       </c>
       <c r="U77" s="1" t="str">
         <f aca="false">IF(D77="1X1","none",IF(E77="skyscraper",CONCATENATE(A77,"_c_north"),IF(E77="landmark",CONCATENATE(A77,"_k_north"),IF(E77="house",CONCATENATE(A77,"_h_north"),CONCATENATE(A77,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>stadium_k_north</v>
       </c>
       <c r="V77" s="1" t="str">
         <f aca="false">IF(OR(D77="1X1",D77="2X1"),"none",IF(E77="skyscraper",CONCATENATE(A77,"_c_east"),IF(E77="landmark",CONCATENATE(A77,"_k_east"),CONCATENATE(A77,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>stadium_k_east</v>
       </c>
       <c r="W77" s="1" t="str">
         <f aca="false">IF(OR(D77="1X1",D77="1X2"),"none",IF(E77="skyscraper",CONCATENATE(A77,"_c_west"),IF(E77="landmark",CONCATENATE(A77,"_k_west"),CONCATENATE(A77,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>stadium_k_west</v>
       </c>
       <c r="X77" s="1" t="str">
         <f aca="false">IF(NOT(D77="2X2"),"none",IF(E77="skyscraper",CONCATENATE(A77,"_c_south"),IF(E77="landmark",CONCATENATE(A77,"_k_south"),CONCATENATE(A77,"_south"))))</f>
+        <v>stadium_k_south</v>
+      </c>
+      <c r="Y77" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G78" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I78" s="4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K78" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L78" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="M78" s="8" t="str">
+        <f aca="false">VLOOKUP(L78,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N78" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="O78" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P78" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q78" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R78" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S78" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="T78" s="1" t="str">
+        <f aca="false">IF(NOT(D78="1X1"),"none",IF(E78="skyscraper",CONCATENATE(A78,"_c"),IF(E78="landmark",CONCATENATE(A78,"_k"),IF(E78="house",CONCATENATE(A78,"_h"),A78))))</f>
+        <v>none</v>
+      </c>
+      <c r="U78" s="1" t="str">
+        <f aca="false">IF(D78="1X1","none",IF(E78="skyscraper",CONCATENATE(A78,"_c_north"),IF(E78="landmark",CONCATENATE(A78,"_k_north"),IF(E78="house",CONCATENATE(A78,"_h_north"),CONCATENATE(A78,"_north")))))</f>
+        <v>temple_k_north</v>
+      </c>
+      <c r="V78" s="1" t="str">
+        <f aca="false">IF(OR(D78="1X1",D78="2X1"),"none",IF(E78="skyscraper",CONCATENATE(A78,"_c_east"),IF(E78="landmark",CONCATENATE(A78,"_k_east"),CONCATENATE(A78,"_east"))))</f>
+        <v>temple_k_east</v>
+      </c>
+      <c r="W78" s="1" t="str">
+        <f aca="false">IF(OR(D78="1X1",D78="1X2"),"none",IF(E78="skyscraper",CONCATENATE(A78,"_c_west"),IF(E78="landmark",CONCATENATE(A78,"_k_west"),CONCATENATE(A78,"_west"))))</f>
+        <v>temple_k_west</v>
+      </c>
+      <c r="X78" s="1" t="str">
+        <f aca="false">IF(NOT(D78="2X2"),"none",IF(E78="skyscraper",CONCATENATE(A78,"_c_south"),IF(E78="landmark",CONCATENATE(A78,"_k_south"),CONCATENATE(A78,"_south"))))</f>
         <v>temple_k_south</v>
       </c>
-      <c r="Y77" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0"/>
-      <c r="D78" s="1"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="6"/>
-      <c r="L78" s="7"/>
-      <c r="M78" s="8"/>
-      <c r="P78" s="5"/>
-      <c r="S78" s="5"/>
+      <c r="Y78" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0"/>
+      <c r="D79" s="1"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="6"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="P79" s="5"/>
+      <c r="S79" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C66 C68:C1048576">
+  <conditionalFormatting sqref="C1:C67 C69:C1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -7456,15 +7545,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L78" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L79" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P78" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P79" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S78" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S79" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7487,33 +7576,34 @@
   <dimension ref="A1:G257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="4" min="3" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>214</v>
+      <c r="A1" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="str">
@@ -7536,7 +7626,7 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="str">
@@ -7559,7 +7649,7 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="str">
@@ -7582,7 +7672,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="str">
@@ -7605,7 +7695,7 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="str">
@@ -7628,7 +7718,7 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="str">
@@ -7651,7 +7741,7 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="str">
@@ -7674,7 +7764,7 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="str">
@@ -7697,7 +7787,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="str">
@@ -7720,7 +7810,7 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="str">
@@ -7743,7 +7833,7 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="str">
@@ -7766,7 +7856,7 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="str">
@@ -7789,7 +7879,7 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="str">
@@ -7812,7 +7902,7 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="str">
@@ -7835,7 +7925,7 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="str">
@@ -7858,7 +7948,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="str">
@@ -7881,7 +7971,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="4" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="str">
@@ -7904,7 +7994,7 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="str">
@@ -7927,7 +8017,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="str">
@@ -7950,7 +8040,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="str">
@@ -7973,7 +8063,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="str">
@@ -7996,7 +8086,7 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="4" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="str">
@@ -8019,30 +8109,30 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="4" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A24,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="false">IF(B24="2X2",4,IF(OR(B24="1X2",B24="2X1"),2,IF(B24="1X1",1,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="n">
         <f aca="false">IF(C24&gt;0,C24,MAX(D23-1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="9" t="n">
         <f aca="false">D24=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="4" t="n">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="str">
@@ -8065,7 +8155,7 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="4" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="str">
@@ -8088,7 +8178,7 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="4" t="n">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="str">
@@ -8111,7 +8201,7 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="4" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="str">
@@ -8134,7 +8224,7 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="4" t="n">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="str">
@@ -8157,7 +8247,7 @@
       <c r="G29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="4" t="n">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="str">
@@ -8180,7 +8270,7 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="4" t="n">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="str">
@@ -8203,7 +8293,7 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="4" t="n">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="str">
@@ -8226,7 +8316,7 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="4" t="n">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="str">
@@ -8249,7 +8339,7 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="4" t="n">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="str">
@@ -8272,7 +8362,7 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="4" t="n">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="str">
@@ -8295,7 +8385,7 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="4" t="n">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="str">
@@ -8318,7 +8408,7 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="4" t="n">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="str">
@@ -8341,7 +8431,7 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="4" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="str">
@@ -8364,7 +8454,7 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="4" t="n">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="str">
@@ -8387,7 +8477,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="4" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="str">
@@ -8410,7 +8500,7 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="4" t="n">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="str">
@@ -8433,7 +8523,7 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="4" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="str">
@@ -8456,7 +8546,7 @@
       <c r="G42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="4" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="str">
@@ -8479,7 +8569,7 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="4" t="n">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="str">
@@ -8502,7 +8592,7 @@
       <c r="G44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="4" t="n">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="str">
@@ -8525,7 +8615,7 @@
       <c r="G45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="4" t="n">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="str">
@@ -8548,7 +8638,7 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="4" t="n">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="str">
@@ -8571,7 +8661,7 @@
       <c r="G47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="4" t="n">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="str">
@@ -8594,7 +8684,7 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="4" t="n">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="str">
@@ -8617,7 +8707,7 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="4" t="n">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="str">
@@ -8640,7 +8730,7 @@
       <c r="G50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="4" t="n">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="str">
@@ -8663,7 +8753,7 @@
       <c r="G51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="4" t="n">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="str">
@@ -8686,7 +8776,7 @@
       <c r="G52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="4" t="n">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="str">
@@ -8709,7 +8799,7 @@
       <c r="G53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="4" t="n">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="str">
@@ -8732,7 +8822,7 @@
       <c r="G54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="4" t="n">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="str">
@@ -8755,7 +8845,7 @@
       <c r="G55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="4" t="n">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="str">
@@ -8778,7 +8868,7 @@
       <c r="G56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="4" t="n">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="str">
@@ -8801,7 +8891,7 @@
       <c r="G57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="4" t="n">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="str">
@@ -8824,7 +8914,7 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="4" t="n">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="str">
@@ -8847,7 +8937,7 @@
       <c r="G59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="4" t="n">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="str">
@@ -8870,7 +8960,7 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="4" t="n">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="str">
@@ -8893,7 +8983,7 @@
       <c r="G61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="4" t="n">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="str">
@@ -8916,7 +9006,7 @@
       <c r="G62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="4" t="n">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="str">
@@ -8939,7 +9029,7 @@
       <c r="G63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="4" t="n">
         <v>62</v>
       </c>
       <c r="B64" s="1" t="str">
@@ -8962,7 +9052,7 @@
       <c r="G64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="4" t="n">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="str">
@@ -8985,7 +9075,7 @@
       <c r="G65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="4" t="n">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="str">
@@ -9008,7 +9098,7 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="4" t="n">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="str">
@@ -9031,7 +9121,7 @@
       <c r="G67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="4" t="n">
         <v>66</v>
       </c>
       <c r="B68" s="1" t="str">
@@ -9054,7 +9144,7 @@
       <c r="G68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="4" t="n">
         <v>67</v>
       </c>
       <c r="B69" s="1" t="str">
@@ -9077,7 +9167,7 @@
       <c r="G69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="4" t="n">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="str">
@@ -9100,7 +9190,7 @@
       <c r="G70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="4" t="n">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="str">
@@ -9123,7 +9213,7 @@
       <c r="G71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="4" t="n">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="str">
@@ -9146,7 +9236,7 @@
       <c r="G72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="4" t="n">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="str">
@@ -9169,7 +9259,7 @@
       <c r="G73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="4" t="n">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="str">
@@ -9192,7 +9282,7 @@
       <c r="G74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="4" t="n">
         <v>73</v>
       </c>
       <c r="B75" s="1" t="str">
@@ -9215,7 +9305,7 @@
       <c r="G75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="4" t="n">
         <v>74</v>
       </c>
       <c r="B76" s="1" t="str">
@@ -9238,7 +9328,7 @@
       <c r="G76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="4" t="n">
         <v>75</v>
       </c>
       <c r="B77" s="1" t="str">
@@ -9261,7 +9351,7 @@
       <c r="G77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="4" t="n">
         <v>76</v>
       </c>
       <c r="B78" s="1" t="str">
@@ -9284,7 +9374,7 @@
       <c r="G78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="4" t="n">
         <v>77</v>
       </c>
       <c r="B79" s="1" t="str">
@@ -9307,7 +9397,7 @@
       <c r="G79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="4" t="n">
         <v>78</v>
       </c>
       <c r="B80" s="1" t="str">
@@ -9330,7 +9420,7 @@
       <c r="G80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="4" t="n">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="str">
@@ -9353,7 +9443,7 @@
       <c r="G81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="4" t="n">
         <v>80</v>
       </c>
       <c r="B82" s="1" t="str">
@@ -9376,7 +9466,7 @@
       <c r="G82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="4" t="n">
         <v>81</v>
       </c>
       <c r="B83" s="1" t="str">
@@ -9399,7 +9489,7 @@
       <c r="G83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="4" t="n">
         <v>82</v>
       </c>
       <c r="B84" s="1" t="str">
@@ -9422,7 +9512,7 @@
       <c r="G84" s="1"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="4" t="n">
         <v>83</v>
       </c>
       <c r="B85" s="1" t="str">
@@ -9445,7 +9535,7 @@
       <c r="G85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="4" t="n">
         <v>84</v>
       </c>
       <c r="B86" s="1" t="str">
@@ -9468,7 +9558,7 @@
       <c r="G86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="4" t="n">
         <v>85</v>
       </c>
       <c r="B87" s="1" t="str">
@@ -9491,7 +9581,7 @@
       <c r="G87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="4" t="n">
         <v>86</v>
       </c>
       <c r="B88" s="1" t="str">
@@ -9514,7 +9604,7 @@
       <c r="G88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="4" t="n">
         <v>87</v>
       </c>
       <c r="B89" s="1" t="str">
@@ -9537,7 +9627,7 @@
       <c r="G89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="4" t="n">
         <v>88</v>
       </c>
       <c r="B90" s="1" t="str">
@@ -9560,7 +9650,7 @@
       <c r="G90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="4" t="n">
         <v>89</v>
       </c>
       <c r="B91" s="1" t="str">
@@ -9583,7 +9673,7 @@
       <c r="G91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="4" t="n">
         <v>90</v>
       </c>
       <c r="B92" s="1" t="str">
@@ -9606,7 +9696,7 @@
       <c r="G92" s="1"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="4" t="n">
         <v>91</v>
       </c>
       <c r="B93" s="1" t="str">
@@ -9629,7 +9719,7 @@
       <c r="G93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="4" t="n">
         <v>92</v>
       </c>
       <c r="B94" s="1" t="str">
@@ -9652,7 +9742,7 @@
       <c r="G94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="4" t="n">
         <v>93</v>
       </c>
       <c r="B95" s="1" t="str">
@@ -9675,7 +9765,7 @@
       <c r="G95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="4" t="n">
         <v>94</v>
       </c>
       <c r="B96" s="1" t="str">
@@ -9698,7 +9788,7 @@
       <c r="G96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="4" t="n">
         <v>95</v>
       </c>
       <c r="B97" s="1" t="str">
@@ -9721,7 +9811,7 @@
       <c r="G97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="4" t="n">
         <v>96</v>
       </c>
       <c r="B98" s="1" t="str">
@@ -9744,7 +9834,7 @@
       <c r="G98" s="1"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="4" t="n">
         <v>97</v>
       </c>
       <c r="B99" s="1" t="str">
@@ -9767,7 +9857,7 @@
       <c r="G99" s="1"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="4" t="n">
         <v>98</v>
       </c>
       <c r="B100" s="1" t="str">
@@ -9790,7 +9880,7 @@
       <c r="G100" s="1"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="4" t="n">
         <v>99</v>
       </c>
       <c r="B101" s="1" t="str">
@@ -9813,7 +9903,7 @@
       <c r="G101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="4" t="n">
         <v>100</v>
       </c>
       <c r="B102" s="1" t="str">
@@ -9836,7 +9926,7 @@
       <c r="G102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="4" t="n">
         <v>101</v>
       </c>
       <c r="B103" s="1" t="str">
@@ -9859,7 +9949,7 @@
       <c r="G103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="4" t="n">
         <v>102</v>
       </c>
       <c r="B104" s="1" t="str">
@@ -9882,7 +9972,7 @@
       <c r="G104" s="1"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="4" t="n">
         <v>103</v>
       </c>
       <c r="B105" s="1" t="str">
@@ -9905,7 +9995,7 @@
       <c r="G105" s="1"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="4" t="n">
         <v>104</v>
       </c>
       <c r="B106" s="1" t="str">
@@ -9928,7 +10018,7 @@
       <c r="G106" s="1"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="4" t="n">
         <v>105</v>
       </c>
       <c r="B107" s="1" t="str">
@@ -9951,7 +10041,7 @@
       <c r="G107" s="1"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="4" t="n">
         <v>106</v>
       </c>
       <c r="B108" s="1" t="str">
@@ -9974,7 +10064,7 @@
       <c r="G108" s="1"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="4" t="n">
         <v>107</v>
       </c>
       <c r="B109" s="1" t="str">
@@ -9997,7 +10087,7 @@
       <c r="G109" s="1"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="4" t="n">
         <v>108</v>
       </c>
       <c r="B110" s="1" t="str">
@@ -10020,7 +10110,7 @@
       <c r="G110" s="1"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="4" t="n">
         <v>109</v>
       </c>
       <c r="B111" s="1" t="str">
@@ -10043,7 +10133,7 @@
       <c r="G111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="4" t="n">
         <v>110</v>
       </c>
       <c r="B112" s="1" t="str">
@@ -10066,7 +10156,7 @@
       <c r="G112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="4" t="n">
         <v>111</v>
       </c>
       <c r="B113" s="1" t="str">
@@ -10089,7 +10179,7 @@
       <c r="G113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="4" t="n">
         <v>112</v>
       </c>
       <c r="B114" s="1" t="str">
@@ -10112,7 +10202,7 @@
       <c r="G114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="4" t="n">
         <v>113</v>
       </c>
       <c r="B115" s="1" t="str">
@@ -10135,7 +10225,7 @@
       <c r="G115" s="1"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="4" t="n">
         <v>114</v>
       </c>
       <c r="B116" s="1" t="str">
@@ -10158,7 +10248,7 @@
       <c r="G116" s="1"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="4" t="n">
         <v>115</v>
       </c>
       <c r="B117" s="1" t="str">
@@ -10181,7 +10271,7 @@
       <c r="G117" s="1"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="4" t="n">
         <v>116</v>
       </c>
       <c r="B118" s="1" t="str">
@@ -10204,7 +10294,7 @@
       <c r="G118" s="1"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="4" t="n">
         <v>117</v>
       </c>
       <c r="B119" s="1" t="str">
@@ -10227,7 +10317,7 @@
       <c r="G119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="4" t="n">
         <v>118</v>
       </c>
       <c r="B120" s="1" t="str">
@@ -10250,7 +10340,7 @@
       <c r="G120" s="1"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="4" t="n">
         <v>119</v>
       </c>
       <c r="B121" s="1" t="str">
@@ -10273,7 +10363,7 @@
       <c r="G121" s="1"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="4" t="n">
         <v>120</v>
       </c>
       <c r="B122" s="1" t="str">
@@ -10296,7 +10386,7 @@
       <c r="G122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="4" t="n">
         <v>121</v>
       </c>
       <c r="B123" s="1" t="str">
@@ -10319,7 +10409,7 @@
       <c r="G123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="4" t="n">
         <v>122</v>
       </c>
       <c r="B124" s="1" t="str">
@@ -10342,7 +10432,7 @@
       <c r="G124" s="1"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="4" t="n">
         <v>123</v>
       </c>
       <c r="B125" s="1" t="str">
@@ -10365,7 +10455,7 @@
       <c r="G125" s="1"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="4" t="n">
         <v>124</v>
       </c>
       <c r="B126" s="1" t="str">
@@ -10388,7 +10478,7 @@
       <c r="G126" s="1"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="4" t="n">
         <v>125</v>
       </c>
       <c r="B127" s="1" t="str">
@@ -10411,7 +10501,7 @@
       <c r="G127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="4" t="n">
         <v>126</v>
       </c>
       <c r="B128" s="1" t="str">
@@ -10434,7 +10524,7 @@
       <c r="G128" s="1"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="4" t="n">
         <v>127</v>
       </c>
       <c r="B129" s="1" t="str">
@@ -10457,7 +10547,7 @@
       <c r="G129" s="1"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="4" t="n">
         <v>128</v>
       </c>
       <c r="B130" s="1" t="str">
@@ -10480,7 +10570,7 @@
       <c r="G130" s="1"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="4" t="n">
         <v>129</v>
       </c>
       <c r="B131" s="1" t="str">
@@ -10503,7 +10593,7 @@
       <c r="G131" s="1"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="4" t="n">
         <v>130</v>
       </c>
       <c r="B132" s="1" t="str">
@@ -10526,7 +10616,7 @@
       <c r="G132" s="1"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="4" t="n">
         <v>131</v>
       </c>
       <c r="B133" s="1" t="str">
@@ -10549,7 +10639,7 @@
       <c r="G133" s="1"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="4" t="n">
         <v>132</v>
       </c>
       <c r="B134" s="1" t="str">
@@ -10572,7 +10662,7 @@
       <c r="G134" s="1"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="4" t="n">
         <v>133</v>
       </c>
       <c r="B135" s="1" t="str">
@@ -10595,7 +10685,7 @@
       <c r="G135" s="1"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="4" t="n">
         <v>134</v>
       </c>
       <c r="B136" s="1" t="str">
@@ -10618,7 +10708,7 @@
       <c r="G136" s="1"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="4" t="n">
         <v>135</v>
       </c>
       <c r="B137" s="1" t="str">
@@ -10641,7 +10731,7 @@
       <c r="G137" s="1"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="4" t="n">
         <v>136</v>
       </c>
       <c r="B138" s="1" t="str">
@@ -10664,7 +10754,7 @@
       <c r="G138" s="1"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="4" t="n">
         <v>137</v>
       </c>
       <c r="B139" s="1" t="str">
@@ -10687,7 +10777,7 @@
       <c r="G139" s="1"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="4" t="n">
         <v>138</v>
       </c>
       <c r="B140" s="1" t="str">
@@ -10710,7 +10800,7 @@
       <c r="G140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="4" t="n">
         <v>139</v>
       </c>
       <c r="B141" s="1" t="str">
@@ -10733,7 +10823,7 @@
       <c r="G141" s="1"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="4" t="n">
         <v>140</v>
       </c>
       <c r="B142" s="1" t="str">
@@ -10756,7 +10846,7 @@
       <c r="G142" s="1"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="4" t="n">
         <v>141</v>
       </c>
       <c r="B143" s="1" t="str">
@@ -10779,7 +10869,7 @@
       <c r="G143" s="1"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="4" t="n">
         <v>142</v>
       </c>
       <c r="B144" s="1" t="str">
@@ -10802,7 +10892,7 @@
       <c r="G144" s="1"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="4" t="n">
         <v>143</v>
       </c>
       <c r="B145" s="1" t="str">
@@ -10825,7 +10915,7 @@
       <c r="G145" s="1"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="4" t="n">
         <v>144</v>
       </c>
       <c r="B146" s="1" t="str">
@@ -10848,7 +10938,7 @@
       <c r="G146" s="1"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="4" t="n">
         <v>145</v>
       </c>
       <c r="B147" s="1" t="str">
@@ -10871,7 +10961,7 @@
       <c r="G147" s="1"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="4" t="n">
         <v>146</v>
       </c>
       <c r="B148" s="1" t="str">
@@ -10894,7 +10984,7 @@
       <c r="G148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="4" t="n">
         <v>147</v>
       </c>
       <c r="B149" s="1" t="str">
@@ -10917,7 +11007,7 @@
       <c r="G149" s="1"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="4" t="n">
         <v>148</v>
       </c>
       <c r="B150" s="1" t="str">
@@ -10940,7 +11030,7 @@
       <c r="G150" s="1"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="4" t="n">
         <v>149</v>
       </c>
       <c r="B151" s="1" t="str">
@@ -10963,7 +11053,7 @@
       <c r="G151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="4" t="n">
         <v>150</v>
       </c>
       <c r="B152" s="1" t="str">
@@ -10986,7 +11076,7 @@
       <c r="G152" s="1"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="4" t="n">
         <v>151</v>
       </c>
       <c r="B153" s="1" t="str">
@@ -11009,7 +11099,7 @@
       <c r="G153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="4" t="n">
         <v>152</v>
       </c>
       <c r="B154" s="1" t="str">
@@ -11032,7 +11122,7 @@
       <c r="G154" s="1"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="4" t="n">
         <v>153</v>
       </c>
       <c r="B155" s="1" t="str">
@@ -11055,7 +11145,7 @@
       <c r="G155" s="1"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="4" t="n">
         <v>154</v>
       </c>
       <c r="B156" s="1" t="str">
@@ -11078,7 +11168,7 @@
       <c r="G156" s="1"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="4" t="n">
         <v>155</v>
       </c>
       <c r="B157" s="1" t="str">
@@ -11101,7 +11191,7 @@
       <c r="G157" s="1"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="4" t="n">
         <v>156</v>
       </c>
       <c r="B158" s="1" t="str">
@@ -11124,7 +11214,7 @@
       <c r="G158" s="1"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="4" t="n">
         <v>157</v>
       </c>
       <c r="B159" s="1" t="str">
@@ -11147,7 +11237,7 @@
       <c r="G159" s="1"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="4" t="n">
         <v>158</v>
       </c>
       <c r="B160" s="1" t="str">
@@ -11170,7 +11260,7 @@
       <c r="G160" s="1"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="4" t="n">
         <v>159</v>
       </c>
       <c r="B161" s="1" t="str">
@@ -11193,7 +11283,7 @@
       <c r="G161" s="1"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="4" t="n">
         <v>160</v>
       </c>
       <c r="B162" s="1" t="str">
@@ -11216,7 +11306,7 @@
       <c r="G162" s="1"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="4" t="n">
         <v>161</v>
       </c>
       <c r="B163" s="1" t="str">
@@ -11239,7 +11329,7 @@
       <c r="G163" s="1"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="n">
+      <c r="A164" s="4" t="n">
         <v>162</v>
       </c>
       <c r="B164" s="1" t="str">
@@ -11262,7 +11352,7 @@
       <c r="G164" s="1"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="n">
+      <c r="A165" s="4" t="n">
         <v>163</v>
       </c>
       <c r="B165" s="1" t="str">
@@ -11285,7 +11375,7 @@
       <c r="G165" s="1"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="n">
+      <c r="A166" s="4" t="n">
         <v>164</v>
       </c>
       <c r="B166" s="1" t="str">
@@ -11308,7 +11398,7 @@
       <c r="G166" s="1"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="n">
+      <c r="A167" s="4" t="n">
         <v>165</v>
       </c>
       <c r="B167" s="1" t="str">
@@ -11331,7 +11421,7 @@
       <c r="G167" s="1"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="n">
+      <c r="A168" s="4" t="n">
         <v>166</v>
       </c>
       <c r="B168" s="1" t="str">
@@ -11354,7 +11444,7 @@
       <c r="G168" s="1"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="n">
+      <c r="A169" s="4" t="n">
         <v>167</v>
       </c>
       <c r="B169" s="1" t="str">
@@ -11377,7 +11467,7 @@
       <c r="G169" s="1"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="n">
+      <c r="A170" s="4" t="n">
         <v>168</v>
       </c>
       <c r="B170" s="1" t="str">
@@ -11400,7 +11490,7 @@
       <c r="G170" s="1"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="n">
+      <c r="A171" s="4" t="n">
         <v>169</v>
       </c>
       <c r="B171" s="1" t="str">
@@ -11423,7 +11513,7 @@
       <c r="G171" s="1"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="n">
+      <c r="A172" s="4" t="n">
         <v>170</v>
       </c>
       <c r="B172" s="1" t="str">
@@ -11446,7 +11536,7 @@
       <c r="G172" s="1"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="n">
+      <c r="A173" s="4" t="n">
         <v>171</v>
       </c>
       <c r="B173" s="1" t="str">
@@ -11469,7 +11559,7 @@
       <c r="G173" s="1"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="n">
+      <c r="A174" s="4" t="n">
         <v>172</v>
       </c>
       <c r="B174" s="1" t="str">
@@ -11492,7 +11582,7 @@
       <c r="G174" s="1"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="n">
+      <c r="A175" s="4" t="n">
         <v>173</v>
       </c>
       <c r="B175" s="1" t="str">
@@ -11515,7 +11605,7 @@
       <c r="G175" s="1"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="n">
+      <c r="A176" s="4" t="n">
         <v>174</v>
       </c>
       <c r="B176" s="1" t="str">
@@ -11538,7 +11628,7 @@
       <c r="G176" s="1"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="n">
+      <c r="A177" s="4" t="n">
         <v>175</v>
       </c>
       <c r="B177" s="1" t="str">
@@ -11561,7 +11651,7 @@
       <c r="G177" s="1"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="n">
+      <c r="A178" s="4" t="n">
         <v>176</v>
       </c>
       <c r="B178" s="1" t="str">
@@ -11584,7 +11674,7 @@
       <c r="G178" s="1"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="n">
+      <c r="A179" s="4" t="n">
         <v>177</v>
       </c>
       <c r="B179" s="1" t="str">
@@ -11607,7 +11697,7 @@
       <c r="G179" s="1"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="n">
+      <c r="A180" s="4" t="n">
         <v>178</v>
       </c>
       <c r="B180" s="1" t="str">
@@ -11630,7 +11720,7 @@
       <c r="G180" s="1"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="n">
+      <c r="A181" s="4" t="n">
         <v>179</v>
       </c>
       <c r="B181" s="1" t="str">
@@ -11653,7 +11743,7 @@
       <c r="G181" s="1"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="n">
+      <c r="A182" s="4" t="n">
         <v>180</v>
       </c>
       <c r="B182" s="1" t="str">
@@ -11676,7 +11766,7 @@
       <c r="G182" s="1"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="n">
+      <c r="A183" s="4" t="n">
         <v>181</v>
       </c>
       <c r="B183" s="1" t="str">
@@ -11699,7 +11789,7 @@
       <c r="G183" s="1"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="n">
+      <c r="A184" s="4" t="n">
         <v>182</v>
       </c>
       <c r="B184" s="1" t="str">
@@ -11722,7 +11812,7 @@
       <c r="G184" s="1"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="n">
+      <c r="A185" s="4" t="n">
         <v>183</v>
       </c>
       <c r="B185" s="1" t="str">
@@ -11745,7 +11835,7 @@
       <c r="G185" s="1"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="1" t="n">
+      <c r="A186" s="4" t="n">
         <v>184</v>
       </c>
       <c r="B186" s="1" t="str">
@@ -11768,7 +11858,7 @@
       <c r="G186" s="1"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="n">
+      <c r="A187" s="4" t="n">
         <v>185</v>
       </c>
       <c r="B187" s="1" t="str">
@@ -11791,7 +11881,7 @@
       <c r="G187" s="1"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="n">
+      <c r="A188" s="4" t="n">
         <v>186</v>
       </c>
       <c r="B188" s="1" t="str">
@@ -11814,7 +11904,7 @@
       <c r="G188" s="1"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="1" t="n">
+      <c r="A189" s="4" t="n">
         <v>187</v>
       </c>
       <c r="B189" s="1" t="str">
@@ -11837,7 +11927,7 @@
       <c r="G189" s="1"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="n">
+      <c r="A190" s="4" t="n">
         <v>188</v>
       </c>
       <c r="B190" s="1" t="str">
@@ -11860,7 +11950,7 @@
       <c r="G190" s="1"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="1" t="n">
+      <c r="A191" s="4" t="n">
         <v>189</v>
       </c>
       <c r="B191" s="1" t="str">
@@ -11883,7 +11973,7 @@
       <c r="G191" s="1"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="1" t="n">
+      <c r="A192" s="4" t="n">
         <v>190</v>
       </c>
       <c r="B192" s="1" t="str">
@@ -11906,7 +11996,7 @@
       <c r="G192" s="1"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="n">
+      <c r="A193" s="4" t="n">
         <v>191</v>
       </c>
       <c r="B193" s="1" t="str">
@@ -11929,7 +12019,7 @@
       <c r="G193" s="1"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="n">
+      <c r="A194" s="4" t="n">
         <v>192</v>
       </c>
       <c r="B194" s="1" t="str">
@@ -11952,7 +12042,7 @@
       <c r="G194" s="1"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="1" t="n">
+      <c r="A195" s="4" t="n">
         <v>193</v>
       </c>
       <c r="B195" s="1" t="str">
@@ -11975,7 +12065,7 @@
       <c r="G195" s="1"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="1" t="n">
+      <c r="A196" s="4" t="n">
         <v>194</v>
       </c>
       <c r="B196" s="1" t="str">
@@ -11998,7 +12088,7 @@
       <c r="G196" s="1"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="n">
+      <c r="A197" s="4" t="n">
         <v>195</v>
       </c>
       <c r="B197" s="1" t="str">
@@ -12021,7 +12111,7 @@
       <c r="G197" s="1"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="n">
+      <c r="A198" s="4" t="n">
         <v>196</v>
       </c>
       <c r="B198" s="1" t="str">
@@ -12044,7 +12134,7 @@
       <c r="G198" s="1"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="1" t="n">
+      <c r="A199" s="4" t="n">
         <v>197</v>
       </c>
       <c r="B199" s="1" t="str">
@@ -12067,7 +12157,7 @@
       <c r="G199" s="1"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="n">
+      <c r="A200" s="4" t="n">
         <v>198</v>
       </c>
       <c r="B200" s="1" t="str">
@@ -12090,7 +12180,7 @@
       <c r="G200" s="1"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1" t="n">
+      <c r="A201" s="4" t="n">
         <v>199</v>
       </c>
       <c r="B201" s="1" t="str">
@@ -12113,7 +12203,7 @@
       <c r="G201" s="1"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="n">
+      <c r="A202" s="4" t="n">
         <v>200</v>
       </c>
       <c r="B202" s="1" t="str">
@@ -12136,7 +12226,7 @@
       <c r="G202" s="1"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="n">
+      <c r="A203" s="4" t="n">
         <v>201</v>
       </c>
       <c r="B203" s="1" t="str">
@@ -12159,7 +12249,7 @@
       <c r="G203" s="1"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1" t="n">
+      <c r="A204" s="4" t="n">
         <v>202</v>
       </c>
       <c r="B204" s="1" t="str">
@@ -12182,7 +12272,7 @@
       <c r="G204" s="1"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="1" t="n">
+      <c r="A205" s="4" t="n">
         <v>203</v>
       </c>
       <c r="B205" s="1" t="str">
@@ -12205,7 +12295,7 @@
       <c r="G205" s="1"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1" t="n">
+      <c r="A206" s="4" t="n">
         <v>204</v>
       </c>
       <c r="B206" s="1" t="str">
@@ -12228,7 +12318,7 @@
       <c r="G206" s="1"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="n">
+      <c r="A207" s="4" t="n">
         <v>205</v>
       </c>
       <c r="B207" s="1" t="str">
@@ -12251,7 +12341,7 @@
       <c r="G207" s="1"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="n">
+      <c r="A208" s="4" t="n">
         <v>206</v>
       </c>
       <c r="B208" s="1" t="str">
@@ -12274,7 +12364,7 @@
       <c r="G208" s="1"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="1" t="n">
+      <c r="A209" s="4" t="n">
         <v>207</v>
       </c>
       <c r="B209" s="1" t="str">
@@ -12297,7 +12387,7 @@
       <c r="G209" s="1"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="1" t="n">
+      <c r="A210" s="4" t="n">
         <v>208</v>
       </c>
       <c r="B210" s="1" t="str">
@@ -12320,7 +12410,7 @@
       <c r="G210" s="1"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1" t="n">
+      <c r="A211" s="4" t="n">
         <v>209</v>
       </c>
       <c r="B211" s="1" t="str">
@@ -12343,7 +12433,7 @@
       <c r="G211" s="1"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="1" t="n">
+      <c r="A212" s="4" t="n">
         <v>210</v>
       </c>
       <c r="B212" s="1" t="str">
@@ -12366,7 +12456,7 @@
       <c r="G212" s="1"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="1" t="n">
+      <c r="A213" s="4" t="n">
         <v>211</v>
       </c>
       <c r="B213" s="1" t="str">
@@ -12389,7 +12479,7 @@
       <c r="G213" s="1"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="1" t="n">
+      <c r="A214" s="4" t="n">
         <v>212</v>
       </c>
       <c r="B214" s="1" t="str">
@@ -12412,7 +12502,7 @@
       <c r="G214" s="1"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="1" t="n">
+      <c r="A215" s="4" t="n">
         <v>213</v>
       </c>
       <c r="B215" s="1" t="str">
@@ -12435,7 +12525,7 @@
       <c r="G215" s="1"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="n">
+      <c r="A216" s="4" t="n">
         <v>214</v>
       </c>
       <c r="B216" s="1" t="str">
@@ -12458,7 +12548,7 @@
       <c r="G216" s="1"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="1" t="n">
+      <c r="A217" s="4" t="n">
         <v>215</v>
       </c>
       <c r="B217" s="1" t="str">
@@ -12481,7 +12571,7 @@
       <c r="G217" s="1"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1" t="n">
+      <c r="A218" s="4" t="n">
         <v>216</v>
       </c>
       <c r="B218" s="1" t="str">
@@ -12504,7 +12594,7 @@
       <c r="G218" s="1"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="n">
+      <c r="A219" s="4" t="n">
         <v>217</v>
       </c>
       <c r="B219" s="1" t="str">
@@ -12527,7 +12617,7 @@
       <c r="G219" s="1"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="1" t="n">
+      <c r="A220" s="4" t="n">
         <v>218</v>
       </c>
       <c r="B220" s="1" t="str">
@@ -12550,7 +12640,7 @@
       <c r="G220" s="1"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="1" t="n">
+      <c r="A221" s="4" t="n">
         <v>219</v>
       </c>
       <c r="B221" s="1" t="str">
@@ -12573,7 +12663,7 @@
       <c r="G221" s="1"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="1" t="n">
+      <c r="A222" s="4" t="n">
         <v>220</v>
       </c>
       <c r="B222" s="1" t="str">
@@ -12596,7 +12686,7 @@
       <c r="G222" s="1"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="1" t="n">
+      <c r="A223" s="4" t="n">
         <v>221</v>
       </c>
       <c r="B223" s="1" t="str">
@@ -12619,7 +12709,7 @@
       <c r="G223" s="1"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="1" t="n">
+      <c r="A224" s="4" t="n">
         <v>222</v>
       </c>
       <c r="B224" s="1" t="str">
@@ -12642,7 +12732,7 @@
       <c r="G224" s="1"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="1" t="n">
+      <c r="A225" s="4" t="n">
         <v>223</v>
       </c>
       <c r="B225" s="1" t="str">
@@ -12665,7 +12755,7 @@
       <c r="G225" s="1"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="1" t="n">
+      <c r="A226" s="4" t="n">
         <v>224</v>
       </c>
       <c r="B226" s="1" t="str">
@@ -12688,7 +12778,7 @@
       <c r="G226" s="1"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="1" t="n">
+      <c r="A227" s="4" t="n">
         <v>225</v>
       </c>
       <c r="B227" s="1" t="str">
@@ -12711,7 +12801,7 @@
       <c r="G227" s="1"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="1" t="n">
+      <c r="A228" s="4" t="n">
         <v>226</v>
       </c>
       <c r="B228" s="1" t="str">
@@ -12734,7 +12824,7 @@
       <c r="G228" s="1"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="1" t="n">
+      <c r="A229" s="4" t="n">
         <v>227</v>
       </c>
       <c r="B229" s="1" t="str">
@@ -12757,7 +12847,7 @@
       <c r="G229" s="1"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="1" t="n">
+      <c r="A230" s="4" t="n">
         <v>228</v>
       </c>
       <c r="B230" s="1" t="str">
@@ -12780,7 +12870,7 @@
       <c r="G230" s="1"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="1" t="n">
+      <c r="A231" s="4" t="n">
         <v>229</v>
       </c>
       <c r="B231" s="1" t="str">
@@ -12803,7 +12893,7 @@
       <c r="G231" s="1"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="1" t="n">
+      <c r="A232" s="4" t="n">
         <v>230</v>
       </c>
       <c r="B232" s="1" t="str">
@@ -12826,7 +12916,7 @@
       <c r="G232" s="1"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="1" t="n">
+      <c r="A233" s="4" t="n">
         <v>231</v>
       </c>
       <c r="B233" s="1" t="str">
@@ -12849,7 +12939,7 @@
       <c r="G233" s="1"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="1" t="n">
+      <c r="A234" s="4" t="n">
         <v>232</v>
       </c>
       <c r="B234" s="1" t="str">
@@ -12872,7 +12962,7 @@
       <c r="G234" s="1"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="1" t="n">
+      <c r="A235" s="4" t="n">
         <v>233</v>
       </c>
       <c r="B235" s="1" t="str">
@@ -12895,7 +12985,7 @@
       <c r="G235" s="1"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="1" t="n">
+      <c r="A236" s="4" t="n">
         <v>234</v>
       </c>
       <c r="B236" s="1" t="str">
@@ -12918,7 +13008,7 @@
       <c r="G236" s="1"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="1" t="n">
+      <c r="A237" s="4" t="n">
         <v>235</v>
       </c>
       <c r="B237" s="1" t="str">
@@ -12941,7 +13031,7 @@
       <c r="G237" s="1"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="1" t="n">
+      <c r="A238" s="4" t="n">
         <v>236</v>
       </c>
       <c r="B238" s="1" t="str">
@@ -12964,7 +13054,7 @@
       <c r="G238" s="1"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="1" t="n">
+      <c r="A239" s="4" t="n">
         <v>237</v>
       </c>
       <c r="B239" s="1" t="str">
@@ -12987,7 +13077,7 @@
       <c r="G239" s="1"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="1" t="n">
+      <c r="A240" s="4" t="n">
         <v>238</v>
       </c>
       <c r="B240" s="1" t="str">
@@ -13010,7 +13100,7 @@
       <c r="G240" s="1"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="1" t="n">
+      <c r="A241" s="4" t="n">
         <v>239</v>
       </c>
       <c r="B241" s="1" t="str">
@@ -13033,7 +13123,7 @@
       <c r="G241" s="1"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="1" t="n">
+      <c r="A242" s="4" t="n">
         <v>240</v>
       </c>
       <c r="B242" s="1" t="str">
@@ -13056,7 +13146,7 @@
       <c r="G242" s="1"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="1" t="n">
+      <c r="A243" s="4" t="n">
         <v>241</v>
       </c>
       <c r="B243" s="1" t="str">
@@ -13079,7 +13169,7 @@
       <c r="G243" s="1"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="1" t="n">
+      <c r="A244" s="4" t="n">
         <v>242</v>
       </c>
       <c r="B244" s="1" t="str">
@@ -13102,7 +13192,7 @@
       <c r="G244" s="1"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="1" t="n">
+      <c r="A245" s="4" t="n">
         <v>243</v>
       </c>
       <c r="B245" s="1" t="str">
@@ -13125,7 +13215,7 @@
       <c r="G245" s="1"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="1" t="n">
+      <c r="A246" s="4" t="n">
         <v>244</v>
       </c>
       <c r="B246" s="1" t="str">
@@ -13148,7 +13238,7 @@
       <c r="G246" s="1"/>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="n">
+      <c r="A247" s="4" t="n">
         <v>245</v>
       </c>
       <c r="B247" s="1" t="str">
@@ -13171,7 +13261,7 @@
       <c r="G247" s="1"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="1" t="n">
+      <c r="A248" s="4" t="n">
         <v>246</v>
       </c>
       <c r="B248" s="1" t="str">
@@ -13194,7 +13284,7 @@
       <c r="G248" s="1"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="n">
+      <c r="A249" s="4" t="n">
         <v>247</v>
       </c>
       <c r="B249" s="1" t="str">
@@ -13217,7 +13307,7 @@
       <c r="G249" s="1"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="1" t="n">
+      <c r="A250" s="4" t="n">
         <v>248</v>
       </c>
       <c r="B250" s="1" t="str">
@@ -13240,7 +13330,7 @@
       <c r="G250" s="1"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="1" t="n">
+      <c r="A251" s="4" t="n">
         <v>249</v>
       </c>
       <c r="B251" s="1" t="str">
@@ -13263,7 +13353,7 @@
       <c r="G251" s="1"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1" t="n">
+      <c r="A252" s="4" t="n">
         <v>250</v>
       </c>
       <c r="B252" s="1" t="str">
@@ -13286,7 +13376,7 @@
       <c r="G252" s="1"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="1" t="n">
+      <c r="A253" s="4" t="n">
         <v>251</v>
       </c>
       <c r="B253" s="1" t="str">
@@ -13309,7 +13399,7 @@
       <c r="G253" s="1"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="1" t="n">
+      <c r="A254" s="4" t="n">
         <v>252</v>
       </c>
       <c r="B254" s="1" t="str">
@@ -13332,7 +13422,7 @@
       <c r="G254" s="1"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="1" t="n">
+      <c r="A255" s="4" t="n">
         <v>253</v>
       </c>
       <c r="B255" s="1" t="str">
@@ -13355,7 +13445,7 @@
       <c r="G255" s="1"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="1" t="n">
+      <c r="A256" s="4" t="n">
         <v>254</v>
       </c>
       <c r="B256" s="1" t="str">
@@ -13378,7 +13468,7 @@
       <c r="G256" s="1"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="1" t="n">
+      <c r="A257" s="4" t="n">
         <v>255</v>
       </c>
       <c r="B257" s="1" t="str">
@@ -13442,25 +13532,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13477,10 +13567,10 @@
         <v>178</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -13503,7 +13593,7 @@
         <v>57</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>122</v>
@@ -13520,13 +13610,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>162</v>
@@ -13537,35 +13627,35 @@
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13573,10 +13663,10 @@
         <v>125</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13587,7 +13677,7 @@
         <v>168</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13595,10 +13685,10 @@
         <v>163</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13606,7 +13696,7 @@
         <v>161</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13614,7 +13704,7 @@
         <v>174</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recode: petrol_station_large & add: pagoda
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="269">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -681,6 +681,21 @@
     <t xml:space="preserve">[PASS, 8],[MAIL, 1],[FOOD, 2]</t>
   </si>
   <si>
+    <t xml:space="preserve">pagoda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME_PAGODA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PASS, 4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shrine_prohibition</t>
+  </si>
+  <si>
     <t xml:space="preserve">petrol_station_large</t>
   </si>
   <si>
@@ -715,15 +730,6 @@
   </si>
   <si>
     <t xml:space="preserve">NAME_SHRINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[PASS, 4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shrine_prohibition</t>
   </si>
   <si>
     <t xml:space="preserve">NAME_SHRINE_PROHIBITION</t>
@@ -1048,14 +1054,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y91"/>
+  <dimension ref="A1:Y92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
-      <selection pane="bottomRight" activeCell="L81" activeCellId="0" sqref="L81"/>
+      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="N83" activeCellId="0" sqref="N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7779,10 +7785,10 @@
         <v>219</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>204</v>
@@ -7791,55 +7797,99 @@
         <v>220</v>
       </c>
       <c r="G81" s="1" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="H81" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I81" s="3" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J81" s="5" t="s">
         <v>30</v>
       </c>
       <c r="K81" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M81" s="7" t="str">
+        <f aca="false">VLOOKUP(L81,dropdowns!E:F,2,0)</f>
+        <v>ALL_TOWNZONES</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q81" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="L81" s="6"/>
-      <c r="M81" s="7"/>
-      <c r="P81" s="4"/>
-      <c r="S81" s="4"/>
+      <c r="R81" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S81" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="T81" s="1" t="str">
+        <f aca="false">IF(NOT(D81="1X1"),"none",IF(E81="skyscraper",CONCATENATE(A81,"_c"),IF(E81="landmark",CONCATENATE(A81,"_k"),IF(E81="house",CONCATENATE(A81,"_h"),A81))))</f>
+        <v>pagoda_k</v>
+      </c>
+      <c r="U81" s="1" t="str">
+        <f aca="false">IF(D81="1X1","none",IF(E81="skyscraper",CONCATENATE(A81,"_c_north"),IF(E81="landmark",CONCATENATE(A81,"_k_north"),IF(E81="house",CONCATENATE(A81,"_h_north"),CONCATENATE(A81,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V81" s="1" t="str">
+        <f aca="false">IF(OR(D81="1X1",D81="2X1"),"none",IF(E81="skyscraper",CONCATENATE(A81,"_c_east"),IF(E81="landmark",CONCATENATE(A81,"_k_east"),CONCATENATE(A81,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W81" s="1" t="str">
+        <f aca="false">IF(OR(D81="1X1",D81="1X2"),"none",IF(E81="skyscraper",CONCATENATE(A81,"_c_west"),IF(E81="landmark",CONCATENATE(A81,"_k_west"),CONCATENATE(A81,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X81" s="1" t="str">
+        <f aca="false">IF(NOT(D81="2X2"),"none",IF(E81="skyscraper",CONCATENATE(A81,"_c_south"),IF(E81="landmark",CONCATENATE(A81,"_k_south"),CONCATENATE(A81,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y81" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>210</v>
+        <v>143</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>204</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G82" s="1" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H82" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I82" s="3" t="n">
-        <v>1950</v>
-      </c>
-      <c r="J82" s="5" t="n">
-        <v>1989</v>
+        <v>1970</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="K82" s="1" t="n">
         <v>10</v>
@@ -7852,7 +7902,7 @@
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N82" s="1" t="n">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="O82" s="1" t="n">
         <v>3</v>
@@ -7875,57 +7925,57 @@
       </c>
       <c r="U82" s="1" t="str">
         <f aca="false">IF(D82="1X1","none",IF(E82="skyscraper",CONCATENATE(A82,"_c_north"),IF(E82="landmark",CONCATENATE(A82,"_k_north"),IF(E82="house",CONCATENATE(A82,"_h_north"),CONCATENATE(A82,"_north")))))</f>
-        <v>petrol_station_old_k_north</v>
+        <v>petrol_station_large_k_north</v>
       </c>
       <c r="V82" s="1" t="str">
         <f aca="false">IF(OR(D82="1X1",D82="2X1"),"none",IF(E82="skyscraper",CONCATENATE(A82,"_c_east"),IF(E82="landmark",CONCATENATE(A82,"_k_east"),CONCATENATE(A82,"_east"))))</f>
-        <v>none</v>
+        <v>petrol_station_large_k_east</v>
       </c>
       <c r="W82" s="1" t="str">
         <f aca="false">IF(OR(D82="1X1",D82="1X2"),"none",IF(E82="skyscraper",CONCATENATE(A82,"_c_west"),IF(E82="landmark",CONCATENATE(A82,"_k_west"),CONCATENATE(A82,"_west"))))</f>
-        <v>petrol_station_old_k_west</v>
+        <v>none</v>
       </c>
       <c r="X82" s="1" t="str">
         <f aca="false">IF(NOT(D82="2X2"),"none",IF(E82="skyscraper",CONCATENATE(A82,"_c_south"),IF(E82="landmark",CONCATENATE(A82,"_k_south"),CONCATENATE(A82,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y82" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>143</v>
+        <v>210</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>204</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G83" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H83" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I83" s="3" t="n">
-        <v>1970</v>
-      </c>
-      <c r="J83" s="5" t="s">
-        <v>30</v>
+        <v>1950</v>
+      </c>
+      <c r="J83" s="5" t="n">
+        <v>1989</v>
       </c>
       <c r="K83" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L83" s="6" t="s">
         <v>175</v>
@@ -7935,7 +7985,7 @@
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N83" s="1" t="n">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="O83" s="1" t="n">
         <v>3</v>
@@ -7950,7 +8000,7 @@
         <v>2</v>
       </c>
       <c r="S83" s="4" t="s">
-        <v>125</v>
+        <v>214</v>
       </c>
       <c r="T83" s="1" t="str">
         <f aca="false">IF(NOT(D83="1X1"),"none",IF(E83="skyscraper",CONCATENATE(A83,"_c"),IF(E83="landmark",CONCATENATE(A83,"_k"),IF(E83="house",CONCATENATE(A83,"_h"),A83))))</f>
@@ -7958,51 +8008,51 @@
       </c>
       <c r="U83" s="1" t="str">
         <f aca="false">IF(D83="1X1","none",IF(E83="skyscraper",CONCATENATE(A83,"_c_north"),IF(E83="landmark",CONCATENATE(A83,"_k_north"),IF(E83="house",CONCATENATE(A83,"_h_north"),CONCATENATE(A83,"_north")))))</f>
-        <v>police_station_k_north</v>
+        <v>petrol_station_old_k_north</v>
       </c>
       <c r="V83" s="1" t="str">
         <f aca="false">IF(OR(D83="1X1",D83="2X1"),"none",IF(E83="skyscraper",CONCATENATE(A83,"_c_east"),IF(E83="landmark",CONCATENATE(A83,"_k_east"),CONCATENATE(A83,"_east"))))</f>
-        <v>police_station_k_east</v>
+        <v>none</v>
       </c>
       <c r="W83" s="1" t="str">
         <f aca="false">IF(OR(D83="1X1",D83="1X2"),"none",IF(E83="skyscraper",CONCATENATE(A83,"_c_west"),IF(E83="landmark",CONCATENATE(A83,"_k_west"),CONCATENATE(A83,"_west"))))</f>
-        <v>none</v>
+        <v>petrol_station_old_k_west</v>
       </c>
       <c r="X83" s="1" t="str">
         <f aca="false">IF(NOT(D83="2X2"),"none",IF(E83="skyscraper",CONCATENATE(A83,"_c_south"),IF(E83="landmark",CONCATENATE(A83,"_k_south"),CONCATENATE(A83,"_south"))))</f>
         <v>none</v>
       </c>
       <c r="Y83" s="1" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C84" s="2" t="n">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>204</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G84" s="1" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H84" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I84" s="3" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J84" s="5" t="s">
         <v>30</v>
@@ -8011,20 +8061,20 @@
         <v>20</v>
       </c>
       <c r="L84" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="M84" s="7" t="str">
         <f aca="false">VLOOKUP(L84,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
       <c r="N84" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O84" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P84" s="4" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q84" s="1" t="n">
         <v>10</v>
@@ -8033,7 +8083,7 @@
         <v>2</v>
       </c>
       <c r="S84" s="4" t="s">
-        <v>218</v>
+        <v>125</v>
       </c>
       <c r="T84" s="1" t="str">
         <f aca="false">IF(NOT(D84="1X1"),"none",IF(E84="skyscraper",CONCATENATE(A84,"_c"),IF(E84="landmark",CONCATENATE(A84,"_k"),IF(E84="house",CONCATENATE(A84,"_h"),A84))))</f>
@@ -8041,73 +8091,73 @@
       </c>
       <c r="U84" s="1" t="str">
         <f aca="false">IF(D84="1X1","none",IF(E84="skyscraper",CONCATENATE(A84,"_c_north"),IF(E84="landmark",CONCATENATE(A84,"_k_north"),IF(E84="house",CONCATENATE(A84,"_h_north"),CONCATENATE(A84,"_north")))))</f>
-        <v>shiro_k_north</v>
+        <v>police_station_k_north</v>
       </c>
       <c r="V84" s="1" t="str">
         <f aca="false">IF(OR(D84="1X1",D84="2X1"),"none",IF(E84="skyscraper",CONCATENATE(A84,"_c_east"),IF(E84="landmark",CONCATENATE(A84,"_k_east"),CONCATENATE(A84,"_east"))))</f>
-        <v>shiro_k_east</v>
+        <v>police_station_k_east</v>
       </c>
       <c r="W84" s="1" t="str">
         <f aca="false">IF(OR(D84="1X1",D84="1X2"),"none",IF(E84="skyscraper",CONCATENATE(A84,"_c_west"),IF(E84="landmark",CONCATENATE(A84,"_k_west"),CONCATENATE(A84,"_west"))))</f>
-        <v>shiro_k_west</v>
+        <v>none</v>
       </c>
       <c r="X84" s="1" t="str">
         <f aca="false">IF(NOT(D84="2X2"),"none",IF(E84="skyscraper",CONCATENATE(A84,"_c_south"),IF(E84="landmark",CONCATENATE(A84,"_k_south"),CONCATENATE(A84,"_south"))))</f>
-        <v>shiro_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y84" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C85" s="2" t="n">
-        <v>7</v>
+        <v>216</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>204</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G85" s="1" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H85" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I85" s="3" t="n">
-        <v>1930</v>
+        <v>1700</v>
       </c>
       <c r="J85" s="5" t="s">
         <v>30</v>
       </c>
       <c r="K85" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L85" s="6" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="M85" s="7" t="str">
         <f aca="false">VLOOKUP(L85,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N85" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O85" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P85" s="4" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="Q85" s="1" t="n">
         <v>10</v>
@@ -8116,41 +8166,41 @@
         <v>2</v>
       </c>
       <c r="S85" s="4" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="T85" s="1" t="str">
         <f aca="false">IF(NOT(D85="1X1"),"none",IF(E85="skyscraper",CONCATENATE(A85,"_c"),IF(E85="landmark",CONCATENATE(A85,"_k"),IF(E85="house",CONCATENATE(A85,"_h"),A85))))</f>
-        <v>shops_small_k</v>
+        <v>none</v>
       </c>
       <c r="U85" s="1" t="str">
         <f aca="false">IF(D85="1X1","none",IF(E85="skyscraper",CONCATENATE(A85,"_c_north"),IF(E85="landmark",CONCATENATE(A85,"_k_north"),IF(E85="house",CONCATENATE(A85,"_h_north"),CONCATENATE(A85,"_north")))))</f>
-        <v>none</v>
+        <v>shiro_k_north</v>
       </c>
       <c r="V85" s="1" t="str">
         <f aca="false">IF(OR(D85="1X1",D85="2X1"),"none",IF(E85="skyscraper",CONCATENATE(A85,"_c_east"),IF(E85="landmark",CONCATENATE(A85,"_k_east"),CONCATENATE(A85,"_east"))))</f>
-        <v>none</v>
+        <v>shiro_k_east</v>
       </c>
       <c r="W85" s="1" t="str">
         <f aca="false">IF(OR(D85="1X1",D85="1X2"),"none",IF(E85="skyscraper",CONCATENATE(A85,"_c_west"),IF(E85="landmark",CONCATENATE(A85,"_k_west"),CONCATENATE(A85,"_west"))))</f>
-        <v>none</v>
+        <v>shiro_k_west</v>
       </c>
       <c r="X85" s="1" t="str">
         <f aca="false">IF(NOT(D85="2X2"),"none",IF(E85="skyscraper",CONCATENATE(A85,"_c_south"),IF(E85="landmark",CONCATENATE(A85,"_k_south"),CONCATENATE(A85,"_south"))))</f>
-        <v>none</v>
+        <v>shiro_k_south</v>
       </c>
       <c r="Y85" s="1" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C86" s="2" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>27</v>
@@ -8159,51 +8209,51 @@
         <v>204</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G86" s="1" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H86" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I86" s="3" t="n">
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="J86" s="5" t="s">
         <v>30</v>
       </c>
       <c r="K86" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L86" s="6" t="s">
-        <v>231</v>
+        <v>31</v>
       </c>
       <c r="M86" s="7" t="str">
         <f aca="false">VLOOKUP(L86,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N86" s="1" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="O86" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P86" s="4" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q86" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R86" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S86" s="4" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="T86" s="1" t="str">
         <f aca="false">IF(NOT(D86="1X1"),"none",IF(E86="skyscraper",CONCATENATE(A86,"_c"),IF(E86="landmark",CONCATENATE(A86,"_k"),IF(E86="house",CONCATENATE(A86,"_h"),A86))))</f>
-        <v>shrine_k</v>
+        <v>shops_small_k</v>
       </c>
       <c r="U86" s="1" t="str">
         <f aca="false">IF(D86="1X1","none",IF(E86="skyscraper",CONCATENATE(A86,"_c_north"),IF(E86="landmark",CONCATENATE(A86,"_k_north"),IF(E86="house",CONCATENATE(A86,"_h_north"),CONCATENATE(A86,"_north")))))</f>
@@ -8222,18 +8272,18 @@
         <v>none</v>
       </c>
       <c r="Y86" s="1" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C87" s="2" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>27</v>
@@ -8242,13 +8292,13 @@
         <v>204</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G87" s="1" t="n">
         <v>5</v>
       </c>
       <c r="H87" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I87" s="3" t="n">
         <v>0</v>
@@ -8260,7 +8310,7 @@
         <v>20</v>
       </c>
       <c r="L87" s="6" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="M87" s="7" t="str">
         <f aca="false">VLOOKUP(L87,dropdowns!E:F,2,0)</f>
@@ -8282,11 +8332,11 @@
         <v>1</v>
       </c>
       <c r="S87" s="4" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="T87" s="1" t="str">
         <f aca="false">IF(NOT(D87="1X1"),"none",IF(E87="skyscraper",CONCATENATE(A87,"_c"),IF(E87="landmark",CONCATENATE(A87,"_k"),IF(E87="house",CONCATENATE(A87,"_h"),A87))))</f>
-        <v>shrine_prohibition_k</v>
+        <v>shrine_k</v>
       </c>
       <c r="U87" s="1" t="str">
         <f aca="false">IF(D87="1X1","none",IF(E87="skyscraper",CONCATENATE(A87,"_c_north"),IF(E87="landmark",CONCATENATE(A87,"_k_north"),IF(E87="house",CONCATENATE(A87,"_h_north"),CONCATENATE(A87,"_north")))))</f>
@@ -8305,21 +8355,21 @@
         <v>none</v>
       </c>
       <c r="Y87" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C88" s="2" t="n">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>159</v>
+        <v>27</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>204</v>
@@ -8328,13 +8378,13 @@
         <v>236</v>
       </c>
       <c r="G88" s="1" t="n">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="H88" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I88" s="3" t="n">
-        <v>1970</v>
+        <v>0</v>
       </c>
       <c r="J88" s="5" t="s">
         <v>30</v>
@@ -8343,52 +8393,52 @@
         <v>20</v>
       </c>
       <c r="L88" s="6" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="M88" s="7" t="str">
         <f aca="false">VLOOKUP(L88,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>ALL_TOWNZONES</v>
       </c>
       <c r="N88" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O88" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P88" s="4" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="Q88" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R88" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S88" s="4" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="T88" s="1" t="str">
         <f aca="false">IF(NOT(D88="1X1"),"none",IF(E88="skyscraper",CONCATENATE(A88,"_c"),IF(E88="landmark",CONCATENATE(A88,"_k"),IF(E88="house",CONCATENATE(A88,"_h"),A88))))</f>
-        <v>none</v>
+        <v>shrine_prohibition_k</v>
       </c>
       <c r="U88" s="1" t="str">
         <f aca="false">IF(D88="1X1","none",IF(E88="skyscraper",CONCATENATE(A88,"_c_north"),IF(E88="landmark",CONCATENATE(A88,"_k_north"),IF(E88="house",CONCATENATE(A88,"_h_north"),CONCATENATE(A88,"_north")))))</f>
-        <v>stadium_k_north</v>
+        <v>none</v>
       </c>
       <c r="V88" s="1" t="str">
         <f aca="false">IF(OR(D88="1X1",D88="2X1"),"none",IF(E88="skyscraper",CONCATENATE(A88,"_c_east"),IF(E88="landmark",CONCATENATE(A88,"_k_east"),CONCATENATE(A88,"_east"))))</f>
-        <v>stadium_k_east</v>
+        <v>none</v>
       </c>
       <c r="W88" s="1" t="str">
         <f aca="false">IF(OR(D88="1X1",D88="1X2"),"none",IF(E88="skyscraper",CONCATENATE(A88,"_c_west"),IF(E88="landmark",CONCATENATE(A88,"_k_west"),CONCATENATE(A88,"_west"))))</f>
-        <v>stadium_k_west</v>
+        <v>none</v>
       </c>
       <c r="X88" s="1" t="str">
         <f aca="false">IF(NOT(D88="2X2"),"none",IF(E88="skyscraper",CONCATENATE(A88,"_c_south"),IF(E88="landmark",CONCATENATE(A88,"_k_south"),CONCATENATE(A88,"_south"))))</f>
-        <v>stadium_k_south</v>
+        <v>none</v>
       </c>
       <c r="Y88" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8399,7 +8449,7 @@
         <v>237</v>
       </c>
       <c r="C89" s="2" t="n">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>159</v>
@@ -8411,13 +8461,13 @@
         <v>238</v>
       </c>
       <c r="G89" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H89" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I89" s="3" t="n">
-        <v>1700</v>
+        <v>1970</v>
       </c>
       <c r="J89" s="5" t="s">
         <v>30</v>
@@ -8426,11 +8476,11 @@
         <v>20</v>
       </c>
       <c r="L89" s="6" t="s">
-        <v>231</v>
+        <v>172</v>
       </c>
       <c r="M89" s="7" t="str">
         <f aca="false">VLOOKUP(L89,dropdowns!E:F,2,0)</f>
-        <v>ALL_TOWNZONES</v>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
       <c r="N89" s="1" t="n">
         <v>20</v>
@@ -8439,16 +8489,16 @@
         <v>3</v>
       </c>
       <c r="P89" s="4" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="Q89" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R89" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S89" s="4" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="T89" s="1" t="str">
         <f aca="false">IF(NOT(D89="1X1"),"none",IF(E89="skyscraper",CONCATENATE(A89,"_c"),IF(E89="landmark",CONCATENATE(A89,"_k"),IF(E89="house",CONCATENATE(A89,"_h"),A89))))</f>
@@ -8456,22 +8506,22 @@
       </c>
       <c r="U89" s="1" t="str">
         <f aca="false">IF(D89="1X1","none",IF(E89="skyscraper",CONCATENATE(A89,"_c_north"),IF(E89="landmark",CONCATENATE(A89,"_k_north"),IF(E89="house",CONCATENATE(A89,"_h_north"),CONCATENATE(A89,"_north")))))</f>
-        <v>temple_k_north</v>
+        <v>stadium_k_north</v>
       </c>
       <c r="V89" s="1" t="str">
         <f aca="false">IF(OR(D89="1X1",D89="2X1"),"none",IF(E89="skyscraper",CONCATENATE(A89,"_c_east"),IF(E89="landmark",CONCATENATE(A89,"_k_east"),CONCATENATE(A89,"_east"))))</f>
-        <v>temple_k_east</v>
+        <v>stadium_k_east</v>
       </c>
       <c r="W89" s="1" t="str">
         <f aca="false">IF(OR(D89="1X1",D89="1X2"),"none",IF(E89="skyscraper",CONCATENATE(A89,"_c_west"),IF(E89="landmark",CONCATENATE(A89,"_k_west"),CONCATENATE(A89,"_west"))))</f>
-        <v>temple_k_west</v>
+        <v>stadium_k_west</v>
       </c>
       <c r="X89" s="1" t="str">
         <f aca="false">IF(NOT(D89="2X2"),"none",IF(E89="skyscraper",CONCATENATE(A89,"_c_south"),IF(E89="landmark",CONCATENATE(A89,"_k_south"),CONCATENATE(A89,"_south"))))</f>
-        <v>temple_k_south</v>
+        <v>stadium_k_south</v>
       </c>
       <c r="Y89" s="1" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8482,10 +8532,10 @@
         <v>239</v>
       </c>
       <c r="C90" s="2" t="n">
-        <v>96</v>
+        <v>208</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>204</v>
@@ -8494,67 +8544,67 @@
         <v>240</v>
       </c>
       <c r="G90" s="1" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H90" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I90" s="3" t="n">
-        <v>1955</v>
+        <v>1700</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>30</v>
       </c>
       <c r="K90" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L90" s="6" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="M90" s="7" t="str">
         <f aca="false">VLOOKUP(L90,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+        <v>ALL_TOWNZONES</v>
       </c>
       <c r="N90" s="1" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O90" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P90" s="4" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="Q90" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R90" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S90" s="4" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="T90" s="1" t="str">
         <f aca="false">IF(NOT(D90="1X1"),"none",IF(E90="skyscraper",CONCATENATE(A90,"_c"),IF(E90="landmark",CONCATENATE(A90,"_k"),IF(E90="house",CONCATENATE(A90,"_h"),A90))))</f>
-        <v>yoshinoya_restaurant_k</v>
+        <v>none</v>
       </c>
       <c r="U90" s="1" t="str">
         <f aca="false">IF(D90="1X1","none",IF(E90="skyscraper",CONCATENATE(A90,"_c_north"),IF(E90="landmark",CONCATENATE(A90,"_k_north"),IF(E90="house",CONCATENATE(A90,"_h_north"),CONCATENATE(A90,"_north")))))</f>
-        <v>none</v>
+        <v>temple_k_north</v>
       </c>
       <c r="V90" s="1" t="str">
         <f aca="false">IF(OR(D90="1X1",D90="2X1"),"none",IF(E90="skyscraper",CONCATENATE(A90,"_c_east"),IF(E90="landmark",CONCATENATE(A90,"_k_east"),CONCATENATE(A90,"_east"))))</f>
-        <v>none</v>
+        <v>temple_k_east</v>
       </c>
       <c r="W90" s="1" t="str">
         <f aca="false">IF(OR(D90="1X1",D90="1X2"),"none",IF(E90="skyscraper",CONCATENATE(A90,"_c_west"),IF(E90="landmark",CONCATENATE(A90,"_k_west"),CONCATENATE(A90,"_west"))))</f>
-        <v>none</v>
+        <v>temple_k_west</v>
       </c>
       <c r="X90" s="1" t="str">
         <f aca="false">IF(NOT(D90="2X2"),"none",IF(E90="skyscraper",CONCATENATE(A90,"_c_south"),IF(E90="landmark",CONCATENATE(A90,"_k_south"),CONCATENATE(A90,"_south"))))</f>
-        <v>none</v>
+        <v>temple_k_south</v>
       </c>
       <c r="Y90" s="1" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8565,7 +8615,7 @@
         <v>241</v>
       </c>
       <c r="C91" s="2" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>27</v>
@@ -8583,7 +8633,7 @@
         <v>1</v>
       </c>
       <c r="I91" s="3" t="n">
-        <v>1960</v>
+        <v>1955</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>30</v>
@@ -8618,7 +8668,7 @@
       </c>
       <c r="T91" s="1" t="str">
         <f aca="false">IF(NOT(D91="1X1"),"none",IF(E91="skyscraper",CONCATENATE(A91,"_c"),IF(E91="landmark",CONCATENATE(A91,"_k"),IF(E91="house",CONCATENATE(A91,"_h"),A91))))</f>
-        <v>yoshinoya_sushi_restaurant_k</v>
+        <v>yoshinoya_restaurant_k</v>
       </c>
       <c r="U91" s="1" t="str">
         <f aca="false">IF(D91="1X1","none",IF(E91="skyscraper",CONCATENATE(A91,"_c_north"),IF(E91="landmark",CONCATENATE(A91,"_k_north"),IF(E91="house",CONCATENATE(A91,"_h_north"),CONCATENATE(A91,"_north")))))</f>
@@ -8637,6 +8687,89 @@
         <v>none</v>
       </c>
       <c r="Y91" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G92" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="H92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I92" s="3" t="n">
+        <v>1960</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K92" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L92" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="M92" s="7" t="str">
+        <f aca="false">VLOOKUP(L92,dropdowns!E:F,2,0)</f>
+        <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
+      </c>
+      <c r="N92" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="O92" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P92" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q92" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R92" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S92" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="T92" s="1" t="str">
+        <f aca="false">IF(NOT(D92="1X1"),"none",IF(E92="skyscraper",CONCATENATE(A92,"_c"),IF(E92="landmark",CONCATENATE(A92,"_k"),IF(E92="house",CONCATENATE(A92,"_h"),A92))))</f>
+        <v>yoshinoya_sushi_restaurant_k</v>
+      </c>
+      <c r="U92" s="1" t="str">
+        <f aca="false">IF(D92="1X1","none",IF(E92="skyscraper",CONCATENATE(A92,"_c_north"),IF(E92="landmark",CONCATENATE(A92,"_k_north"),IF(E92="house",CONCATENATE(A92,"_h_north"),CONCATENATE(A92,"_north")))))</f>
+        <v>none</v>
+      </c>
+      <c r="V92" s="1" t="str">
+        <f aca="false">IF(OR(D92="1X1",D92="2X1"),"none",IF(E92="skyscraper",CONCATENATE(A92,"_c_east"),IF(E92="landmark",CONCATENATE(A92,"_k_east"),CONCATENATE(A92,"_east"))))</f>
+        <v>none</v>
+      </c>
+      <c r="W92" s="1" t="str">
+        <f aca="false">IF(OR(D92="1X1",D92="1X2"),"none",IF(E92="skyscraper",CONCATENATE(A92,"_c_west"),IF(E92="landmark",CONCATENATE(A92,"_k_west"),CONCATENATE(A92,"_west"))))</f>
+        <v>none</v>
+      </c>
+      <c r="X92" s="1" t="str">
+        <f aca="false">IF(NOT(D92="2X2"),"none",IF(E92="skyscraper",CONCATENATE(A92,"_c_south"),IF(E92="landmark",CONCATENATE(A92,"_k_south"),CONCATENATE(A92,"_south"))))</f>
+        <v>none</v>
+      </c>
+      <c r="Y92" s="1" t="s">
         <v>208</v>
       </c>
     </row>
@@ -8649,15 +8782,15 @@
       <formula1>dropdowns!$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L91" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L92" type="list">
       <formula1>dropdowns!$E:$E</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P91" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P92" type="list">
       <formula1>dropdowns!$G:$G</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S91" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S92" type="list">
       <formula1>dropdowns!$D:$D</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8679,7 +8812,7 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B113" activeCellId="0" sqref="B113"/>
     </sheetView>
   </sheetViews>
@@ -8691,16 +8824,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -8727,11 +8860,11 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H2" s="0" t="n">
+        <v>249</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <f aca="false">COUNTIF(E:E,"FALSE")</f>
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8756,11 +8889,11 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H3" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <f aca="false">COUNTIF(E:E,"TRUE")</f>
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11736,19 +11869,19 @@
       </c>
       <c r="B133" s="1" t="str">
         <f aca="false">IFERROR(VLOOKUP(A133,items!C:D,2,0),"ID not in use")</f>
-        <v>ID not in use</v>
+        <v>1X1</v>
       </c>
       <c r="C133" s="1" t="n">
         <f aca="false">IF(B133="2X2",4,IF(OR(B133="1X2",B133="2X1"),2,IF(B133="1X1",1,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133" s="1" t="n">
         <f aca="false">IF(C133&gt;0,C133,MAX(D132-1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" s="8" t="b">
         <f aca="false">D133=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -14647,25 +14780,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14682,10 +14815,10 @@
         <v>214</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
@@ -14708,7 +14841,7 @@
         <v>57</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>122</v>
@@ -14731,7 +14864,7 @@
         <v>31</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>162</v>
@@ -14748,7 +14881,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14759,7 +14892,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14770,18 +14903,18 @@
         <v>206</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>172</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14792,7 +14925,7 @@
         <v>175</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14803,7 +14936,7 @@
         <v>190</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14811,7 +14944,7 @@
         <v>161</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14819,7 +14952,7 @@
         <v>181</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redraw: yano & recode: ConstructionChecks
</commit_message>
<xml_diff>
--- a/docs/buildings.xlsx
+++ b/docs/buildings.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ID checks" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="dropdowns" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="rule of thumbs" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="townzones" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">items!$A$1:$AA$128</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="416">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -301,39 +302,39 @@
     <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOKI_OFFICE),string(MEDIUM)</t>
   </si>
   <si>
+    <t xml:space="preserve">4 only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aoki_office_l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOKI_OFFICE),string(LARGE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aoki_office_x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOKI_OFFICE),string(XTRA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aoyama_office_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aoyama_office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOYAMA_OFFICE),string(MEDIUM)</t>
+  </si>
+  <si>
     <t xml:space="preserve">4,3,2</t>
   </si>
   <si>
-    <t xml:space="preserve">aoki_office_l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">large</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOKI_OFFICE),string(LARGE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aoki_office_x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xtra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOKI_OFFICE),string(XTRA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aoyama_office_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aoyama_office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STR_CONCAT_2, string(NAME_AOYAMA_OFFICE),string(MEDIUM)</t>
-  </si>
-  <si>
     <t xml:space="preserve">aoyama_office_l</t>
   </si>
   <si>
@@ -1232,6 +1233,48 @@
   </si>
   <si>
     <t xml:space="preserve">9L, 10L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WideRoad() + PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!WideRoad() + PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!Medium</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1286,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1265,21 +1308,59 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF819E"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB4C7DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -1308,7 +1389,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1341,11 +1422,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1405,19 +1530,19 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1439,7 +1564,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCCCC"/>
@@ -1450,7 +1575,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1475,12 +1600,12 @@
   </sheetPr>
   <dimension ref="A1:AC128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="F55" activeCellId="0" sqref="F55"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1642,7 +1767,7 @@
       <c r="N2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="8" t="str">
+      <c r="O2" s="3" t="str">
         <f aca="false">VLOOKUP(N2,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -1735,7 +1860,7 @@
       <c r="N3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="8" t="str">
+      <c r="O3" s="3" t="str">
         <f aca="false">VLOOKUP(N3,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -1828,7 +1953,7 @@
       <c r="N4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="8" t="str">
+      <c r="O4" s="3" t="str">
         <f aca="false">VLOOKUP(N4,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -1921,7 +2046,7 @@
       <c r="N5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="8" t="str">
+      <c r="O5" s="3" t="str">
         <f aca="false">VLOOKUP(N5,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -2014,7 +2139,7 @@
       <c r="N6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="8" t="str">
+      <c r="O6" s="3" t="str">
         <f aca="false">VLOOKUP(N6,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -2107,7 +2232,7 @@
       <c r="N7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="8" t="str">
+      <c r="O7" s="3" t="str">
         <f aca="false">VLOOKUP(N7,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -2192,7 +2317,7 @@
         <v>1700</v>
       </c>
       <c r="L8" s="6" t="n">
-        <v>1988</v>
+        <v>1944</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>5</v>
@@ -2200,7 +2325,7 @@
       <c r="N8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O8" s="8" t="str">
+      <c r="O8" s="3" t="str">
         <f aca="false">VLOOKUP(N8,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -2293,7 +2418,7 @@
       <c r="N9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O9" s="8" t="str">
+      <c r="O9" s="3" t="str">
         <f aca="false">VLOOKUP(N9,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -2386,7 +2511,7 @@
       <c r="N10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O10" s="8" t="str">
+      <c r="O10" s="3" t="str">
         <f aca="false">VLOOKUP(N10,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -2479,7 +2604,7 @@
       <c r="N11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O11" s="8" t="str">
+      <c r="O11" s="3" t="str">
         <f aca="false">VLOOKUP(N11,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_EDGE )</v>
       </c>
@@ -2572,7 +2697,7 @@
       <c r="N12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O12" s="8" t="str">
+      <c r="O12" s="3" t="str">
         <f aca="false">VLOOKUP(N12,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
@@ -2665,7 +2790,7 @@
       <c r="N13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="8" t="str">
+      <c r="O13" s="3" t="str">
         <f aca="false">VLOOKUP(N13,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -2758,7 +2883,7 @@
       <c r="N14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="O14" s="8" t="str">
+      <c r="O14" s="3" t="str">
         <f aca="false">VLOOKUP(N14,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT)</v>
       </c>
@@ -2851,7 +2976,7 @@
       <c r="N15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="8" t="str">
+      <c r="O15" s="3" t="str">
         <f aca="false">VLOOKUP(N15,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -2944,7 +3069,7 @@
       <c r="N16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O16" s="8" t="str">
+      <c r="O16" s="3" t="str">
         <f aca="false">VLOOKUP(N16,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -3037,7 +3162,7 @@
       <c r="N17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O17" s="8" t="str">
+      <c r="O17" s="3" t="str">
         <f aca="false">VLOOKUP(N17,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -3130,7 +3255,7 @@
       <c r="N18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="8" t="str">
+      <c r="O18" s="3" t="str">
         <f aca="false">VLOOKUP(N18,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -3223,7 +3348,7 @@
       <c r="N19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O19" s="8" t="str">
+      <c r="O19" s="3" t="str">
         <f aca="false">VLOOKUP(N19,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -3316,7 +3441,7 @@
       <c r="N20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O20" s="8" t="str">
+      <c r="O20" s="3" t="str">
         <f aca="false">VLOOKUP(N20,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -3409,9 +3534,9 @@
       <c r="N21" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="O21" s="8" t="str">
+      <c r="O21" s="3" t="str">
         <f aca="false">VLOOKUP(N21,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="P21" s="1" t="n">
         <v>27</v>
@@ -3502,11 +3627,11 @@
         <v>10</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="O22" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O22" s="3" t="str">
         <f aca="false">VLOOKUP(N22,dropdowns!E:F,2,0)</f>
-        <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
+        <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
       <c r="P22" s="1" t="n">
         <v>27</v>
@@ -3595,9 +3720,9 @@
         <v>15</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O23" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O23" s="3" t="str">
         <f aca="false">VLOOKUP(N23,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -3651,10 +3776,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>126</v>
@@ -3670,7 +3795,7 @@
         <v>89</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>100</v>
@@ -3688,9 +3813,9 @@
         <v>7</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O24" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O24" s="3" t="str">
         <f aca="false">VLOOKUP(N24,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -3749,7 +3874,7 @@
         <v>102</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>127</v>
@@ -3785,7 +3910,7 @@
       <c r="N25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O25" s="8" t="str">
+      <c r="O25" s="3" t="str">
         <f aca="false">VLOOKUP(N25,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -3876,9 +4001,9 @@
         <v>7</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O26" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O26" s="3" t="str">
         <f aca="false">VLOOKUP(N26,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -3973,7 +4098,7 @@
       <c r="N27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O27" s="8" t="str">
+      <c r="O27" s="3" t="str">
         <f aca="false">VLOOKUP(N27,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -4066,9 +4191,9 @@
         <v>7</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O28" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O28" s="3" t="str">
         <f aca="false">VLOOKUP(N28,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -4163,7 +4288,7 @@
       <c r="N29" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O29" s="8" t="str">
+      <c r="O29" s="3" t="str">
         <f aca="false">VLOOKUP(N29,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -4256,9 +4381,9 @@
         <v>7</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O30" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O30" s="3" t="str">
         <f aca="false">VLOOKUP(N30,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -4353,7 +4478,7 @@
       <c r="N31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O31" s="8" t="str">
+      <c r="O31" s="3" t="str">
         <f aca="false">VLOOKUP(N31,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -4448,7 +4573,7 @@
       <c r="N32" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O32" s="8" t="str">
+      <c r="O32" s="3" t="str">
         <f aca="false">VLOOKUP(N32,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -4539,9 +4664,9 @@
         <v>15</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O33" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O33" s="3" t="str">
         <f aca="false">VLOOKUP(N33,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -4603,7 +4728,8 @@
       <c r="C34" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D34" s="5" t="b">
+      <c r="D34" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -4636,7 +4762,7 @@
       <c r="N34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O34" s="8" t="str">
+      <c r="O34" s="3" t="str">
         <f aca="false">VLOOKUP(N34,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -4700,7 +4826,8 @@
       <c r="C35" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="D35" s="5" t="b">
+      <c r="D35" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -4731,9 +4858,9 @@
         <v>7</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O35" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O35" s="3" t="str">
         <f aca="false">VLOOKUP(N35,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -4831,7 +4958,7 @@
       <c r="N36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O36" s="8" t="str">
+      <c r="O36" s="3" t="str">
         <f aca="false">VLOOKUP(N36,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -4927,9 +5054,9 @@
         <v>7</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O37" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O37" s="3" t="str">
         <f aca="false">VLOOKUP(N37,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -4993,7 +5120,8 @@
       <c r="C38" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D38" s="5" t="b">
+      <c r="D38" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -5026,7 +5154,7 @@
       <c r="N38" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O38" s="8" t="str">
+      <c r="O38" s="3" t="str">
         <f aca="false">VLOOKUP(N38,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -5090,7 +5218,8 @@
       <c r="C39" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="D39" s="5" t="b">
+      <c r="D39" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -5121,9 +5250,9 @@
         <v>7</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O39" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O39" s="3" t="str">
         <f aca="false">VLOOKUP(N39,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -5216,9 +5345,9 @@
         <v>7</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O40" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O40" s="3" t="str">
         <f aca="false">VLOOKUP(N40,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -5311,9 +5440,9 @@
         <v>7</v>
       </c>
       <c r="N41" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O41" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O41" s="3" t="str">
         <f aca="false">VLOOKUP(N41,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -5408,7 +5537,7 @@
       <c r="N42" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O42" s="8" t="str">
+      <c r="O42" s="3" t="str">
         <f aca="false">VLOOKUP(N42,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -5499,9 +5628,9 @@
         <v>15</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O43" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O43" s="3" t="str">
         <f aca="false">VLOOKUP(N43,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -5594,7 +5723,7 @@
       <c r="N44" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O44" s="8" t="str">
+      <c r="O44" s="3" t="str">
         <f aca="false">VLOOKUP(N44,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -5685,9 +5814,9 @@
         <v>15</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O45" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O45" s="3" t="str">
         <f aca="false">VLOOKUP(N45,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -5780,7 +5909,7 @@
       <c r="N46" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O46" s="8" t="str">
+      <c r="O46" s="3" t="str">
         <f aca="false">VLOOKUP(N46,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -5871,9 +6000,9 @@
         <v>15</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O47" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O47" s="3" t="str">
         <f aca="false">VLOOKUP(N47,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -5935,7 +6064,8 @@
       <c r="C48" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="D48" s="5" t="b">
+      <c r="D48" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -5968,7 +6098,7 @@
       <c r="N48" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O48" s="8" t="str">
+      <c r="O48" s="3" t="str">
         <f aca="false">VLOOKUP(N48,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -6032,7 +6162,8 @@
       <c r="C49" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="D49" s="5" t="b">
+      <c r="D49" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -6063,9 +6194,9 @@
         <v>7</v>
       </c>
       <c r="N49" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O49" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O49" s="3" t="str">
         <f aca="false">VLOOKUP(N49,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -6158,9 +6289,9 @@
         <v>7</v>
       </c>
       <c r="N50" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O50" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O50" s="3" t="str">
         <f aca="false">VLOOKUP(N50,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -6255,7 +6386,7 @@
       <c r="N51" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O51" s="8" t="str">
+      <c r="O51" s="3" t="str">
         <f aca="false">VLOOKUP(N51,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -6351,7 +6482,7 @@
       <c r="N52" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O52" s="8" t="str">
+      <c r="O52" s="3" t="str">
         <f aca="false">VLOOKUP(N52,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -6447,9 +6578,9 @@
         <v>7</v>
       </c>
       <c r="N53" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O53" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O53" s="3" t="str">
         <f aca="false">VLOOKUP(N53,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -6513,7 +6644,8 @@
       <c r="C54" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="D54" s="5" t="b">
+      <c r="D54" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -6546,7 +6678,7 @@
       <c r="N54" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O54" s="8" t="str">
+      <c r="O54" s="3" t="str">
         <f aca="false">VLOOKUP(N54,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -6610,7 +6742,8 @@
       <c r="C55" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="D55" s="5" t="b">
+      <c r="D55" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -6641,9 +6774,9 @@
         <v>7</v>
       </c>
       <c r="N55" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O55" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O55" s="3" t="str">
         <f aca="false">VLOOKUP(N55,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -6736,9 +6869,9 @@
         <v>7</v>
       </c>
       <c r="N56" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O56" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O56" s="3" t="str">
         <f aca="false">VLOOKUP(N56,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -6836,7 +6969,7 @@
       <c r="N57" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O57" s="8" t="str">
+      <c r="O57" s="3" t="str">
         <f aca="false">VLOOKUP(N57,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -6932,9 +7065,9 @@
         <v>7</v>
       </c>
       <c r="N58" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O58" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O58" s="3" t="str">
         <f aca="false">VLOOKUP(N58,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -7027,9 +7160,9 @@
         <v>7</v>
       </c>
       <c r="N59" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O59" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O59" s="3" t="str">
         <f aca="false">VLOOKUP(N59,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -7124,7 +7257,7 @@
       <c r="N60" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O60" s="8" t="str">
+      <c r="O60" s="3" t="str">
         <f aca="false">VLOOKUP(N60,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -7215,9 +7348,9 @@
         <v>7</v>
       </c>
       <c r="N61" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O61" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O61" s="3" t="str">
         <f aca="false">VLOOKUP(N61,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -7310,9 +7443,9 @@
         <v>10</v>
       </c>
       <c r="N62" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O62" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O62" s="3" t="str">
         <f aca="false">VLOOKUP(N62,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -7403,9 +7536,9 @@
         <v>15</v>
       </c>
       <c r="N63" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O63" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O63" s="3" t="str">
         <f aca="false">VLOOKUP(N63,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -7496,9 +7629,9 @@
         <v>7</v>
       </c>
       <c r="N64" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O64" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O64" s="3" t="str">
         <f aca="false">VLOOKUP(N64,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -7589,9 +7722,9 @@
         <v>10</v>
       </c>
       <c r="N65" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O65" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O65" s="3" t="str">
         <f aca="false">VLOOKUP(N65,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -7682,9 +7815,9 @@
         <v>7</v>
       </c>
       <c r="N66" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O66" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O66" s="3" t="str">
         <f aca="false">VLOOKUP(N66,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -7777,7 +7910,7 @@
       <c r="N67" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O67" s="8" t="str">
+      <c r="O67" s="3" t="str">
         <f aca="false">VLOOKUP(N67,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -7868,9 +8001,9 @@
         <v>15</v>
       </c>
       <c r="N68" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O68" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O68" s="3" t="str">
         <f aca="false">VLOOKUP(N68,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -7961,9 +8094,9 @@
         <v>7</v>
       </c>
       <c r="N69" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O69" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O69" s="3" t="str">
         <f aca="false">VLOOKUP(N69,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -8056,7 +8189,7 @@
       <c r="N70" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O70" s="8" t="str">
+      <c r="O70" s="3" t="str">
         <f aca="false">VLOOKUP(N70,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -8147,9 +8280,9 @@
         <v>7</v>
       </c>
       <c r="N71" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O71" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O71" s="3" t="str">
         <f aca="false">VLOOKUP(N71,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -8242,7 +8375,7 @@
       <c r="N72" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O72" s="8" t="str">
+      <c r="O72" s="3" t="str">
         <f aca="false">VLOOKUP(N72,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -8333,9 +8466,9 @@
         <v>15</v>
       </c>
       <c r="N73" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O73" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O73" s="3" t="str">
         <f aca="false">VLOOKUP(N73,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -8426,9 +8559,9 @@
         <v>15</v>
       </c>
       <c r="N74" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O74" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O74" s="3" t="str">
         <f aca="false">VLOOKUP(N74,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -8521,7 +8654,7 @@
       <c r="N75" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O75" s="8" t="str">
+      <c r="O75" s="3" t="str">
         <f aca="false">VLOOKUP(N75,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -8614,7 +8747,7 @@
       <c r="N76" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O76" s="8" t="str">
+      <c r="O76" s="3" t="str">
         <f aca="false">VLOOKUP(N76,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -8705,9 +8838,9 @@
         <v>15</v>
       </c>
       <c r="N77" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O77" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O77" s="3" t="str">
         <f aca="false">VLOOKUP(N77,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -8798,9 +8931,9 @@
         <v>7</v>
       </c>
       <c r="N78" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O78" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O78" s="3" t="str">
         <f aca="false">VLOOKUP(N78,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -8893,7 +9026,7 @@
       <c r="N79" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O79" s="8" t="str">
+      <c r="O79" s="3" t="str">
         <f aca="false">VLOOKUP(N79,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -8984,9 +9117,9 @@
         <v>15</v>
       </c>
       <c r="N80" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O80" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O80" s="3" t="str">
         <f aca="false">VLOOKUP(N80,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -9082,7 +9215,7 @@
       <c r="N81" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O81" s="8" t="str">
+      <c r="O81" s="3" t="str">
         <f aca="false">VLOOKUP(N81,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -9176,9 +9309,9 @@
         <v>7</v>
       </c>
       <c r="N82" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O82" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O82" s="3" t="str">
         <f aca="false">VLOOKUP(N82,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -9269,9 +9402,9 @@
         <v>7</v>
       </c>
       <c r="N83" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O83" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O83" s="3" t="str">
         <f aca="false">VLOOKUP(N83,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -9364,7 +9497,7 @@
       <c r="N84" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O84" s="8" t="str">
+      <c r="O84" s="3" t="str">
         <f aca="false">VLOOKUP(N84,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -9455,9 +9588,9 @@
         <v>7</v>
       </c>
       <c r="N85" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O85" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O85" s="3" t="str">
         <f aca="false">VLOOKUP(N85,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -9550,9 +9683,9 @@
         <v>15</v>
       </c>
       <c r="N86" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O86" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O86" s="3" t="str">
         <f aca="false">VLOOKUP(N86,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -9643,9 +9776,9 @@
         <v>15</v>
       </c>
       <c r="N87" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O87" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O87" s="3" t="str">
         <f aca="false">VLOOKUP(N87,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -9736,9 +9869,9 @@
         <v>15</v>
       </c>
       <c r="N88" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O88" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O88" s="3" t="str">
         <f aca="false">VLOOKUP(N88,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -9829,9 +9962,9 @@
         <v>7</v>
       </c>
       <c r="N89" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O89" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O89" s="3" t="str">
         <f aca="false">VLOOKUP(N89,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -9924,9 +10057,9 @@
         <v>10</v>
       </c>
       <c r="N90" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O90" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O90" s="3" t="str">
         <f aca="false">VLOOKUP(N90,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10017,9 +10150,9 @@
         <v>15</v>
       </c>
       <c r="N91" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O91" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O91" s="3" t="str">
         <f aca="false">VLOOKUP(N91,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10110,9 +10243,9 @@
         <v>7</v>
       </c>
       <c r="N92" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O92" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O92" s="3" t="str">
         <f aca="false">VLOOKUP(N92,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -10205,7 +10338,7 @@
       <c r="N93" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O93" s="8" t="str">
+      <c r="O93" s="3" t="str">
         <f aca="false">VLOOKUP(N93,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB )</v>
       </c>
@@ -10296,9 +10429,9 @@
         <v>7</v>
       </c>
       <c r="N94" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O94" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O94" s="3" t="str">
         <f aca="false">VLOOKUP(N94,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -10389,9 +10522,9 @@
         <v>15</v>
       </c>
       <c r="N95" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O95" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O95" s="3" t="str">
         <f aca="false">VLOOKUP(N95,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10482,9 +10615,9 @@
         <v>25</v>
       </c>
       <c r="N96" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O96" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O96" s="3" t="str">
         <f aca="false">VLOOKUP(N96,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10575,9 +10708,9 @@
         <v>25</v>
       </c>
       <c r="N97" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O97" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O97" s="3" t="str">
         <f aca="false">VLOOKUP(N97,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10668,9 +10801,9 @@
         <v>25</v>
       </c>
       <c r="N98" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O98" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O98" s="3" t="str">
         <f aca="false">VLOOKUP(N98,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10761,9 +10894,9 @@
         <v>25</v>
       </c>
       <c r="N99" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O99" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O99" s="3" t="str">
         <f aca="false">VLOOKUP(N99,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10854,9 +10987,9 @@
         <v>25</v>
       </c>
       <c r="N100" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O100" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O100" s="3" t="str">
         <f aca="false">VLOOKUP(N100,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -10947,9 +11080,9 @@
         <v>25</v>
       </c>
       <c r="N101" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O101" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O101" s="3" t="str">
         <f aca="false">VLOOKUP(N101,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11040,9 +11173,9 @@
         <v>25</v>
       </c>
       <c r="N102" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O102" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O102" s="3" t="str">
         <f aca="false">VLOOKUP(N102,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11133,9 +11266,9 @@
         <v>25</v>
       </c>
       <c r="N103" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O103" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O103" s="3" t="str">
         <f aca="false">VLOOKUP(N103,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11226,9 +11359,9 @@
         <v>25</v>
       </c>
       <c r="N104" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O104" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O104" s="3" t="str">
         <f aca="false">VLOOKUP(N104,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11319,9 +11452,9 @@
         <v>25</v>
       </c>
       <c r="N105" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O105" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O105" s="3" t="str">
         <f aca="false">VLOOKUP(N105,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11412,9 +11545,9 @@
         <v>25</v>
       </c>
       <c r="N106" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O106" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O106" s="3" t="str">
         <f aca="false">VLOOKUP(N106,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11505,9 +11638,9 @@
         <v>25</v>
       </c>
       <c r="N107" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O107" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O107" s="3" t="str">
         <f aca="false">VLOOKUP(N107,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11598,9 +11731,9 @@
         <v>25</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O108" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O108" s="3" t="str">
         <f aca="false">VLOOKUP(N108,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11691,9 +11824,9 @@
         <v>25</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O109" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O109" s="3" t="str">
         <f aca="false">VLOOKUP(N109,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11784,9 +11917,9 @@
         <v>25</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O110" s="8" t="str">
+        <v>91</v>
+      </c>
+      <c r="O110" s="3" t="str">
         <f aca="false">VLOOKUP(N110,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE)</v>
       </c>
@@ -11879,7 +12012,7 @@
       <c r="N111" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="O111" s="8" t="str">
+      <c r="O111" s="3" t="str">
         <f aca="false">VLOOKUP(N111,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
@@ -11972,7 +12105,7 @@
       <c r="N112" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O112" s="8" t="str">
+      <c r="O112" s="3" t="str">
         <f aca="false">VLOOKUP(N112,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -12065,7 +12198,7 @@
       <c r="N113" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O113" s="8" t="str">
+      <c r="O113" s="3" t="str">
         <f aca="false">VLOOKUP(N113,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -12158,7 +12291,7 @@
       <c r="N114" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="O114" s="8" t="str">
+      <c r="O114" s="3" t="str">
         <f aca="false">VLOOKUP(N114,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
@@ -12251,7 +12384,7 @@
       <c r="N115" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O115" s="8" t="str">
+      <c r="O115" s="3" t="str">
         <f aca="false">VLOOKUP(N115,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES &amp; ~bitmask(TOWNZONE_EDGE)</v>
       </c>
@@ -12344,7 +12477,7 @@
       <c r="N116" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O116" s="8" t="str">
+      <c r="O116" s="3" t="str">
         <f aca="false">VLOOKUP(N116,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
@@ -12437,7 +12570,7 @@
       <c r="N117" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O117" s="8" t="str">
+      <c r="O117" s="3" t="str">
         <f aca="false">VLOOKUP(N117,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -12530,7 +12663,7 @@
       <c r="N118" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O118" s="8" t="str">
+      <c r="O118" s="3" t="str">
         <f aca="false">VLOOKUP(N118,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -12623,7 +12756,7 @@
       <c r="N119" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O119" s="8" t="str">
+      <c r="O119" s="3" t="str">
         <f aca="false">VLOOKUP(N119,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -12716,7 +12849,7 @@
       <c r="N120" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O120" s="8" t="str">
+      <c r="O120" s="3" t="str">
         <f aca="false">VLOOKUP(N120,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_OUTER_SUBURB , TOWNZONE_OUTSKIRT, TOWNZONE_EDGE )</v>
       </c>
@@ -12809,7 +12942,7 @@
       <c r="N121" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O121" s="8" t="str">
+      <c r="O121" s="3" t="str">
         <f aca="false">VLOOKUP(N121,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -12900,9 +13033,9 @@
         <v>10</v>
       </c>
       <c r="N122" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O122" s="8" t="str">
+        <v>101</v>
+      </c>
+      <c r="O122" s="3" t="str">
         <f aca="false">VLOOKUP(N122,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_CENTRE, TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -12995,7 +13128,7 @@
       <c r="N123" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O123" s="8" t="str">
+      <c r="O123" s="3" t="str">
         <f aca="false">VLOOKUP(N123,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
@@ -13088,7 +13221,7 @@
       <c r="N124" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O124" s="8" t="str">
+      <c r="O124" s="3" t="str">
         <f aca="false">VLOOKUP(N124,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
@@ -13181,7 +13314,7 @@
       <c r="N125" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O125" s="8" t="str">
+      <c r="O125" s="3" t="str">
         <f aca="false">VLOOKUP(N125,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB )</v>
       </c>
@@ -13274,7 +13407,7 @@
       <c r="N126" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O126" s="8" t="str">
+      <c r="O126" s="3" t="str">
         <f aca="false">VLOOKUP(N126,dropdowns!E:F,2,0)</f>
         <v>ALL_TOWNZONES</v>
       </c>
@@ -13367,7 +13500,7 @@
       <c r="N127" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="O127" s="8" t="str">
+      <c r="O127" s="3" t="str">
         <f aca="false">VLOOKUP(N127,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
@@ -13460,7 +13593,7 @@
       <c r="N128" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="O128" s="8" t="str">
+      <c r="O128" s="3" t="str">
         <f aca="false">VLOOKUP(N128,dropdowns!E:F,2,0)</f>
         <v>bitmask(TOWNZONE_INNER_SUBURB, TOWNZONE_OUTER_SUBURB, TOWNZONE_OUTSKIRT)</v>
       </c>
@@ -13595,7 +13728,7 @@
         <f aca="false">IF(C2&gt;0,C2,MAX(D1-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="b">
+      <c r="E2" s="8" t="b">
         <f aca="false">D2=0</f>
         <v>0</v>
       </c>
@@ -13624,7 +13757,7 @@
         <f aca="false">IF(C3&gt;0,C3,MAX(D2-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="b">
+      <c r="E3" s="8" t="b">
         <f aca="false">D3=0</f>
         <v>0</v>
       </c>
@@ -13653,7 +13786,7 @@
         <f aca="false">IF(C4&gt;0,C4,MAX(D3-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="b">
+      <c r="E4" s="8" t="b">
         <f aca="false">D4=0</f>
         <v>0</v>
       </c>
@@ -13676,7 +13809,7 @@
         <f aca="false">IF(C5&gt;0,C5,MAX(D4-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="b">
+      <c r="E5" s="8" t="b">
         <f aca="false">D5=0</f>
         <v>0</v>
       </c>
@@ -13699,7 +13832,7 @@
         <f aca="false">IF(C6&gt;0,C6,MAX(D5-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E6" s="9" t="b">
+      <c r="E6" s="8" t="b">
         <f aca="false">D6=0</f>
         <v>0</v>
       </c>
@@ -13722,7 +13855,7 @@
         <f aca="false">IF(C7&gt;0,C7,MAX(D6-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E7" s="9" t="b">
+      <c r="E7" s="8" t="b">
         <f aca="false">D7=0</f>
         <v>0</v>
       </c>
@@ -13745,7 +13878,7 @@
         <f aca="false">IF(C8&gt;0,C8,MAX(D7-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E8" s="9" t="b">
+      <c r="E8" s="8" t="b">
         <f aca="false">D8=0</f>
         <v>0</v>
       </c>
@@ -13768,7 +13901,7 @@
         <f aca="false">IF(C9&gt;0,C9,MAX(D8-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E9" s="9" t="b">
+      <c r="E9" s="8" t="b">
         <f aca="false">D9=0</f>
         <v>0</v>
       </c>
@@ -13791,7 +13924,7 @@
         <f aca="false">IF(C10&gt;0,C10,MAX(D9-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E10" s="9" t="b">
+      <c r="E10" s="8" t="b">
         <f aca="false">D10=0</f>
         <v>0</v>
       </c>
@@ -13814,7 +13947,7 @@
         <f aca="false">IF(C11&gt;0,C11,MAX(D10-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E11" s="9" t="b">
+      <c r="E11" s="8" t="b">
         <f aca="false">D11=0</f>
         <v>0</v>
       </c>
@@ -13837,7 +13970,7 @@
         <f aca="false">IF(C12&gt;0,C12,MAX(D11-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E12" s="9" t="b">
+      <c r="E12" s="8" t="b">
         <f aca="false">D12=0</f>
         <v>0</v>
       </c>
@@ -13860,7 +13993,7 @@
         <f aca="false">IF(C13&gt;0,C13,MAX(D12-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E13" s="9" t="b">
+      <c r="E13" s="8" t="b">
         <f aca="false">D13=0</f>
         <v>0</v>
       </c>
@@ -13883,7 +14016,7 @@
         <f aca="false">IF(C14&gt;0,C14,MAX(D13-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E14" s="9" t="b">
+      <c r="E14" s="8" t="b">
         <f aca="false">D14=0</f>
         <v>0</v>
       </c>
@@ -13906,7 +14039,7 @@
         <f aca="false">IF(C15&gt;0,C15,MAX(D14-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E15" s="9" t="b">
+      <c r="E15" s="8" t="b">
         <f aca="false">D15=0</f>
         <v>0</v>
       </c>
@@ -13929,7 +14062,7 @@
         <f aca="false">IF(C16&gt;0,C16,MAX(D15-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E16" s="9" t="b">
+      <c r="E16" s="8" t="b">
         <f aca="false">D16=0</f>
         <v>0</v>
       </c>
@@ -13952,7 +14085,7 @@
         <f aca="false">IF(C17&gt;0,C17,MAX(D16-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E17" s="9" t="b">
+      <c r="E17" s="8" t="b">
         <f aca="false">D17=0</f>
         <v>0</v>
       </c>
@@ -13975,7 +14108,7 @@
         <f aca="false">IF(C18&gt;0,C18,MAX(D17-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E18" s="9" t="b">
+      <c r="E18" s="8" t="b">
         <f aca="false">D18=0</f>
         <v>0</v>
       </c>
@@ -13998,7 +14131,7 @@
         <f aca="false">IF(C19&gt;0,C19,MAX(D18-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E19" s="9" t="b">
+      <c r="E19" s="8" t="b">
         <f aca="false">D19=0</f>
         <v>0</v>
       </c>
@@ -14021,7 +14154,7 @@
         <f aca="false">IF(C20&gt;0,C20,MAX(D19-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E20" s="9" t="b">
+      <c r="E20" s="8" t="b">
         <f aca="false">D20=0</f>
         <v>0</v>
       </c>
@@ -14044,7 +14177,7 @@
         <f aca="false">IF(C21&gt;0,C21,MAX(D20-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E21" s="9" t="b">
+      <c r="E21" s="8" t="b">
         <f aca="false">D21=0</f>
         <v>0</v>
       </c>
@@ -14067,7 +14200,7 @@
         <f aca="false">IF(C22&gt;0,C22,MAX(D21-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E22" s="9" t="b">
+      <c r="E22" s="8" t="b">
         <f aca="false">D22=0</f>
         <v>0</v>
       </c>
@@ -14090,7 +14223,7 @@
         <f aca="false">IF(C23&gt;0,C23,MAX(D22-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E23" s="9" t="b">
+      <c r="E23" s="8" t="b">
         <f aca="false">D23=0</f>
         <v>0</v>
       </c>
@@ -14113,7 +14246,7 @@
         <f aca="false">IF(C24&gt;0,C24,MAX(D23-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E24" s="9" t="b">
+      <c r="E24" s="8" t="b">
         <f aca="false">D24=0</f>
         <v>0</v>
       </c>
@@ -14136,7 +14269,7 @@
         <f aca="false">IF(C25&gt;0,C25,MAX(D24-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E25" s="9" t="b">
+      <c r="E25" s="8" t="b">
         <f aca="false">D25=0</f>
         <v>0</v>
       </c>
@@ -14159,7 +14292,7 @@
         <f aca="false">IF(C26&gt;0,C26,MAX(D25-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E26" s="9" t="b">
+      <c r="E26" s="8" t="b">
         <f aca="false">D26=0</f>
         <v>0</v>
       </c>
@@ -14182,7 +14315,7 @@
         <f aca="false">IF(C27&gt;0,C27,MAX(D26-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E27" s="9" t="b">
+      <c r="E27" s="8" t="b">
         <f aca="false">D27=0</f>
         <v>0</v>
       </c>
@@ -14205,7 +14338,7 @@
         <f aca="false">IF(C28&gt;0,C28,MAX(D27-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E28" s="9" t="b">
+      <c r="E28" s="8" t="b">
         <f aca="false">D28=0</f>
         <v>0</v>
       </c>
@@ -14228,7 +14361,7 @@
         <f aca="false">IF(C29&gt;0,C29,MAX(D28-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E29" s="9" t="b">
+      <c r="E29" s="8" t="b">
         <f aca="false">D29=0</f>
         <v>0</v>
       </c>
@@ -14251,7 +14384,7 @@
         <f aca="false">IF(C30&gt;0,C30,MAX(D29-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E30" s="9" t="b">
+      <c r="E30" s="8" t="b">
         <f aca="false">D30=0</f>
         <v>0</v>
       </c>
@@ -14274,7 +14407,7 @@
         <f aca="false">IF(C31&gt;0,C31,MAX(D30-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E31" s="9" t="b">
+      <c r="E31" s="8" t="b">
         <f aca="false">D31=0</f>
         <v>0</v>
       </c>
@@ -14297,7 +14430,7 @@
         <f aca="false">IF(C32&gt;0,C32,MAX(D31-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E32" s="9" t="b">
+      <c r="E32" s="8" t="b">
         <f aca="false">D32=0</f>
         <v>0</v>
       </c>
@@ -14320,7 +14453,7 @@
         <f aca="false">IF(C33&gt;0,C33,MAX(D32-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E33" s="9" t="b">
+      <c r="E33" s="8" t="b">
         <f aca="false">D33=0</f>
         <v>0</v>
       </c>
@@ -14343,7 +14476,7 @@
         <f aca="false">IF(C34&gt;0,C34,MAX(D33-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E34" s="9" t="b">
+      <c r="E34" s="8" t="b">
         <f aca="false">D34=0</f>
         <v>0</v>
       </c>
@@ -14366,7 +14499,7 @@
         <f aca="false">IF(C35&gt;0,C35,MAX(D34-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E35" s="9" t="b">
+      <c r="E35" s="8" t="b">
         <f aca="false">D35=0</f>
         <v>0</v>
       </c>
@@ -14389,7 +14522,7 @@
         <f aca="false">IF(C36&gt;0,C36,MAX(D35-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E36" s="9" t="b">
+      <c r="E36" s="8" t="b">
         <f aca="false">D36=0</f>
         <v>0</v>
       </c>
@@ -14412,7 +14545,7 @@
         <f aca="false">IF(C37&gt;0,C37,MAX(D36-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E37" s="9" t="b">
+      <c r="E37" s="8" t="b">
         <f aca="false">D37=0</f>
         <v>0</v>
       </c>
@@ -14435,7 +14568,7 @@
         <f aca="false">IF(C38&gt;0,C38,MAX(D37-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E38" s="9" t="b">
+      <c r="E38" s="8" t="b">
         <f aca="false">D38=0</f>
         <v>0</v>
       </c>
@@ -14458,7 +14591,7 @@
         <f aca="false">IF(C39&gt;0,C39,MAX(D38-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E39" s="9" t="b">
+      <c r="E39" s="8" t="b">
         <f aca="false">D39=0</f>
         <v>0</v>
       </c>
@@ -14481,7 +14614,7 @@
         <f aca="false">IF(C40&gt;0,C40,MAX(D39-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E40" s="9" t="b">
+      <c r="E40" s="8" t="b">
         <f aca="false">D40=0</f>
         <v>0</v>
       </c>
@@ -14504,7 +14637,7 @@
         <f aca="false">IF(C41&gt;0,C41,MAX(D40-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E41" s="9" t="b">
+      <c r="E41" s="8" t="b">
         <f aca="false">D41=0</f>
         <v>0</v>
       </c>
@@ -14527,7 +14660,7 @@
         <f aca="false">IF(C42&gt;0,C42,MAX(D41-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E42" s="9" t="b">
+      <c r="E42" s="8" t="b">
         <f aca="false">D42=0</f>
         <v>0</v>
       </c>
@@ -14550,7 +14683,7 @@
         <f aca="false">IF(C43&gt;0,C43,MAX(D42-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E43" s="9" t="b">
+      <c r="E43" s="8" t="b">
         <f aca="false">D43=0</f>
         <v>0</v>
       </c>
@@ -14573,7 +14706,7 @@
         <f aca="false">IF(C44&gt;0,C44,MAX(D43-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E44" s="9" t="b">
+      <c r="E44" s="8" t="b">
         <f aca="false">D44=0</f>
         <v>0</v>
       </c>
@@ -14596,7 +14729,7 @@
         <f aca="false">IF(C45&gt;0,C45,MAX(D44-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E45" s="9" t="b">
+      <c r="E45" s="8" t="b">
         <f aca="false">D45=0</f>
         <v>0</v>
       </c>
@@ -14619,7 +14752,7 @@
         <f aca="false">IF(C46&gt;0,C46,MAX(D45-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E46" s="9" t="b">
+      <c r="E46" s="8" t="b">
         <f aca="false">D46=0</f>
         <v>0</v>
       </c>
@@ -14642,7 +14775,7 @@
         <f aca="false">IF(C47&gt;0,C47,MAX(D46-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E47" s="9" t="b">
+      <c r="E47" s="8" t="b">
         <f aca="false">D47=0</f>
         <v>0</v>
       </c>
@@ -14665,7 +14798,7 @@
         <f aca="false">IF(C48&gt;0,C48,MAX(D47-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E48" s="9" t="b">
+      <c r="E48" s="8" t="b">
         <f aca="false">D48=0</f>
         <v>0</v>
       </c>
@@ -14688,7 +14821,7 @@
         <f aca="false">IF(C49&gt;0,C49,MAX(D48-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E49" s="9" t="b">
+      <c r="E49" s="8" t="b">
         <f aca="false">D49=0</f>
         <v>0</v>
       </c>
@@ -14711,7 +14844,7 @@
         <f aca="false">IF(C50&gt;0,C50,MAX(D49-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E50" s="9" t="b">
+      <c r="E50" s="8" t="b">
         <f aca="false">D50=0</f>
         <v>0</v>
       </c>
@@ -14734,7 +14867,7 @@
         <f aca="false">IF(C51&gt;0,C51,MAX(D50-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E51" s="9" t="b">
+      <c r="E51" s="8" t="b">
         <f aca="false">D51=0</f>
         <v>0</v>
       </c>
@@ -14757,7 +14890,7 @@
         <f aca="false">IF(C52&gt;0,C52,MAX(D51-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E52" s="9" t="b">
+      <c r="E52" s="8" t="b">
         <f aca="false">D52=0</f>
         <v>0</v>
       </c>
@@ -14780,7 +14913,7 @@
         <f aca="false">IF(C53&gt;0,C53,MAX(D52-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E53" s="9" t="b">
+      <c r="E53" s="8" t="b">
         <f aca="false">D53=0</f>
         <v>0</v>
       </c>
@@ -14803,7 +14936,7 @@
         <f aca="false">IF(C54&gt;0,C54,MAX(D53-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E54" s="9" t="b">
+      <c r="E54" s="8" t="b">
         <f aca="false">D54=0</f>
         <v>0</v>
       </c>
@@ -14826,7 +14959,7 @@
         <f aca="false">IF(C55&gt;0,C55,MAX(D54-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E55" s="9" t="b">
+      <c r="E55" s="8" t="b">
         <f aca="false">D55=0</f>
         <v>0</v>
       </c>
@@ -14849,7 +14982,7 @@
         <f aca="false">IF(C56&gt;0,C56,MAX(D55-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E56" s="9" t="b">
+      <c r="E56" s="8" t="b">
         <f aca="false">D56=0</f>
         <v>1</v>
       </c>
@@ -14872,7 +15005,7 @@
         <f aca="false">IF(C57&gt;0,C57,MAX(D56-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E57" s="9" t="b">
+      <c r="E57" s="8" t="b">
         <f aca="false">D57=0</f>
         <v>1</v>
       </c>
@@ -14895,7 +15028,7 @@
         <f aca="false">IF(C58&gt;0,C58,MAX(D57-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E58" s="9" t="b">
+      <c r="E58" s="8" t="b">
         <f aca="false">D58=0</f>
         <v>0</v>
       </c>
@@ -14918,7 +15051,7 @@
         <f aca="false">IF(C59&gt;0,C59,MAX(D58-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E59" s="9" t="b">
+      <c r="E59" s="8" t="b">
         <f aca="false">D59=0</f>
         <v>0</v>
       </c>
@@ -14941,7 +15074,7 @@
         <f aca="false">IF(C60&gt;0,C60,MAX(D59-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E60" s="9" t="b">
+      <c r="E60" s="8" t="b">
         <f aca="false">D60=0</f>
         <v>0</v>
       </c>
@@ -14964,7 +15097,7 @@
         <f aca="false">IF(C61&gt;0,C61,MAX(D60-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E61" s="9" t="b">
+      <c r="E61" s="8" t="b">
         <f aca="false">D61=0</f>
         <v>1</v>
       </c>
@@ -14987,7 +15120,7 @@
         <f aca="false">IF(C62&gt;0,C62,MAX(D61-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E62" s="9" t="b">
+      <c r="E62" s="8" t="b">
         <f aca="false">D62=0</f>
         <v>1</v>
       </c>
@@ -15010,7 +15143,7 @@
         <f aca="false">IF(C63&gt;0,C63,MAX(D62-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E63" s="9" t="b">
+      <c r="E63" s="8" t="b">
         <f aca="false">D63=0</f>
         <v>1</v>
       </c>
@@ -15033,7 +15166,7 @@
         <f aca="false">IF(C64&gt;0,C64,MAX(D63-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E64" s="9" t="b">
+      <c r="E64" s="8" t="b">
         <f aca="false">D64=0</f>
         <v>1</v>
       </c>
@@ -15056,7 +15189,7 @@
         <f aca="false">IF(C65&gt;0,C65,MAX(D64-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E65" s="9" t="b">
+      <c r="E65" s="8" t="b">
         <f aca="false">D65=0</f>
         <v>1</v>
       </c>
@@ -15079,7 +15212,7 @@
         <f aca="false">IF(C66&gt;0,C66,MAX(D65-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E66" s="9" t="b">
+      <c r="E66" s="8" t="b">
         <f aca="false">D66=0</f>
         <v>0</v>
       </c>
@@ -15102,7 +15235,7 @@
         <f aca="false">IF(C67&gt;0,C67,MAX(D66-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E67" s="9" t="b">
+      <c r="E67" s="8" t="b">
         <f aca="false">D67=0</f>
         <v>0</v>
       </c>
@@ -15125,7 +15258,7 @@
         <f aca="false">IF(C68&gt;0,C68,MAX(D67-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E68" s="9" t="b">
+      <c r="E68" s="8" t="b">
         <f aca="false">D68=0</f>
         <v>1</v>
       </c>
@@ -15148,7 +15281,7 @@
         <f aca="false">IF(C69&gt;0,C69,MAX(D68-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E69" s="9" t="b">
+      <c r="E69" s="8" t="b">
         <f aca="false">D69=0</f>
         <v>1</v>
       </c>
@@ -15171,7 +15304,7 @@
         <f aca="false">IF(C70&gt;0,C70,MAX(D69-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E70" s="9" t="b">
+      <c r="E70" s="8" t="b">
         <f aca="false">D70=0</f>
         <v>1</v>
       </c>
@@ -15194,7 +15327,7 @@
         <f aca="false">IF(C71&gt;0,C71,MAX(D70-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E71" s="9" t="b">
+      <c r="E71" s="8" t="b">
         <f aca="false">D71=0</f>
         <v>1</v>
       </c>
@@ -15217,7 +15350,7 @@
         <f aca="false">IF(C72&gt;0,C72,MAX(D71-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E72" s="9" t="b">
+      <c r="E72" s="8" t="b">
         <f aca="false">D72=0</f>
         <v>1</v>
       </c>
@@ -15240,7 +15373,7 @@
         <f aca="false">IF(C73&gt;0,C73,MAX(D72-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E73" s="9" t="b">
+      <c r="E73" s="8" t="b">
         <f aca="false">D73=0</f>
         <v>1</v>
       </c>
@@ -15263,7 +15396,7 @@
         <f aca="false">IF(C74&gt;0,C74,MAX(D73-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E74" s="9" t="b">
+      <c r="E74" s="8" t="b">
         <f aca="false">D74=0</f>
         <v>1</v>
       </c>
@@ -15286,7 +15419,7 @@
         <f aca="false">IF(C75&gt;0,C75,MAX(D74-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E75" s="9" t="b">
+      <c r="E75" s="8" t="b">
         <f aca="false">D75=0</f>
         <v>1</v>
       </c>
@@ -15309,7 +15442,7 @@
         <f aca="false">IF(C76&gt;0,C76,MAX(D75-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E76" s="9" t="b">
+      <c r="E76" s="8" t="b">
         <f aca="false">D76=0</f>
         <v>0</v>
       </c>
@@ -15332,7 +15465,7 @@
         <f aca="false">IF(C77&gt;0,C77,MAX(D76-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E77" s="9" t="b">
+      <c r="E77" s="8" t="b">
         <f aca="false">D77=0</f>
         <v>0</v>
       </c>
@@ -15355,7 +15488,7 @@
         <f aca="false">IF(C78&gt;0,C78,MAX(D77-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E78" s="9" t="b">
+      <c r="E78" s="8" t="b">
         <f aca="false">D78=0</f>
         <v>0</v>
       </c>
@@ -15378,7 +15511,7 @@
         <f aca="false">IF(C79&gt;0,C79,MAX(D78-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E79" s="9" t="b">
+      <c r="E79" s="8" t="b">
         <f aca="false">D79=0</f>
         <v>0</v>
       </c>
@@ -15401,7 +15534,7 @@
         <f aca="false">IF(C80&gt;0,C80,MAX(D79-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E80" s="9" t="b">
+      <c r="E80" s="8" t="b">
         <f aca="false">D80=0</f>
         <v>0</v>
       </c>
@@ -15424,7 +15557,7 @@
         <f aca="false">IF(C81&gt;0,C81,MAX(D80-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E81" s="9" t="b">
+      <c r="E81" s="8" t="b">
         <f aca="false">D81=0</f>
         <v>0</v>
       </c>
@@ -15447,7 +15580,7 @@
         <f aca="false">IF(C82&gt;0,C82,MAX(D81-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E82" s="9" t="b">
+      <c r="E82" s="8" t="b">
         <f aca="false">D82=0</f>
         <v>0</v>
       </c>
@@ -15470,7 +15603,7 @@
         <f aca="false">IF(C83&gt;0,C83,MAX(D82-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E83" s="9" t="b">
+      <c r="E83" s="8" t="b">
         <f aca="false">D83=0</f>
         <v>0</v>
       </c>
@@ -15493,7 +15626,7 @@
         <f aca="false">IF(C84&gt;0,C84,MAX(D83-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E84" s="9" t="b">
+      <c r="E84" s="8" t="b">
         <f aca="false">D84=0</f>
         <v>0</v>
       </c>
@@ -15516,7 +15649,7 @@
         <f aca="false">IF(C85&gt;0,C85,MAX(D84-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E85" s="9" t="b">
+      <c r="E85" s="8" t="b">
         <f aca="false">D85=0</f>
         <v>0</v>
       </c>
@@ -15539,7 +15672,7 @@
         <f aca="false">IF(C86&gt;0,C86,MAX(D85-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E86" s="9" t="b">
+      <c r="E86" s="8" t="b">
         <f aca="false">D86=0</f>
         <v>0</v>
       </c>
@@ -15562,7 +15695,7 @@
         <f aca="false">IF(C87&gt;0,C87,MAX(D86-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E87" s="9" t="b">
+      <c r="E87" s="8" t="b">
         <f aca="false">D87=0</f>
         <v>0</v>
       </c>
@@ -15585,7 +15718,7 @@
         <f aca="false">IF(C88&gt;0,C88,MAX(D87-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E88" s="9" t="b">
+      <c r="E88" s="8" t="b">
         <f aca="false">D88=0</f>
         <v>0</v>
       </c>
@@ -15608,7 +15741,7 @@
         <f aca="false">IF(C89&gt;0,C89,MAX(D88-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E89" s="9" t="b">
+      <c r="E89" s="8" t="b">
         <f aca="false">D89=0</f>
         <v>0</v>
       </c>
@@ -15631,7 +15764,7 @@
         <f aca="false">IF(C90&gt;0,C90,MAX(D89-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E90" s="9" t="b">
+      <c r="E90" s="8" t="b">
         <f aca="false">D90=0</f>
         <v>1</v>
       </c>
@@ -15654,7 +15787,7 @@
         <f aca="false">IF(C91&gt;0,C91,MAX(D90-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E91" s="9" t="b">
+      <c r="E91" s="8" t="b">
         <f aca="false">D91=0</f>
         <v>0</v>
       </c>
@@ -15677,7 +15810,7 @@
         <f aca="false">IF(C92&gt;0,C92,MAX(D91-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E92" s="9" t="b">
+      <c r="E92" s="8" t="b">
         <f aca="false">D92=0</f>
         <v>1</v>
       </c>
@@ -15700,7 +15833,7 @@
         <f aca="false">IF(C93&gt;0,C93,MAX(D92-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E93" s="9" t="b">
+      <c r="E93" s="8" t="b">
         <f aca="false">D93=0</f>
         <v>0</v>
       </c>
@@ -15723,7 +15856,7 @@
         <f aca="false">IF(C94&gt;0,C94,MAX(D93-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E94" s="9" t="b">
+      <c r="E94" s="8" t="b">
         <f aca="false">D94=0</f>
         <v>1</v>
       </c>
@@ -15746,7 +15879,7 @@
         <f aca="false">IF(C95&gt;0,C95,MAX(D94-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E95" s="9" t="b">
+      <c r="E95" s="8" t="b">
         <f aca="false">D95=0</f>
         <v>0</v>
       </c>
@@ -15769,7 +15902,7 @@
         <f aca="false">IF(C96&gt;0,C96,MAX(D95-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E96" s="9" t="b">
+      <c r="E96" s="8" t="b">
         <f aca="false">D96=0</f>
         <v>0</v>
       </c>
@@ -15792,7 +15925,7 @@
         <f aca="false">IF(C97&gt;0,C97,MAX(D96-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E97" s="9" t="b">
+      <c r="E97" s="8" t="b">
         <f aca="false">D97=0</f>
         <v>0</v>
       </c>
@@ -15815,7 +15948,7 @@
         <f aca="false">IF(C98&gt;0,C98,MAX(D97-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E98" s="9" t="b">
+      <c r="E98" s="8" t="b">
         <f aca="false">D98=0</f>
         <v>0</v>
       </c>
@@ -15838,7 +15971,7 @@
         <f aca="false">IF(C99&gt;0,C99,MAX(D98-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E99" s="9" t="b">
+      <c r="E99" s="8" t="b">
         <f aca="false">D99=0</f>
         <v>1</v>
       </c>
@@ -15861,7 +15994,7 @@
         <f aca="false">IF(C100&gt;0,C100,MAX(D99-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E100" s="9" t="b">
+      <c r="E100" s="8" t="b">
         <f aca="false">D100=0</f>
         <v>1</v>
       </c>
@@ -15884,7 +16017,7 @@
         <f aca="false">IF(C101&gt;0,C101,MAX(D100-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E101" s="9" t="b">
+      <c r="E101" s="8" t="b">
         <f aca="false">D101=0</f>
         <v>1</v>
       </c>
@@ -15907,7 +16040,7 @@
         <f aca="false">IF(C102&gt;0,C102,MAX(D101-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E102" s="9" t="b">
+      <c r="E102" s="8" t="b">
         <f aca="false">D102=0</f>
         <v>1</v>
       </c>
@@ -15930,7 +16063,7 @@
         <f aca="false">IF(C103&gt;0,C103,MAX(D102-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E103" s="9" t="b">
+      <c r="E103" s="8" t="b">
         <f aca="false">D103=0</f>
         <v>0</v>
       </c>
@@ -15953,7 +16086,7 @@
         <f aca="false">IF(C104&gt;0,C104,MAX(D103-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E104" s="9" t="b">
+      <c r="E104" s="8" t="b">
         <f aca="false">D104=0</f>
         <v>0</v>
       </c>
@@ -15976,7 +16109,7 @@
         <f aca="false">IF(C105&gt;0,C105,MAX(D104-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E105" s="9" t="b">
+      <c r="E105" s="8" t="b">
         <f aca="false">D105=0</f>
         <v>1</v>
       </c>
@@ -15999,7 +16132,7 @@
         <f aca="false">IF(C106&gt;0,C106,MAX(D105-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E106" s="9" t="b">
+      <c r="E106" s="8" t="b">
         <f aca="false">D106=0</f>
         <v>1</v>
       </c>
@@ -16022,7 +16155,7 @@
         <f aca="false">IF(C107&gt;0,C107,MAX(D106-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E107" s="9" t="b">
+      <c r="E107" s="8" t="b">
         <f aca="false">D107=0</f>
         <v>0</v>
       </c>
@@ -16045,7 +16178,7 @@
         <f aca="false">IF(C108&gt;0,C108,MAX(D107-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E108" s="9" t="b">
+      <c r="E108" s="8" t="b">
         <f aca="false">D108=0</f>
         <v>0</v>
       </c>
@@ -16068,7 +16201,7 @@
         <f aca="false">IF(C109&gt;0,C109,MAX(D108-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E109" s="9" t="b">
+      <c r="E109" s="8" t="b">
         <f aca="false">D109=0</f>
         <v>0</v>
       </c>
@@ -16091,7 +16224,7 @@
         <f aca="false">IF(C110&gt;0,C110,MAX(D109-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E110" s="9" t="b">
+      <c r="E110" s="8" t="b">
         <f aca="false">D110=0</f>
         <v>0</v>
       </c>
@@ -16114,7 +16247,7 @@
         <f aca="false">IF(C111&gt;0,C111,MAX(D110-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E111" s="9" t="b">
+      <c r="E111" s="8" t="b">
         <f aca="false">D111=0</f>
         <v>0</v>
       </c>
@@ -16137,7 +16270,7 @@
         <f aca="false">IF(C112&gt;0,C112,MAX(D111-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E112" s="9" t="b">
+      <c r="E112" s="8" t="b">
         <f aca="false">D112=0</f>
         <v>0</v>
       </c>
@@ -16160,7 +16293,7 @@
         <f aca="false">IF(C113&gt;0,C113,MAX(D112-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E113" s="9" t="b">
+      <c r="E113" s="8" t="b">
         <f aca="false">D113=0</f>
         <v>0</v>
       </c>
@@ -16183,7 +16316,7 @@
         <f aca="false">IF(C114&gt;0,C114,MAX(D113-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E114" s="9" t="b">
+      <c r="E114" s="8" t="b">
         <f aca="false">D114=0</f>
         <v>1</v>
       </c>
@@ -16206,7 +16339,7 @@
         <f aca="false">IF(C115&gt;0,C115,MAX(D114-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E115" s="9" t="b">
+      <c r="E115" s="8" t="b">
         <f aca="false">D115=0</f>
         <v>0</v>
       </c>
@@ -16229,7 +16362,7 @@
         <f aca="false">IF(C116&gt;0,C116,MAX(D115-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E116" s="9" t="b">
+      <c r="E116" s="8" t="b">
         <f aca="false">D116=0</f>
         <v>0</v>
       </c>
@@ -16252,7 +16385,7 @@
         <f aca="false">IF(C117&gt;0,C117,MAX(D116-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E117" s="9" t="b">
+      <c r="E117" s="8" t="b">
         <f aca="false">D117=0</f>
         <v>0</v>
       </c>
@@ -16275,7 +16408,7 @@
         <f aca="false">IF(C118&gt;0,C118,MAX(D117-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E118" s="9" t="b">
+      <c r="E118" s="8" t="b">
         <f aca="false">D118=0</f>
         <v>0</v>
       </c>
@@ -16298,7 +16431,7 @@
         <f aca="false">IF(C119&gt;0,C119,MAX(D118-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E119" s="9" t="b">
+      <c r="E119" s="8" t="b">
         <f aca="false">D119=0</f>
         <v>1</v>
       </c>
@@ -16321,7 +16454,7 @@
         <f aca="false">IF(C120&gt;0,C120,MAX(D119-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E120" s="9" t="b">
+      <c r="E120" s="8" t="b">
         <f aca="false">D120=0</f>
         <v>0</v>
       </c>
@@ -16344,7 +16477,7 @@
         <f aca="false">IF(C121&gt;0,C121,MAX(D120-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E121" s="9" t="b">
+      <c r="E121" s="8" t="b">
         <f aca="false">D121=0</f>
         <v>1</v>
       </c>
@@ -16367,7 +16500,7 @@
         <f aca="false">IF(C122&gt;0,C122,MAX(D121-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E122" s="9" t="b">
+      <c r="E122" s="8" t="b">
         <f aca="false">D122=0</f>
         <v>0</v>
       </c>
@@ -16390,7 +16523,7 @@
         <f aca="false">IF(C123&gt;0,C123,MAX(D122-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E123" s="9" t="b">
+      <c r="E123" s="8" t="b">
         <f aca="false">D123=0</f>
         <v>0</v>
       </c>
@@ -16413,7 +16546,7 @@
         <f aca="false">IF(C124&gt;0,C124,MAX(D123-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E124" s="9" t="b">
+      <c r="E124" s="8" t="b">
         <f aca="false">D124=0</f>
         <v>0</v>
       </c>
@@ -16436,7 +16569,7 @@
         <f aca="false">IF(C125&gt;0,C125,MAX(D124-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E125" s="9" t="b">
+      <c r="E125" s="8" t="b">
         <f aca="false">D125=0</f>
         <v>0</v>
       </c>
@@ -16459,7 +16592,7 @@
         <f aca="false">IF(C126&gt;0,C126,MAX(D125-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E126" s="9" t="b">
+      <c r="E126" s="8" t="b">
         <f aca="false">D126=0</f>
         <v>0</v>
       </c>
@@ -16482,7 +16615,7 @@
         <f aca="false">IF(C127&gt;0,C127,MAX(D126-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E127" s="9" t="b">
+      <c r="E127" s="8" t="b">
         <f aca="false">D127=0</f>
         <v>0</v>
       </c>
@@ -16505,7 +16638,7 @@
         <f aca="false">IF(C128&gt;0,C128,MAX(D127-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E128" s="9" t="b">
+      <c r="E128" s="8" t="b">
         <f aca="false">D128=0</f>
         <v>0</v>
       </c>
@@ -16528,7 +16661,7 @@
         <f aca="false">IF(C129&gt;0,C129,MAX(D128-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E129" s="9" t="b">
+      <c r="E129" s="8" t="b">
         <f aca="false">D129=0</f>
         <v>0</v>
       </c>
@@ -16551,7 +16684,7 @@
         <f aca="false">IF(C130&gt;0,C130,MAX(D129-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E130" s="9" t="b">
+      <c r="E130" s="8" t="b">
         <f aca="false">D130=0</f>
         <v>0</v>
       </c>
@@ -16574,7 +16707,7 @@
         <f aca="false">IF(C131&gt;0,C131,MAX(D130-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E131" s="9" t="b">
+      <c r="E131" s="8" t="b">
         <f aca="false">D131=0</f>
         <v>0</v>
       </c>
@@ -16597,7 +16730,7 @@
         <f aca="false">IF(C132&gt;0,C132,MAX(D131-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E132" s="9" t="b">
+      <c r="E132" s="8" t="b">
         <f aca="false">D132=0</f>
         <v>0</v>
       </c>
@@ -16620,7 +16753,7 @@
         <f aca="false">IF(C133&gt;0,C133,MAX(D132-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E133" s="9" t="b">
+      <c r="E133" s="8" t="b">
         <f aca="false">D133=0</f>
         <v>0</v>
       </c>
@@ -16643,7 +16776,7 @@
         <f aca="false">IF(C134&gt;0,C134,MAX(D133-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E134" s="9" t="b">
+      <c r="E134" s="8" t="b">
         <f aca="false">D134=0</f>
         <v>0</v>
       </c>
@@ -16666,7 +16799,7 @@
         <f aca="false">IF(C135&gt;0,C135,MAX(D134-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E135" s="9" t="b">
+      <c r="E135" s="8" t="b">
         <f aca="false">D135=0</f>
         <v>0</v>
       </c>
@@ -16689,7 +16822,7 @@
         <f aca="false">IF(C136&gt;0,C136,MAX(D135-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E136" s="9" t="b">
+      <c r="E136" s="8" t="b">
         <f aca="false">D136=0</f>
         <v>0</v>
       </c>
@@ -16712,7 +16845,7 @@
         <f aca="false">IF(C137&gt;0,C137,MAX(D136-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E137" s="9" t="b">
+      <c r="E137" s="8" t="b">
         <f aca="false">D137=0</f>
         <v>0</v>
       </c>
@@ -16735,7 +16868,7 @@
         <f aca="false">IF(C138&gt;0,C138,MAX(D137-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E138" s="9" t="b">
+      <c r="E138" s="8" t="b">
         <f aca="false">D138=0</f>
         <v>0</v>
       </c>
@@ -16758,7 +16891,7 @@
         <f aca="false">IF(C139&gt;0,C139,MAX(D138-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E139" s="9" t="b">
+      <c r="E139" s="8" t="b">
         <f aca="false">D139=0</f>
         <v>0</v>
       </c>
@@ -16781,7 +16914,7 @@
         <f aca="false">IF(C140&gt;0,C140,MAX(D139-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E140" s="9" t="b">
+      <c r="E140" s="8" t="b">
         <f aca="false">D140=0</f>
         <v>0</v>
       </c>
@@ -16804,7 +16937,7 @@
         <f aca="false">IF(C141&gt;0,C141,MAX(D140-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E141" s="9" t="b">
+      <c r="E141" s="8" t="b">
         <f aca="false">D141=0</f>
         <v>0</v>
       </c>
@@ -16827,7 +16960,7 @@
         <f aca="false">IF(C142&gt;0,C142,MAX(D141-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E142" s="9" t="b">
+      <c r="E142" s="8" t="b">
         <f aca="false">D142=0</f>
         <v>0</v>
       </c>
@@ -16850,7 +16983,7 @@
         <f aca="false">IF(C143&gt;0,C143,MAX(D142-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E143" s="9" t="b">
+      <c r="E143" s="8" t="b">
         <f aca="false">D143=0</f>
         <v>0</v>
       </c>
@@ -16873,7 +17006,7 @@
         <f aca="false">IF(C144&gt;0,C144,MAX(D143-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E144" s="9" t="b">
+      <c r="E144" s="8" t="b">
         <f aca="false">D144=0</f>
         <v>0</v>
       </c>
@@ -16896,7 +17029,7 @@
         <f aca="false">IF(C145&gt;0,C145,MAX(D144-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E145" s="9" t="b">
+      <c r="E145" s="8" t="b">
         <f aca="false">D145=0</f>
         <v>0</v>
       </c>
@@ -16919,7 +17052,7 @@
         <f aca="false">IF(C146&gt;0,C146,MAX(D145-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E146" s="9" t="b">
+      <c r="E146" s="8" t="b">
         <f aca="false">D146=0</f>
         <v>0</v>
       </c>
@@ -16942,7 +17075,7 @@
         <f aca="false">IF(C147&gt;0,C147,MAX(D146-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E147" s="9" t="b">
+      <c r="E147" s="8" t="b">
         <f aca="false">D147=0</f>
         <v>0</v>
       </c>
@@ -16965,7 +17098,7 @@
         <f aca="false">IF(C148&gt;0,C148,MAX(D147-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E148" s="9" t="b">
+      <c r="E148" s="8" t="b">
         <f aca="false">D148=0</f>
         <v>0</v>
       </c>
@@ -16988,7 +17121,7 @@
         <f aca="false">IF(C149&gt;0,C149,MAX(D148-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E149" s="9" t="b">
+      <c r="E149" s="8" t="b">
         <f aca="false">D149=0</f>
         <v>0</v>
       </c>
@@ -17011,7 +17144,7 @@
         <f aca="false">IF(C150&gt;0,C150,MAX(D149-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E150" s="9" t="b">
+      <c r="E150" s="8" t="b">
         <f aca="false">D150=0</f>
         <v>0</v>
       </c>
@@ -17034,7 +17167,7 @@
         <f aca="false">IF(C151&gt;0,C151,MAX(D150-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E151" s="9" t="b">
+      <c r="E151" s="8" t="b">
         <f aca="false">D151=0</f>
         <v>0</v>
       </c>
@@ -17057,7 +17190,7 @@
         <f aca="false">IF(C152&gt;0,C152,MAX(D151-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E152" s="9" t="b">
+      <c r="E152" s="8" t="b">
         <f aca="false">D152=0</f>
         <v>0</v>
       </c>
@@ -17080,7 +17213,7 @@
         <f aca="false">IF(C153&gt;0,C153,MAX(D152-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E153" s="9" t="b">
+      <c r="E153" s="8" t="b">
         <f aca="false">D153=0</f>
         <v>0</v>
       </c>
@@ -17103,7 +17236,7 @@
         <f aca="false">IF(C154&gt;0,C154,MAX(D153-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E154" s="9" t="b">
+      <c r="E154" s="8" t="b">
         <f aca="false">D154=0</f>
         <v>0</v>
       </c>
@@ -17126,7 +17259,7 @@
         <f aca="false">IF(C155&gt;0,C155,MAX(D154-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E155" s="9" t="b">
+      <c r="E155" s="8" t="b">
         <f aca="false">D155=0</f>
         <v>0</v>
       </c>
@@ -17149,7 +17282,7 @@
         <f aca="false">IF(C156&gt;0,C156,MAX(D155-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E156" s="9" t="b">
+      <c r="E156" s="8" t="b">
         <f aca="false">D156=0</f>
         <v>0</v>
       </c>
@@ -17172,7 +17305,7 @@
         <f aca="false">IF(C157&gt;0,C157,MAX(D156-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E157" s="9" t="b">
+      <c r="E157" s="8" t="b">
         <f aca="false">D157=0</f>
         <v>1</v>
       </c>
@@ -17195,7 +17328,7 @@
         <f aca="false">IF(C158&gt;0,C158,MAX(D157-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E158" s="9" t="b">
+      <c r="E158" s="8" t="b">
         <f aca="false">D158=0</f>
         <v>1</v>
       </c>
@@ -17218,7 +17351,7 @@
         <f aca="false">IF(C159&gt;0,C159,MAX(D158-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E159" s="9" t="b">
+      <c r="E159" s="8" t="b">
         <f aca="false">D159=0</f>
         <v>1</v>
       </c>
@@ -17241,7 +17374,7 @@
         <f aca="false">IF(C160&gt;0,C160,MAX(D159-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E160" s="9" t="b">
+      <c r="E160" s="8" t="b">
         <f aca="false">D160=0</f>
         <v>1</v>
       </c>
@@ -17264,7 +17397,7 @@
         <f aca="false">IF(C161&gt;0,C161,MAX(D160-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E161" s="9" t="b">
+      <c r="E161" s="8" t="b">
         <f aca="false">D161=0</f>
         <v>1</v>
       </c>
@@ -17287,7 +17420,7 @@
         <f aca="false">IF(C162&gt;0,C162,MAX(D161-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E162" s="9" t="b">
+      <c r="E162" s="8" t="b">
         <f aca="false">D162=0</f>
         <v>1</v>
       </c>
@@ -17310,7 +17443,7 @@
         <f aca="false">IF(C163&gt;0,C163,MAX(D162-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E163" s="9" t="b">
+      <c r="E163" s="8" t="b">
         <f aca="false">D163=0</f>
         <v>1</v>
       </c>
@@ -17333,7 +17466,7 @@
         <f aca="false">IF(C164&gt;0,C164,MAX(D163-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E164" s="9" t="b">
+      <c r="E164" s="8" t="b">
         <f aca="false">D164=0</f>
         <v>1</v>
       </c>
@@ -17356,7 +17489,7 @@
         <f aca="false">IF(C165&gt;0,C165,MAX(D164-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E165" s="9" t="b">
+      <c r="E165" s="8" t="b">
         <f aca="false">D165=0</f>
         <v>1</v>
       </c>
@@ -17379,7 +17512,7 @@
         <f aca="false">IF(C166&gt;0,C166,MAX(D165-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E166" s="9" t="b">
+      <c r="E166" s="8" t="b">
         <f aca="false">D166=0</f>
         <v>1</v>
       </c>
@@ -17402,7 +17535,7 @@
         <f aca="false">IF(C167&gt;0,C167,MAX(D166-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E167" s="9" t="b">
+      <c r="E167" s="8" t="b">
         <f aca="false">D167=0</f>
         <v>1</v>
       </c>
@@ -17425,7 +17558,7 @@
         <f aca="false">IF(C168&gt;0,C168,MAX(D167-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E168" s="9" t="b">
+      <c r="E168" s="8" t="b">
         <f aca="false">D168=0</f>
         <v>1</v>
       </c>
@@ -17448,7 +17581,7 @@
         <f aca="false">IF(C169&gt;0,C169,MAX(D168-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E169" s="9" t="b">
+      <c r="E169" s="8" t="b">
         <f aca="false">D169=0</f>
         <v>1</v>
       </c>
@@ -17471,7 +17604,7 @@
         <f aca="false">IF(C170&gt;0,C170,MAX(D169-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E170" s="9" t="b">
+      <c r="E170" s="8" t="b">
         <f aca="false">D170=0</f>
         <v>1</v>
       </c>
@@ -17494,7 +17627,7 @@
         <f aca="false">IF(C171&gt;0,C171,MAX(D170-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E171" s="9" t="b">
+      <c r="E171" s="8" t="b">
         <f aca="false">D171=0</f>
         <v>1</v>
       </c>
@@ -17517,7 +17650,7 @@
         <f aca="false">IF(C172&gt;0,C172,MAX(D171-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E172" s="9" t="b">
+      <c r="E172" s="8" t="b">
         <f aca="false">D172=0</f>
         <v>1</v>
       </c>
@@ -17540,7 +17673,7 @@
         <f aca="false">IF(C173&gt;0,C173,MAX(D172-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E173" s="9" t="b">
+      <c r="E173" s="8" t="b">
         <f aca="false">D173=0</f>
         <v>1</v>
       </c>
@@ -17563,7 +17696,7 @@
         <f aca="false">IF(C174&gt;0,C174,MAX(D173-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E174" s="9" t="b">
+      <c r="E174" s="8" t="b">
         <f aca="false">D174=0</f>
         <v>1</v>
       </c>
@@ -17586,7 +17719,7 @@
         <f aca="false">IF(C175&gt;0,C175,MAX(D174-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E175" s="9" t="b">
+      <c r="E175" s="8" t="b">
         <f aca="false">D175=0</f>
         <v>1</v>
       </c>
@@ -17609,7 +17742,7 @@
         <f aca="false">IF(C176&gt;0,C176,MAX(D175-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E176" s="9" t="b">
+      <c r="E176" s="8" t="b">
         <f aca="false">D176=0</f>
         <v>1</v>
       </c>
@@ -17632,7 +17765,7 @@
         <f aca="false">IF(C177&gt;0,C177,MAX(D176-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E177" s="9" t="b">
+      <c r="E177" s="8" t="b">
         <f aca="false">D177=0</f>
         <v>1</v>
       </c>
@@ -17655,7 +17788,7 @@
         <f aca="false">IF(C178&gt;0,C178,MAX(D177-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E178" s="9" t="b">
+      <c r="E178" s="8" t="b">
         <f aca="false">D178=0</f>
         <v>1</v>
       </c>
@@ -17678,7 +17811,7 @@
         <f aca="false">IF(C179&gt;0,C179,MAX(D178-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E179" s="9" t="b">
+      <c r="E179" s="8" t="b">
         <f aca="false">D179=0</f>
         <v>1</v>
       </c>
@@ -17701,7 +17834,7 @@
         <f aca="false">IF(C180&gt;0,C180,MAX(D179-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E180" s="9" t="b">
+      <c r="E180" s="8" t="b">
         <f aca="false">D180=0</f>
         <v>1</v>
       </c>
@@ -17724,7 +17857,7 @@
         <f aca="false">IF(C181&gt;0,C181,MAX(D180-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E181" s="9" t="b">
+      <c r="E181" s="8" t="b">
         <f aca="false">D181=0</f>
         <v>1</v>
       </c>
@@ -17747,7 +17880,7 @@
         <f aca="false">IF(C182&gt;0,C182,MAX(D181-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E182" s="9" t="b">
+      <c r="E182" s="8" t="b">
         <f aca="false">D182=0</f>
         <v>1</v>
       </c>
@@ -17770,7 +17903,7 @@
         <f aca="false">IF(C183&gt;0,C183,MAX(D182-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E183" s="9" t="b">
+      <c r="E183" s="8" t="b">
         <f aca="false">D183=0</f>
         <v>1</v>
       </c>
@@ -17793,7 +17926,7 @@
         <f aca="false">IF(C184&gt;0,C184,MAX(D183-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E184" s="9" t="b">
+      <c r="E184" s="8" t="b">
         <f aca="false">D184=0</f>
         <v>1</v>
       </c>
@@ -17816,7 +17949,7 @@
         <f aca="false">IF(C185&gt;0,C185,MAX(D184-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E185" s="9" t="b">
+      <c r="E185" s="8" t="b">
         <f aca="false">D185=0</f>
         <v>1</v>
       </c>
@@ -17839,7 +17972,7 @@
         <f aca="false">IF(C186&gt;0,C186,MAX(D185-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E186" s="9" t="b">
+      <c r="E186" s="8" t="b">
         <f aca="false">D186=0</f>
         <v>1</v>
       </c>
@@ -17862,7 +17995,7 @@
         <f aca="false">IF(C187&gt;0,C187,MAX(D186-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E187" s="9" t="b">
+      <c r="E187" s="8" t="b">
         <f aca="false">D187=0</f>
         <v>1</v>
       </c>
@@ -17885,7 +18018,7 @@
         <f aca="false">IF(C188&gt;0,C188,MAX(D187-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E188" s="9" t="b">
+      <c r="E188" s="8" t="b">
         <f aca="false">D188=0</f>
         <v>1</v>
       </c>
@@ -17908,7 +18041,7 @@
         <f aca="false">IF(C189&gt;0,C189,MAX(D188-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E189" s="9" t="b">
+      <c r="E189" s="8" t="b">
         <f aca="false">D189=0</f>
         <v>1</v>
       </c>
@@ -17931,7 +18064,7 @@
         <f aca="false">IF(C190&gt;0,C190,MAX(D189-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E190" s="9" t="b">
+      <c r="E190" s="8" t="b">
         <f aca="false">D190=0</f>
         <v>1</v>
       </c>
@@ -17954,7 +18087,7 @@
         <f aca="false">IF(C191&gt;0,C191,MAX(D190-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E191" s="9" t="b">
+      <c r="E191" s="8" t="b">
         <f aca="false">D191=0</f>
         <v>1</v>
       </c>
@@ -17977,7 +18110,7 @@
         <f aca="false">IF(C192&gt;0,C192,MAX(D191-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E192" s="9" t="b">
+      <c r="E192" s="8" t="b">
         <f aca="false">D192=0</f>
         <v>1</v>
       </c>
@@ -18000,7 +18133,7 @@
         <f aca="false">IF(C193&gt;0,C193,MAX(D192-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E193" s="9" t="b">
+      <c r="E193" s="8" t="b">
         <f aca="false">D193=0</f>
         <v>1</v>
       </c>
@@ -18023,7 +18156,7 @@
         <f aca="false">IF(C194&gt;0,C194,MAX(D193-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E194" s="9" t="b">
+      <c r="E194" s="8" t="b">
         <f aca="false">D194=0</f>
         <v>1</v>
       </c>
@@ -18046,7 +18179,7 @@
         <f aca="false">IF(C195&gt;0,C195,MAX(D194-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E195" s="9" t="b">
+      <c r="E195" s="8" t="b">
         <f aca="false">D195=0</f>
         <v>1</v>
       </c>
@@ -18069,7 +18202,7 @@
         <f aca="false">IF(C196&gt;0,C196,MAX(D195-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E196" s="9" t="b">
+      <c r="E196" s="8" t="b">
         <f aca="false">D196=0</f>
         <v>1</v>
       </c>
@@ -18092,7 +18225,7 @@
         <f aca="false">IF(C197&gt;0,C197,MAX(D196-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E197" s="9" t="b">
+      <c r="E197" s="8" t="b">
         <f aca="false">D197=0</f>
         <v>1</v>
       </c>
@@ -18115,7 +18248,7 @@
         <f aca="false">IF(C198&gt;0,C198,MAX(D197-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E198" s="9" t="b">
+      <c r="E198" s="8" t="b">
         <f aca="false">D198=0</f>
         <v>1</v>
       </c>
@@ -18138,7 +18271,7 @@
         <f aca="false">IF(C199&gt;0,C199,MAX(D198-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E199" s="9" t="b">
+      <c r="E199" s="8" t="b">
         <f aca="false">D199=0</f>
         <v>1</v>
       </c>
@@ -18161,7 +18294,7 @@
         <f aca="false">IF(C200&gt;0,C200,MAX(D199-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E200" s="9" t="b">
+      <c r="E200" s="8" t="b">
         <f aca="false">D200=0</f>
         <v>1</v>
       </c>
@@ -18184,7 +18317,7 @@
         <f aca="false">IF(C201&gt;0,C201,MAX(D200-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E201" s="9" t="b">
+      <c r="E201" s="8" t="b">
         <f aca="false">D201=0</f>
         <v>1</v>
       </c>
@@ -18207,7 +18340,7 @@
         <f aca="false">IF(C202&gt;0,C202,MAX(D201-1,0))</f>
         <v>4</v>
       </c>
-      <c r="E202" s="9" t="b">
+      <c r="E202" s="8" t="b">
         <f aca="false">D202=0</f>
         <v>0</v>
       </c>
@@ -18230,7 +18363,7 @@
         <f aca="false">IF(C203&gt;0,C203,MAX(D202-1,0))</f>
         <v>3</v>
       </c>
-      <c r="E203" s="9" t="b">
+      <c r="E203" s="8" t="b">
         <f aca="false">D203=0</f>
         <v>0</v>
       </c>
@@ -18253,7 +18386,7 @@
         <f aca="false">IF(C204&gt;0,C204,MAX(D203-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E204" s="9" t="b">
+      <c r="E204" s="8" t="b">
         <f aca="false">D204=0</f>
         <v>0</v>
       </c>
@@ -18276,7 +18409,7 @@
         <f aca="false">IF(C205&gt;0,C205,MAX(D204-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E205" s="9" t="b">
+      <c r="E205" s="8" t="b">
         <f aca="false">D205=0</f>
         <v>0</v>
       </c>
@@ -18299,7 +18432,7 @@
         <f aca="false">IF(C206&gt;0,C206,MAX(D205-1,0))</f>
         <v>4</v>
       </c>
-      <c r="E206" s="9" t="b">
+      <c r="E206" s="8" t="b">
         <f aca="false">D206=0</f>
         <v>0</v>
       </c>
@@ -18322,7 +18455,7 @@
         <f aca="false">IF(C207&gt;0,C207,MAX(D206-1,0))</f>
         <v>3</v>
       </c>
-      <c r="E207" s="9" t="b">
+      <c r="E207" s="8" t="b">
         <f aca="false">D207=0</f>
         <v>0</v>
       </c>
@@ -18345,7 +18478,7 @@
         <f aca="false">IF(C208&gt;0,C208,MAX(D207-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E208" s="9" t="b">
+      <c r="E208" s="8" t="b">
         <f aca="false">D208=0</f>
         <v>0</v>
       </c>
@@ -18368,7 +18501,7 @@
         <f aca="false">IF(C209&gt;0,C209,MAX(D208-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E209" s="9" t="b">
+      <c r="E209" s="8" t="b">
         <f aca="false">D209=0</f>
         <v>0</v>
       </c>
@@ -18391,7 +18524,7 @@
         <f aca="false">IF(C210&gt;0,C210,MAX(D209-1,0))</f>
         <v>4</v>
       </c>
-      <c r="E210" s="9" t="b">
+      <c r="E210" s="8" t="b">
         <f aca="false">D210=0</f>
         <v>0</v>
       </c>
@@ -18414,7 +18547,7 @@
         <f aca="false">IF(C211&gt;0,C211,MAX(D210-1,0))</f>
         <v>3</v>
       </c>
-      <c r="E211" s="9" t="b">
+      <c r="E211" s="8" t="b">
         <f aca="false">D211=0</f>
         <v>0</v>
       </c>
@@ -18437,7 +18570,7 @@
         <f aca="false">IF(C212&gt;0,C212,MAX(D211-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E212" s="9" t="b">
+      <c r="E212" s="8" t="b">
         <f aca="false">D212=0</f>
         <v>0</v>
       </c>
@@ -18460,7 +18593,7 @@
         <f aca="false">IF(C213&gt;0,C213,MAX(D212-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E213" s="9" t="b">
+      <c r="E213" s="8" t="b">
         <f aca="false">D213=0</f>
         <v>0</v>
       </c>
@@ -18483,7 +18616,7 @@
         <f aca="false">IF(C214&gt;0,C214,MAX(D213-1,0))</f>
         <v>4</v>
       </c>
-      <c r="E214" s="9" t="b">
+      <c r="E214" s="8" t="b">
         <f aca="false">D214=0</f>
         <v>0</v>
       </c>
@@ -18506,7 +18639,7 @@
         <f aca="false">IF(C215&gt;0,C215,MAX(D214-1,0))</f>
         <v>3</v>
       </c>
-      <c r="E215" s="9" t="b">
+      <c r="E215" s="8" t="b">
         <f aca="false">D215=0</f>
         <v>0</v>
       </c>
@@ -18529,7 +18662,7 @@
         <f aca="false">IF(C216&gt;0,C216,MAX(D215-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E216" s="9" t="b">
+      <c r="E216" s="8" t="b">
         <f aca="false">D216=0</f>
         <v>0</v>
       </c>
@@ -18552,7 +18685,7 @@
         <f aca="false">IF(C217&gt;0,C217,MAX(D216-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E217" s="9" t="b">
+      <c r="E217" s="8" t="b">
         <f aca="false">D217=0</f>
         <v>0</v>
       </c>
@@ -18575,7 +18708,7 @@
         <f aca="false">IF(C218&gt;0,C218,MAX(D217-1,0))</f>
         <v>4</v>
       </c>
-      <c r="E218" s="9" t="b">
+      <c r="E218" s="8" t="b">
         <f aca="false">D218=0</f>
         <v>0</v>
       </c>
@@ -18598,7 +18731,7 @@
         <f aca="false">IF(C219&gt;0,C219,MAX(D218-1,0))</f>
         <v>3</v>
       </c>
-      <c r="E219" s="9" t="b">
+      <c r="E219" s="8" t="b">
         <f aca="false">D219=0</f>
         <v>0</v>
       </c>
@@ -18621,7 +18754,7 @@
         <f aca="false">IF(C220&gt;0,C220,MAX(D219-1,0))</f>
         <v>2</v>
       </c>
-      <c r="E220" s="9" t="b">
+      <c r="E220" s="8" t="b">
         <f aca="false">D220=0</f>
         <v>0</v>
       </c>
@@ -18644,7 +18777,7 @@
         <f aca="false">IF(C221&gt;0,C221,MAX(D220-1,0))</f>
         <v>1</v>
       </c>
-      <c r="E221" s="9" t="b">
+      <c r="E221" s="8" t="b">
         <f aca="false">D221=0</f>
         <v>0</v>
       </c>
@@ -18667,7 +18800,7 @@
         <f aca="false">IF(C222&gt;0,C222,MAX(D221-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E222" s="9" t="b">
+      <c r="E222" s="8" t="b">
         <f aca="false">D222=0</f>
         <v>1</v>
       </c>
@@ -18690,7 +18823,7 @@
         <f aca="false">IF(C223&gt;0,C223,MAX(D222-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E223" s="9" t="b">
+      <c r="E223" s="8" t="b">
         <f aca="false">D223=0</f>
         <v>1</v>
       </c>
@@ -18713,7 +18846,7 @@
         <f aca="false">IF(C224&gt;0,C224,MAX(D223-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E224" s="9" t="b">
+      <c r="E224" s="8" t="b">
         <f aca="false">D224=0</f>
         <v>1</v>
       </c>
@@ -18736,7 +18869,7 @@
         <f aca="false">IF(C225&gt;0,C225,MAX(D224-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E225" s="9" t="b">
+      <c r="E225" s="8" t="b">
         <f aca="false">D225=0</f>
         <v>1</v>
       </c>
@@ -18759,7 +18892,7 @@
         <f aca="false">IF(C226&gt;0,C226,MAX(D225-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E226" s="9" t="b">
+      <c r="E226" s="8" t="b">
         <f aca="false">D226=0</f>
         <v>1</v>
       </c>
@@ -18782,7 +18915,7 @@
         <f aca="false">IF(C227&gt;0,C227,MAX(D226-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E227" s="9" t="b">
+      <c r="E227" s="8" t="b">
         <f aca="false">D227=0</f>
         <v>1</v>
       </c>
@@ -18805,7 +18938,7 @@
         <f aca="false">IF(C228&gt;0,C228,MAX(D227-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E228" s="9" t="b">
+      <c r="E228" s="8" t="b">
         <f aca="false">D228=0</f>
         <v>1</v>
       </c>
@@ -18828,7 +18961,7 @@
         <f aca="false">IF(C229&gt;0,C229,MAX(D228-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E229" s="9" t="b">
+      <c r="E229" s="8" t="b">
         <f aca="false">D229=0</f>
         <v>1</v>
       </c>
@@ -18851,7 +18984,7 @@
         <f aca="false">IF(C230&gt;0,C230,MAX(D229-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E230" s="9" t="b">
+      <c r="E230" s="8" t="b">
         <f aca="false">D230=0</f>
         <v>1</v>
       </c>
@@ -18874,7 +19007,7 @@
         <f aca="false">IF(C231&gt;0,C231,MAX(D230-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E231" s="9" t="b">
+      <c r="E231" s="8" t="b">
         <f aca="false">D231=0</f>
         <v>1</v>
       </c>
@@ -18897,7 +19030,7 @@
         <f aca="false">IF(C232&gt;0,C232,MAX(D231-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E232" s="9" t="b">
+      <c r="E232" s="8" t="b">
         <f aca="false">D232=0</f>
         <v>1</v>
       </c>
@@ -18920,7 +19053,7 @@
         <f aca="false">IF(C233&gt;0,C233,MAX(D232-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E233" s="9" t="b">
+      <c r="E233" s="8" t="b">
         <f aca="false">D233=0</f>
         <v>1</v>
       </c>
@@ -18943,7 +19076,7 @@
         <f aca="false">IF(C234&gt;0,C234,MAX(D233-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E234" s="9" t="b">
+      <c r="E234" s="8" t="b">
         <f aca="false">D234=0</f>
         <v>1</v>
       </c>
@@ -18966,7 +19099,7 @@
         <f aca="false">IF(C235&gt;0,C235,MAX(D234-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E235" s="9" t="b">
+      <c r="E235" s="8" t="b">
         <f aca="false">D235=0</f>
         <v>1</v>
       </c>
@@ -18989,7 +19122,7 @@
         <f aca="false">IF(C236&gt;0,C236,MAX(D235-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E236" s="9" t="b">
+      <c r="E236" s="8" t="b">
         <f aca="false">D236=0</f>
         <v>1</v>
       </c>
@@ -19012,7 +19145,7 @@
         <f aca="false">IF(C237&gt;0,C237,MAX(D236-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E237" s="9" t="b">
+      <c r="E237" s="8" t="b">
         <f aca="false">D237=0</f>
         <v>1</v>
       </c>
@@ -19035,7 +19168,7 @@
         <f aca="false">IF(C238&gt;0,C238,MAX(D237-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E238" s="9" t="b">
+      <c r="E238" s="8" t="b">
         <f aca="false">D238=0</f>
         <v>1</v>
       </c>
@@ -19058,7 +19191,7 @@
         <f aca="false">IF(C239&gt;0,C239,MAX(D238-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E239" s="9" t="b">
+      <c r="E239" s="8" t="b">
         <f aca="false">D239=0</f>
         <v>1</v>
       </c>
@@ -19081,7 +19214,7 @@
         <f aca="false">IF(C240&gt;0,C240,MAX(D239-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E240" s="9" t="b">
+      <c r="E240" s="8" t="b">
         <f aca="false">D240=0</f>
         <v>1</v>
       </c>
@@ -19104,7 +19237,7 @@
         <f aca="false">IF(C241&gt;0,C241,MAX(D240-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E241" s="9" t="b">
+      <c r="E241" s="8" t="b">
         <f aca="false">D241=0</f>
         <v>1</v>
       </c>
@@ -19127,7 +19260,7 @@
         <f aca="false">IF(C242&gt;0,C242,MAX(D241-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E242" s="9" t="b">
+      <c r="E242" s="8" t="b">
         <f aca="false">D242=0</f>
         <v>1</v>
       </c>
@@ -19150,7 +19283,7 @@
         <f aca="false">IF(C243&gt;0,C243,MAX(D242-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E243" s="9" t="b">
+      <c r="E243" s="8" t="b">
         <f aca="false">D243=0</f>
         <v>1</v>
       </c>
@@ -19173,7 +19306,7 @@
         <f aca="false">IF(C244&gt;0,C244,MAX(D243-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E244" s="9" t="b">
+      <c r="E244" s="8" t="b">
         <f aca="false">D244=0</f>
         <v>1</v>
       </c>
@@ -19196,7 +19329,7 @@
         <f aca="false">IF(C245&gt;0,C245,MAX(D244-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E245" s="9" t="b">
+      <c r="E245" s="8" t="b">
         <f aca="false">D245=0</f>
         <v>1</v>
       </c>
@@ -19219,7 +19352,7 @@
         <f aca="false">IF(C246&gt;0,C246,MAX(D245-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E246" s="9" t="b">
+      <c r="E246" s="8" t="b">
         <f aca="false">D246=0</f>
         <v>1</v>
       </c>
@@ -19242,7 +19375,7 @@
         <f aca="false">IF(C247&gt;0,C247,MAX(D246-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E247" s="9" t="b">
+      <c r="E247" s="8" t="b">
         <f aca="false">D247=0</f>
         <v>1</v>
       </c>
@@ -19265,7 +19398,7 @@
         <f aca="false">IF(C248&gt;0,C248,MAX(D247-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E248" s="9" t="b">
+      <c r="E248" s="8" t="b">
         <f aca="false">D248=0</f>
         <v>1</v>
       </c>
@@ -19288,7 +19421,7 @@
         <f aca="false">IF(C249&gt;0,C249,MAX(D248-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E249" s="9" t="b">
+      <c r="E249" s="8" t="b">
         <f aca="false">D249=0</f>
         <v>1</v>
       </c>
@@ -19311,7 +19444,7 @@
         <f aca="false">IF(C250&gt;0,C250,MAX(D249-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E250" s="9" t="b">
+      <c r="E250" s="8" t="b">
         <f aca="false">D250=0</f>
         <v>1</v>
       </c>
@@ -19334,7 +19467,7 @@
         <f aca="false">IF(C251&gt;0,C251,MAX(D250-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E251" s="9" t="b">
+      <c r="E251" s="8" t="b">
         <f aca="false">D251=0</f>
         <v>1</v>
       </c>
@@ -19357,7 +19490,7 @@
         <f aca="false">IF(C252&gt;0,C252,MAX(D251-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E252" s="9" t="b">
+      <c r="E252" s="8" t="b">
         <f aca="false">D252=0</f>
         <v>1</v>
       </c>
@@ -19380,7 +19513,7 @@
         <f aca="false">IF(C253&gt;0,C253,MAX(D252-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E253" s="9" t="b">
+      <c r="E253" s="8" t="b">
         <f aca="false">D253=0</f>
         <v>1</v>
       </c>
@@ -19403,7 +19536,7 @@
         <f aca="false">IF(C254&gt;0,C254,MAX(D253-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E254" s="9" t="b">
+      <c r="E254" s="8" t="b">
         <f aca="false">D254=0</f>
         <v>1</v>
       </c>
@@ -19426,7 +19559,7 @@
         <f aca="false">IF(C255&gt;0,C255,MAX(D254-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E255" s="9" t="b">
+      <c r="E255" s="8" t="b">
         <f aca="false">D255=0</f>
         <v>1</v>
       </c>
@@ -19449,7 +19582,7 @@
         <f aca="false">IF(C256&gt;0,C256,MAX(D255-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E256" s="9" t="b">
+      <c r="E256" s="8" t="b">
         <f aca="false">D256=0</f>
         <v>1</v>
       </c>
@@ -19472,7 +19605,7 @@
         <f aca="false">IF(C257&gt;0,C257,MAX(D256-1,0))</f>
         <v>0</v>
       </c>
-      <c r="E257" s="9" t="b">
+      <c r="E257" s="8" t="b">
         <f aca="false">D257=0</f>
         <v>1</v>
       </c>
@@ -19581,7 +19714,7 @@
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="3" t="s">
         <v>384</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -19602,9 +19735,9 @@
         <v>340</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>385</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -19621,7 +19754,7 @@
       <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="3" t="s">
         <v>386</v>
       </c>
     </row>
@@ -19630,9 +19763,9 @@
         <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>387</v>
       </c>
     </row>
@@ -19643,7 +19776,7 @@
       <c r="E7" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="3" t="s">
         <v>388</v>
       </c>
     </row>
@@ -19654,7 +19787,7 @@
       <c r="E8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="3" t="s">
         <v>389</v>
       </c>
     </row>
@@ -19665,7 +19798,7 @@
       <c r="E9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="3" t="s">
         <v>390</v>
       </c>
     </row>
@@ -19676,7 +19809,7 @@
       <c r="E10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="3" t="s">
         <v>391</v>
       </c>
     </row>
@@ -19684,7 +19817,7 @@
       <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="3" t="s">
         <v>392</v>
       </c>
     </row>
@@ -19692,7 +19825,7 @@
       <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="3" t="s">
         <v>393</v>
       </c>
     </row>
@@ -19761,4 +19894,322 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:F22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.54"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="12"/>
+      <c r="C4" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="E15:F18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:F22"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>